<commit_message>
remove old commented out code
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4483B5C1-7ACF-48EB-A23B-ABC2B4B1A103}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E2D17A-D99F-43EB-B9B1-267213C107EF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="10635" activeTab="2" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="87">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -2265,6 +2265,15 @@
   </si>
   <si>
     <t>from PhotoPlaybackWidget.js:</t>
+  </si>
+  <si>
+    <t>I'll do for photos myself, then let T fill in for video.</t>
+  </si>
+  <si>
+    <t>Make generic function to find correct width/height for given panel &amp; aspect ratio</t>
+  </si>
+  <si>
+    <t>This will be used for both setting IMG/YT element dimensions and for setting photo request width</t>
   </si>
 </sst>
 </file>
@@ -2477,7 +2486,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2555,6 +2564,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3421,72 +3433,76 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267B328E-A616-48A5-B37D-5A675A5748D9}">
-  <dimension ref="A1:A51"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="109.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>52</v>
       </c>
@@ -3544,78 +3560,86 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="28"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C38" s="30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C39" s="30"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C40" s="30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C41" s="30"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="28"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="27" t="s">
         <v>80</v>
       </c>
@@ -3636,6 +3660,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C38:C39"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed problem caused by Dojo register include
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9636856-9373-43D3-B051-053F52E5EFF2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8390CFF0-3F88-49B9-B36D-AB0870995500}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="10635" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="10635" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="to do" sheetId="1" r:id="rId1"/>
-    <sheet name="dgrid reorder" sheetId="6" r:id="rId2"/>
-    <sheet name="resize imagery on splitter drag" sheetId="7" r:id="rId3"/>
+    <sheet name="extent history" sheetId="8" r:id="rId2"/>
+    <sheet name="dgrid reorder" sheetId="6" r:id="rId3"/>
+    <sheet name="resize imagery on splitter drag" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'to do'!$A$1:$H$31</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="143">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -2278,12 +2279,2895 @@
   <si>
     <t>Settings panel</t>
   </si>
+  <si>
+    <t>/* For extent history and prev/next extent navigation*/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">var </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">prevNextBtnsHtml </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"&lt;img id='btn_prevExtent' src='assets/images/backward.png' onclick='</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>gotoSavedExtent</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(-1)' title='Click to go to previous extent' height='32px' width='32px' /&gt;&lt;hr&gt;"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">prevNextBtnsHtml </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">+= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"&lt;img id='btn_nextExtent' src='assets/images/forward.png' onclick='</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>gotoSavedExtent</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(1)' title='Click to go to next extent in history' height='32px' width='32px' style='opacity: 0.2' /&gt;"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">var </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">savedExtentsWidget </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">var </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">bookmarkSelected </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">var </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">currentBookmarkNumber </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>= -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">function </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>gotoSavedExtent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(offset) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">var </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">l </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>savedExtentsWidget</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.bookmarks.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">currentBookmarkNumber </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>=== -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">currentBookmarkNumber </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">l </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">var </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">n </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">currentBookmarkNumber </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>+ offset;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">0 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">&amp;&amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF808080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>//</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF0073BF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>TODO: handle this:  Uncaught Error: li had a span child removed, but there is now more than one. You must add unique key properties to make them distinguishable.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF808080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>//savedExtentsWidget.bookmarks.items[currentBookmarkNumber].thumbnail = "";</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    //savedExtentsWidget.bookmarks.items[n].thumbnail = "assets/images/w_right_green.png";</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">var </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">currentBookmark </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>savedExtentsWidget</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.bookmarks.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>items</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>];</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF808080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>//currentBookmark.thumbnail.url = "assets/images/w_right_green.png";</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>savedExtentsWidget</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.goTo(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>currentBookmark</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">var </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">prevButton </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>getEl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"btn_prevExtent"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">var </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">nextButton </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>getEl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"btn_nextExtent"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>prevButton</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>style</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">opacity </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>nextButton</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>style</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">opacity </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">n </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">=== </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>prevButton</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>style</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">opacity </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">n </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">=== </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">l </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>nextButton</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>style</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">opacity </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">currentBookmarkNumber </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  }</t>
+  </si>
+  <si>
+    <t>GlobalVars.js</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">var </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">prevNextBtnsDiv </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>document</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7A7A43"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>createElement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"DIV"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>prevNextBtnsDiv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">innerHTML </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>prevNextBtnsHtml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>view</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.ui.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7A7A43"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>add</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>prevNextBtnsDiv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"top-left"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">savedExtentsWidget </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>Bookmarks({</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>view</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>view</t>
+    </r>
+  </si>
+  <si>
+    <t>});</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">var </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">savedExtentsExpand </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>Expand({</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>expandIconClass</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"esri-icon-collection"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">,  </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF808080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>// see https://developers.arcgis.com/javascript/latest/guide/esri-icon-font/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>expandTooltip</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Show extents history"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF808080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>// optional, defaults to "Expand" for English locale</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>view</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>view</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>content</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>savedExtentsWidget</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>view</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.ui.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7A7A43"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>add</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>savedExtentsExpand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>, {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>position</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"top-left"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>savedExtentsWidget</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.on(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"select-bookmark"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(event){</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">currentBookmarkNumber </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>parseInt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(event.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>target</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.activeBookmark.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7A7A43"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>split</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>)[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>]);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">bookmarkSelected </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>MapStuffWidget.js</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>bookmarkSelected</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">bookmarkSelected </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>return</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">var </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">km </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>Math</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7A7A43"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>round</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(newExtent.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>" km"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">var </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">bookmark </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>Bookmark({</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>savedExtentsWidget</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.bookmarks.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>items</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">length </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">+ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">":" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>km</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>extent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>: newExtent});</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF808080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>//bookmark.thumbnail = "assets/images/noaa_wb.png";</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>savedExtentsWidget</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.bookmarks.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7A7A43"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>add</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF458383"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>bookmark</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">currentBookmarkNumber </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>savedExtentsWidget</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.bookmarks.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">length </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MapStuffWidget.js  (handleExtentChange </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2447,6 +5331,28 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF008000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF0073BF"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2489,7 +5395,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2570,6 +5476,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3102,7 +6041,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -3330,6 +6269,350 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE45D646-5865-4DD3-B066-A6FB8031C09E}">
+  <dimension ref="A1:A74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="112.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="35" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="35" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="35" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="38" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="37" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="34"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="34"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="35" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="37" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="37" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="35" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="35" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="35" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="35" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="35" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCD9E72-3AC1-432D-84D6-99D2A7F07F80}">
   <dimension ref="A2:H42"/>
   <sheetViews>
@@ -3439,7 +6722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267B328E-A616-48A5-B37D-5A675A5748D9}">
   <dimension ref="A1:C51"/>
   <sheetViews>

</xml_diff>

<commit_message>
Can now sort Units table by column without messing up links to graphic features
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8390CFF0-3F88-49B9-B36D-AB0870995500}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A42E903-7CF7-4317-82A2-E127A95B972D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="10635" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="10635" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="to do" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="resize imagery on splitter drag" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'to do'!$A$1:$H$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'to do'!$A$1:$H$32</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="144">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -5161,6 +5161,9 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>Generalize QueryBasedTablePanelWidget, so not specific to SZ Units</t>
   </si>
 </sst>
 </file>
@@ -5474,9 +5477,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -5509,6 +5509,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -6039,10 +6042,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6126,9 +6129,12 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>42</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>6</v>
@@ -6154,91 +6160,97 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="D12" s="15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="15" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="19" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D16" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D17" s="15" t="s">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D18" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D20" s="15" t="s">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D21" s="15" t="s">
         <v>21</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>26</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="D22" s="15" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="15" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D23" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="2" t="s">
+      <c r="H23" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D26" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D28" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D28" s="15" t="s">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D29" s="15" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -6246,16 +6258,27 @@
         <v>42</v>
       </c>
       <c r="D31" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="15" t="s">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="15" t="s">
         <v>87</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H31" xr:uid="{FA7CAD96-383D-486D-B6C7-EAC38E698684}">
+  <autoFilter ref="A1:H32" xr:uid="{FA7CAD96-383D-486D-B6C7-EAC38E698684}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
@@ -6272,7 +6295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE45D646-5865-4DD3-B066-A6FB8031C09E}">
   <dimension ref="A1:A74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -6288,103 +6311,103 @@
     </row>
     <row r="2" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="32" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="32" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
+      <c r="A6" s="32"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="32" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="39" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="40" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="34" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="36" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="36" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="34" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="34" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="32" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="34" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="34" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
+      <c r="A19" s="33"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="38" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="34" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="34" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="34" t="s">
         <v>122</v>
       </c>
     </row>
@@ -6395,52 +6418,52 @@
     </row>
     <row r="28" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="34" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="34" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="34" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="34" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="34" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="34" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="38" t="s">
+      <c r="A35" s="37" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="37" t="s">
+      <c r="A36" s="36" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="34" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="34" t="s">
         <v>51</v>
       </c>
     </row>
@@ -6451,158 +6474,158 @@
     </row>
     <row r="42" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="30" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="31" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="32" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="34"/>
+      <c r="A46" s="33"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="32" t="s">
+      <c r="A47" s="31" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="32" t="s">
+      <c r="A48" s="31" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="32" t="s">
+      <c r="A49" s="31" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="34"/>
+      <c r="A50" s="33"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="32" t="s">
+      <c r="A51" s="31" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="35" t="s">
+      <c r="A52" s="34" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="35" t="s">
+      <c r="A53" s="34" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="35" t="s">
+      <c r="A54" s="34" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="34" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="34" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="34" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="36" t="s">
+      <c r="A58" s="35" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="37" t="s">
+      <c r="A59" s="36" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="37" t="s">
+      <c r="A60" s="36" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="35" t="s">
+      <c r="A61" s="34" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="37" t="s">
+      <c r="A62" s="36" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="35" t="s">
+      <c r="A63" s="34" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="35" t="s">
+      <c r="A64" s="34" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="35" t="s">
+      <c r="A65" s="34" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="35" t="s">
+      <c r="A66" s="34" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="35" t="s">
+      <c r="A67" s="34" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="35" t="s">
+      <c r="A68" s="34" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="35" t="s">
+      <c r="A69" s="34" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="35" t="s">
+      <c r="A70" s="34" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="35" t="s">
+      <c r="A71" s="34" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="35" t="s">
+      <c r="A72" s="34" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="35" t="s">
+      <c r="A73" s="34" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="37" t="s">
+      <c r="A74" s="36" t="s">
         <v>88</v>
       </c>
     </row>
@@ -6878,7 +6901,7 @@
       <c r="A38" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="41" t="s">
         <v>84</v>
       </c>
     </row>
@@ -6886,13 +6909,13 @@
       <c r="A39" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="30"/>
+      <c r="C39" s="41"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="30" t="s">
+      <c r="C40" s="41" t="s">
         <v>85</v>
       </c>
     </row>
@@ -6900,7 +6923,7 @@
       <c r="A41" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="C41" s="30"/>
+      <c r="C41" s="41"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">

</xml_diff>

<commit_message>
sort Units table by column: Generalize, so it works with Fish Atlas tables
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A42E903-7CF7-4317-82A2-E127A95B972D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A26C2C3-57A2-4F88-86CA-AA52F4A6F81F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="10635" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="144">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -6045,7 +6045,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6168,8 +6168,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="15" t="s">

</xml_diff>

<commit_message>
Add zoom-in to Fish Atlas table entries
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A26C2C3-57A2-4F88-86CA-AA52F4A6F81F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356B5E82-88A1-4E45-BED2-59618C966200}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="10635" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="resize imagery on splitter drag" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'to do'!$A$1:$H$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'to do'!$A$1:$H$35</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="147">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t>Steve request</t>
-  </si>
-  <si>
-    <t>4.9 API update</t>
   </si>
   <si>
     <t>check Python code for remaining ArcGIS functions</t>
@@ -289,9 +286,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>problems using this version</t>
-  </si>
-  <si>
     <t>TS</t>
   </si>
   <si>
@@ -5164,6 +5158,21 @@
   </si>
   <si>
     <t>Generalize QueryBasedTablePanelWidget, so not specific to SZ Units</t>
+  </si>
+  <si>
+    <t>Steve request.  Instead, JN made them smaller, so you can still see which points are selected when not using autoRefresh</t>
+  </si>
+  <si>
+    <t>JN:  I think the API now adjusts positioning of popups so they don't force an extent change</t>
+  </si>
+  <si>
+    <t>Graphics objects are now limited minimal pixel spacing, set in website settings panel</t>
+  </si>
+  <si>
+    <t>minimal pixel distance for video points, like for photos?</t>
+  </si>
+  <si>
+    <t>Useful now that points can be queried at greater extents</t>
   </si>
 </sst>
 </file>
@@ -5398,7 +5407,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5512,6 +5521,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -6045,7 +6060,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6055,8 +6070,8 @@
     <col min="4" max="4" width="69" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.5" style="15" customWidth="1"/>
     <col min="6" max="6" width="37.75" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.25" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.25" style="15" customWidth="1"/>
+    <col min="7" max="7" width="5.75" style="15" customWidth="1"/>
+    <col min="8" max="8" width="55.875" style="42" customWidth="1"/>
     <col min="9" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
@@ -6076,24 +6091,25 @@
       <c r="F1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>40</v>
+      <c r="H1" s="43" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>12</v>
       </c>
+      <c r="H2" s="18"/>
     </row>
     <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>11</v>
@@ -6104,17 +6120,19 @@
       <c r="G4" s="15" t="s">
         <v>9</v>
       </c>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>8</v>
       </c>
+      <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -6131,10 +6149,10 @@
     </row>
     <row r="8" spans="1:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>6</v>
@@ -6146,50 +6164,60 @@
         <v>4</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>2</v>
       </c>
+      <c r="H10" s="15"/>
     </row>
     <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>1</v>
       </c>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>143</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="H13" s="18"/>
     </row>
     <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" spans="1:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="D16" s="19" t="s">
         <v>0</v>
+      </c>
+      <c r="H16" s="42" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -6197,91 +6225,98 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="D21" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="42" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="H22" s="42" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="D23" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="H23" s="42" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D24" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="15" t="s">
+      <c r="H24" s="42" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>25</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="H26" s="18"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D29" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C34" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H32" xr:uid="{FA7CAD96-383D-486D-B6C7-EAC38E698684}">
+  <autoFilter ref="A1:H35" xr:uid="{13923B3E-52AC-4114-8064-97A62885AB12}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
@@ -6309,23 +6344,23 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -6333,62 +6368,62 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -6396,99 +6431,99 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="34" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="34" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="37" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="36" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="34" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
@@ -6496,17 +6531,17 @@
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
@@ -6514,122 +6549,122 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="34" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="34" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="34" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="36" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="36" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="34" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -6655,19 +6690,19 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" s="7"/>
     </row>
@@ -6676,10 +6711,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -6690,7 +6725,7 @@
     <row r="9" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -6698,7 +6733,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -6712,7 +6747,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
@@ -6720,7 +6755,7 @@
     </row>
     <row r="31" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -6734,7 +6769,7 @@
     </row>
     <row r="42" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -6764,33 +6799,33 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6798,35 +6833,35 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -6834,67 +6869,67 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -6902,55 +6937,55 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C39" s="41"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C40" s="41" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C41" s="41"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -6958,22 +6993,22 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add select subarea and zoom-in to Fish Atlas table entries
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356B5E82-88A1-4E45-BED2-59618C966200}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2426D24D-9C4F-4F62-826F-47C23580D72A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="10635" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="149">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -5173,6 +5173,12 @@
   </si>
   <si>
     <t>Useful now that points can be queried at greater extents</t>
+  </si>
+  <si>
+    <t>Hide SZ stuff when in FA tab, and vice-versa</t>
+  </si>
+  <si>
+    <t>Things don't work if you start zooming before initial draw of SZ video lines</t>
   </si>
 </sst>
 </file>
@@ -5519,14 +5525,14 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -6057,10 +6063,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6071,7 +6077,7 @@
     <col min="5" max="5" width="4.5" style="15" customWidth="1"/>
     <col min="6" max="6" width="37.75" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.75" style="15" customWidth="1"/>
-    <col min="8" max="8" width="55.875" style="42" customWidth="1"/>
+    <col min="8" max="8" width="55.875" style="41" customWidth="1"/>
     <col min="9" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
@@ -6091,7 +6097,7 @@
       <c r="F1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="42" t="s">
         <v>39</v>
       </c>
     </row>
@@ -6216,60 +6222,63 @@
       <c r="D16" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="41" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D18" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H21" s="42" t="s">
+      <c r="H21" s="41" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="H22" s="42" t="s">
+      <c r="H22" s="41" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="H23" s="42" t="s">
+      <c r="H23" s="41" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>13</v>
+      </c>
       <c r="B24" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H24" s="42" t="s">
+      <c r="H24" s="41" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
         <v>37</v>
       </c>
@@ -6278,7 +6287,7 @@
       </c>
       <c r="H26" s="18"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>40</v>
       </c>
@@ -6286,12 +6295,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D29" s="15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>40</v>
       </c>
@@ -6299,7 +6308,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>40</v>
       </c>
@@ -6307,7 +6316,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="3:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="C34" s="2" t="s">
         <v>37</v>
       </c>
@@ -6315,8 +6324,24 @@
         <v>85</v>
       </c>
     </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H35" xr:uid="{13923B3E-52AC-4114-8064-97A62885AB12}">
+  <autoFilter ref="A1:H35" xr:uid="{046495F1-3543-4F8C-98E4-A4049F15EBF9}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
@@ -6939,7 +6964,7 @@
       <c r="A38" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="41" t="s">
+      <c r="C38" s="43" t="s">
         <v>82</v>
       </c>
     </row>
@@ -6947,13 +6972,13 @@
       <c r="A39" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C39" s="41"/>
+      <c r="C39" s="43"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="41" t="s">
+      <c r="C40" s="43" t="s">
         <v>83</v>
       </c>
     </row>
@@ -6961,7 +6986,7 @@
       <c r="A41" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="41"/>
+      <c r="C41" s="43"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">

</xml_diff>

<commit_message>
Added explicit widths for CMECS columns
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2426D24D-9C4F-4F62-826F-47C23580D72A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF76820D-2200-4DFC-9009-B9BE5515D99E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="10635" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="resize imagery on splitter drag" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'to do'!$A$1:$H$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'to do'!$A$1:$I$36</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="161">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -70,9 +70,6 @@
     <t>T</t>
   </si>
   <si>
-    <t>photo: processPicasaData()</t>
-  </si>
-  <si>
     <t>VideoPanelWidget.js, PhotoPlaybackWidget</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>tooltips for video/photo controls</t>
   </si>
   <si>
-    <t>var "speedHTML"</t>
-  </si>
-  <si>
     <t>VideoPanelWidget.js, youtube.js</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
   </si>
   <si>
     <t>Completed by</t>
-  </si>
-  <si>
-    <t>where to look</t>
   </si>
   <si>
     <t>QueryBasedTablePanelWidget.js</t>
@@ -5179,6 +5170,73 @@
   </si>
   <si>
     <t>Things don't work if you start zooming before initial draw of SZ video lines</t>
+  </si>
+  <si>
+    <t>functions</t>
+  </si>
+  <si>
+    <t>files</t>
+  </si>
+  <si>
+    <t>vars</t>
+  </si>
+  <si>
+    <t>speedHTML</t>
+  </si>
+  <si>
+    <t>processPicasaData()</t>
+  </si>
+  <si>
+    <t>Better column widths for tables</t>
+  </si>
+  <si>
+    <t>mapStuffWidget.js</t>
+  </si>
+  <si>
+    <t>faWidget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add width info for columns to specialFormatting property </t>
+  </si>
+  <si>
+    <t>Bug:  Adding TextSymbol to Locales causes problems</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>possible solutions:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  Either change GraphicLayer to FeatureLayer with labelingInfo, or put TextSymbols in separate layer</t>
+    </r>
+  </si>
+  <si>
+    <t>get mouseover of graphic object to highlight row in table</t>
+  </si>
+  <si>
+    <t>QueryBasedPanelWidget</t>
+  </si>
+  <si>
+    <t>makeClickableGraphics</t>
+  </si>
+  <si>
+    <t>textOverlayPars property in faWidget</t>
   </si>
 </sst>
 </file>
@@ -5413,7 +5471,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5533,6 +5591,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -6063,10 +6124,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6076,272 +6137,337 @@
     <col min="4" max="4" width="69" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.5" style="15" customWidth="1"/>
     <col min="6" max="6" width="37.75" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.75" style="15" customWidth="1"/>
-    <col min="8" max="8" width="55.875" style="41" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="15"/>
+    <col min="7" max="7" width="21.625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="20" style="18" customWidth="1"/>
+    <col min="9" max="9" width="55.875" style="41" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="12" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>18</v>
-      </c>
       <c r="D1" s="12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="42" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="15"/>
+      <c r="I2" s="18"/>
+    </row>
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="18"/>
-    </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="I4" s="15"/>
+    </row>
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+    </row>
+    <row r="6" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>11</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="15"/>
-    </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="15"/>
-    </row>
-    <row r="6" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" s="15"/>
+      <c r="I8" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="15"/>
-    </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="15"/>
+    </row>
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="18"/>
-    </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="15"/>
+      <c r="I12" s="18"/>
+    </row>
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="H13" s="15"/>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="H15" s="15"/>
+      <c r="I15" s="18"/>
+    </row>
+    <row r="16" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="41" t="s">
+      <c r="H16" s="15"/>
+      <c r="I16" s="41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="15"/>
+      <c r="I21" s="41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="15"/>
+      <c r="I22" s="41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="I23" s="41" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="2" t="s">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="15"/>
+      <c r="I24" s="41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="15"/>
+      <c r="I26" s="18"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="41" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="2" t="s">
+      <c r="D28" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D29" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="41" t="s">
+      <c r="D31" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H34" s="15"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="15" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="H23" s="41" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="41" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H26" s="18"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D29" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>148</v>
+      <c r="D38" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="I38" s="41" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D40" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="I40" s="41" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D42" s="15" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H35" xr:uid="{046495F1-3543-4F8C-98E4-A4049F15EBF9}">
+  <autoFilter ref="A1:I36" xr:uid="{046495F1-3543-4F8C-98E4-A4049F15EBF9}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
@@ -6369,23 +6495,23 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -6393,62 +6519,62 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -6456,99 +6582,99 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="34" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="34" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="34" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="34" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="34" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="37" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="36" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="34" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="34" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="10" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
@@ -6556,17 +6682,17 @@
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
@@ -6574,122 +6700,122 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="31" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="34" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="34" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="34" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="34" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="34" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="34" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="35" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="36" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="36" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="34" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="36" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="34" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="34" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="34" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="34" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="34" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="34" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="34" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="34" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="34" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="34" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="34" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="36" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -6715,19 +6841,19 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H3" s="7"/>
     </row>
@@ -6736,21 +6862,21 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -6758,7 +6884,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -6772,7 +6898,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
@@ -6780,7 +6906,7 @@
     </row>
     <row r="31" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -6794,7 +6920,7 @@
     </row>
     <row r="42" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -6824,33 +6950,33 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6858,35 +6984,35 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -6894,67 +7020,67 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -6962,55 +7088,55 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C38" s="43" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C39" s="43"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C40" s="43" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C41" s="43"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -7018,22 +7144,22 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="27" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="29" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added envelope info to dropdowns, to allow for zooming to subarea
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF76820D-2200-4DFC-9009-B9BE5515D99E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090C2953-DF8B-46BC-90BF-33A1E796E8FD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="10635" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="resize imagery on splitter drag" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'to do'!$A$1:$I$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'to do'!$A$1:$I$100</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="162">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -5202,31 +5202,6 @@
     <t>Bug:  Adding TextSymbol to Locales causes problems</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>possible solutions:</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  Either change GraphicLayer to FeatureLayer with labelingInfo, or put TextSymbols in separate layer</t>
-    </r>
-  </si>
-  <si>
     <t>get mouseover of graphic object to highlight row in table</t>
   </si>
   <si>
@@ -5237,6 +5212,12 @@
   </si>
   <si>
     <t>textOverlayPars property in faWidget</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> put TextSymbols in separate layer</t>
+  </si>
+  <si>
+    <t>totals query is processed like table?</t>
   </si>
 </sst>
 </file>
@@ -6124,10 +6105,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6302,7 +6286,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
@@ -6444,30 +6428,46 @@
         <v>154</v>
       </c>
     </row>
-    <row r="40" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D40" s="15" t="s">
         <v>155</v>
       </c>
       <c r="F40" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="G40" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="G40" s="15" t="s">
+      <c r="H40" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="H40" s="18" t="s">
+      <c r="I40" s="41" t="s">
         <v>160</v>
-      </c>
-      <c r="I40" s="41" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D42" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I36" xr:uid="{046495F1-3543-4F8C-98E4-A4049F15EBF9}">
+  <autoFilter ref="A1:I100" xr:uid="{6CDD44CA-3159-4ADC-A892-9FFB6DB01C72}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Added highlighting of row via graphic object mouseover
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090C2953-DF8B-46BC-90BF-33A1E796E8FD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBCA6A8-A70A-4583-9FCE-639F7C1202C5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="10635" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="165">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -5218,6 +5218,15 @@
   </si>
   <si>
     <t>totals query is processed like table?</t>
+  </si>
+  <si>
+    <t>dGrid Selection module API</t>
+  </si>
+  <si>
+    <t>displayPlayButton</t>
+  </si>
+  <si>
+    <t>QueryBasedPanelWidget.js</t>
   </si>
 </sst>
 </file>
@@ -5452,7 +5461,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5484,9 +5493,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5573,8 +5579,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -6105,30 +6123,31 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I100"/>
+  <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.375" style="15" customWidth="1"/>
+    <col min="1" max="1" width="3.75" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="69" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.5" style="15" customWidth="1"/>
-    <col min="6" max="6" width="37.75" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="20" style="18" customWidth="1"/>
-    <col min="9" max="9" width="55.875" style="41" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="15"/>
+    <col min="4" max="4" width="69" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5" style="14" customWidth="1"/>
+    <col min="6" max="6" width="24.625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="16.75" style="14" customWidth="1"/>
+    <col min="8" max="8" width="20" style="17" customWidth="1"/>
+    <col min="9" max="9" width="49.25" style="40" customWidth="1"/>
+    <col min="10" max="10" width="23.125" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="12" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="47" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="13" t="s">
@@ -6140,16 +6159,16 @@
       <c r="D1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="H1" s="44" t="s">
+      <c r="H1" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="41" t="s">
         <v>36</v>
       </c>
     </row>
@@ -6157,11 +6176,11 @@
       <c r="C2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="18"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -6170,16 +6189,16 @@
       <c r="C4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="I4" s="15"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -6188,11 +6207,11 @@
       <c r="C5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -6214,17 +6233,17 @@
       <c r="C8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="18" t="s">
+      <c r="H8" s="14"/>
+      <c r="I8" s="17" t="s">
         <v>38</v>
       </c>
     </row>
@@ -6235,21 +6254,21 @@
       <c r="C10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
     </row>
     <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="18"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="17"/>
     </row>
     <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
@@ -6258,31 +6277,31 @@
       <c r="C13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="18"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="17"/>
     </row>
     <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="18"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="17"/>
     </row>
     <row r="16" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="15"/>
-      <c r="I16" s="41" t="s">
+      <c r="H16" s="14"/>
+      <c r="I16" s="40" t="s">
         <v>140</v>
       </c>
     </row>
@@ -6293,7 +6312,7 @@
       <c r="C18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>13</v>
       </c>
     </row>
@@ -6301,11 +6320,11 @@
       <c r="C21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="15"/>
-      <c r="I21" s="41" t="s">
+      <c r="H21" s="14"/>
+      <c r="I21" s="40" t="s">
         <v>139</v>
       </c>
     </row>
@@ -6313,11 +6332,11 @@
       <c r="C22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="15"/>
-      <c r="I22" s="41" t="s">
+      <c r="H22" s="14"/>
+      <c r="I22" s="40" t="s">
         <v>141</v>
       </c>
     </row>
@@ -6325,25 +6344,25 @@
       <c r="B23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="I23" s="41" t="s">
+      <c r="I23" s="40" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="15"/>
-      <c r="I24" s="41" t="s">
+      <c r="H24" s="14"/>
+      <c r="I24" s="40" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6351,22 +6370,22 @@
       <c r="C26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H26" s="15"/>
-      <c r="I26" s="18"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="17"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="14" t="s">
         <v>39</v>
       </c>
     </row>
@@ -6374,7 +6393,7 @@
       <c r="B31" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="14" t="s">
         <v>40</v>
       </c>
     </row>
@@ -6382,87 +6401,99 @@
       <c r="B32" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="H34" s="15"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="14"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="14" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="14" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="F38" s="16" t="s">
+      <c r="F38" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="H38" s="18" t="s">
+      <c r="H38" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="I38" s="41" t="s">
+      <c r="I38" s="40" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="40" spans="2:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C40" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="F40" s="16" t="s">
+      <c r="F40" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="G40" s="15" t="s">
+      <c r="G40" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="H40" s="18" t="s">
+      <c r="H40" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="I40" s="41" t="s">
+      <c r="I40" s="40" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D42" s="15" t="s">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="14" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F42" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="J42" s="43" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="14" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="15">
+      <c r="A100" s="14">
         <v>0</v>
       </c>
     </row>
@@ -6475,8 +6506,11 @@
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="J42" r:id="rId1" display="https://github.com/SitePen/dgrid/blob/master/doc/components/mixins/Selection.md" xr:uid="{B02003EC-0D72-4D32-86B5-BCB2E4740BDA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6500,103 +6534,103 @@
     </row>
     <row r="2" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="A6" s="31"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="38" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="39" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="33" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="35" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="35" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="33" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="33" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="31" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="33" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="33" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
+      <c r="A19" s="32"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="37" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="33" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="33" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="33" t="s">
         <v>117</v>
       </c>
     </row>
@@ -6607,52 +6641,52 @@
     </row>
     <row r="28" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="33" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="33" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="33" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="33" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="33" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="33" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="36" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="35" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="33" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="33" t="s">
         <v>46</v>
       </c>
     </row>
@@ -6663,158 +6697,158 @@
     </row>
     <row r="42" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="29" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="30" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="31" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="33"/>
+      <c r="A46" s="32"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="30" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="30" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="30" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="33"/>
+      <c r="A50" s="32"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="30" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="34" t="s">
+      <c r="A52" s="33" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="34" t="s">
+      <c r="A53" s="33" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="34" t="s">
+      <c r="A54" s="33" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="34" t="s">
+      <c r="A55" s="33" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="34" t="s">
+      <c r="A56" s="33" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="34" t="s">
+      <c r="A57" s="33" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="35" t="s">
+      <c r="A58" s="34" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="36" t="s">
+      <c r="A59" s="35" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="36" t="s">
+      <c r="A60" s="35" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="34" t="s">
+      <c r="A61" s="33" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="36" t="s">
+      <c r="A62" s="35" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="34" t="s">
+      <c r="A63" s="33" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="34" t="s">
+      <c r="A64" s="33" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="34" t="s">
+      <c r="A65" s="33" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="34" t="s">
+      <c r="A66" s="33" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="34" t="s">
+      <c r="A67" s="33" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="34" t="s">
+      <c r="A68" s="33" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="34" t="s">
+      <c r="A69" s="33" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="34" t="s">
+      <c r="A70" s="33" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="34" t="s">
+      <c r="A71" s="33" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="34" t="s">
+      <c r="A72" s="33" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="34" t="s">
+      <c r="A73" s="33" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="36" t="s">
+      <c r="A74" s="35" t="s">
         <v>83</v>
       </c>
     </row>
@@ -6955,35 +6989,35 @@
     </row>
     <row r="2" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="20" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="20" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="21"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>47</v>
       </c>
       <c r="C11" t="s">
@@ -6991,174 +7025,174 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="20" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="20" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="22" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
+      <c r="A19" s="23"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="22" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="24" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="25" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="24" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="25" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="23" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="19" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="20" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="20" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="20" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="20" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="20" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="26" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
+      <c r="A37" s="27"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="43" t="s">
+      <c r="C38" s="42" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C39" s="43"/>
+      <c r="C39" s="42"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="29" t="s">
+      <c r="A40" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C40" s="43" t="s">
+      <c r="C40" s="42" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="27" t="s">
+      <c r="A41" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C41" s="43"/>
+      <c r="C41" s="42"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="28" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="29" t="s">
+      <c r="A43" s="28" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="26" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="26" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="28" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="28"/>
+      <c r="A47" s="27"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="27" t="s">
+      <c r="A48" s="26" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="27" t="s">
+      <c r="A49" s="26" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="28" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="29" t="s">
+      <c r="A51" s="28" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Start Shore Stations add-on, with Regions tab
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708F5C94-D8D9-47E6-B134-0C5F15C0AF6B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DA4310-7A00-4E83-8878-F29D55FF79AA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="10635" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -5513,11 +5513,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -5851,7 +5851,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G107" sqref="G107"/>
+      <selection pane="bottomRight" activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5878,7 +5878,7 @@
       <c r="C1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="40" t="s">
         <v>15</v>
       </c>
       <c r="F1" s="36" t="s">
@@ -5978,7 +5978,7 @@
     <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="63" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
@@ -6062,7 +6062,7 @@
     <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:9" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
         <v>22</v>
       </c>
@@ -6086,11 +6086,11 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="10" t="s">
         <v>130</v>
       </c>
       <c r="I23" s="33" t="s">
@@ -6175,26 +6175,26 @@
       </c>
       <c r="H34" s="7"/>
     </row>
-    <row r="35" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="10" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="37" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="D37" s="7"/>
     </row>
-    <row r="38" spans="2:10" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" ht="126" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>25</v>
       </c>
@@ -6237,11 +6237,11 @@
     <row r="41" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="2:10" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="10" t="s">
         <v>141</v>
       </c>
       <c r="F42" s="8" t="s">
@@ -6260,19 +6260,19 @@
     <row r="43" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="10" t="s">
         <v>150</v>
       </c>
     </row>
@@ -6466,10 +6466,9 @@
       <filters blank="1"/>
     </filterColumn>
     <filterColumn colId="1">
-      <filters>
-        <filter val="TS"/>
-        <filter val="TS?"/>
-      </filters>
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
     <filterColumn colId="2">
       <filters blank="1"/>
@@ -6983,7 +6982,7 @@
       <c r="A38" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="40" t="s">
+      <c r="C38" s="41" t="s">
         <v>67</v>
       </c>
     </row>
@@ -6991,13 +6990,13 @@
       <c r="A39" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="40"/>
+      <c r="C39" s="41"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="40" t="s">
+      <c r="C40" s="41" t="s">
         <v>68</v>
       </c>
     </row>
@@ -7005,7 +7004,7 @@
       <c r="A41" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="40"/>
+      <c r="C41" s="41"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">

</xml_diff>

<commit_message>
Reconfigured changeState function, incl. setting visibility of graphic layers
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DA4310-7A00-4E83-8878-F29D55FF79AA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5D5129-999E-4C41-84DE-6E952B358B70}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="10635" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="2025" yWindow="150" windowWidth="24615" windowHeight="15390" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="to do" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="resize imagery on splitter drag" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'to do'!$A$1:$I$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'to do'!$A$1:$I$102</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="168">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -103,9 +104,6 @@
   </si>
   <si>
     <t>Task</t>
-  </si>
-  <si>
-    <t>Completed by</t>
   </si>
   <si>
     <t>graphics layers:  no display until mouseover</t>
@@ -152,9 +150,6 @@
 Still need to get BorderContainer splitter event</t>
   </si>
   <si>
-    <t>other tooltips</t>
-  </si>
-  <si>
     <t>semi-transparent background for text over imagery, so it's more visible</t>
   </si>
   <si>
@@ -5168,6 +5163,36 @@
       <t xml:space="preserve"> property.
 (Leave the CMECS fields unchanged, and don't do anything with labels of 3-4 characters.)</t>
     </r>
+  </si>
+  <si>
+    <t>The Picasa API is deprecated. See https://developers.google.com/picasa-web/ for more details and the migration guide.</t>
+  </si>
+  <si>
+    <t>Deal with "more videos" on YouTube video pause</t>
+  </si>
+  <si>
+    <t>YouTube API no longer allows disabling showing of "more videos" when video is paused</t>
+  </si>
+  <si>
+    <t>works okay on server?</t>
+  </si>
+  <si>
+    <t>Deal with Picasa deprecation</t>
+  </si>
+  <si>
+    <t>Add links to REST services for SZ, FA, SS</t>
+  </si>
+  <si>
+    <t>Use AOOS service?</t>
+  </si>
+  <si>
+    <t>Completed?</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -5402,7 +5427,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5515,6 +5540,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -5844,14 +5875,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:J100"/>
+  <sheetPr codeName="Sheet1" filterMode="1"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F106" sqref="F106"/>
+      <selection pane="bottomRight" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5862,9 +5893,9 @@
     <col min="5" max="5" width="4.5" style="7" customWidth="1"/>
     <col min="6" max="6" width="24.625" style="8" customWidth="1"/>
     <col min="7" max="7" width="16.75" style="7" customWidth="1"/>
-    <col min="8" max="8" width="20" style="10" customWidth="1"/>
+    <col min="8" max="8" width="14.75" style="10" customWidth="1"/>
     <col min="9" max="9" width="62.75" style="33" customWidth="1"/>
-    <col min="10" max="10" width="23.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.125" style="7" customWidth="1"/>
     <col min="11" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
@@ -5875,28 +5906,28 @@
       <c r="B1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>16</v>
+      <c r="C1" s="42" t="s">
+        <v>165</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>15</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G1" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="38" t="s">
-        <v>136</v>
-      </c>
       <c r="I1" s="34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>167</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>10</v>
@@ -5904,15 +5935,15 @@
       <c r="H2" s="7"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>9</v>
@@ -5921,16 +5952,16 @@
         <v>8</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>7</v>
@@ -5951,15 +5982,15 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>5</v>
@@ -5968,22 +5999,22 @@
         <v>4</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:9" ht="63" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>2</v>
@@ -5991,12 +6022,12 @@
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>167</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>1</v>
@@ -6006,95 +6037,98 @@
     </row>
     <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>22</v>
+        <v>167</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>167</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>166</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>0</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="33" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>167</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
-        <v>22</v>
+        <v>166</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
-        <v>22</v>
+        <v>167</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="I23" s="33" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="I23" s="33" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -6102,46 +6136,49 @@
         <v>11</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
-        <v>22</v>
+        <v>166</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D29" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -6149,326 +6186,363 @@
         <v>11</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D33" s="7"/>
     </row>
     <row r="34" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C34" s="2" t="s">
-        <v>22</v>
+        <v>167</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="I36" s="33" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D37" s="7"/>
     </row>
-    <row r="38" spans="2:10" ht="126" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" ht="126" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F38" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="I38" s="33" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D39" s="7"/>
+    </row>
+    <row r="40" spans="2:10" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="I40" s="33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D41" s="7"/>
+    </row>
+    <row r="42" spans="2:10" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D42" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="H38" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="I38" s="33" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="7"/>
-    </row>
-    <row r="40" spans="2:10" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="H40" s="10" t="s">
+      <c r="F42" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="I42" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="J42" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="I40" s="33" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D41" s="7"/>
-    </row>
-    <row r="42" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B42" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="I42" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="J42" s="35" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D43" s="7"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D45" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D46" s="7"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D47" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="46" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D46" s="7"/>
-    </row>
-    <row r="47" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D47" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D48" s="7"/>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="2" t="s">
+      <c r="D49" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="F49" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="H49" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="I49" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="F49" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="H49" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="I49" s="33" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D50" s="7"/>
     </row>
-    <row r="51" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D51" s="7"/>
-    </row>
-    <row r="52" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D52" s="7"/>
-    </row>
-    <row r="53" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="I51" s="41" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="I52" s="41" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D53" s="7"/>
     </row>
-    <row r="54" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D54" s="7"/>
     </row>
-    <row r="55" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D56" s="7"/>
     </row>
-    <row r="57" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D57" s="7"/>
     </row>
-    <row r="58" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D58" s="7"/>
     </row>
-    <row r="59" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D60" s="7"/>
     </row>
-    <row r="61" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D61" s="7"/>
     </row>
-    <row r="62" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D63" s="7"/>
     </row>
-    <row r="64" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D64" s="7"/>
     </row>
-    <row r="65" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="7"/>
     </row>
-    <row r="66" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="7"/>
     </row>
-    <row r="67" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="7"/>
     </row>
-    <row r="68" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="7"/>
     </row>
-    <row r="69" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="7"/>
     </row>
-    <row r="71" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="7"/>
     </row>
-    <row r="72" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="7"/>
     </row>
-    <row r="73" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73" s="7"/>
     </row>
-    <row r="74" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74" s="7"/>
     </row>
-    <row r="75" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75" s="7"/>
     </row>
-    <row r="76" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77" s="7"/>
     </row>
-    <row r="78" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D78" s="7"/>
     </row>
-    <row r="79" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D79" s="7"/>
     </row>
-    <row r="80" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80" s="7"/>
     </row>
-    <row r="81" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81" s="7"/>
     </row>
-    <row r="82" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D82" s="7"/>
     </row>
-    <row r="83" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83" s="7"/>
     </row>
-    <row r="84" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D84" s="7"/>
     </row>
-    <row r="85" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D85" s="7"/>
     </row>
-    <row r="86" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D86" s="7"/>
     </row>
-    <row r="87" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D87" s="7"/>
     </row>
-    <row r="88" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D88" s="7"/>
     </row>
-    <row r="89" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D89" s="7"/>
     </row>
-    <row r="90" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D90" s="7"/>
     </row>
-    <row r="91" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D91" s="7"/>
     </row>
-    <row r="92" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D92" s="7"/>
     </row>
-    <row r="93" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D93" s="7"/>
     </row>
-    <row r="94" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D94" s="7"/>
     </row>
-    <row r="95" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D95" s="7"/>
     </row>
-    <row r="96" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D96" s="7"/>
     </row>
-    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D97" s="7"/>
     </row>
-    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D98" s="7"/>
     </row>
-    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D99" s="7"/>
     </row>
-    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="7">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="7"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="7"/>
+    </row>
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="7">
         <v>0</v>
       </c>
-      <c r="D100" s="7"/>
+      <c r="D102" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I100" xr:uid="{6CDD44CA-3159-4ADC-A892-9FFB6DB01C72}">
+  <autoFilter ref="A1:I102" xr:uid="{6CDD44CA-3159-4ADC-A892-9FFB6DB01C72}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
     <filterColumn colId="1">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+      <filters blank="1">
+        <filter val="JN"/>
+      </filters>
     </filterColumn>
     <filterColumn colId="2">
       <filters blank="1"/>
@@ -6476,14 +6550,17 @@
   </autoFilter>
   <hyperlinks>
     <hyperlink ref="J42" r:id="rId1" display="https://github.com/SitePen/dgrid/blob/master/doc/components/mixins/Selection.md" xr:uid="{B02003EC-0D72-4D32-86B5-BCB2E4740BDA}"/>
+    <hyperlink ref="I51" r:id="rId2" xr:uid="{D7280C89-055C-482B-859C-78DDF371D8BE}"/>
+    <hyperlink ref="I52" r:id="rId3" location="release_notes_08_23_2018" display="Can no longer disable showing of &quot;more videos&quot; when video is paused" xr:uid="{75869B48-9B1F-4352-8C34-D2F55186219A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE45D646-5865-4DD3-B066-A6FB8031C09E}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6497,23 +6574,23 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -6521,62 +6598,62 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -6584,99 +6661,99 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
@@ -6684,17 +6761,17 @@
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
@@ -6702,122 +6779,122 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -6828,6 +6905,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267B328E-A616-48A5-B37D-5A675A5748D9}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -6842,33 +6920,33 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6876,35 +6954,35 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -6912,67 +6990,67 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -6980,55 +7058,55 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="41" t="s">
-        <v>67</v>
+        <v>51</v>
+      </c>
+      <c r="C38" s="43" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C39" s="41"/>
+        <v>52</v>
+      </c>
+      <c r="C39" s="43"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C40" s="41" t="s">
-        <v>68</v>
+        <v>53</v>
+      </c>
+      <c r="C40" s="43" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="41"/>
+        <v>54</v>
+      </c>
+      <c r="C41" s="43"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -7036,22 +7114,22 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit rest of files
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimnoel/WebstormProjects/ShoreZoneDev_JS4x/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5D5129-999E-4C41-84DE-6E952B358B70}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB60EDC1-8BB3-A64C-B96C-276748820EDA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="150" windowWidth="24615" windowHeight="15390" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="2020" yWindow="460" windowWidth="24620" windowHeight="15400" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="to do" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="168">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -5199,7 +5199,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5879,27 +5879,27 @@
   <dimension ref="A1:J102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C47" sqref="C47"/>
+      <selection pane="bottomRight" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.75" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="45.375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.33203125" style="10" customWidth="1"/>
     <col min="5" max="5" width="4.5" style="7" customWidth="1"/>
-    <col min="6" max="6" width="24.625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="16.75" style="7" customWidth="1"/>
-    <col min="8" max="8" width="14.75" style="10" customWidth="1"/>
-    <col min="9" max="9" width="62.75" style="33" customWidth="1"/>
-    <col min="10" max="10" width="32.125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="62.6640625" style="33" customWidth="1"/>
+    <col min="10" max="10" width="32.1640625" style="7" customWidth="1"/>
     <col min="11" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="86.25" customHeight="1">
       <c r="A1" s="39" t="s">
         <v>12</v>
       </c>
@@ -5925,7 +5925,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" hidden="1">
       <c r="C2" s="2" t="s">
         <v>167</v>
       </c>
@@ -5935,10 +5935,10 @@
       <c r="H2" s="7"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1">
       <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
@@ -5956,7 +5956,7 @@
       </c>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1">
       <c r="B5" s="2" t="s">
         <v>24</v>
       </c>
@@ -5969,7 +5969,7 @@
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" customFormat="1" hidden="1">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -5982,10 +5982,10 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="34" hidden="1">
       <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
@@ -6006,10 +6006,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="63" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="68" hidden="1">
       <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
@@ -6022,10 +6022,10 @@
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1">
       <c r="C12" s="2" t="s">
         <v>167</v>
       </c>
@@ -6035,7 +6035,7 @@
       <c r="H12" s="7"/>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1">
       <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
@@ -6048,10 +6048,10 @@
       <c r="H13" s="7"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1">
       <c r="C15" s="2" t="s">
         <v>167</v>
       </c>
@@ -6061,7 +6061,7 @@
       <c r="H15" s="7"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="34" hidden="1">
       <c r="C16" s="2" t="s">
         <v>166</v>
       </c>
@@ -6073,10 +6073,10 @@
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1">
       <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
@@ -6087,13 +6087,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="34" hidden="1">
       <c r="C21" s="2" t="s">
         <v>166</v>
       </c>
@@ -6105,7 +6105,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="34" hidden="1">
       <c r="C22" s="2" t="s">
         <v>167</v>
       </c>
@@ -6117,7 +6117,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="34" hidden="1">
       <c r="A23" s="7" t="s">
         <v>11</v>
       </c>
@@ -6131,7 +6131,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="17" hidden="1">
       <c r="A24" s="7" t="s">
         <v>11</v>
       </c>
@@ -6146,10 +6146,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1">
       <c r="C26" s="2" t="s">
         <v>166</v>
       </c>
@@ -6159,10 +6159,10 @@
       <c r="H26" s="7"/>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="34" hidden="1">
       <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
@@ -6170,7 +6170,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="B29" s="2" t="s">
         <v>21</v>
       </c>
@@ -6178,10 +6178,10 @@
         <v>163</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1">
       <c r="A31" s="7" t="s">
         <v>11</v>
       </c>
@@ -6192,7 +6192,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="17" hidden="1">
       <c r="B32" s="2" t="s">
         <v>24</v>
       </c>
@@ -6200,10 +6200,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10">
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" hidden="1">
       <c r="C34" s="2" t="s">
         <v>167</v>
       </c>
@@ -6212,15 +6212,18 @@
       </c>
       <c r="H34" s="7"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" ht="17" hidden="1">
       <c r="B35" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="C35" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="D35" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" ht="34" hidden="1">
       <c r="B36" s="2" t="s">
         <v>21</v>
       </c>
@@ -6234,10 +6237,10 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10">
       <c r="D37" s="7"/>
     </row>
-    <row r="38" spans="2:10" ht="126" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" ht="136" hidden="1">
       <c r="B38" s="2" t="s">
         <v>24</v>
       </c>
@@ -6254,10 +6257,10 @@
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10">
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="2:10" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" ht="51" hidden="1">
       <c r="C40" s="2" t="s">
         <v>166</v>
       </c>
@@ -6277,10 +6280,10 @@
         <v>143</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10">
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="2:10" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" ht="34" hidden="1">
       <c r="B42" s="2" t="s">
         <v>21</v>
       </c>
@@ -6303,18 +6306,21 @@
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10">
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" ht="17" hidden="1">
       <c r="B44" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="C44" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="D44" s="10" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="45" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" ht="34">
       <c r="B45" s="2" t="s">
         <v>21</v>
       </c>
@@ -6322,18 +6328,18 @@
         <v>148</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10">
       <c r="D46" s="7"/>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10">
       <c r="D47" s="7" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10">
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" ht="17" hidden="1">
       <c r="B49" s="2" t="s">
         <v>150</v>
       </c>
@@ -6350,10 +6356,10 @@
         <v>154</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9">
       <c r="D50" s="7"/>
     </row>
-    <row r="51" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" ht="34" hidden="1">
       <c r="B51" s="2" t="s">
         <v>21</v>
       </c>
@@ -6370,7 +6376,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="52" spans="2:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" ht="34" hidden="1">
       <c r="C52" s="2" t="s">
         <v>166</v>
       </c>
@@ -6381,154 +6387,154 @@
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9">
       <c r="D53" s="7"/>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9">
       <c r="D54" s="7"/>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9">
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9">
       <c r="D56" s="7"/>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9">
       <c r="D57" s="7"/>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9">
       <c r="D58" s="7"/>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9">
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9">
       <c r="D60" s="7"/>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9">
       <c r="D61" s="7"/>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9">
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9">
       <c r="D63" s="7"/>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9">
       <c r="D64" s="7"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:4">
       <c r="D65" s="7"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:4">
       <c r="D66" s="7"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:4">
       <c r="D67" s="7"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:4">
       <c r="D68" s="7"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:4">
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:4">
       <c r="D70" s="7"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:4">
       <c r="D71" s="7"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:4">
       <c r="D72" s="7"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:4">
       <c r="D73" s="7"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:4">
       <c r="D74" s="7"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:4">
       <c r="D75" s="7"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4">
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:4">
       <c r="D77" s="7"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:4">
       <c r="D78" s="7"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:4">
       <c r="D79" s="7"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:4">
       <c r="D80" s="7"/>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:4">
       <c r="D81" s="7"/>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:4">
       <c r="D82" s="7"/>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:4">
       <c r="D83" s="7"/>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:4">
       <c r="D84" s="7"/>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:4">
       <c r="D85" s="7"/>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:4">
       <c r="D86" s="7"/>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:4">
       <c r="D87" s="7"/>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:4">
       <c r="D88" s="7"/>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:4">
       <c r="D89" s="7"/>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:4">
       <c r="D90" s="7"/>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:4">
       <c r="D91" s="7"/>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:4">
       <c r="D92" s="7"/>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:4">
       <c r="D93" s="7"/>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:4">
       <c r="D94" s="7"/>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:4">
       <c r="D95" s="7"/>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:4">
       <c r="D96" s="7"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="D97" s="7"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="D98" s="7"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="D99" s="7"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="D100" s="7"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="D101" s="7"/>
     </row>
-    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" hidden="1">
       <c r="A102" s="7">
         <v>0</v>
       </c>
@@ -6567,332 +6573,332 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="112.75" customWidth="1"/>
+    <col min="1" max="1" width="112.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="17" thickTop="1"/>
+    <row r="3" spans="1:1">
       <c r="A3" s="24" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="24" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="24" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="24"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="31" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="32" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="26" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="28" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="26" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="26" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="24" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="26" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="26" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="25"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="30" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="26" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="26" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="26" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" ht="18" thickBot="1">
       <c r="A27" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" ht="17" thickTop="1"/>
+    <row r="29" spans="1:1">
       <c r="A29" s="26" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="26" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="26" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="26" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="26" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="26" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="29" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="28" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="26" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" ht="18" thickBot="1">
       <c r="A41" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" ht="17" thickTop="1"/>
+    <row r="43" spans="1:1">
       <c r="A43" s="22" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="24" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="25"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="23" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="23" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="25"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="23" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1">
       <c r="A52" s="26" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1">
       <c r="A53" s="26" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1">
       <c r="A54" s="26" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1">
       <c r="A55" s="26" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1">
       <c r="A56" s="26" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1">
       <c r="A57" s="26" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1">
       <c r="A58" s="27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1">
       <c r="A59" s="28" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1">
       <c r="A60" s="28" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1">
       <c r="A61" s="26" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1">
       <c r="A62" s="28" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1">
       <c r="A63" s="26" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1">
       <c r="A64" s="26" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1">
       <c r="A65" s="26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1">
       <c r="A66" s="26" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1">
       <c r="A67" s="26" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1">
       <c r="A68" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1">
       <c r="A69" s="26" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1">
       <c r="A70" s="26" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1">
       <c r="A71" s="26" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1">
       <c r="A72" s="26" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1">
       <c r="A73" s="26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1">
       <c r="A74" s="28" t="s">
         <v>69</v>
       </c>
@@ -6912,47 +6918,47 @@
       <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="109.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="109.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="17" thickTop="1"/>
+    <row r="4" spans="1:3">
       <c r="A4" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="14"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="12" t="s">
         <v>33</v>
       </c>
@@ -6960,103 +6966,103 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="17">
       <c r="A18" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="16"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="17">
       <c r="A20" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="17">
       <c r="A21" s="17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="17">
       <c r="A22" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="17">
       <c r="A23" s="17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="34">
       <c r="A24" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" s="20"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" s="19" t="s">
         <v>51</v>
       </c>
@@ -7064,13 +7070,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C39" s="43"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" s="21" t="s">
         <v>53</v>
       </c>
@@ -7078,56 +7084,56 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="19" t="s">
         <v>54</v>
       </c>
       <c r="C41" s="43"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="21" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="20"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="19" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="21" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Handle table with 0 rows
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimnoel/WebstormProjects/ShoreZoneDev_JS4x/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB60EDC1-8BB3-A64C-B96C-276748820EDA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2F29BD-E6E6-0E47-B1B3-B0BED52FC23D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2020" yWindow="460" windowWidth="24620" windowHeight="15400" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="170">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -5083,9 +5083,6 @@
     <t>2 queries when click on "go to subarea"?</t>
   </si>
   <si>
-    <t>When in Locales, click of Regions tab needs to lose region selection</t>
-  </si>
-  <si>
     <t>saved extents</t>
   </si>
   <si>
@@ -5194,12 +5191,21 @@
   <si>
     <t>y</t>
   </si>
+  <si>
+    <t>Locale marker background transparency</t>
+  </si>
+  <si>
+    <t>Leave dropdown selection out of query where clause when dropdown is not visible</t>
+  </si>
+  <si>
+    <t>textOverlayPars</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5385,6 +5391,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF660E7A"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -5427,7 +5440,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5550,6 +5563,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Heading 2" xfId="6" builtinId="17"/>
@@ -5882,7 +5896,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D45" sqref="D45"/>
+      <selection pane="bottomRight" activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -5907,7 +5921,7 @@
         <v>14</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>15</v>
@@ -5927,7 +5941,7 @@
     </row>
     <row r="2" spans="1:9" hidden="1">
       <c r="C2" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>10</v>
@@ -6027,7 +6041,7 @@
     </row>
     <row r="12" spans="1:9" hidden="1">
       <c r="C12" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>1</v>
@@ -6040,7 +6054,7 @@
         <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>124</v>
@@ -6053,7 +6067,7 @@
     </row>
     <row r="15" spans="1:9" hidden="1">
       <c r="C15" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>67</v>
@@ -6063,7 +6077,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" hidden="1">
       <c r="C16" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>0</v>
@@ -6081,7 +6095,7 @@
         <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>13</v>
@@ -6095,7 +6109,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" hidden="1">
       <c r="C21" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>16</v>
@@ -6107,7 +6121,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" hidden="1">
       <c r="C22" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>20</v>
@@ -6151,7 +6165,7 @@
     </row>
     <row r="26" spans="1:9" hidden="1">
       <c r="C26" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>19</v>
@@ -6175,7 +6189,7 @@
         <v>21</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -6205,7 +6219,7 @@
     </row>
     <row r="34" spans="2:10" hidden="1">
       <c r="C34" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>68</v>
@@ -6217,7 +6231,7 @@
         <v>21</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>130</v>
@@ -6228,13 +6242,13 @@
         <v>21</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>131</v>
       </c>
       <c r="I36" s="33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="2:10">
@@ -6245,16 +6259,16 @@
         <v>24</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>137</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I38" s="33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="2:10">
@@ -6262,7 +6276,7 @@
     </row>
     <row r="40" spans="2:10" ht="51" hidden="1">
       <c r="C40" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>138</v>
@@ -6288,7 +6302,7 @@
         <v>21</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>139</v>
@@ -6300,7 +6314,7 @@
         <v>145</v>
       </c>
       <c r="I42" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J42" s="35" t="s">
         <v>144</v>
@@ -6314,26 +6328,34 @@
         <v>21</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="45" spans="2:10" ht="34">
+    <row r="45" spans="2:10" ht="34" hidden="1">
       <c r="B45" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="C45" s="2" t="s">
+        <v>166</v>
+      </c>
       <c r="D45" s="10" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="2:10">
-      <c r="D46" s="7"/>
+      <c r="D46" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="I46" s="44" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="47" spans="2:10">
       <c r="D47" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="2:10">
@@ -6341,19 +6363,19 @@
     </row>
     <row r="49" spans="2:9" ht="17" hidden="1">
       <c r="B49" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>137</v>
       </c>
       <c r="H49" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="I49" s="33" t="s">
         <v>153</v>
-      </c>
-      <c r="I49" s="33" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="50" spans="2:9">
@@ -6364,27 +6386,27 @@
         <v>21</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I51" s="41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="2:9" ht="34" hidden="1">
       <c r="C52" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D52" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="I52" s="41" t="s">
         <v>159</v>
-      </c>
-      <c r="I52" s="41" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="53" spans="2:9">

</xml_diff>

<commit_message>
Rearrange and modify widget icons, modify map/table panel sizes
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimnoel/WebstormProjects/ShoreZoneDev_JS4x/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2F29BD-E6E6-0E47-B1B3-B0BED52FC23D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC1D2E9-2C5F-3449-9E37-3C4C1611C089}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="460" windowWidth="24620" windowHeight="15400" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="1060" yWindow="460" windowWidth="24620" windowHeight="15400" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="to do" sheetId="1" r:id="rId1"/>
     <sheet name="extent history" sheetId="8" r:id="rId2"/>
     <sheet name="resize imagery on splitter drag" sheetId="7" r:id="rId3"/>
+    <sheet name="possible Tristan jobs" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'to do'!$A$1:$I$102</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="171">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -5199,6 +5200,9 @@
   </si>
   <si>
     <t>textOverlayPars</t>
+  </si>
+  <si>
+    <t>bring up to ES5/ES6</t>
   </si>
 </sst>
 </file>
@@ -5560,10 +5564,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Heading 2" xfId="6" builtinId="17"/>
@@ -5893,7 +5897,7 @@
   <dimension ref="A1:J102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="I46" sqref="I46"/>
@@ -6349,7 +6353,7 @@
       <c r="D46" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="I46" s="44" t="s">
+      <c r="I46" s="43" t="s">
         <v>169</v>
       </c>
     </row>
@@ -7088,7 +7092,7 @@
       <c r="A38" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="43" t="s">
+      <c r="C38" s="44" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7096,13 +7100,13 @@
       <c r="A39" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="43"/>
+      <c r="C39" s="44"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="43" t="s">
+      <c r="C40" s="44" t="s">
         <v>66</v>
       </c>
     </row>
@@ -7110,7 +7114,7 @@
       <c r="A41" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="43"/>
+      <c r="C41" s="44"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="21" t="s">
@@ -7168,4 +7172,27 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E19437AE-572B-6E4F-9B26-5FD12EFDDDFB}">
+  <dimension ref="B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Expand LayerList & Legend widgets by default, for pub.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimnoel/WebstormProjects/ShoreZoneDev_JS4x/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC1D2E9-2C5F-3449-9E37-3C4C1611C089}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB36ADE-0EA7-FF40-B29B-6EBED7BEF14A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="460" windowWidth="24620" windowHeight="15400" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="172">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -5203,6 +5203,12 @@
   </si>
   <si>
     <t>bring up to ES5/ES6</t>
+  </si>
+  <si>
+    <t>FA/Sites tab:  Choose locale from different region:
+     Flex: no DD for Regions, so it works fine
+     JS:  need to either ignore Region DD selection, 
+          or limit Locale options to current Region</t>
   </si>
 </sst>
 </file>
@@ -5897,10 +5903,10 @@
   <dimension ref="A1:J102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I46" sqref="I46"/>
+      <selection pane="bottomRight" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -6413,8 +6419,10 @@
         <v>159</v>
       </c>
     </row>
-    <row r="53" spans="2:9">
-      <c r="D53" s="7"/>
+    <row r="53" spans="2:9" ht="68">
+      <c r="D53" s="10" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="54" spans="2:9">
       <c r="D54" s="7"/>

</xml_diff>

<commit_message>
Use AOOS photos by default
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimnoel/WebstormProjects/ShoreZoneDev_JS4x/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E54B64-1A44-1E46-8B25-60C53147B721}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1C9422-0089-6F4C-9F99-4C0693C28A7E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="460" windowWidth="24620" windowHeight="15400" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="175">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -5215,6 +5215,9 @@
   </si>
   <si>
     <t xml:space="preserve">CSS settings?  </t>
+  </si>
+  <si>
+    <t>set correct initial photo size for photos from Axiom</t>
   </si>
 </sst>
 </file>
@@ -5912,7 +5915,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I55" sqref="I55"/>
+      <selection pane="bottomRight" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -6448,7 +6451,9 @@
       <c r="D56" s="7"/>
     </row>
     <row r="57" spans="2:9">
-      <c r="D57" s="7"/>
+      <c r="D57" s="7" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="58" spans="2:9">
       <c r="D58" s="7"/>

</xml_diff>

<commit_message>
Data download:  Hide vidcaps options when none are available
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimnoel/WebstormProjects/ShoreZoneDev_JS4x/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1C9422-0089-6F4C-9F99-4C0693C28A7E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291E8C2A-9431-904F-9884-D05932F2C1E8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="460" windowWidth="24620" windowHeight="15400" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="1060" yWindow="460" windowWidth="24620" windowHeight="15400" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="to do" sheetId="1" r:id="rId1"/>
-    <sheet name="extent history" sheetId="8" r:id="rId2"/>
-    <sheet name="resize imagery on splitter drag" sheetId="7" r:id="rId3"/>
-    <sheet name="possible Tristan jobs" sheetId="9" r:id="rId4"/>
+    <sheet name="screen captures" sheetId="10" r:id="rId2"/>
+    <sheet name="extent history" sheetId="8" r:id="rId3"/>
+    <sheet name="resize imagery on splitter drag" sheetId="7" r:id="rId4"/>
+    <sheet name="possible Tristan jobs" sheetId="9" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'to do'!$A$1:$I$102</definedName>
@@ -5611,6 +5612,55 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{548AA073-8E6D-8048-AB60-33CDCDBE8A9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5753100" cy="3568700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5911,7 +5961,7 @@
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -6618,6 +6668,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C0E0CA-5258-DA42-9AFB-0582B12738D1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE45D646-5865-4DD3-B066-A6FB8031C09E}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A74"/>
@@ -6962,7 +7025,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267B328E-A616-48A5-B37D-5A675A5748D9}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C51"/>
@@ -7201,7 +7264,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E19437AE-572B-6E4F-9B26-5FD12EFDDDFB}">
   <dimension ref="B3"/>
   <sheetViews>

</xml_diff>

<commit_message>
SS PhotoPlaybackWidget runQuery and processData
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimnoel/WebstormProjects/ShoreZoneDev_JS4x/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291E8C2A-9431-904F-9884-D05932F2C1E8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEE1A35-426A-4FD2-BF52-E9808B74BDCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="460" windowWidth="24620" windowHeight="15400" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
-    <sheet name="to do" sheetId="1" r:id="rId1"/>
-    <sheet name="screen captures" sheetId="10" r:id="rId2"/>
-    <sheet name="extent history" sheetId="8" r:id="rId3"/>
-    <sheet name="resize imagery on splitter drag" sheetId="7" r:id="rId4"/>
-    <sheet name="possible Tristan jobs" sheetId="9" r:id="rId5"/>
+    <sheet name="sync_photos" sheetId="11" r:id="rId1"/>
+    <sheet name="to do" sheetId="1" r:id="rId2"/>
+    <sheet name="screen captures" sheetId="10" r:id="rId3"/>
+    <sheet name="extent history" sheetId="8" r:id="rId4"/>
+    <sheet name="resize imagery on splitter drag" sheetId="7" r:id="rId5"/>
+    <sheet name="possible Tristan jobs" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'to do'!$A$1:$I$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$102</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="178">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -5220,14 +5221,30 @@
   <si>
     <t>set correct initial photo size for photos from Axiom</t>
   </si>
+  <si>
+    <t>szPhotoWidget.syncFrom = szVideoWidget</t>
+  </si>
+  <si>
+    <t>szVideoWidget.syncTo = szPhotoWidget</t>
+  </si>
+  <si>
+    <t>Replace with (?):</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="29">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -5418,6 +5435,22 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF660E7A"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -5451,141 +5484,147 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="6"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="6"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="7" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Heading 2" xfId="6" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5593,6 +5632,7 @@
     <cellStyle name="Normal 2 2" xfId="4" xr:uid="{97D9842F-BF32-4166-B6CE-BB3D7E981AD6}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{33E71147-3CE4-45CE-8876-5FF661A1EB4E}"/>
     <cellStyle name="Normal 4" xfId="5" xr:uid="{F641EBF2-1CDA-425E-B5C3-517AF90F4C7A}"/>
+    <cellStyle name="Normal 5" xfId="7" xr:uid="{9FC96886-235B-415D-910B-05AF22994145}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5613,6 +5653,50 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="8866667" cy="3961905"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8DED24D-4DDE-482E-AA46-9AE983789186}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8866667" cy="3961905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -5957,6 +6041,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB0B7B4-8613-440E-8760-4618937ED99C}">
+  <dimension ref="B23:B25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9" style="45"/>
+    <col min="2" max="2" width="36.625" style="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="45"/>
+  </cols>
+  <sheetData>
+    <row r="23" spans="2:2">
+      <c r="B23" s="47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="46" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="46" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:J102"/>
@@ -5968,17 +6089,17 @@
       <selection pane="bottomRight" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="45.33203125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="3.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.375" style="10" customWidth="1"/>
     <col min="5" max="5" width="4.5" style="7" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="62.6640625" style="33" customWidth="1"/>
-    <col min="10" max="10" width="32.1640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="24.625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="16.625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="14.625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="62.625" style="33" customWidth="1"/>
+    <col min="10" max="10" width="32.125" style="7" customWidth="1"/>
     <col min="11" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
@@ -6068,7 +6189,7 @@
     <row r="7" spans="1:9">
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="34" hidden="1">
+    <row r="8" spans="1:9" ht="31.5" hidden="1">
       <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
@@ -6092,7 +6213,7 @@
     <row r="9" spans="1:9">
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="68" hidden="1">
+    <row r="10" spans="1:9" ht="63" hidden="1">
       <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
@@ -6144,7 +6265,7 @@
       <c r="H15" s="7"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" ht="34" hidden="1">
+    <row r="16" spans="1:9" ht="31.5" hidden="1">
       <c r="C16" s="2" t="s">
         <v>165</v>
       </c>
@@ -6176,7 +6297,7 @@
     <row r="20" spans="1:9">
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:9" ht="34" hidden="1">
+    <row r="21" spans="1:9" ht="31.5" hidden="1">
       <c r="C21" s="2" t="s">
         <v>165</v>
       </c>
@@ -6188,7 +6309,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="34" hidden="1">
+    <row r="22" spans="1:9" ht="31.5" hidden="1">
       <c r="C22" s="2" t="s">
         <v>166</v>
       </c>
@@ -6200,7 +6321,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="34" hidden="1">
+    <row r="23" spans="1:9" ht="31.5" hidden="1">
       <c r="A23" s="7" t="s">
         <v>11</v>
       </c>
@@ -6214,7 +6335,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="17" hidden="1">
+    <row r="24" spans="1:9" hidden="1">
       <c r="A24" s="7" t="s">
         <v>11</v>
       </c>
@@ -6245,7 +6366,7 @@
     <row r="27" spans="1:9">
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:9" ht="34" hidden="1">
+    <row r="28" spans="1:9" ht="31.5" hidden="1">
       <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
@@ -6275,7 +6396,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="17" hidden="1">
+    <row r="32" spans="1:9" hidden="1">
       <c r="B32" s="2" t="s">
         <v>24</v>
       </c>
@@ -6295,7 +6416,7 @@
       </c>
       <c r="H34" s="7"/>
     </row>
-    <row r="35" spans="2:10" ht="17" hidden="1">
+    <row r="35" spans="2:10" hidden="1">
       <c r="B35" s="2" t="s">
         <v>21</v>
       </c>
@@ -6306,7 +6427,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="34" hidden="1">
+    <row r="36" spans="2:10" ht="31.5" hidden="1">
       <c r="B36" s="2" t="s">
         <v>21</v>
       </c>
@@ -6323,7 +6444,7 @@
     <row r="37" spans="2:10">
       <c r="D37" s="7"/>
     </row>
-    <row r="38" spans="2:10" ht="136" hidden="1">
+    <row r="38" spans="2:10" ht="126" hidden="1">
       <c r="B38" s="2" t="s">
         <v>24</v>
       </c>
@@ -6343,7 +6464,7 @@
     <row r="39" spans="2:10">
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="2:10" ht="51" hidden="1">
+    <row r="40" spans="2:10" ht="47.25" hidden="1">
       <c r="C40" s="2" t="s">
         <v>165</v>
       </c>
@@ -6366,7 +6487,7 @@
     <row r="41" spans="2:10">
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="2:10" ht="34" hidden="1">
+    <row r="42" spans="2:10" ht="31.5" hidden="1">
       <c r="B42" s="2" t="s">
         <v>21</v>
       </c>
@@ -6392,7 +6513,7 @@
     <row r="43" spans="2:10">
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="2:10" ht="17" hidden="1">
+    <row r="44" spans="2:10" hidden="1">
       <c r="B44" s="2" t="s">
         <v>21</v>
       </c>
@@ -6403,7 +6524,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="45" spans="2:10" ht="34" hidden="1">
+    <row r="45" spans="2:10" ht="31.5" hidden="1">
       <c r="B45" s="2" t="s">
         <v>21</v>
       </c>
@@ -6430,7 +6551,7 @@
     <row r="48" spans="2:10">
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="2:9" ht="17" hidden="1">
+    <row r="49" spans="2:9" hidden="1">
       <c r="B49" s="2" t="s">
         <v>149</v>
       </c>
@@ -6450,7 +6571,7 @@
     <row r="50" spans="2:9">
       <c r="D50" s="7"/>
     </row>
-    <row r="51" spans="2:9" ht="34" hidden="1">
+    <row r="51" spans="2:9" ht="31.5" hidden="1">
       <c r="B51" s="2" t="s">
         <v>21</v>
       </c>
@@ -6467,7 +6588,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="2:9" ht="34" hidden="1">
+    <row r="52" spans="2:9" ht="31.5" hidden="1">
       <c r="C52" s="2" t="s">
         <v>165</v>
       </c>
@@ -6478,7 +6599,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="53" spans="2:9" ht="68">
+    <row r="53" spans="2:9" ht="63">
       <c r="D53" s="10" t="s">
         <v>171</v>
       </c>
@@ -6486,7 +6607,7 @@
     <row r="54" spans="2:9">
       <c r="D54" s="7"/>
     </row>
-    <row r="55" spans="2:9" ht="17">
+    <row r="55" spans="2:9">
       <c r="B55" s="2" t="s">
         <v>24</v>
       </c>
@@ -6667,20 +6788,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C0E0CA-5258-DA42-9AFB-0582B12738D1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE45D646-5865-4DD3-B066-A6FB8031C09E}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A74"/>
@@ -6689,9 +6810,9 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="112.6640625" customWidth="1"/>
+    <col min="1" max="1" width="112.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18" thickBot="1">
@@ -6699,7 +6820,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17" thickTop="1"/>
+    <row r="2" spans="1:1" ht="16.5" thickTop="1"/>
     <row r="3" spans="1:1">
       <c r="A3" s="24" t="s">
         <v>98</v>
@@ -6806,7 +6927,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="17" thickTop="1"/>
+    <row r="28" spans="1:1" ht="16.5" thickTop="1"/>
     <row r="29" spans="1:1">
       <c r="A29" s="26" t="s">
         <v>115</v>
@@ -6862,7 +6983,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="17" thickTop="1"/>
+    <row r="42" spans="1:1" ht="16.5" thickTop="1"/>
     <row r="43" spans="1:1">
       <c r="A43" s="22" t="s">
         <v>69</v>
@@ -7025,7 +7146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267B328E-A616-48A5-B37D-5A675A5748D9}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C51"/>
@@ -7034,9 +7155,9 @@
       <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="109.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="109.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7045,7 +7166,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" thickTop="1"/>
+    <row r="2" spans="1:3" ht="16.5" thickTop="1"/>
     <row r="4" spans="1:3">
       <c r="A4" s="16" t="s">
         <v>37</v>
@@ -7102,7 +7223,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="17">
+    <row r="18" spans="1:1" ht="31.5">
       <c r="A18" s="15" t="s">
         <v>38</v>
       </c>
@@ -7110,27 +7231,27 @@
     <row r="19" spans="1:1">
       <c r="A19" s="16"/>
     </row>
-    <row r="20" spans="1:1" ht="17">
+    <row r="20" spans="1:1">
       <c r="A20" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="17">
+    <row r="21" spans="1:1">
       <c r="A21" s="17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="17">
+    <row r="22" spans="1:1">
       <c r="A22" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="17">
+    <row r="23" spans="1:1">
       <c r="A23" s="17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="34">
+    <row r="24" spans="1:1" ht="31.5">
       <c r="A24" s="18" t="s">
         <v>43</v>
       </c>
@@ -7264,7 +7385,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E19437AE-572B-6E4F-9B26-5FD12EFDDDFB}">
   <dimension ref="B3"/>
   <sheetViews>
@@ -7272,7 +7393,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Add photoServer, photoResInsert, relPathField, fileNameField parameters to PhotoPlaybackWidget
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEE1A35-426A-4FD2-BF52-E9808B74BDCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E231A1DB-514B-4E62-A80A-7103B9A3352C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
-    <sheet name="sync_photos" sheetId="11" r:id="rId1"/>
+    <sheet name="photoImage" sheetId="12" r:id="rId1"/>
     <sheet name="to do" sheetId="1" r:id="rId2"/>
     <sheet name="screen captures" sheetId="10" r:id="rId3"/>
     <sheet name="extent history" sheetId="8" r:id="rId4"/>
     <sheet name="resize imagery on splitter drag" sheetId="7" r:id="rId5"/>
     <sheet name="possible Tristan jobs" sheetId="9" r:id="rId6"/>
+    <sheet name="DONE_sync_photos" sheetId="11" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$102</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="180">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -5230,12 +5231,18 @@
   <si>
     <t>Replace with (?):</t>
   </si>
+  <si>
+    <t>szPhotoWidget.sync_photos = [True/False]</t>
+  </si>
+  <si>
+    <t>rename photoImage as szPhotoImage and ssPhotoImage?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29">
+  <fonts count="31">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5451,8 +5458,23 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9.8000000000000007"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF008000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5462,6 +5484,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5494,7 +5522,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5615,14 +5643,20 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="7" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Heading 2" xfId="6" builtinId="17"/>
@@ -5654,20 +5688,25 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="8866667" cy="3961905"/>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>379924</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123309</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8DED24D-4DDE-482E-AA46-9AE983789186}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F33BB346-53EC-4945-83AA-49D63D3B57FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5684,7 +5723,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8866667" cy="3961905"/>
+          <a:ext cx="8609524" cy="4123809"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5692,7 +5731,51 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1122609</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>151931</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6D8D733-FEC0-4FF5-A9E7-C689396C5286}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4600575"/>
+          <a:ext cx="10723809" cy="3752381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5742,6 +5825,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="8866667" cy="3961905"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8DED24D-4DDE-482E-AA46-9AE983789186}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8866667" cy="3961905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6041,33 +6168,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB0B7B4-8613-440E-8760-4618937ED99C}">
-  <dimension ref="B23:B25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C107A0-3D2A-4B99-B594-96B25D57F2E7}">
+  <dimension ref="O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9" style="45"/>
-    <col min="2" max="2" width="36.625" style="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="45"/>
+    <col min="15" max="15" width="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="23" spans="2:2">
-      <c r="B23" s="47" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" s="46" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" s="46" t="s">
-        <v>175</v>
+    <row r="5" spans="15:15">
+      <c r="O5" s="49" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -6086,7 +6201,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D58" sqref="D58"/>
+      <selection pane="bottomRight" activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -7303,7 +7418,7 @@
       <c r="A38" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="44" t="s">
+      <c r="C38" s="48" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7311,13 +7426,13 @@
       <c r="A39" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="44"/>
+      <c r="C39" s="48"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="44" t="s">
+      <c r="C40" s="48" t="s">
         <v>66</v>
       </c>
     </row>
@@ -7325,7 +7440,7 @@
       <c r="A41" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="44"/>
+      <c r="C41" s="48"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="21" t="s">
@@ -7406,4 +7521,46 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB0B7B4-8613-440E-8760-4618937ED99C}">
+  <dimension ref="B23:B27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9" style="44"/>
+    <col min="2" max="2" width="36.625" style="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="44"/>
+  </cols>
+  <sheetData>
+    <row r="23" spans="2:2">
+      <c r="B23" s="45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="46" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="46" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="47" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change more column widths, correlate photo/video point visibility between map layers & clickableLayers
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimnoel/WebstormProjects/ShoreZoneDev_JS4x/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CE8CC2-30A9-6047-BD1E-704AAD1073F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DD491C-6052-F247-A600-F4DFBCEBE495}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$111</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="96">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -414,6 +414,18 @@
   </si>
   <si>
     <t>not using Axiom anymore, so moot point</t>
+  </si>
+  <si>
+    <t>Site/Station zoom to some specific scale</t>
+  </si>
+  <si>
+    <t>regions table sometimes disappears when going bak from subareas tab</t>
+  </si>
+  <si>
+    <t>remove "search result" popup on using locator</t>
+  </si>
+  <si>
+    <t>new SZ fields not done yet</t>
   </si>
 </sst>
 </file>
@@ -1297,13 +1309,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J107"/>
+  <dimension ref="A1:J111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D112" sqref="D112"/>
+      <selection pane="bottomRight" activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -1989,49 +2001,72 @@
     <row r="96" spans="4:4" hidden="1">
       <c r="D96" s="6"/>
     </row>
-    <row r="97" spans="1:4" hidden="1">
+    <row r="97" spans="1:9" hidden="1">
       <c r="D97" s="6"/>
     </row>
-    <row r="98" spans="1:4" hidden="1">
+    <row r="98" spans="1:9" hidden="1">
       <c r="D98" s="6"/>
     </row>
-    <row r="99" spans="1:4" hidden="1">
+    <row r="99" spans="1:9" hidden="1">
       <c r="D99" s="6"/>
     </row>
-    <row r="100" spans="1:4" hidden="1">
+    <row r="100" spans="1:9" hidden="1">
       <c r="D100" s="6"/>
     </row>
-    <row r="101" spans="1:4" hidden="1">
+    <row r="101" spans="1:9" hidden="1">
       <c r="D101" s="6"/>
     </row>
-    <row r="102" spans="1:4" hidden="1">
+    <row r="102" spans="1:9" hidden="1">
       <c r="A102" s="6">
         <v>0</v>
       </c>
       <c r="D102" s="6"/>
     </row>
-    <row r="104" spans="1:4" ht="34">
+    <row r="103" spans="1:9" hidden="1"/>
+    <row r="104" spans="1:9" ht="34">
       <c r="D104" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="17">
+    <row r="105" spans="1:9" ht="17">
       <c r="D105" s="9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="17">
+    <row r="106" spans="1:9" ht="17" hidden="1">
+      <c r="C106" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="D106" s="9" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" ht="17">
+      <c r="I106" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="17">
       <c r="D107" s="9" t="s">
         <v>90</v>
       </c>
     </row>
+    <row r="108" spans="1:9" ht="17">
+      <c r="D108" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" hidden="1"/>
+    <row r="110" spans="1:9" ht="34">
+      <c r="D110" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="17">
+      <c r="D111" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I102" xr:uid="{6CDD44CA-3159-4ADC-A892-9FFB6DB01C72}">
+  <autoFilter ref="A1:I111" xr:uid="{9828EF7F-101C-E647-87AD-55E99BD78B9A}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Initialize with FA or SS, "Simple ShoreZone" with Units panel collapsed.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimnoel/WebstormProjects/ShoreZoneDev_JS4x/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DD491C-6052-F247-A600-F4DFBCEBE495}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9951B6AE-62FD-4B44-9A61-8EEBBBCE6CE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -419,13 +419,25 @@
     <t>Site/Station zoom to some specific scale</t>
   </si>
   <si>
-    <t>regions table sometimes disappears when going bak from subareas tab</t>
-  </si>
-  <si>
     <t>remove "search result" popup on using locator</t>
   </si>
   <si>
     <t>new SZ fields not done yet</t>
+  </si>
+  <si>
+    <t>show/hide Video Flightline legend</t>
+  </si>
+  <si>
+    <t>regions table sometimes disappears when going back from subareas tab</t>
+  </si>
+  <si>
+    <t>smaller popups</t>
+  </si>
+  <si>
+    <t>track widths of cell contents for each column, and use to set column width</t>
+  </si>
+  <si>
+    <t>compress SS photos</t>
   </si>
 </sst>
 </file>
@@ -1309,13 +1321,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J111"/>
+  <dimension ref="A1:J117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D116" sqref="D116"/>
+      <selection pane="bottomRight" activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -2023,7 +2035,10 @@
       <c r="D102" s="6"/>
     </row>
     <row r="103" spans="1:9" hidden="1"/>
-    <row r="104" spans="1:9" ht="34">
+    <row r="104" spans="1:9" ht="34" hidden="1">
+      <c r="C104" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="D104" s="9" t="s">
         <v>87</v>
       </c>
@@ -2041,7 +2056,7 @@
         <v>89</v>
       </c>
       <c r="I106" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="17">
@@ -2057,12 +2072,32 @@
     <row r="109" spans="1:9" hidden="1"/>
     <row r="110" spans="1:9" ht="34">
       <c r="D110" s="9" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="17">
       <c r="D111" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="113" spans="4:4" ht="17">
+      <c r="D113" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="114" spans="4:4" ht="17">
+      <c r="D114" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="116" spans="4:4" ht="34">
+      <c r="D116" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="117" spans="4:4" ht="17">
+      <c r="D117" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tooltip text for lock and link buttons.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimnoel/WebstormProjects/ShoreZoneDev_JS4x/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9951B6AE-62FD-4B44-9A61-8EEBBBCE6CE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11EBFAF-ACB3-6646-B610-C88A6A6FDE01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="101">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>compress SS photos</t>
+  </si>
+  <si>
+    <t>get highres verson of photo on right-click:download</t>
   </si>
 </sst>
 </file>
@@ -1321,13 +1324,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J117"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D118" sqref="D118"/>
+      <selection pane="bottomRight" activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -2098,6 +2101,11 @@
     <row r="117" spans="4:4" ht="17">
       <c r="D117" s="9" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="118" spans="4:4" ht="17">
+      <c r="D118" s="9" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix initial layout selection for default.htm
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimnoel/WebstormProjects/ShoreZoneDev_JS4x/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11EBFAF-ACB3-6646-B610-C88A6A6FDE01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14759F52-F2D9-4748-A435-8A6A74FD9869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$118</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="103">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -441,6 +441,12 @@
   </si>
   <si>
     <t>get highres verson of photo on right-click:download</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>bring up to 10.14  (and make bookmarks work under this)</t>
   </si>
 </sst>
 </file>
@@ -1262,23 +1268,23 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="21"/>
   <cols>
     <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="21.875" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="26">
+    <row r="1" spans="1:2" ht="26.25">
       <c r="A1" s="21" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="24">
+    <row r="3" spans="1:2" ht="23.25">
       <c r="A3" s="22">
         <v>4.13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409" customHeight="1">
+    <row r="4" spans="1:2" ht="408.95" customHeight="1">
       <c r="B4" s="23" t="s">
         <v>82</v>
       </c>
@@ -1289,28 +1295,28 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="398" customHeight="1">
+    <row r="7" spans="1:2" ht="398.1" customHeight="1">
       <c r="B7" s="23" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="24">
+    <row r="8" spans="1:2" ht="23.25">
       <c r="A8" s="22">
         <v>4.12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="76" customHeight="1">
+    <row r="9" spans="1:2" ht="75.95" customHeight="1">
       <c r="B9" s="23" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="409" customHeight="1">
+    <row r="10" spans="1:2" ht="408.95" customHeight="1">
       <c r="B10" s="23" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="177" customHeight="1"/>
-    <row r="12" spans="1:2" ht="185" customHeight="1"/>
+    <row r="12" spans="1:2" ht="185.1" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="https://developers.arcgis.com/javascript/latest/guide/release-notes/" xr:uid="{9B90A93B-81C7-0348-B902-045AB450F6B0}"/>
@@ -1324,26 +1330,26 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J118"/>
+  <dimension ref="A1:J120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D119" sqref="D119"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.625" style="2" customWidth="1"/>
     <col min="4" max="4" width="53.5" style="9" customWidth="1"/>
     <col min="5" max="5" width="4.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="62.6640625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="32.1640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="24.625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="16.625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="14.625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="62.625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="32.125" style="6" customWidth="1"/>
     <col min="11" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -1433,7 +1439,7 @@
     <row r="7" spans="1:9" hidden="1">
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:9" ht="34" hidden="1">
+    <row r="8" spans="1:9" ht="31.5" hidden="1">
       <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1457,7 +1463,7 @@
     <row r="9" spans="1:9" hidden="1">
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="68" hidden="1">
+    <row r="10" spans="1:9" ht="63" hidden="1">
       <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1509,7 +1515,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" spans="1:9" ht="34" hidden="1">
+    <row r="16" spans="1:9" ht="31.5" hidden="1">
       <c r="C16" s="2" t="s">
         <v>71</v>
       </c>
@@ -1541,7 +1547,7 @@
     <row r="20" spans="1:9" hidden="1">
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:9" ht="34" hidden="1">
+    <row r="21" spans="1:9" ht="31.5" hidden="1">
       <c r="C21" s="2" t="s">
         <v>71</v>
       </c>
@@ -1553,7 +1559,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="34" hidden="1">
+    <row r="22" spans="1:9" ht="31.5" hidden="1">
       <c r="C22" s="2" t="s">
         <v>72</v>
       </c>
@@ -1565,7 +1571,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="17" hidden="1">
+    <row r="23" spans="1:9" hidden="1">
       <c r="A23" s="6" t="s">
         <v>11</v>
       </c>
@@ -1579,7 +1585,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="17" hidden="1">
+    <row r="24" spans="1:9" hidden="1">
       <c r="A24" s="6" t="s">
         <v>11</v>
       </c>
@@ -1610,7 +1616,7 @@
     <row r="27" spans="1:9" hidden="1">
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:9" ht="34">
+    <row r="28" spans="1:9" ht="39.950000000000003" customHeight="1">
       <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
@@ -1643,18 +1649,21 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="17">
+    <row r="32" spans="1:9" hidden="1">
       <c r="B32" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="C32" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="D32" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="2:10" hidden="1">
+    <row r="33" spans="1:10" hidden="1">
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="2:10" hidden="1">
+    <row r="34" spans="1:10" hidden="1">
       <c r="C34" s="2" t="s">
         <v>72</v>
       </c>
@@ -1663,7 +1672,7 @@
       </c>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="2:10" ht="17" hidden="1">
+    <row r="35" spans="1:10" hidden="1">
       <c r="B35" s="2" t="s">
         <v>21</v>
       </c>
@@ -1674,7 +1683,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="34" hidden="1">
+    <row r="36" spans="1:10" ht="31.5" hidden="1">
       <c r="B36" s="2" t="s">
         <v>21</v>
       </c>
@@ -1688,10 +1697,10 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="2:10" hidden="1">
+    <row r="37" spans="1:10" hidden="1">
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="2:10" ht="136" hidden="1">
+    <row r="38" spans="1:10" ht="126" hidden="1">
       <c r="B38" s="2" t="s">
         <v>24</v>
       </c>
@@ -1711,10 +1720,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="2:10" hidden="1">
+    <row r="39" spans="1:10" hidden="1">
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="2:10" ht="51" hidden="1">
+    <row r="40" spans="1:10" ht="47.25" hidden="1">
       <c r="C40" s="2" t="s">
         <v>71</v>
       </c>
@@ -1734,10 +1743,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="2:10" hidden="1">
+    <row r="41" spans="1:10" hidden="1">
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="2:10" ht="34" hidden="1">
+    <row r="42" spans="1:10" ht="31.5" hidden="1">
       <c r="B42" s="2" t="s">
         <v>21</v>
       </c>
@@ -1760,10 +1769,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="2:10" hidden="1">
+    <row r="43" spans="1:10" hidden="1">
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="2:10" ht="17" hidden="1">
+    <row r="44" spans="1:10" hidden="1">
       <c r="B44" s="2" t="s">
         <v>21</v>
       </c>
@@ -1774,7 +1783,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="2:10" ht="34" hidden="1">
+    <row r="45" spans="1:10" ht="31.5" hidden="1">
       <c r="B45" s="2" t="s">
         <v>21</v>
       </c>
@@ -1785,7 +1794,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="2:10">
+    <row r="46" spans="1:10" hidden="1">
+      <c r="A46" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="D46" s="6" t="s">
         <v>73</v>
       </c>
@@ -1793,7 +1805,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="2:10" hidden="1">
+    <row r="47" spans="1:10" hidden="1">
       <c r="C47" s="2" t="s">
         <v>72</v>
       </c>
@@ -1801,10 +1813,10 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="2:10" hidden="1">
+    <row r="48" spans="1:10" hidden="1">
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:9" ht="17" hidden="1">
+    <row r="49" spans="1:9" hidden="1">
       <c r="B49" s="2" t="s">
         <v>55</v>
       </c>
@@ -1827,7 +1839,7 @@
     <row r="50" spans="1:9" hidden="1">
       <c r="D50" s="6"/>
     </row>
-    <row r="51" spans="1:9" ht="34" hidden="1">
+    <row r="51" spans="1:9" ht="31.5" hidden="1">
       <c r="B51" s="2" t="s">
         <v>21</v>
       </c>
@@ -1844,7 +1856,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="34" hidden="1">
+    <row r="52" spans="1:9" ht="31.5" hidden="1">
       <c r="C52" s="2" t="s">
         <v>71</v>
       </c>
@@ -1855,7 +1867,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="68" hidden="1">
+    <row r="53" spans="1:9" ht="63" hidden="1">
       <c r="A53" s="6" t="s">
         <v>11</v>
       </c>
@@ -1866,7 +1878,7 @@
     <row r="54" spans="1:9" hidden="1">
       <c r="D54" s="6"/>
     </row>
-    <row r="55" spans="1:9" ht="17" hidden="1">
+    <row r="55" spans="1:9" hidden="1">
       <c r="B55" s="2" t="s">
         <v>24</v>
       </c>
@@ -1883,7 +1895,7 @@
     <row r="56" spans="1:9" hidden="1">
       <c r="D56" s="6"/>
     </row>
-    <row r="57" spans="1:9" ht="17" hidden="1">
+    <row r="57" spans="1:9" hidden="1">
       <c r="C57" s="2" t="s">
         <v>71</v>
       </c>
@@ -1908,208 +1920,143 @@
     <row r="60" spans="1:9" hidden="1">
       <c r="D60" s="6"/>
     </row>
-    <row r="61" spans="1:9" hidden="1">
-      <c r="D61" s="6"/>
-    </row>
-    <row r="62" spans="1:9" hidden="1">
-      <c r="D62" s="6"/>
-    </row>
-    <row r="63" spans="1:9" hidden="1">
-      <c r="D63" s="6"/>
+    <row r="61" spans="1:9" hidden="1"/>
+    <row r="62" spans="1:9" ht="31.5" hidden="1">
+      <c r="C62" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="20.100000000000001" hidden="1" customHeight="1">
+      <c r="A63" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="64" spans="1:9" hidden="1">
-      <c r="D64" s="6"/>
-    </row>
-    <row r="65" spans="4:4" hidden="1">
-      <c r="D65" s="6"/>
-    </row>
-    <row r="66" spans="4:4" hidden="1">
-      <c r="D66" s="6"/>
-    </row>
-    <row r="67" spans="4:4" hidden="1">
-      <c r="D67" s="6"/>
-    </row>
-    <row r="68" spans="4:4" hidden="1">
-      <c r="D68" s="6"/>
-    </row>
-    <row r="69" spans="4:4" hidden="1">
-      <c r="D69" s="6"/>
-    </row>
-    <row r="70" spans="4:4" hidden="1">
-      <c r="D70" s="6"/>
-    </row>
-    <row r="71" spans="4:4" hidden="1">
-      <c r="D71" s="6"/>
-    </row>
-    <row r="72" spans="4:4" hidden="1">
-      <c r="D72" s="6"/>
-    </row>
-    <row r="73" spans="4:4" hidden="1">
-      <c r="D73" s="6"/>
-    </row>
-    <row r="74" spans="4:4" hidden="1">
-      <c r="D74" s="6"/>
-    </row>
-    <row r="75" spans="4:4" hidden="1">
-      <c r="D75" s="6"/>
-    </row>
-    <row r="76" spans="4:4" hidden="1">
-      <c r="D76" s="6"/>
-    </row>
-    <row r="77" spans="4:4" hidden="1">
-      <c r="D77" s="6"/>
-    </row>
-    <row r="78" spans="4:4" hidden="1">
-      <c r="D78" s="6"/>
-    </row>
-    <row r="79" spans="4:4" hidden="1">
-      <c r="D79" s="6"/>
-    </row>
-    <row r="80" spans="4:4" hidden="1">
-      <c r="D80" s="6"/>
-    </row>
-    <row r="81" spans="4:4" hidden="1">
-      <c r="D81" s="6"/>
-    </row>
-    <row r="82" spans="4:4" hidden="1">
-      <c r="D82" s="6"/>
-    </row>
-    <row r="83" spans="4:4" hidden="1">
-      <c r="D83" s="6"/>
-    </row>
-    <row r="84" spans="4:4" hidden="1">
-      <c r="D84" s="6"/>
-    </row>
-    <row r="85" spans="4:4" hidden="1">
-      <c r="D85" s="6"/>
-    </row>
-    <row r="86" spans="4:4" hidden="1">
-      <c r="D86" s="6"/>
-    </row>
-    <row r="87" spans="4:4" hidden="1">
-      <c r="D87" s="6"/>
-    </row>
-    <row r="88" spans="4:4" hidden="1">
-      <c r="D88" s="6"/>
-    </row>
-    <row r="89" spans="4:4" hidden="1">
-      <c r="D89" s="6"/>
-    </row>
-    <row r="90" spans="4:4" hidden="1">
-      <c r="D90" s="6"/>
-    </row>
-    <row r="91" spans="4:4" hidden="1">
-      <c r="D91" s="6"/>
-    </row>
-    <row r="92" spans="4:4" hidden="1">
-      <c r="D92" s="6"/>
-    </row>
-    <row r="93" spans="4:4" hidden="1">
-      <c r="D93" s="6"/>
-    </row>
-    <row r="94" spans="4:4" hidden="1">
-      <c r="D94" s="6"/>
-    </row>
-    <row r="95" spans="4:4" hidden="1">
-      <c r="D95" s="6"/>
-    </row>
-    <row r="96" spans="4:4" hidden="1">
-      <c r="D96" s="6"/>
-    </row>
-    <row r="97" spans="1:9" hidden="1">
-      <c r="D97" s="6"/>
-    </row>
-    <row r="98" spans="1:9" hidden="1">
-      <c r="D98" s="6"/>
-    </row>
-    <row r="99" spans="1:9" hidden="1">
-      <c r="D99" s="6"/>
-    </row>
-    <row r="100" spans="1:9" hidden="1">
-      <c r="D100" s="6"/>
-    </row>
-    <row r="101" spans="1:9" hidden="1">
-      <c r="D101" s="6"/>
-    </row>
-    <row r="102" spans="1:9" hidden="1">
-      <c r="A102" s="6">
-        <v>0</v>
-      </c>
-      <c r="D102" s="6"/>
-    </row>
-    <row r="103" spans="1:9" hidden="1"/>
-    <row r="104" spans="1:9" ht="34" hidden="1">
-      <c r="C104" s="2" t="s">
+      <c r="C64" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="I64" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" hidden="1">
+      <c r="C65" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D104" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" ht="17">
-      <c r="D105" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" ht="17" hidden="1">
-      <c r="C106" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D106" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="I106" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" ht="17">
-      <c r="D107" s="9" t="s">
+      <c r="D65" s="9" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="17">
-      <c r="D108" s="9" t="s">
+    <row r="66" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="D66" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="109" spans="1:9" hidden="1"/>
-    <row r="110" spans="1:9" ht="34">
-      <c r="D110" s="9" t="s">
+    <row r="67" spans="1:4" hidden="1"/>
+    <row r="68" spans="1:4" ht="39.950000000000003" customHeight="1">
+      <c r="D68" s="9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="17">
-      <c r="D111" s="9" t="s">
+    <row r="69" spans="1:4" hidden="1">
+      <c r="C69" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D69" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="113" spans="4:4" ht="17">
-      <c r="D113" s="9" t="s">
+    <row r="70" spans="1:4" hidden="1"/>
+    <row r="71" spans="1:4" hidden="1">
+      <c r="C71" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D71" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="114" spans="4:4" ht="17">
-      <c r="D114" s="9" t="s">
+    <row r="72" spans="1:4" ht="20.100000000000001" hidden="1" customHeight="1">
+      <c r="A72" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D72" s="9" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="116" spans="4:4" ht="34">
-      <c r="D116" s="9" t="s">
+    <row r="73" spans="1:4" hidden="1"/>
+    <row r="74" spans="1:4" ht="39.950000000000003" customHeight="1">
+      <c r="D74" s="9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="117" spans="4:4" ht="17">
-      <c r="D117" s="9" t="s">
+    <row r="75" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="D75" s="9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="118" spans="4:4" ht="17">
-      <c r="D118" s="9" t="s">
+    <row r="76" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="D76" s="9" t="s">
         <v>100</v>
       </c>
     </row>
+    <row r="77" spans="1:4" hidden="1"/>
+    <row r="78" spans="1:4" hidden="1"/>
+    <row r="79" spans="1:4" hidden="1"/>
+    <row r="80" spans="1:4" hidden="1"/>
+    <row r="81" hidden="1"/>
+    <row r="82" hidden="1"/>
+    <row r="83" hidden="1"/>
+    <row r="84" hidden="1"/>
+    <row r="85" hidden="1"/>
+    <row r="86" hidden="1"/>
+    <row r="87" hidden="1"/>
+    <row r="88" hidden="1"/>
+    <row r="89" hidden="1"/>
+    <row r="90" hidden="1"/>
+    <row r="91" hidden="1"/>
+    <row r="92" hidden="1"/>
+    <row r="93" hidden="1"/>
+    <row r="94" hidden="1"/>
+    <row r="95" hidden="1"/>
+    <row r="96" hidden="1"/>
+    <row r="97" hidden="1"/>
+    <row r="98" hidden="1"/>
+    <row r="99" hidden="1"/>
+    <row r="100" hidden="1"/>
+    <row r="101" hidden="1"/>
+    <row r="102" hidden="1"/>
+    <row r="103" hidden="1"/>
+    <row r="104" hidden="1"/>
+    <row r="105" hidden="1"/>
+    <row r="106" hidden="1"/>
+    <row r="107" hidden="1"/>
+    <row r="108" hidden="1"/>
+    <row r="109" hidden="1"/>
+    <row r="110" hidden="1"/>
+    <row r="111" hidden="1"/>
+    <row r="112" hidden="1"/>
+    <row r="113" spans="4:4" hidden="1"/>
+    <row r="114" spans="4:4" hidden="1"/>
+    <row r="115" spans="4:4" hidden="1"/>
+    <row r="116" spans="4:4" hidden="1"/>
+    <row r="117" spans="4:4" hidden="1"/>
+    <row r="118" spans="4:4" hidden="1"/>
+    <row r="120" spans="4:4">
+      <c r="D120" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I111" xr:uid="{9828EF7F-101C-E647-87AD-55E99BD78B9A}">
+  <autoFilter ref="A1:I118" xr:uid="{3D8B8C54-31AE-4B49-AB74-3ED34CE5744B}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Use compressed SS photos, hide LL when not in SZ, plus/minus icons for video speed.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14759F52-F2D9-4748-A435-8A6A74FD9869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF849F7-318A-4F8D-BCBF-D22CF84B9AF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="4245" yWindow="885" windowWidth="23415" windowHeight="14715" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$118</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$500</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="111">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -447,6 +447,30 @@
   </si>
   <si>
     <t>bring up to 10.14  (and make bookmarks work under this)</t>
+  </si>
+  <si>
+    <t>checkbox for global/inView on searchWidget</t>
+  </si>
+  <si>
+    <t>hide LayerList when in FA/SS?</t>
+  </si>
+  <si>
+    <t>change "eye" checkbox in LayerList to regular box?</t>
+  </si>
+  <si>
+    <t>compare speeds of services on NOAA &amp; PSMFC servers</t>
+  </si>
+  <si>
+    <t>go to locale/site from maptip</t>
+  </si>
+  <si>
+    <t>put widget inside DIV, add checkbox at bottom of DIV?</t>
+  </si>
+  <si>
+    <t>keep track of user state, so stays off in SZ mode when user has turned off?</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -1330,13 +1354,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D125" sqref="D125"/>
+      <selection pane="bottomRight" activeCell="D506" sqref="D506"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1345,9 +1369,9 @@
     <col min="2" max="3" width="5.625" style="2" customWidth="1"/>
     <col min="4" max="4" width="53.5" style="9" customWidth="1"/>
     <col min="5" max="5" width="4.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="24.625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="16.625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="14.625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="11.25" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="8.125" style="9" customWidth="1"/>
     <col min="9" max="9" width="62.625" style="11" customWidth="1"/>
     <col min="10" max="10" width="32.125" style="6" customWidth="1"/>
     <col min="11" max="16384" width="9" style="6"/>
@@ -1998,7 +2022,10 @@
         <v>98</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="75" spans="1:4" ht="20.100000000000001" hidden="1" customHeight="1">
+      <c r="C75" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="D75" s="9" t="s">
         <v>99</v>
       </c>
@@ -2044,19 +2071,433 @@
     <row r="110" hidden="1"/>
     <row r="111" hidden="1"/>
     <row r="112" hidden="1"/>
-    <row r="113" spans="4:4" hidden="1"/>
-    <row r="114" spans="4:4" hidden="1"/>
-    <row r="115" spans="4:4" hidden="1"/>
-    <row r="116" spans="4:4" hidden="1"/>
-    <row r="117" spans="4:4" hidden="1"/>
-    <row r="118" spans="4:4" hidden="1"/>
-    <row r="120" spans="4:4">
+    <row r="113" spans="3:9" hidden="1"/>
+    <row r="114" spans="3:9" hidden="1"/>
+    <row r="115" spans="3:9" hidden="1"/>
+    <row r="116" spans="3:9" hidden="1"/>
+    <row r="117" spans="3:9" hidden="1"/>
+    <row r="118" spans="3:9" hidden="1"/>
+    <row r="119" spans="3:9" hidden="1"/>
+    <row r="120" spans="3:9">
       <c r="D120" s="9" t="s">
         <v>102</v>
       </c>
     </row>
+    <row r="121" spans="3:9" hidden="1"/>
+    <row r="122" spans="3:9">
+      <c r="D122" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I122" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="123" spans="3:9" hidden="1"/>
+    <row r="124" spans="3:9" hidden="1">
+      <c r="C124" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D124" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I124" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="125" spans="3:9" hidden="1"/>
+    <row r="126" spans="3:9">
+      <c r="D126" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="127" spans="3:9" hidden="1"/>
+    <row r="128" spans="3:9">
+      <c r="D128" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="129" spans="4:4" hidden="1"/>
+    <row r="130" spans="4:4">
+      <c r="D130" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="131" spans="4:4" hidden="1"/>
+    <row r="132" spans="4:4" hidden="1"/>
+    <row r="133" spans="4:4" hidden="1"/>
+    <row r="134" spans="4:4" hidden="1"/>
+    <row r="135" spans="4:4" hidden="1"/>
+    <row r="136" spans="4:4" hidden="1"/>
+    <row r="137" spans="4:4" hidden="1"/>
+    <row r="138" spans="4:4" hidden="1"/>
+    <row r="139" spans="4:4" hidden="1"/>
+    <row r="140" spans="4:4" hidden="1"/>
+    <row r="141" spans="4:4" hidden="1"/>
+    <row r="142" spans="4:4" hidden="1"/>
+    <row r="143" spans="4:4" hidden="1"/>
+    <row r="144" spans="4:4" hidden="1"/>
+    <row r="145" hidden="1"/>
+    <row r="146" hidden="1"/>
+    <row r="147" hidden="1"/>
+    <row r="148" hidden="1"/>
+    <row r="149" hidden="1"/>
+    <row r="150" hidden="1"/>
+    <row r="151" hidden="1"/>
+    <row r="152" hidden="1"/>
+    <row r="153" hidden="1"/>
+    <row r="154" hidden="1"/>
+    <row r="155" hidden="1"/>
+    <row r="156" hidden="1"/>
+    <row r="157" hidden="1"/>
+    <row r="158" hidden="1"/>
+    <row r="159" hidden="1"/>
+    <row r="160" hidden="1"/>
+    <row r="161" hidden="1"/>
+    <row r="162" hidden="1"/>
+    <row r="163" hidden="1"/>
+    <row r="164" hidden="1"/>
+    <row r="165" hidden="1"/>
+    <row r="166" hidden="1"/>
+    <row r="167" hidden="1"/>
+    <row r="168" hidden="1"/>
+    <row r="169" hidden="1"/>
+    <row r="170" hidden="1"/>
+    <row r="171" hidden="1"/>
+    <row r="172" hidden="1"/>
+    <row r="173" hidden="1"/>
+    <row r="174" hidden="1"/>
+    <row r="175" hidden="1"/>
+    <row r="176" hidden="1"/>
+    <row r="177" hidden="1"/>
+    <row r="178" hidden="1"/>
+    <row r="179" hidden="1"/>
+    <row r="180" hidden="1"/>
+    <row r="181" hidden="1"/>
+    <row r="182" hidden="1"/>
+    <row r="183" hidden="1"/>
+    <row r="184" hidden="1"/>
+    <row r="185" hidden="1"/>
+    <row r="186" hidden="1"/>
+    <row r="187" hidden="1"/>
+    <row r="188" hidden="1"/>
+    <row r="189" hidden="1"/>
+    <row r="190" hidden="1"/>
+    <row r="191" hidden="1"/>
+    <row r="192" hidden="1"/>
+    <row r="193" hidden="1"/>
+    <row r="194" hidden="1"/>
+    <row r="195" hidden="1"/>
+    <row r="196" hidden="1"/>
+    <row r="197" hidden="1"/>
+    <row r="198" hidden="1"/>
+    <row r="199" hidden="1"/>
+    <row r="200" hidden="1"/>
+    <row r="201" hidden="1"/>
+    <row r="202" hidden="1"/>
+    <row r="203" hidden="1"/>
+    <row r="204" hidden="1"/>
+    <row r="205" hidden="1"/>
+    <row r="206" hidden="1"/>
+    <row r="207" hidden="1"/>
+    <row r="208" hidden="1"/>
+    <row r="209" hidden="1"/>
+    <row r="210" hidden="1"/>
+    <row r="211" hidden="1"/>
+    <row r="212" hidden="1"/>
+    <row r="213" hidden="1"/>
+    <row r="214" hidden="1"/>
+    <row r="215" hidden="1"/>
+    <row r="216" hidden="1"/>
+    <row r="217" hidden="1"/>
+    <row r="218" hidden="1"/>
+    <row r="219" hidden="1"/>
+    <row r="220" hidden="1"/>
+    <row r="221" hidden="1"/>
+    <row r="222" hidden="1"/>
+    <row r="223" hidden="1"/>
+    <row r="224" hidden="1"/>
+    <row r="225" hidden="1"/>
+    <row r="226" hidden="1"/>
+    <row r="227" hidden="1"/>
+    <row r="228" hidden="1"/>
+    <row r="229" hidden="1"/>
+    <row r="230" hidden="1"/>
+    <row r="231" hidden="1"/>
+    <row r="232" hidden="1"/>
+    <row r="233" hidden="1"/>
+    <row r="234" hidden="1"/>
+    <row r="235" hidden="1"/>
+    <row r="236" hidden="1"/>
+    <row r="237" hidden="1"/>
+    <row r="238" hidden="1"/>
+    <row r="239" hidden="1"/>
+    <row r="240" hidden="1"/>
+    <row r="241" hidden="1"/>
+    <row r="242" hidden="1"/>
+    <row r="243" hidden="1"/>
+    <row r="244" hidden="1"/>
+    <row r="245" hidden="1"/>
+    <row r="246" hidden="1"/>
+    <row r="247" hidden="1"/>
+    <row r="248" hidden="1"/>
+    <row r="249" hidden="1"/>
+    <row r="250" hidden="1"/>
+    <row r="251" hidden="1"/>
+    <row r="252" hidden="1"/>
+    <row r="253" hidden="1"/>
+    <row r="254" hidden="1"/>
+    <row r="255" hidden="1"/>
+    <row r="256" hidden="1"/>
+    <row r="257" hidden="1"/>
+    <row r="258" hidden="1"/>
+    <row r="259" hidden="1"/>
+    <row r="260" hidden="1"/>
+    <row r="261" hidden="1"/>
+    <row r="262" hidden="1"/>
+    <row r="263" hidden="1"/>
+    <row r="264" hidden="1"/>
+    <row r="265" hidden="1"/>
+    <row r="266" hidden="1"/>
+    <row r="267" hidden="1"/>
+    <row r="268" hidden="1"/>
+    <row r="269" hidden="1"/>
+    <row r="270" hidden="1"/>
+    <row r="271" hidden="1"/>
+    <row r="272" hidden="1"/>
+    <row r="273" hidden="1"/>
+    <row r="274" hidden="1"/>
+    <row r="275" hidden="1"/>
+    <row r="276" hidden="1"/>
+    <row r="277" hidden="1"/>
+    <row r="278" hidden="1"/>
+    <row r="279" hidden="1"/>
+    <row r="280" hidden="1"/>
+    <row r="281" hidden="1"/>
+    <row r="282" hidden="1"/>
+    <row r="283" hidden="1"/>
+    <row r="284" hidden="1"/>
+    <row r="285" hidden="1"/>
+    <row r="286" hidden="1"/>
+    <row r="287" hidden="1"/>
+    <row r="288" hidden="1"/>
+    <row r="289" hidden="1"/>
+    <row r="290" hidden="1"/>
+    <row r="291" hidden="1"/>
+    <row r="292" hidden="1"/>
+    <row r="293" hidden="1"/>
+    <row r="294" hidden="1"/>
+    <row r="295" hidden="1"/>
+    <row r="296" hidden="1"/>
+    <row r="297" hidden="1"/>
+    <row r="298" hidden="1"/>
+    <row r="299" hidden="1"/>
+    <row r="300" hidden="1"/>
+    <row r="301" hidden="1"/>
+    <row r="302" hidden="1"/>
+    <row r="303" hidden="1"/>
+    <row r="304" hidden="1"/>
+    <row r="305" hidden="1"/>
+    <row r="306" hidden="1"/>
+    <row r="307" hidden="1"/>
+    <row r="308" hidden="1"/>
+    <row r="309" hidden="1"/>
+    <row r="310" hidden="1"/>
+    <row r="311" hidden="1"/>
+    <row r="312" hidden="1"/>
+    <row r="313" hidden="1"/>
+    <row r="314" hidden="1"/>
+    <row r="315" hidden="1"/>
+    <row r="316" hidden="1"/>
+    <row r="317" hidden="1"/>
+    <row r="318" hidden="1"/>
+    <row r="319" hidden="1"/>
+    <row r="320" hidden="1"/>
+    <row r="321" hidden="1"/>
+    <row r="322" hidden="1"/>
+    <row r="323" hidden="1"/>
+    <row r="324" hidden="1"/>
+    <row r="325" hidden="1"/>
+    <row r="326" hidden="1"/>
+    <row r="327" hidden="1"/>
+    <row r="328" hidden="1"/>
+    <row r="329" hidden="1"/>
+    <row r="330" hidden="1"/>
+    <row r="331" hidden="1"/>
+    <row r="332" hidden="1"/>
+    <row r="333" hidden="1"/>
+    <row r="334" hidden="1"/>
+    <row r="335" hidden="1"/>
+    <row r="336" hidden="1"/>
+    <row r="337" hidden="1"/>
+    <row r="338" hidden="1"/>
+    <row r="339" hidden="1"/>
+    <row r="340" hidden="1"/>
+    <row r="341" hidden="1"/>
+    <row r="342" hidden="1"/>
+    <row r="343" hidden="1"/>
+    <row r="344" hidden="1"/>
+    <row r="345" hidden="1"/>
+    <row r="346" hidden="1"/>
+    <row r="347" hidden="1"/>
+    <row r="348" hidden="1"/>
+    <row r="349" hidden="1"/>
+    <row r="350" hidden="1"/>
+    <row r="351" hidden="1"/>
+    <row r="352" hidden="1"/>
+    <row r="353" hidden="1"/>
+    <row r="354" hidden="1"/>
+    <row r="355" hidden="1"/>
+    <row r="356" hidden="1"/>
+    <row r="357" hidden="1"/>
+    <row r="358" hidden="1"/>
+    <row r="359" hidden="1"/>
+    <row r="360" hidden="1"/>
+    <row r="361" hidden="1"/>
+    <row r="362" hidden="1"/>
+    <row r="363" hidden="1"/>
+    <row r="364" hidden="1"/>
+    <row r="365" hidden="1"/>
+    <row r="366" hidden="1"/>
+    <row r="367" hidden="1"/>
+    <row r="368" hidden="1"/>
+    <row r="369" hidden="1"/>
+    <row r="370" hidden="1"/>
+    <row r="371" hidden="1"/>
+    <row r="372" hidden="1"/>
+    <row r="373" hidden="1"/>
+    <row r="374" hidden="1"/>
+    <row r="375" hidden="1"/>
+    <row r="376" hidden="1"/>
+    <row r="377" hidden="1"/>
+    <row r="378" hidden="1"/>
+    <row r="379" hidden="1"/>
+    <row r="380" hidden="1"/>
+    <row r="381" hidden="1"/>
+    <row r="382" hidden="1"/>
+    <row r="383" hidden="1"/>
+    <row r="384" hidden="1"/>
+    <row r="385" hidden="1"/>
+    <row r="386" hidden="1"/>
+    <row r="387" hidden="1"/>
+    <row r="388" hidden="1"/>
+    <row r="389" hidden="1"/>
+    <row r="390" hidden="1"/>
+    <row r="391" hidden="1"/>
+    <row r="392" hidden="1"/>
+    <row r="393" hidden="1"/>
+    <row r="394" hidden="1"/>
+    <row r="395" hidden="1"/>
+    <row r="396" hidden="1"/>
+    <row r="397" hidden="1"/>
+    <row r="398" hidden="1"/>
+    <row r="399" hidden="1"/>
+    <row r="400" hidden="1"/>
+    <row r="401" hidden="1"/>
+    <row r="402" hidden="1"/>
+    <row r="403" hidden="1"/>
+    <row r="404" hidden="1"/>
+    <row r="405" hidden="1"/>
+    <row r="406" hidden="1"/>
+    <row r="407" hidden="1"/>
+    <row r="408" hidden="1"/>
+    <row r="409" hidden="1"/>
+    <row r="410" hidden="1"/>
+    <row r="411" hidden="1"/>
+    <row r="412" hidden="1"/>
+    <row r="413" hidden="1"/>
+    <row r="414" hidden="1"/>
+    <row r="415" hidden="1"/>
+    <row r="416" hidden="1"/>
+    <row r="417" hidden="1"/>
+    <row r="418" hidden="1"/>
+    <row r="419" hidden="1"/>
+    <row r="420" hidden="1"/>
+    <row r="421" hidden="1"/>
+    <row r="422" hidden="1"/>
+    <row r="423" hidden="1"/>
+    <row r="424" hidden="1"/>
+    <row r="425" hidden="1"/>
+    <row r="426" hidden="1"/>
+    <row r="427" hidden="1"/>
+    <row r="428" hidden="1"/>
+    <row r="429" hidden="1"/>
+    <row r="430" hidden="1"/>
+    <row r="431" hidden="1"/>
+    <row r="432" hidden="1"/>
+    <row r="433" hidden="1"/>
+    <row r="434" hidden="1"/>
+    <row r="435" hidden="1"/>
+    <row r="436" hidden="1"/>
+    <row r="437" hidden="1"/>
+    <row r="438" hidden="1"/>
+    <row r="439" hidden="1"/>
+    <row r="440" hidden="1"/>
+    <row r="441" hidden="1"/>
+    <row r="442" hidden="1"/>
+    <row r="443" hidden="1"/>
+    <row r="444" hidden="1"/>
+    <row r="445" hidden="1"/>
+    <row r="446" hidden="1"/>
+    <row r="447" hidden="1"/>
+    <row r="448" hidden="1"/>
+    <row r="449" hidden="1"/>
+    <row r="450" hidden="1"/>
+    <row r="451" hidden="1"/>
+    <row r="452" hidden="1"/>
+    <row r="453" hidden="1"/>
+    <row r="454" hidden="1"/>
+    <row r="455" hidden="1"/>
+    <row r="456" hidden="1"/>
+    <row r="457" hidden="1"/>
+    <row r="458" hidden="1"/>
+    <row r="459" hidden="1"/>
+    <row r="460" hidden="1"/>
+    <row r="461" hidden="1"/>
+    <row r="462" hidden="1"/>
+    <row r="463" hidden="1"/>
+    <row r="464" hidden="1"/>
+    <row r="465" hidden="1"/>
+    <row r="466" hidden="1"/>
+    <row r="467" hidden="1"/>
+    <row r="468" hidden="1"/>
+    <row r="469" hidden="1"/>
+    <row r="470" hidden="1"/>
+    <row r="471" hidden="1"/>
+    <row r="472" hidden="1"/>
+    <row r="473" hidden="1"/>
+    <row r="474" hidden="1"/>
+    <row r="475" hidden="1"/>
+    <row r="476" hidden="1"/>
+    <row r="477" hidden="1"/>
+    <row r="478" hidden="1"/>
+    <row r="479" hidden="1"/>
+    <row r="480" hidden="1"/>
+    <row r="481" hidden="1"/>
+    <row r="482" hidden="1"/>
+    <row r="483" hidden="1"/>
+    <row r="484" hidden="1"/>
+    <row r="485" hidden="1"/>
+    <row r="486" hidden="1"/>
+    <row r="487" hidden="1"/>
+    <row r="488" hidden="1"/>
+    <row r="489" hidden="1"/>
+    <row r="490" hidden="1"/>
+    <row r="491" hidden="1"/>
+    <row r="492" hidden="1"/>
+    <row r="493" hidden="1"/>
+    <row r="494" hidden="1"/>
+    <row r="495" hidden="1"/>
+    <row r="496" hidden="1"/>
+    <row r="497" spans="1:1" hidden="1"/>
+    <row r="498" spans="1:1" hidden="1"/>
+    <row r="499" spans="1:1" hidden="1"/>
+    <row r="500" spans="1:1" hidden="1">
+      <c r="A500" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I118" xr:uid="{3D8B8C54-31AE-4B49-AB74-3ED34CE5744B}">
+  <autoFilter ref="A1:I500" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Replaced video speed slider with +/- increment controls.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF849F7-318A-4F8D-BCBF-D22CF84B9AF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098AC9B4-AC05-467D-AD89-127A89CCA20B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4245" yWindow="885" windowWidth="23415" windowHeight="14715" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="112">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -461,9 +461,6 @@
     <t>compare speeds of services on NOAA &amp; PSMFC servers</t>
   </si>
   <si>
-    <t>go to locale/site from maptip</t>
-  </si>
-  <si>
     <t>put widget inside DIV, add checkbox at bottom of DIV?</t>
   </si>
   <si>
@@ -471,6 +468,12 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>go to locale/site from popup</t>
+  </si>
+  <si>
+    <t>basically there -- update where "playbackRate" appears</t>
   </si>
 </sst>
 </file>
@@ -1357,10 +1360,10 @@
   <dimension ref="A1:J500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D55" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D506" sqref="D506"/>
+      <selection pane="bottomRight" activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1647,6 +1650,9 @@
       <c r="D28" s="9" t="s">
         <v>22</v>
       </c>
+      <c r="I28" s="11" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="29" spans="1:9" hidden="1">
       <c r="B29" s="2" t="s">
@@ -1747,7 +1753,7 @@
     <row r="39" spans="1:10" hidden="1">
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:10" ht="47.25" hidden="1">
+    <row r="40" spans="1:10" ht="94.5" hidden="1">
       <c r="C40" s="2" t="s">
         <v>71</v>
       </c>
@@ -1840,7 +1846,7 @@
     <row r="48" spans="1:10" hidden="1">
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:9" hidden="1">
+    <row r="49" spans="1:9" ht="31.5" hidden="1">
       <c r="B49" s="2" t="s">
         <v>55</v>
       </c>
@@ -2089,7 +2095,7 @@
         <v>103</v>
       </c>
       <c r="I122" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="123" spans="3:9" hidden="1"/>
@@ -2101,7 +2107,7 @@
         <v>104</v>
       </c>
       <c r="I124" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="125" spans="3:9" hidden="1"/>
@@ -2119,7 +2125,7 @@
     <row r="129" spans="4:4" hidden="1"/>
     <row r="130" spans="4:4">
       <c r="D130" s="9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="131" spans="4:4" hidden="1"/>
@@ -2493,7 +2499,7 @@
     <row r="499" spans="1:1" hidden="1"/>
     <row r="500" spans="1:1" hidden="1">
       <c r="A500" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LayerList Icons, download original-res photo.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098AC9B4-AC05-467D-AD89-127A89CCA20B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F0BD0C-44FD-43BA-9C64-84762603A8A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4245" yWindow="885" windowWidth="23415" windowHeight="14715" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="645" yWindow="885" windowWidth="27885" windowHeight="14715" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="113">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -474,6 +474,9 @@
   </si>
   <si>
     <t>basically there -- update where "playbackRate" appears</t>
+  </si>
+  <si>
+    <t>Still can't get it to download straight to file file rather than open in new tab.</t>
   </si>
 </sst>
 </file>
@@ -1363,7 +1366,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I66" sqref="I66"/>
+      <selection pane="bottomRight" activeCell="D506" sqref="D506"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1643,9 +1646,12 @@
     <row r="27" spans="1:9" hidden="1">
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:9" ht="39.950000000000003" customHeight="1">
+    <row r="28" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1">
       <c r="B28" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>22</v>
@@ -1978,7 +1984,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="1:4" hidden="1">
+    <row r="65" spans="1:9" hidden="1">
       <c r="C65" s="2" t="s">
         <v>72</v>
       </c>
@@ -1986,18 +1992,18 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="66" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="D66" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:4" hidden="1"/>
-    <row r="68" spans="1:4" ht="39.950000000000003" customHeight="1">
+    <row r="67" spans="1:9" hidden="1"/>
+    <row r="68" spans="1:9" ht="39.950000000000003" customHeight="1">
       <c r="D68" s="9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="1:4" hidden="1">
+    <row r="69" spans="1:9" hidden="1">
       <c r="C69" s="2" t="s">
         <v>101</v>
       </c>
@@ -2005,8 +2011,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:4" hidden="1"/>
-    <row r="71" spans="1:4" hidden="1">
+    <row r="70" spans="1:9" hidden="1"/>
+    <row r="71" spans="1:9" hidden="1">
       <c r="C71" s="2" t="s">
         <v>72</v>
       </c>
@@ -2014,7 +2020,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="72" spans="1:9" ht="20.100000000000001" hidden="1" customHeight="1">
       <c r="A72" s="6" t="s">
         <v>11</v>
       </c>
@@ -2022,13 +2028,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="73" spans="1:4" hidden="1"/>
-    <row r="74" spans="1:4" ht="39.950000000000003" customHeight="1">
+    <row r="73" spans="1:9" hidden="1"/>
+    <row r="74" spans="1:9" ht="39.950000000000003" customHeight="1">
       <c r="D74" s="9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="75" spans="1:9" ht="20.100000000000001" hidden="1" customHeight="1">
       <c r="C75" s="2" t="s">
         <v>72</v>
       </c>
@@ -2036,15 +2042,21 @@
         <v>99</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="76" spans="1:9" ht="20.100000000000001" hidden="1" customHeight="1">
+      <c r="C76" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="D76" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" hidden="1"/>
-    <row r="78" spans="1:4" hidden="1"/>
-    <row r="79" spans="1:4" hidden="1"/>
-    <row r="80" spans="1:4" hidden="1"/>
+      <c r="I76" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" hidden="1"/>
+    <row r="78" spans="1:9" hidden="1"/>
+    <row r="79" spans="1:9" hidden="1"/>
+    <row r="80" spans="1:9" hidden="1"/>
     <row r="81" hidden="1"/>
     <row r="82" hidden="1"/>
     <row r="83" hidden="1"/>
@@ -2090,7 +2102,10 @@
       </c>
     </row>
     <row r="121" spans="3:9" hidden="1"/>
-    <row r="122" spans="3:9">
+    <row r="122" spans="3:9" hidden="1">
+      <c r="C122" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D122" s="9" t="s">
         <v>103</v>
       </c>
@@ -2111,7 +2126,10 @@
       </c>
     </row>
     <row r="125" spans="3:9" hidden="1"/>
-    <row r="126" spans="3:9">
+    <row r="126" spans="3:9" hidden="1">
+      <c r="C126" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D126" s="9" t="s">
         <v>105</v>
       </c>

</xml_diff>

<commit_message>
Download orig. res. photo, popup info from table row.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F0BD0C-44FD-43BA-9C64-84762603A8A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF1B88E-4599-4482-8687-3BE9893CF7D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="885" windowWidth="27885" windowHeight="14715" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="915" yWindow="1485" windowWidth="27885" windowHeight="14715" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="113">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -1366,7 +1366,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D506" sqref="D506"/>
+      <selection pane="bottomRight" activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1992,7 +1992,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="66" spans="1:9" ht="20.100000000000001" hidden="1" customHeight="1">
+      <c r="C66" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D66" s="9" t="s">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
Finished popup info from table row.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF1B88E-4599-4482-8687-3BE9893CF7D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E34067A-D0C2-4EA4-BC44-9A5127C326D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="1485" windowWidth="27885" windowHeight="14715" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="915" yWindow="885" windowWidth="27885" windowHeight="14715" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="113">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -1366,7 +1366,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C130" sqref="C130"/>
+      <selection pane="bottomRight" activeCell="D509" sqref="D509"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -2143,26 +2143,29 @@
         <v>106</v>
       </c>
     </row>
-    <row r="129" spans="4:4" hidden="1"/>
-    <row r="130" spans="4:4">
+    <row r="129" spans="3:4" hidden="1"/>
+    <row r="130" spans="3:4" hidden="1">
+      <c r="C130" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D130" s="9" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="131" spans="4:4" hidden="1"/>
-    <row r="132" spans="4:4" hidden="1"/>
-    <row r="133" spans="4:4" hidden="1"/>
-    <row r="134" spans="4:4" hidden="1"/>
-    <row r="135" spans="4:4" hidden="1"/>
-    <row r="136" spans="4:4" hidden="1"/>
-    <row r="137" spans="4:4" hidden="1"/>
-    <row r="138" spans="4:4" hidden="1"/>
-    <row r="139" spans="4:4" hidden="1"/>
-    <row r="140" spans="4:4" hidden="1"/>
-    <row r="141" spans="4:4" hidden="1"/>
-    <row r="142" spans="4:4" hidden="1"/>
-    <row r="143" spans="4:4" hidden="1"/>
-    <row r="144" spans="4:4" hidden="1"/>
+    <row r="131" spans="3:4" hidden="1"/>
+    <row r="132" spans="3:4" hidden="1"/>
+    <row r="133" spans="3:4" hidden="1"/>
+    <row r="134" spans="3:4" hidden="1"/>
+    <row r="135" spans="3:4" hidden="1"/>
+    <row r="136" spans="3:4" hidden="1"/>
+    <row r="137" spans="3:4" hidden="1"/>
+    <row r="138" spans="3:4" hidden="1"/>
+    <row r="139" spans="3:4" hidden="1"/>
+    <row r="140" spans="3:4" hidden="1"/>
+    <row r="141" spans="3:4" hidden="1"/>
+    <row r="142" spans="3:4" hidden="1"/>
+    <row r="143" spans="3:4" hidden="1"/>
+    <row r="144" spans="3:4" hidden="1"/>
     <row r="145" hidden="1"/>
     <row r="146" hidden="1"/>
     <row r="147" hidden="1"/>

</xml_diff>

<commit_message>
4.14, extent bookmarks with thumbnails
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E34067A-D0C2-4EA4-BC44-9A5127C326D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4E0585-BF29-4F2B-AE23-06C12B27791B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="915" yWindow="885" windowWidth="27885" windowHeight="14715" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$500</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$427</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="117">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -477,6 +477,43 @@
   </si>
   <si>
     <t>Still can't get it to download straight to file file rather than open in new tab.</t>
+  </si>
+  <si>
+    <t>populate species dropdowns</t>
+  </si>
+  <si>
+    <t>filter video point query when zoomed out</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">propose using [modulo n] on MP4_Seconds, with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> determined by extent</t>
+    </r>
+  </si>
+  <si>
+    <t>look into Slider widgets?</t>
   </si>
 </sst>
 </file>
@@ -611,12 +648,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE5FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -637,7 +692,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -698,6 +753,15 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -712,6 +776,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFE5FF"/>
       <color rgb="FFFFCCFF"/>
     </mruColors>
   </colors>
@@ -1294,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2BFB56-BD70-FD45-AC33-49638CF763A3}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A3" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="21"/>
@@ -1360,16 +1425,16 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J500"/>
+  <dimension ref="A1:J427"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D509" sqref="D509"/>
+      <selection pane="bottomRight" activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5.625" style="2" customWidth="1"/>
@@ -1383,7 +1448,7 @@
     <col min="11" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="86.25" customHeight="1">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="97.5" customHeight="1">
       <c r="A1" s="17" t="s">
         <v>12</v>
       </c>
@@ -1396,6 +1461,7 @@
       <c r="D1" s="18" t="s">
         <v>15</v>
       </c>
+      <c r="E1" s="6"/>
       <c r="F1" s="14" t="s">
         <v>39</v>
       </c>
@@ -1409,7 +1475,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1">
+    <row r="2" spans="1:9" ht="15.75" hidden="1">
       <c r="C2" s="2" t="s">
         <v>72</v>
       </c>
@@ -1419,10 +1485,25 @@
       <c r="H2" s="6"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" hidden="1">
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" hidden="1">
+    <row r="3" spans="1:9" ht="15.75" hidden="1">
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" hidden="1">
       <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
@@ -1430,1120 +1511,634 @@
         <v>24</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>41</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" hidden="1">
+    <row r="5" spans="1:9" customFormat="1" ht="15.75" hidden="1">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
       <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="31.5" hidden="1">
+      <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="63" hidden="1">
+      <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" customFormat="1" hidden="1">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" hidden="1">
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" ht="31.5" hidden="1">
-      <c r="B8" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="D7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" hidden="1">
       <c r="C8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" hidden="1">
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" hidden="1">
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" ht="63" hidden="1">
-      <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="C9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" hidden="1">
       <c r="C10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>2</v>
+        <v>72</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" hidden="1">
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" hidden="1">
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" ht="31.5" hidden="1">
+      <c r="C11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" hidden="1">
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:9" hidden="1">
-      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="31.5" hidden="1">
+      <c r="C13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="31.5" hidden="1">
+      <c r="C14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" hidden="1">
+      <c r="A15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:9" hidden="1">
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" hidden="1">
-      <c r="C15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" ht="31.5" hidden="1">
-      <c r="C16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>0</v>
+      <c r="D15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" hidden="1">
+      <c r="A16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" hidden="1">
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" hidden="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" hidden="1">
+      <c r="C17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:10" ht="31.5" hidden="1">
       <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" hidden="1">
+      <c r="B19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" hidden="1">
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" hidden="1">
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:9" ht="31.5" hidden="1">
+      <c r="D19" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" hidden="1">
+      <c r="A20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" hidden="1">
+      <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="C21" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="31.5" hidden="1">
+        <v>72</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" hidden="1">
       <c r="C22" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="H22" s="6"/>
-      <c r="I22" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" hidden="1">
-      <c r="A23" s="6" t="s">
-        <v>11</v>
-      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" hidden="1">
       <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="C23" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="D23" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" hidden="1">
-      <c r="A24" s="6" t="s">
-        <v>11</v>
-      </c>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="31.5" hidden="1">
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="6"/>
+      <c r="C24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="I24" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" hidden="1">
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="1:9" hidden="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="126" hidden="1">
+      <c r="B25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="94.5" hidden="1">
       <c r="C26" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="6"/>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" hidden="1">
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1">
+        <v>44</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="31.5" hidden="1">
+      <c r="B27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" hidden="1">
       <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" hidden="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="31.5" hidden="1">
       <c r="B29" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" hidden="1">
-      <c r="D30" s="6"/>
-    </row>
-    <row r="31" spans="1:9" hidden="1">
-      <c r="A31" s="6" t="s">
+      <c r="D29" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" hidden="1">
+      <c r="A30" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="D30" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" hidden="1">
+      <c r="C31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="31.5" hidden="1">
+      <c r="B32" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="31.5" hidden="1">
+      <c r="B33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I33" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="31.5" hidden="1">
+      <c r="C34" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I34" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="63" hidden="1">
+      <c r="A35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" hidden="1">
+      <c r="B36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" hidden="1">
-      <c r="B32" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="C36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" hidden="1">
+      <c r="C37" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" hidden="1">
+      <c r="C38" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" hidden="1">
-      <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="1:10" hidden="1">
-      <c r="C34" s="2" t="s">
+      <c r="D38" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="31.5" hidden="1">
+      <c r="C39" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D34" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H34" s="6"/>
-    </row>
-    <row r="35" spans="1:10" hidden="1">
-      <c r="B35" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="31.5" hidden="1">
-      <c r="B36" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="D39" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" hidden="1">
+      <c r="A40" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" hidden="1">
+      <c r="C41" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I36" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" hidden="1">
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="1:10" ht="126" hidden="1">
-      <c r="B38" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" hidden="1">
-      <c r="D39" s="6"/>
-    </row>
-    <row r="40" spans="1:10" ht="94.5" hidden="1">
-      <c r="C40" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" hidden="1">
-      <c r="D41" s="6"/>
-    </row>
-    <row r="42" spans="1:10" ht="31.5" hidden="1">
-      <c r="B42" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="D41" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" hidden="1">
       <c r="C42" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I42" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="J42" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" hidden="1">
-      <c r="D43" s="6"/>
-    </row>
-    <row r="44" spans="1:10" hidden="1">
-      <c r="B44" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" hidden="1">
+      <c r="C43" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D43" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="39.75" customHeight="1">
+      <c r="D44" s="25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" hidden="1">
+      <c r="C45" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" hidden="1">
+      <c r="C46" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="31.5" hidden="1">
-      <c r="B45" s="2" t="s">
+      <c r="D46" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="9.75" hidden="1" customHeight="1">
+      <c r="A47" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="42" customHeight="1">
+      <c r="D48" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="3:9" ht="15.75" hidden="1">
+      <c r="C49" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="3:9" ht="31.5" hidden="1">
+      <c r="C50" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" ht="24.95" hidden="1" customHeight="1">
+      <c r="C51" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="3:9" ht="15.75" hidden="1">
+      <c r="C52" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" hidden="1">
-      <c r="A46" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I46" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" hidden="1">
-      <c r="C47" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" hidden="1">
-      <c r="D48" s="6"/>
-    </row>
-    <row r="49" spans="1:9" ht="31.5" hidden="1">
-      <c r="B49" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="D52" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I52" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="3:9" ht="15.75" hidden="1">
+      <c r="C53" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="3:9" ht="15.75" hidden="1">
+      <c r="C54" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D49" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H49" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I49" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" hidden="1">
-      <c r="D50" s="6"/>
-    </row>
-    <row r="51" spans="1:9" ht="31.5" hidden="1">
-      <c r="B51" s="2" t="s">
+      <c r="D54" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="3:9" ht="24.95" customHeight="1">
+      <c r="D55" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="3:9" ht="24.95" customHeight="1">
+      <c r="D56" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="3:9" ht="15.75" hidden="1">
+      <c r="C57" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I51" s="19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="31.5" hidden="1">
-      <c r="C52" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="I52" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="63" hidden="1">
-      <c r="A53" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" hidden="1">
-      <c r="D54" s="6"/>
-    </row>
-    <row r="55" spans="1:9" hidden="1">
-      <c r="B55" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="I55" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" hidden="1">
-      <c r="D56" s="6"/>
-    </row>
-    <row r="57" spans="1:9" hidden="1">
-      <c r="C57" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="I57" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" hidden="1">
-      <c r="D58" s="6"/>
-    </row>
-    <row r="59" spans="1:9" hidden="1">
-      <c r="C59" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" hidden="1">
-      <c r="D60" s="6"/>
-    </row>
-    <row r="61" spans="1:9" hidden="1"/>
-    <row r="62" spans="1:9" ht="31.5" hidden="1">
-      <c r="C62" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="20.100000000000001" hidden="1" customHeight="1">
-      <c r="A63" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" hidden="1">
-      <c r="C64" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="I64" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" hidden="1">
-      <c r="C65" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="20.100000000000001" hidden="1" customHeight="1">
-      <c r="C66" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" hidden="1"/>
-    <row r="68" spans="1:9" ht="39.950000000000003" customHeight="1">
-      <c r="D68" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" hidden="1">
-      <c r="C69" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D69" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" hidden="1"/>
-    <row r="71" spans="1:9" hidden="1">
-      <c r="C71" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="20.100000000000001" hidden="1" customHeight="1">
-      <c r="A72" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" hidden="1"/>
-    <row r="74" spans="1:9" ht="39.950000000000003" customHeight="1">
-      <c r="D74" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="20.100000000000001" hidden="1" customHeight="1">
-      <c r="C75" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="20.100000000000001" hidden="1" customHeight="1">
-      <c r="C76" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="I76" s="11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" hidden="1"/>
-    <row r="78" spans="1:9" hidden="1"/>
-    <row r="79" spans="1:9" hidden="1"/>
-    <row r="80" spans="1:9" hidden="1"/>
-    <row r="81" hidden="1"/>
-    <row r="82" hidden="1"/>
-    <row r="83" hidden="1"/>
-    <row r="84" hidden="1"/>
-    <row r="85" hidden="1"/>
-    <row r="86" hidden="1"/>
-    <row r="87" hidden="1"/>
-    <row r="88" hidden="1"/>
-    <row r="89" hidden="1"/>
-    <row r="90" hidden="1"/>
-    <row r="91" hidden="1"/>
-    <row r="92" hidden="1"/>
-    <row r="93" hidden="1"/>
-    <row r="94" hidden="1"/>
-    <row r="95" hidden="1"/>
-    <row r="96" hidden="1"/>
-    <row r="97" hidden="1"/>
-    <row r="98" hidden="1"/>
-    <row r="99" hidden="1"/>
-    <row r="100" hidden="1"/>
-    <row r="101" hidden="1"/>
-    <row r="102" hidden="1"/>
-    <row r="103" hidden="1"/>
-    <row r="104" hidden="1"/>
-    <row r="105" hidden="1"/>
-    <row r="106" hidden="1"/>
-    <row r="107" hidden="1"/>
-    <row r="108" hidden="1"/>
-    <row r="109" hidden="1"/>
-    <row r="110" hidden="1"/>
-    <row r="111" hidden="1"/>
-    <row r="112" hidden="1"/>
-    <row r="113" spans="3:9" hidden="1"/>
-    <row r="114" spans="3:9" hidden="1"/>
-    <row r="115" spans="3:9" hidden="1"/>
-    <row r="116" spans="3:9" hidden="1"/>
-    <row r="117" spans="3:9" hidden="1"/>
-    <row r="118" spans="3:9" hidden="1"/>
-    <row r="119" spans="3:9" hidden="1"/>
-    <row r="120" spans="3:9">
-      <c r="D120" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="121" spans="3:9" hidden="1"/>
-    <row r="122" spans="3:9" hidden="1">
-      <c r="C122" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D122" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="I122" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="123" spans="3:9" hidden="1"/>
-    <row r="124" spans="3:9" hidden="1">
-      <c r="C124" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D124" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="I124" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="125" spans="3:9" hidden="1"/>
-    <row r="126" spans="3:9" hidden="1">
-      <c r="C126" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D126" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="127" spans="3:9" hidden="1"/>
-    <row r="128" spans="3:9">
-      <c r="D128" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="129" spans="3:4" hidden="1"/>
-    <row r="130" spans="3:4" hidden="1">
-      <c r="C130" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D130" s="9" t="s">
+      <c r="D57" s="9" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="131" spans="3:4" hidden="1"/>
-    <row r="132" spans="3:4" hidden="1"/>
-    <row r="133" spans="3:4" hidden="1"/>
-    <row r="134" spans="3:4" hidden="1"/>
-    <row r="135" spans="3:4" hidden="1"/>
-    <row r="136" spans="3:4" hidden="1"/>
-    <row r="137" spans="3:4" hidden="1"/>
-    <row r="138" spans="3:4" hidden="1"/>
-    <row r="139" spans="3:4" hidden="1"/>
-    <row r="140" spans="3:4" hidden="1"/>
-    <row r="141" spans="3:4" hidden="1"/>
-    <row r="142" spans="3:4" hidden="1"/>
-    <row r="143" spans="3:4" hidden="1"/>
-    <row r="144" spans="3:4" hidden="1"/>
-    <row r="145" hidden="1"/>
-    <row r="146" hidden="1"/>
-    <row r="147" hidden="1"/>
-    <row r="148" hidden="1"/>
-    <row r="149" hidden="1"/>
-    <row r="150" hidden="1"/>
-    <row r="151" hidden="1"/>
-    <row r="152" hidden="1"/>
-    <row r="153" hidden="1"/>
-    <row r="154" hidden="1"/>
-    <row r="155" hidden="1"/>
-    <row r="156" hidden="1"/>
-    <row r="157" hidden="1"/>
-    <row r="158" hidden="1"/>
-    <row r="159" hidden="1"/>
-    <row r="160" hidden="1"/>
-    <row r="161" hidden="1"/>
-    <row r="162" hidden="1"/>
-    <row r="163" hidden="1"/>
-    <row r="164" hidden="1"/>
-    <row r="165" hidden="1"/>
-    <row r="166" hidden="1"/>
-    <row r="167" hidden="1"/>
-    <row r="168" hidden="1"/>
-    <row r="169" hidden="1"/>
-    <row r="170" hidden="1"/>
-    <row r="171" hidden="1"/>
-    <row r="172" hidden="1"/>
-    <row r="173" hidden="1"/>
-    <row r="174" hidden="1"/>
-    <row r="175" hidden="1"/>
-    <row r="176" hidden="1"/>
-    <row r="177" hidden="1"/>
-    <row r="178" hidden="1"/>
-    <row r="179" hidden="1"/>
-    <row r="180" hidden="1"/>
-    <row r="181" hidden="1"/>
-    <row r="182" hidden="1"/>
-    <row r="183" hidden="1"/>
-    <row r="184" hidden="1"/>
-    <row r="185" hidden="1"/>
-    <row r="186" hidden="1"/>
-    <row r="187" hidden="1"/>
-    <row r="188" hidden="1"/>
-    <row r="189" hidden="1"/>
-    <row r="190" hidden="1"/>
-    <row r="191" hidden="1"/>
-    <row r="192" hidden="1"/>
-    <row r="193" hidden="1"/>
-    <row r="194" hidden="1"/>
-    <row r="195" hidden="1"/>
-    <row r="196" hidden="1"/>
-    <row r="197" hidden="1"/>
-    <row r="198" hidden="1"/>
-    <row r="199" hidden="1"/>
-    <row r="200" hidden="1"/>
-    <row r="201" hidden="1"/>
-    <row r="202" hidden="1"/>
-    <row r="203" hidden="1"/>
-    <row r="204" hidden="1"/>
-    <row r="205" hidden="1"/>
-    <row r="206" hidden="1"/>
-    <row r="207" hidden="1"/>
-    <row r="208" hidden="1"/>
-    <row r="209" hidden="1"/>
-    <row r="210" hidden="1"/>
-    <row r="211" hidden="1"/>
-    <row r="212" hidden="1"/>
-    <row r="213" hidden="1"/>
-    <row r="214" hidden="1"/>
-    <row r="215" hidden="1"/>
-    <row r="216" hidden="1"/>
-    <row r="217" hidden="1"/>
-    <row r="218" hidden="1"/>
-    <row r="219" hidden="1"/>
-    <row r="220" hidden="1"/>
-    <row r="221" hidden="1"/>
-    <row r="222" hidden="1"/>
-    <row r="223" hidden="1"/>
-    <row r="224" hidden="1"/>
-    <row r="225" hidden="1"/>
-    <row r="226" hidden="1"/>
-    <row r="227" hidden="1"/>
-    <row r="228" hidden="1"/>
-    <row r="229" hidden="1"/>
-    <row r="230" hidden="1"/>
-    <row r="231" hidden="1"/>
-    <row r="232" hidden="1"/>
-    <row r="233" hidden="1"/>
-    <row r="234" hidden="1"/>
-    <row r="235" hidden="1"/>
-    <row r="236" hidden="1"/>
-    <row r="237" hidden="1"/>
-    <row r="238" hidden="1"/>
-    <row r="239" hidden="1"/>
-    <row r="240" hidden="1"/>
-    <row r="241" hidden="1"/>
-    <row r="242" hidden="1"/>
-    <row r="243" hidden="1"/>
-    <row r="244" hidden="1"/>
-    <row r="245" hidden="1"/>
-    <row r="246" hidden="1"/>
-    <row r="247" hidden="1"/>
-    <row r="248" hidden="1"/>
-    <row r="249" hidden="1"/>
-    <row r="250" hidden="1"/>
-    <row r="251" hidden="1"/>
-    <row r="252" hidden="1"/>
-    <row r="253" hidden="1"/>
-    <row r="254" hidden="1"/>
-    <row r="255" hidden="1"/>
-    <row r="256" hidden="1"/>
-    <row r="257" hidden="1"/>
-    <row r="258" hidden="1"/>
-    <row r="259" hidden="1"/>
-    <row r="260" hidden="1"/>
-    <row r="261" hidden="1"/>
-    <row r="262" hidden="1"/>
-    <row r="263" hidden="1"/>
-    <row r="264" hidden="1"/>
-    <row r="265" hidden="1"/>
-    <row r="266" hidden="1"/>
-    <row r="267" hidden="1"/>
-    <row r="268" hidden="1"/>
-    <row r="269" hidden="1"/>
-    <row r="270" hidden="1"/>
-    <row r="271" hidden="1"/>
-    <row r="272" hidden="1"/>
-    <row r="273" hidden="1"/>
-    <row r="274" hidden="1"/>
-    <row r="275" hidden="1"/>
-    <row r="276" hidden="1"/>
-    <row r="277" hidden="1"/>
-    <row r="278" hidden="1"/>
-    <row r="279" hidden="1"/>
-    <row r="280" hidden="1"/>
-    <row r="281" hidden="1"/>
-    <row r="282" hidden="1"/>
-    <row r="283" hidden="1"/>
-    <row r="284" hidden="1"/>
-    <row r="285" hidden="1"/>
-    <row r="286" hidden="1"/>
-    <row r="287" hidden="1"/>
-    <row r="288" hidden="1"/>
-    <row r="289" hidden="1"/>
-    <row r="290" hidden="1"/>
-    <row r="291" hidden="1"/>
-    <row r="292" hidden="1"/>
-    <row r="293" hidden="1"/>
-    <row r="294" hidden="1"/>
-    <row r="295" hidden="1"/>
-    <row r="296" hidden="1"/>
-    <row r="297" hidden="1"/>
-    <row r="298" hidden="1"/>
-    <row r="299" hidden="1"/>
-    <row r="300" hidden="1"/>
-    <row r="301" hidden="1"/>
-    <row r="302" hidden="1"/>
-    <row r="303" hidden="1"/>
-    <row r="304" hidden="1"/>
-    <row r="305" hidden="1"/>
-    <row r="306" hidden="1"/>
-    <row r="307" hidden="1"/>
-    <row r="308" hidden="1"/>
-    <row r="309" hidden="1"/>
-    <row r="310" hidden="1"/>
-    <row r="311" hidden="1"/>
-    <row r="312" hidden="1"/>
-    <row r="313" hidden="1"/>
-    <row r="314" hidden="1"/>
-    <row r="315" hidden="1"/>
-    <row r="316" hidden="1"/>
-    <row r="317" hidden="1"/>
-    <row r="318" hidden="1"/>
-    <row r="319" hidden="1"/>
-    <row r="320" hidden="1"/>
-    <row r="321" hidden="1"/>
-    <row r="322" hidden="1"/>
-    <row r="323" hidden="1"/>
-    <row r="324" hidden="1"/>
-    <row r="325" hidden="1"/>
-    <row r="326" hidden="1"/>
-    <row r="327" hidden="1"/>
-    <row r="328" hidden="1"/>
-    <row r="329" hidden="1"/>
-    <row r="330" hidden="1"/>
-    <row r="331" hidden="1"/>
-    <row r="332" hidden="1"/>
-    <row r="333" hidden="1"/>
-    <row r="334" hidden="1"/>
-    <row r="335" hidden="1"/>
-    <row r="336" hidden="1"/>
-    <row r="337" hidden="1"/>
-    <row r="338" hidden="1"/>
-    <row r="339" hidden="1"/>
-    <row r="340" hidden="1"/>
-    <row r="341" hidden="1"/>
-    <row r="342" hidden="1"/>
-    <row r="343" hidden="1"/>
-    <row r="344" hidden="1"/>
-    <row r="345" hidden="1"/>
-    <row r="346" hidden="1"/>
-    <row r="347" hidden="1"/>
-    <row r="348" hidden="1"/>
-    <row r="349" hidden="1"/>
-    <row r="350" hidden="1"/>
-    <row r="351" hidden="1"/>
-    <row r="352" hidden="1"/>
-    <row r="353" hidden="1"/>
-    <row r="354" hidden="1"/>
-    <row r="355" hidden="1"/>
-    <row r="356" hidden="1"/>
-    <row r="357" hidden="1"/>
-    <row r="358" hidden="1"/>
-    <row r="359" hidden="1"/>
-    <row r="360" hidden="1"/>
-    <row r="361" hidden="1"/>
-    <row r="362" hidden="1"/>
-    <row r="363" hidden="1"/>
-    <row r="364" hidden="1"/>
-    <row r="365" hidden="1"/>
-    <row r="366" hidden="1"/>
-    <row r="367" hidden="1"/>
-    <row r="368" hidden="1"/>
-    <row r="369" hidden="1"/>
-    <row r="370" hidden="1"/>
-    <row r="371" hidden="1"/>
-    <row r="372" hidden="1"/>
-    <row r="373" hidden="1"/>
-    <row r="374" hidden="1"/>
-    <row r="375" hidden="1"/>
-    <row r="376" hidden="1"/>
-    <row r="377" hidden="1"/>
-    <row r="378" hidden="1"/>
-    <row r="379" hidden="1"/>
-    <row r="380" hidden="1"/>
-    <row r="381" hidden="1"/>
-    <row r="382" hidden="1"/>
-    <row r="383" hidden="1"/>
-    <row r="384" hidden="1"/>
-    <row r="385" hidden="1"/>
-    <row r="386" hidden="1"/>
-    <row r="387" hidden="1"/>
-    <row r="388" hidden="1"/>
-    <row r="389" hidden="1"/>
-    <row r="390" hidden="1"/>
-    <row r="391" hidden="1"/>
-    <row r="392" hidden="1"/>
-    <row r="393" hidden="1"/>
-    <row r="394" hidden="1"/>
-    <row r="395" hidden="1"/>
-    <row r="396" hidden="1"/>
-    <row r="397" hidden="1"/>
-    <row r="398" hidden="1"/>
-    <row r="399" hidden="1"/>
-    <row r="400" hidden="1"/>
-    <row r="401" hidden="1"/>
-    <row r="402" hidden="1"/>
-    <row r="403" hidden="1"/>
-    <row r="404" hidden="1"/>
-    <row r="405" hidden="1"/>
-    <row r="406" hidden="1"/>
-    <row r="407" hidden="1"/>
-    <row r="408" hidden="1"/>
-    <row r="409" hidden="1"/>
-    <row r="410" hidden="1"/>
-    <row r="411" hidden="1"/>
-    <row r="412" hidden="1"/>
-    <row r="413" hidden="1"/>
-    <row r="414" hidden="1"/>
-    <row r="415" hidden="1"/>
-    <row r="416" hidden="1"/>
-    <row r="417" hidden="1"/>
-    <row r="418" hidden="1"/>
-    <row r="419" hidden="1"/>
-    <row r="420" hidden="1"/>
-    <row r="421" hidden="1"/>
-    <row r="422" hidden="1"/>
-    <row r="423" hidden="1"/>
-    <row r="424" hidden="1"/>
-    <row r="425" hidden="1"/>
-    <row r="426" hidden="1"/>
-    <row r="427" hidden="1"/>
-    <row r="428" hidden="1"/>
-    <row r="429" hidden="1"/>
-    <row r="430" hidden="1"/>
-    <row r="431" hidden="1"/>
-    <row r="432" hidden="1"/>
-    <row r="433" hidden="1"/>
-    <row r="434" hidden="1"/>
-    <row r="435" hidden="1"/>
-    <row r="436" hidden="1"/>
-    <row r="437" hidden="1"/>
-    <row r="438" hidden="1"/>
-    <row r="439" hidden="1"/>
-    <row r="440" hidden="1"/>
-    <row r="441" hidden="1"/>
-    <row r="442" hidden="1"/>
-    <row r="443" hidden="1"/>
-    <row r="444" hidden="1"/>
-    <row r="445" hidden="1"/>
-    <row r="446" hidden="1"/>
-    <row r="447" hidden="1"/>
-    <row r="448" hidden="1"/>
-    <row r="449" hidden="1"/>
-    <row r="450" hidden="1"/>
-    <row r="451" hidden="1"/>
-    <row r="452" hidden="1"/>
-    <row r="453" hidden="1"/>
-    <row r="454" hidden="1"/>
-    <row r="455" hidden="1"/>
-    <row r="456" hidden="1"/>
-    <row r="457" hidden="1"/>
-    <row r="458" hidden="1"/>
-    <row r="459" hidden="1"/>
-    <row r="460" hidden="1"/>
-    <row r="461" hidden="1"/>
-    <row r="462" hidden="1"/>
-    <row r="463" hidden="1"/>
-    <row r="464" hidden="1"/>
-    <row r="465" hidden="1"/>
-    <row r="466" hidden="1"/>
-    <row r="467" hidden="1"/>
-    <row r="468" hidden="1"/>
-    <row r="469" hidden="1"/>
-    <row r="470" hidden="1"/>
-    <row r="471" hidden="1"/>
-    <row r="472" hidden="1"/>
-    <row r="473" hidden="1"/>
-    <row r="474" hidden="1"/>
-    <row r="475" hidden="1"/>
-    <row r="476" hidden="1"/>
-    <row r="477" hidden="1"/>
-    <row r="478" hidden="1"/>
-    <row r="479" hidden="1"/>
-    <row r="480" hidden="1"/>
-    <row r="481" hidden="1"/>
-    <row r="482" hidden="1"/>
-    <row r="483" hidden="1"/>
-    <row r="484" hidden="1"/>
-    <row r="485" hidden="1"/>
-    <row r="486" hidden="1"/>
-    <row r="487" hidden="1"/>
-    <row r="488" hidden="1"/>
-    <row r="489" hidden="1"/>
-    <row r="490" hidden="1"/>
-    <row r="491" hidden="1"/>
-    <row r="492" hidden="1"/>
-    <row r="493" hidden="1"/>
-    <row r="494" hidden="1"/>
-    <row r="495" hidden="1"/>
-    <row r="496" hidden="1"/>
-    <row r="497" spans="1:1" hidden="1"/>
-    <row r="498" spans="1:1" hidden="1"/>
-    <row r="499" spans="1:1" hidden="1"/>
-    <row r="500" spans="1:1" hidden="1">
-      <c r="A500" s="2" t="s">
+    <row r="58" spans="3:9" ht="24.95" customHeight="1">
+      <c r="D58" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="3:9" ht="24.95" customHeight="1">
+      <c r="D59" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" ht="15.75" hidden="1">
+      <c r="A427" s="2" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I500" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
+  <autoFilter ref="A1:I427" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>
-    <filterColumn colId="3">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="J42" r:id="rId1" display="https://github.com/SitePen/dgrid/blob/master/doc/components/mixins/Selection.md" xr:uid="{B02003EC-0D72-4D32-86B5-BCB2E4740BDA}"/>
-    <hyperlink ref="I51" r:id="rId2" xr:uid="{D7280C89-055C-482B-859C-78DDF371D8BE}"/>
-    <hyperlink ref="I52" r:id="rId3" location="release_notes_08_23_2018" display="Can no longer disable showing of &quot;more videos&quot; when video is paused" xr:uid="{75869B48-9B1F-4352-8C34-D2F55186219A}"/>
+    <hyperlink ref="J27" r:id="rId1" display="https://github.com/SitePen/dgrid/blob/master/doc/components/mixins/Selection.md" xr:uid="{B02003EC-0D72-4D32-86B5-BCB2E4740BDA}"/>
+    <hyperlink ref="I33" r:id="rId2" xr:uid="{D7280C89-055C-482B-859C-78DDF371D8BE}"/>
+    <hyperlink ref="I34" r:id="rId3" location="release_notes_08_23_2018" display="Can no longer disable showing of &quot;more videos&quot; when video is paused" xr:uid="{75869B48-9B1F-4352-8C34-D2F55186219A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId4"/>

</xml_diff>

<commit_message>
Set up Fish Atlas species dropdown filter
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4E0585-BF29-4F2B-AE23-06C12B27791B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8A4399-E8EE-4B78-9475-AC64E9E7E1BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="885" windowWidth="27885" windowHeight="14715" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="6900" yWindow="480" windowWidth="21315" windowHeight="14490" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="120">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -514,6 +514,15 @@
   </si>
   <si>
     <t>look into Slider widgets?</t>
+  </si>
+  <si>
+    <t>done for FA</t>
+  </si>
+  <si>
+    <t>check if filtering affects display of points on map?</t>
+  </si>
+  <si>
+    <t>new icons for map widgets</t>
   </si>
 </sst>
 </file>
@@ -648,7 +657,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -673,6 +682,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -692,7 +707,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -760,6 +775,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1431,7 +1452,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C55" sqref="C55"/>
+      <selection pane="bottomRight" activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2099,6 +2120,9 @@
       <c r="D56" s="9" t="s">
         <v>113</v>
       </c>
+      <c r="I56" s="27" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="57" spans="3:9" ht="15.75" hidden="1">
       <c r="C57" s="2" t="s">
@@ -2119,6 +2143,16 @@
     <row r="59" spans="3:9" ht="24.95" customHeight="1">
       <c r="D59" s="9" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="3:9" ht="24.95" customHeight="1">
+      <c r="D60" s="28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" spans="3:9" ht="24.95" customHeight="1">
+      <c r="D61" s="9" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="427" spans="1:1" ht="15.75" hidden="1">

</xml_diff>

<commit_message>
Make habitat dropdowns independents between Region/Locale/Habitat tabs
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8A4399-E8EE-4B78-9475-AC64E9E7E1BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F150C52-15D4-4118-9614-552BF6A2382B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="480" windowWidth="21315" windowHeight="14490" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="5025" yWindow="480" windowWidth="23190" windowHeight="14490" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="121">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -519,10 +519,13 @@
     <t>done for FA</t>
   </si>
   <si>
-    <t>check if filtering affects display of points on map?</t>
-  </si>
-  <si>
     <t>new icons for map widgets</t>
+  </si>
+  <si>
+    <t>Flex site:  1) restore mapping/DotNet folder?     2)  ArcGis Server queries set to return in AMF format, which is no longer supported.</t>
+  </si>
+  <si>
+    <t>default to independent habitat dropdowns between Region/Locale/Site tabs</t>
   </si>
 </sst>
 </file>
@@ -657,7 +660,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -672,12 +675,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFE5FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -685,6 +682,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA7A7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -707,7 +716,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -774,13 +783,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -797,6 +809,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFA7A7"/>
       <color rgb="FFFFE5FF"/>
       <color rgb="FFFFCCFF"/>
     </mruColors>
@@ -1452,14 +1465,14 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D62" sqref="D62"/>
+      <selection pane="bottomRight" activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="53.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="62.75" style="9" customWidth="1"/>
     <col min="5" max="5" width="4.5" style="6" customWidth="1"/>
     <col min="6" max="6" width="11.25" style="7" customWidth="1"/>
     <col min="7" max="7" width="13.875" style="6" customWidth="1"/>
@@ -1571,7 +1584,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="63" hidden="1">
+    <row r="7" spans="1:9" ht="47.25" hidden="1">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1770,7 +1783,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="31.5" hidden="1">
+    <row r="24" spans="1:10" ht="15.75" hidden="1">
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
@@ -2021,7 +2034,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="39.75" customHeight="1">
-      <c r="D44" s="25" t="s">
+      <c r="D44" s="29" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2054,7 +2067,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="3:9" ht="15.75" hidden="1">
+    <row r="49" spans="1:9" ht="15.75" hidden="1">
       <c r="C49" s="2" t="s">
         <v>72</v>
       </c>
@@ -2062,7 +2075,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="3:9" ht="31.5" hidden="1">
+    <row r="50" spans="1:9" ht="31.5" hidden="1">
       <c r="C50" s="2" t="s">
         <v>71</v>
       </c>
@@ -2073,7 +2086,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="3:9" ht="24.95" hidden="1" customHeight="1">
+    <row r="51" spans="1:9" ht="24.95" hidden="1" customHeight="1">
       <c r="C51" s="2" t="s">
         <v>72</v>
       </c>
@@ -2081,7 +2094,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="3:9" ht="15.75" hidden="1">
+    <row r="52" spans="1:9" ht="15.75" hidden="1">
       <c r="C52" s="2" t="s">
         <v>21</v>
       </c>
@@ -2092,7 +2105,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="3:9" ht="15.75" hidden="1">
+    <row r="53" spans="1:9" ht="15.75" hidden="1">
       <c r="C53" s="2" t="s">
         <v>71</v>
       </c>
@@ -2103,7 +2116,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="3:9" ht="15.75" hidden="1">
+    <row r="54" spans="1:9" ht="15.75" hidden="1">
       <c r="C54" s="2" t="s">
         <v>21</v>
       </c>
@@ -2111,20 +2124,23 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="3:9" ht="24.95" customHeight="1">
+    <row r="55" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+      <c r="A55" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="D55" s="24" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="3:9" ht="24.95" customHeight="1">
+    <row r="56" spans="1:9" ht="24.95" customHeight="1">
       <c r="D56" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I56" s="27" t="s">
+      <c r="I56" s="26" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="3:9" ht="15.75" hidden="1">
+    <row r="57" spans="1:9" ht="15.75" hidden="1">
       <c r="C57" s="2" t="s">
         <v>21</v>
       </c>
@@ -2132,26 +2148,34 @@
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="3:9" ht="24.95" customHeight="1">
-      <c r="D58" s="26" t="s">
+    <row r="58" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D58" s="25" t="s">
         <v>114</v>
       </c>
       <c r="I58" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="59" spans="3:9" ht="24.95" customHeight="1">
+    <row r="59" spans="1:9" ht="24.95" customHeight="1">
       <c r="D59" s="9" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="60" spans="3:9" ht="24.95" customHeight="1">
-      <c r="D60" s="28" t="s">
+    <row r="60" spans="1:9" ht="31.5" hidden="1">
+      <c r="C60" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D60" s="27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D61" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="61" spans="3:9" ht="24.95" customHeight="1">
-      <c r="D61" s="9" t="s">
+    <row r="66" spans="4:4" ht="34.5" customHeight="1">
+      <c r="D66" s="28" t="s">
         <v>119</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Coordinate Fish Atlas layer display when filtering data
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F150C52-15D4-4118-9614-552BF6A2382B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E012FB62-9A54-4DF1-9B31-93E8F3D9A8FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5025" yWindow="480" windowWidth="23190" windowHeight="14490" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -35,8 +35,45 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jim</author>
+  </authors>
+  <commentList>
+    <comment ref="D59" authorId="0" shapeId="0" xr:uid="{8BE8D365-4202-41D2-8F8C-D33F0829961C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>4.14 feature</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D62" authorId="0" shapeId="0" xr:uid="{F4FBDC21-E4A6-4952-845B-FA2AABFC0B3B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Make clickable features invisible, hovering over MapService features?
+(Use views to limit features.)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="122">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -527,12 +564,15 @@
   <si>
     <t>default to independent habitat dropdowns between Region/Locale/Site tabs</t>
   </si>
+  <si>
+    <t>Do something about Locale labels</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -658,6 +698,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1457,7 +1503,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:J427"/>
   <sheetViews>
@@ -1465,7 +1511,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H63" sqref="H63"/>
+      <selection pane="bottomRight" activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2156,7 +2202,10 @@
         <v>115</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="24.95" customHeight="1">
+    <row r="59" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+      <c r="A59" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="D59" s="9" t="s">
         <v>116</v>
       </c>
@@ -2172,6 +2221,11 @@
     <row r="61" spans="1:9" ht="24.95" customHeight="1">
       <c r="D61" s="9" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D62" s="9" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="66" spans="4:4" ht="34.5" customHeight="1">
@@ -2200,5 +2254,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Setup species filter for Shore Stations
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E012FB62-9A54-4DF1-9B31-93E8F3D9A8FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27ABE492-51A1-484E-AAF5-E35463B8067A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="480" windowWidth="23190" windowHeight="14490" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="14430" yWindow="105" windowWidth="14085" windowHeight="14490" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="122">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -1511,7 +1511,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H64" sqref="H64"/>
+      <selection pane="bottomRight" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2223,7 +2223,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="24.95" customHeight="1">
+    <row r="62" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+      <c r="C62" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D62" s="9" t="s">
         <v>121</v>
       </c>

</xml_diff>

<commit_message>
Hide table but keep table headers when there is no disabledMsgInfix property (FA & SS tables)
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27ABE492-51A1-484E-AAF5-E35463B8067A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70201B59-3145-48C1-BBFE-B723443FB361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14430" yWindow="105" windowWidth="14085" windowHeight="14490" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="14085" windowHeight="14490" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="123">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -566,6 +566,9 @@
   </si>
   <si>
     <t>Do something about Locale labels</t>
+  </si>
+  <si>
+    <t>fix when whole table &amp; headers disappear on empty query results</t>
   </si>
 </sst>
 </file>
@@ -1511,7 +1514,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C61" sqref="C61"/>
+      <selection pane="bottomRight" activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2231,6 +2234,11 @@
         <v>121</v>
       </c>
     </row>
+    <row r="63" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D63" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
     <row r="66" spans="4:4" ht="34.5" customHeight="1">
       <c r="D66" s="28" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
Streamlined processFeatures method and submethods for tables
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70201B59-3145-48C1-BBFE-B723443FB361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC70A415-3895-4E4C-9B72-65FAA371BD77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="14085" windowHeight="14490" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="123">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -1514,7 +1514,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D64" sqref="D64"/>
+      <selection pane="bottomRight" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2082,7 +2082,10 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="39.75" customHeight="1">
+    <row r="44" spans="1:9" ht="39.75" hidden="1" customHeight="1">
+      <c r="C44" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="D44" s="29" t="s">
         <v>96</v>
       </c>
@@ -2234,7 +2237,10 @@
         <v>121</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="24.95" customHeight="1">
+    <row r="63" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+      <c r="C63" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D63" s="9" t="s">
         <v>122</v>
       </c>

</xml_diff>

<commit_message>
Fix timing issue on starting in FA or SS mode
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC70A415-3895-4E4C-9B72-65FAA371BD77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC795E9B-1F21-40E5-9D23-45413169420D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="14085" windowHeight="14490" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="22140" windowHeight="14490" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="125">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -553,9 +553,6 @@
     <t>look into Slider widgets?</t>
   </si>
   <si>
-    <t>done for FA</t>
-  </si>
-  <si>
     <t>new icons for map widgets</t>
   </si>
   <si>
@@ -569,6 +566,38 @@
   </si>
   <si>
     <t>fix when whole table &amp; headers disappear on empty query results</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">check </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>setTimeout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> references, see if can be replaced by "promise"</t>
+    </r>
+  </si>
+  <si>
+    <t>make visibility of SZ, FA &amp; SS services settable</t>
+  </si>
+  <si>
+    <t>simple dropdowns there, now need dialog box</t>
   </si>
 </sst>
 </file>
@@ -1511,10 +1540,10 @@
   <dimension ref="A1:J427"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C64" sqref="C64"/>
+      <selection pane="bottomRight" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2189,7 +2218,7 @@
         <v>113</v>
       </c>
       <c r="I56" s="26" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" hidden="1">
@@ -2221,12 +2250,12 @@
         <v>72</v>
       </c>
       <c r="D60" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="24.95" customHeight="1">
       <c r="D61" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="24.95" hidden="1" customHeight="1">
@@ -2234,7 +2263,7 @@
         <v>21</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="24.95" hidden="1" customHeight="1">
@@ -2242,12 +2271,22 @@
         <v>21</v>
       </c>
       <c r="D63" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D64" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" ht="24.95" customHeight="1">
+      <c r="D67" s="9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="4:4" ht="34.5" customHeight="1">
-      <c r="D66" s="28" t="s">
-        <v>119</v>
+    <row r="68" spans="4:4" ht="34.5" customHeight="1">
+      <c r="D68" s="28" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="427" spans="1:1" ht="15.75" hidden="1">

</xml_diff>

<commit_message>
Remove Temp/Eelgrass, make map service root selectable, start on species selection dialogs
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC795E9B-1F21-40E5-9D23-45413169420D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A613BA21-2C38-4234-A9EA-7F405EFD8A7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="22140" windowHeight="14490" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$427</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$428</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="127">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -594,17 +594,35 @@
     </r>
   </si>
   <si>
-    <t>make visibility of SZ, FA &amp; SS services settable</t>
-  </si>
-  <si>
     <t>simple dropdowns there, now need dialog box</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">adjust alignment of map service visibility checkbox in LayerList     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>make visibility of SZ, FA &amp; SS services settable</t>
+    </r>
+  </si>
+  <si>
+    <t>FA statewide query panel</t>
+  </si>
+  <si>
+    <t>download table data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -736,6 +754,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1537,13 +1562,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J427"/>
+  <dimension ref="A1:J428"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D65" sqref="D65"/>
+      <selection pane="bottomRight" activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2218,7 +2243,7 @@
         <v>113</v>
       </c>
       <c r="I56" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" hidden="1">
@@ -2274,28 +2299,41 @@
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="24.95" customHeight="1">
+    <row r="64" spans="1:9" ht="32.25" hidden="1" customHeight="1">
+      <c r="C64" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D64" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="67" spans="4:4" ht="24.95" customHeight="1">
-      <c r="D67" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" ht="24.95" customHeight="1">
+      <c r="D65" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" ht="24.95" customHeight="1">
+      <c r="D66" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" ht="24.95" customHeight="1">
+      <c r="D68" s="9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="4:4" ht="34.5" customHeight="1">
-      <c r="D68" s="28" t="s">
+    <row r="69" spans="4:4" ht="34.5" customHeight="1">
+      <c r="D69" s="28" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="427" spans="1:1" ht="15.75" hidden="1">
-      <c r="A427" s="2" t="s">
+    <row r="428" spans="1:1" ht="15.75" hidden="1">
+      <c r="A428" s="2" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I427" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
+  <autoFilter ref="A1:I428" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Make dropdown panel filtering selections work together
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A613BA21-2C38-4234-A9EA-7F405EFD8A7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6799D7-2BA8-4240-A0E0-FE12C480C85B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="22140" windowHeight="14490" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="6405" yWindow="1440" windowWidth="22140" windowHeight="12270" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="128">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -594,9 +594,6 @@
     </r>
   </si>
   <si>
-    <t>simple dropdowns there, now need dialog box</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">adjust alignment of map service visibility checkbox in LayerList     </t>
     </r>
@@ -616,6 +613,12 @@
   </si>
   <si>
     <t>download table data</t>
+  </si>
+  <si>
+    <t>have dialog box for FA, now need for SS</t>
+  </si>
+  <si>
+    <t>do combined dropdown selections sometimes not work?  (e.g. FA Sites)</t>
   </si>
 </sst>
 </file>
@@ -763,7 +766,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -800,6 +803,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE5FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -819,7 +828,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -896,6 +905,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -912,8 +924,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFE5FF"/>
       <color rgb="FFFFA7A7"/>
-      <color rgb="FFFFE5FF"/>
       <color rgb="FFFFCCFF"/>
     </mruColors>
   </colors>
@@ -1565,10 +1577,10 @@
   <dimension ref="A1:J428"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D73" sqref="D73"/>
+      <selection pane="bottomRight" activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2243,7 +2255,7 @@
         <v>113</v>
       </c>
       <c r="I56" s="26" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" hidden="1">
@@ -2304,17 +2316,17 @@
         <v>21</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="4:4" ht="24.95" customHeight="1">
       <c r="D65" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="4:4" ht="24.95" customHeight="1">
       <c r="D66" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68" spans="4:4" ht="24.95" customHeight="1">
@@ -2325,6 +2337,11 @@
     <row r="69" spans="4:4" ht="34.5" customHeight="1">
       <c r="D69" s="28" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="70" spans="4:4" ht="24.95" customHeight="1">
+      <c r="D70" s="30" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="428" spans="1:1" ht="15.75" hidden="1">

</xml_diff>

<commit_message>
Set up species dropdown panel for Shore Stations
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6799D7-2BA8-4240-A0E0-FE12C480C85B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D55FE52-C5F6-47B8-AC23-0901700FAF1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6405" yWindow="1440" windowWidth="22140" windowHeight="12270" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="128">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -1580,7 +1580,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F48" sqref="F48"/>
+      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2319,27 +2319,30 @@
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="4:4" ht="24.95" customHeight="1">
+    <row r="65" spans="3:4" ht="24.95" customHeight="1">
       <c r="D65" s="9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="66" spans="4:4" ht="24.95" customHeight="1">
+    <row r="66" spans="3:4" ht="24.95" hidden="1" customHeight="1">
+      <c r="C66" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D66" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="68" spans="4:4" ht="24.95" customHeight="1">
+    <row r="68" spans="3:4" ht="24.95" customHeight="1">
       <c r="D68" s="9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="69" spans="4:4" ht="34.5" customHeight="1">
+    <row r="69" spans="3:4" ht="34.5" customHeight="1">
       <c r="D69" s="28" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="70" spans="4:4" ht="24.95" customHeight="1">
+    <row r="70" spans="3:4" ht="24.95" customHeight="1">
       <c r="D70" s="30" t="s">
         <v>127</v>
       </c>

</xml_diff>

<commit_message>
Add Shore Stations Group and Subgroup dropdowns.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D55FE52-C5F6-47B8-AC23-0901700FAF1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946CAC6D-D0F6-4BFD-A90D-291E7FE7B1A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6405" yWindow="1440" windowWidth="22140" windowHeight="12270" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="2730" yWindow="2295" windowWidth="22665" windowHeight="13905" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$428</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$431</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="129">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -615,10 +615,13 @@
     <t>download table data</t>
   </si>
   <si>
-    <t>have dialog box for FA, now need for SS</t>
-  </si>
-  <si>
     <t>do combined dropdown selections sometimes not work?  (e.g. FA Sites)</t>
+  </si>
+  <si>
+    <t>add download of video clip (from video panel)</t>
+  </si>
+  <si>
+    <t>limit dropdown lists based on other dropdown selections</t>
   </si>
 </sst>
 </file>
@@ -1574,13 +1577,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J428"/>
+  <dimension ref="A1:J431"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
+      <selection pane="bottomRight" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2250,13 +2253,14 @@
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="24.95" customHeight="1">
+    <row r="56" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+      <c r="C56" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D56" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I56" s="26" t="s">
-        <v>126</v>
-      </c>
+      <c r="I56" s="26"/>
     </row>
     <row r="57" spans="1:9" ht="15.75" hidden="1">
       <c r="C57" s="2" t="s">
@@ -2332,28 +2336,38 @@
         <v>125</v>
       </c>
     </row>
+    <row r="67" spans="3:4" ht="24.95" customHeight="1">
+      <c r="D67" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
     <row r="68" spans="3:4" ht="24.95" customHeight="1">
       <c r="D68" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4" ht="24.95" customHeight="1">
+      <c r="D71" s="9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="69" spans="3:4" ht="34.5" customHeight="1">
-      <c r="D69" s="28" t="s">
+    <row r="72" spans="3:4" ht="34.5" customHeight="1">
+      <c r="D72" s="28" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="70" spans="3:4" ht="24.95" customHeight="1">
-      <c r="D70" s="30" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="428" spans="1:1" ht="15.75" hidden="1">
-      <c r="A428" s="2" t="s">
+    <row r="73" spans="3:4" ht="24.95" customHeight="1">
+      <c r="D73" s="30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" ht="15.75" hidden="1">
+      <c r="A431" s="2" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I428" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
+  <autoFilter ref="A1:I431" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Manage WHERE clause for dropdown panels involving several dropdowns.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946CAC6D-D0F6-4BFD-A90D-291E7FE7B1A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50103DB-7509-455F-81F1-C4A127AA0289}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2295" windowWidth="22665" windowHeight="13905" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -1583,7 +1583,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C58" sqref="C58"/>
+      <selection pane="bottomRight" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>

</xml_diff>

<commit_message>
test window.innerHeight on file download
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50103DB-7509-455F-81F1-C4A127AA0289}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD692B2-E3D7-4C3A-81BA-2FB7E0382477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2295" windowWidth="22665" windowHeight="13905" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="5745" yWindow="1590" windowWidth="22215" windowHeight="13905" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="132">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -622,6 +622,15 @@
   </si>
   <si>
     <t>limit dropdown lists based on other dropdown selections</t>
+  </si>
+  <si>
+    <t>SZ:  If (Chrome) downloads panel appears and changes map panel size, don't requery points</t>
+  </si>
+  <si>
+    <t>Google search</t>
+  </si>
+  <si>
+    <t>set some kind of flag to let app know it's not a real map panel resize?</t>
   </si>
 </sst>
 </file>
@@ -1583,7 +1592,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D68" sqref="D68"/>
+      <selection pane="bottomRight" activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2323,12 +2332,12 @@
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="3:4" ht="24.95" customHeight="1">
+    <row r="65" spans="3:9" ht="24.95" customHeight="1">
       <c r="D65" s="9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="66" spans="3:4" ht="24.95" hidden="1" customHeight="1">
+    <row r="66" spans="3:9" ht="24.95" hidden="1" customHeight="1">
       <c r="C66" s="2" t="s">
         <v>21</v>
       </c>
@@ -2336,27 +2345,38 @@
         <v>125</v>
       </c>
     </row>
-    <row r="67" spans="3:4" ht="24.95" customHeight="1">
+    <row r="67" spans="3:9" ht="24.95" customHeight="1">
       <c r="D67" s="9" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="68" spans="3:4" ht="24.95" customHeight="1">
+    <row r="68" spans="3:9" ht="24.95" customHeight="1">
       <c r="D68" s="9" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="71" spans="3:4" ht="24.95" customHeight="1">
+    <row r="69" spans="3:9" ht="31.5">
+      <c r="D69" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G69" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="I69" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="3:9" ht="24.95" customHeight="1">
       <c r="D71" s="9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="72" spans="3:4" ht="34.5" customHeight="1">
+    <row r="72" spans="3:9" ht="34.5" customHeight="1">
       <c r="D72" s="28" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="73" spans="3:4" ht="24.95" customHeight="1">
+    <row r="73" spans="3:9" ht="24.95" customHeight="1">
       <c r="D73" s="30" t="s">
         <v>126</v>
       </c>
@@ -2379,9 +2399,10 @@
     <hyperlink ref="J27" r:id="rId1" display="https://github.com/SitePen/dgrid/blob/master/doc/components/mixins/Selection.md" xr:uid="{B02003EC-0D72-4D32-86B5-BCB2E4740BDA}"/>
     <hyperlink ref="I33" r:id="rId2" xr:uid="{D7280C89-055C-482B-859C-78DDF371D8BE}"/>
     <hyperlink ref="I34" r:id="rId3" location="release_notes_08_23_2018" display="Can no longer disable showing of &quot;more videos&quot; when video is paused" xr:uid="{75869B48-9B1F-4352-8C34-D2F55186219A}"/>
+    <hyperlink ref="G69" r:id="rId4" display="https://www.google.com/search?sxsrf=ALeKk03fRI45rxW7duPejqDWYRNo315xnA%3A1589067316875Google search" xr:uid="{B59445F6-07F3-4CDD-950F-C113A43BEE63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Attempts at bypassing SZ point regeneration on downloads bar show/hide.  (commented out)
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD692B2-E3D7-4C3A-81BA-2FB7E0382477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FEEB57-7A1F-4DFB-AE8F-FB8332F1F85C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5745" yWindow="1590" windowWidth="22215" windowHeight="13905" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="1050" yWindow="45" windowWidth="26190" windowHeight="15555" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
     <sheet name="to do" sheetId="1" r:id="rId2"/>
+    <sheet name="SZ point regeneration rethink" sheetId="14" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$8</definedName>
@@ -68,6 +69,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="D69" authorId="0" shapeId="0" xr:uid="{E4E7D546-5501-4B22-B4CB-2D44BAC24129}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">see </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>SZ point regeneration rethink</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> tab</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -624,20 +657,46 @@
     <t>limit dropdown lists based on other dropdown selections</t>
   </si>
   <si>
-    <t>SZ:  If (Chrome) downloads panel appears and changes map panel size, don't requery points</t>
-  </si>
-  <si>
     <t>Google search</t>
   </si>
   <si>
     <t>set some kind of flag to let app know it's not a real map panel resize?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SZ:  Make manual point regeneration the default, and add map tool for setting this.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">old task:  </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If (Chrome) downloads panel appears and changes map panel size, don't requery points</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -776,6 +835,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1221,6 +1293,61 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>142879</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133354</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>633226</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>65028</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F523197-4540-4E3B-BAB1-FA9387155FFF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="142879" y="133354"/>
+          <a:ext cx="4605147" cy="6932549"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1592,7 +1719,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I70" sqref="I70"/>
+      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2355,15 +2482,15 @@
         <v>128</v>
       </c>
     </row>
-    <row r="69" spans="3:9" ht="31.5">
+    <row r="69" spans="3:9" ht="63">
       <c r="D69" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G69" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="G69" s="19" t="s">
+      <c r="I69" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="I69" s="11" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="71" spans="3:9" ht="24.95" customHeight="1">
@@ -2405,4 +2532,19 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId5"/>
   <legacyDrawing r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3521A2-0E46-4626-A556-F81B8258D1DB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Panel with link to SZapps page for table downloads, add FA & SS to SZapps page.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FEEB57-7A1F-4DFB-AE8F-FB8332F1F85C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE3E888-EED8-4358-A418-A599C5EDB039}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="45" windowWidth="26190" windowHeight="15555" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
     <sheet name="to do" sheetId="1" r:id="rId2"/>
     <sheet name="SZ point regeneration rethink" sheetId="14" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$431</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$432</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -105,8 +106,32 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jim</author>
+  </authors>
+  <commentList>
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{79327622-38C1-4F4F-A8CA-2FE4024A7825}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>not there yet</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="145">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -691,12 +716,51 @@
       <t>If (Chrome) downloads panel appears and changes map panel size, don't requery points</t>
     </r>
   </si>
+  <si>
+    <t>add link to download FA (and SS?) GDB</t>
+  </si>
+  <si>
+    <t>Downloads</t>
+  </si>
+  <si>
+    <t>offline app</t>
+  </si>
+  <si>
+    <t>FCs and media</t>
+  </si>
+  <si>
+    <t>map widget</t>
+  </si>
+  <si>
+    <t>disc icon</t>
+  </si>
+  <si>
+    <t>table DL as CSV</t>
+  </si>
+  <si>
+    <t>(disc icon)</t>
+  </si>
+  <si>
+    <t>video clip</t>
+  </si>
+  <si>
+    <t>top-right links</t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>MPKs</t>
+  </si>
+  <si>
+    <t>link from table download panel?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -849,6 +913,21 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -894,7 +973,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -902,8 +981,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
@@ -911,8 +999,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -994,8 +1083,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="7"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
+    <cellStyle name="Heading 2" xfId="7" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{1147CFDD-9E92-4003-90A5-A177F72C7D95}"/>
@@ -1713,13 +1804,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J431"/>
+  <dimension ref="A1:J432"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
+      <selection pane="bottomRight" activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2493,28 +2584,34 @@
         <v>130</v>
       </c>
     </row>
-    <row r="71" spans="3:9" ht="24.95" customHeight="1">
-      <c r="D71" s="9" t="s">
+    <row r="70" spans="3:9" ht="15.75">
+      <c r="D70" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G70" s="19"/>
+    </row>
+    <row r="72" spans="3:9" ht="24.95" customHeight="1">
+      <c r="D72" s="9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="72" spans="3:9" ht="34.5" customHeight="1">
-      <c r="D72" s="28" t="s">
+    <row r="73" spans="3:9" ht="34.5" customHeight="1">
+      <c r="D73" s="28" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="73" spans="3:9" ht="24.95" customHeight="1">
-      <c r="D73" s="30" t="s">
+    <row r="74" spans="3:9" ht="24.95" customHeight="1">
+      <c r="D74" s="30" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="431" spans="1:1" ht="15.75" hidden="1">
-      <c r="A431" s="2" t="s">
+    <row r="432" spans="1:1" ht="15.75" hidden="1">
+      <c r="A432" s="2" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I431" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
+  <autoFilter ref="A1:I432" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
@@ -2547,4 +2644,78 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D90DEFD-D6A8-4BFB-97A2-600F5E7E4446}">
+  <dimension ref="B2:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="18" thickBot="1">
+      <c r="B2" s="31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="16.5" thickTop="1"/>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed Url generation for NOAA/PSMFC, fixed display of staions with Bioband/Species filter
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2D0E76-F634-4ACF-B0F3-A250A26011C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66973CDE-200B-47C4-AAF1-504771CABFC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13965" yWindow="45" windowWidth="14655" windowHeight="15555" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="270" yWindow="45" windowWidth="19695" windowHeight="15555" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$433</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$434</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="148">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -673,9 +673,6 @@
     <t>download table data</t>
   </si>
   <si>
-    <t>do combined dropdown selections sometimes not work?  (e.g. FA Sites)</t>
-  </si>
-  <si>
     <t>add download of video clip (from video panel)</t>
   </si>
   <si>
@@ -757,6 +754,15 @@
   </si>
   <si>
     <t>When "All" is selected in SS species filter panel, do not close and run query if something is selected in upper dropdown</t>
+  </si>
+  <si>
+    <t>Check photos/video on server, arrange original photos for PSMFC, check when last updates were done, figure out everything that goes to PSMFC</t>
+  </si>
+  <si>
+    <t>Set up fallback to PSMFC for all services &amp; imagery</t>
+  </si>
+  <si>
+    <t>get table back after previous query returns no rows</t>
   </si>
 </sst>
 </file>
@@ -976,7 +982,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -993,6 +999,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1004,7 +1025,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1087,6 +1108,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="7"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Heading 2" xfId="7" builtinId="17"/>
@@ -1807,13 +1831,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J433"/>
+  <dimension ref="A1:J434"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F71" sqref="F71"/>
+      <selection pane="bottomRight" activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2568,23 +2592,23 @@
     </row>
     <row r="67" spans="3:9" ht="24.95" customHeight="1">
       <c r="D67" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" spans="3:9" ht="24.95" customHeight="1">
       <c r="D68" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="3:9" ht="63">
       <c r="D69" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G69" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="I69" s="11" t="s">
         <v>129</v>
-      </c>
-      <c r="I69" s="11" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="70" spans="3:9" ht="15.75" hidden="1">
@@ -2592,38 +2616,50 @@
         <v>21</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G70" s="19"/>
     </row>
-    <row r="71" spans="3:9" ht="42" customHeight="1">
-      <c r="D71" s="9" t="s">
+    <row r="71" spans="3:9" ht="24.95" customHeight="1">
+      <c r="D71" s="30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="72" spans="3:9" ht="42" customHeight="1" thickBot="1">
+      <c r="D72" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="G72" s="19"/>
+    </row>
+    <row r="73" spans="3:9" ht="16.5" thickBot="1">
+      <c r="D73" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="G73" s="19"/>
+    </row>
+    <row r="75" spans="3:9" ht="24.95" customHeight="1">
+      <c r="D75" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="3:9" ht="34.5" customHeight="1">
+      <c r="D76" s="28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="77" spans="3:9" ht="24.95" customHeight="1" thickBot="1"/>
+    <row r="78" spans="3:9" ht="32.25" thickBot="1">
+      <c r="D78" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="G71" s="19"/>
-    </row>
-    <row r="73" spans="3:9" ht="24.95" customHeight="1">
-      <c r="D73" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="74" spans="3:9" ht="34.5" customHeight="1">
-      <c r="D74" s="28" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="75" spans="3:9" ht="24.95" customHeight="1">
-      <c r="D75" s="30" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="433" spans="1:1" ht="15.75" hidden="1">
-      <c r="A433" s="2" t="s">
+    </row>
+    <row r="434" spans="1:1" ht="15.75" hidden="1">
+      <c r="A434" s="2" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I433" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
+  <autoFilter ref="A1:I434" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
@@ -2674,56 +2710,56 @@
   <sheetData>
     <row r="2" spans="2:3" ht="18" thickBot="1">
       <c r="B2" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="16.5" thickTop="1"/>
     <row r="4" spans="2:3">
       <c r="B4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" t="s">
         <v>137</v>
-      </c>
-      <c r="C7" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" t="s">
         <v>139</v>
-      </c>
-      <c r="C8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" t="s">
         <v>141</v>
-      </c>
-      <c r="C10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
On switching DBs, retain previous state if data is present.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66973CDE-200B-47C4-AAF1-504771CABFC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ED8489-6696-4A03-8627-3E4699ECDE7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="45" windowWidth="19695" windowHeight="15555" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="270" yWindow="45" windowWidth="24810" windowHeight="15555" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="148">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -1837,7 +1837,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H72" sqref="H72"/>
+      <selection pane="bottomRight" activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2600,7 +2600,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="3:9" ht="63">
+    <row r="69" spans="3:9" ht="63.75" thickBot="1">
       <c r="D69" s="9" t="s">
         <v>130</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="3:9" ht="15.75" hidden="1">
+    <row r="70" spans="3:9" ht="16.5" hidden="1" thickBot="1">
       <c r="C70" s="2" t="s">
         <v>21</v>
       </c>
@@ -2620,12 +2620,18 @@
       </c>
       <c r="G70" s="19"/>
     </row>
-    <row r="71" spans="3:9" ht="24.95" customHeight="1">
+    <row r="71" spans="3:9" ht="24.95" hidden="1" customHeight="1" thickBot="1">
+      <c r="C71" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D71" s="30" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="72" spans="3:9" ht="42" customHeight="1" thickBot="1">
+    <row r="72" spans="3:9" ht="42" hidden="1" customHeight="1" thickBot="1">
+      <c r="C72" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D72" s="9" t="s">
         <v>144</v>
       </c>

</xml_diff>

<commit_message>
Map service URLs as 2-element arrays (for PS or NOAA)
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D54622-059E-46F8-BA2E-15AF3FE01838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870278A3-04B6-4822-A0E9-95D40F95C4AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="45" windowWidth="24810" windowHeight="15555" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="270" yWindow="45" windowWidth="27030" windowHeight="15555" activeTab="2" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
     <sheet name="to do" sheetId="1" r:id="rId2"/>
-    <sheet name="SZ point regeneration rethink" sheetId="14" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="15" r:id="rId4"/>
+    <sheet name="to do - SS" sheetId="16" r:id="rId3"/>
+    <sheet name="SZ point regeneration rethink" sheetId="14" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$435</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'to do - SS'!$A$1:$I$435</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -131,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="154">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -759,9 +761,6 @@
     <t>Check photos/video on server, arrange original photos for PSMFC, check when last updates were done, figure out everything that goes to PSMFC</t>
   </si>
   <si>
-    <t>Set up fallback to PSMFC for all services &amp; imagery</t>
-  </si>
-  <si>
     <t>get table back after previous query returns no rows</t>
   </si>
   <si>
@@ -795,6 +794,41 @@
   </si>
   <si>
     <t>new in 4.15, still in beta</t>
+  </si>
+  <si>
+    <t>Set up fallback to alternate server for all services &amp; imagery</t>
+  </si>
+  <si>
+    <t>enable common/scientific radio button</t>
+  </si>
+  <si>
+    <t>Species table:  algae/invert filters</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Species table:  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>show biobands</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> option</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -970,7 +1004,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -980,12 +1014,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1010,6 +1038,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFE5FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1057,7 +1097,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1121,13 +1161,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1136,11 +1173,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="7"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="7"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1158,9 +1201,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCFF"/>
       <color rgb="FFFFE5FF"/>
       <color rgb="FFFFA7A7"/>
-      <color rgb="FFFFCCFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1444,6 +1487,55 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1723224</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>75975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB1CF29C-8624-44D6-8DB4-E3C63A6C32D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8877300" y="1314450"/>
+          <a:ext cx="6409524" cy="1800000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1865,11 +1957,11 @@
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:J435"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I81" sqref="I81"/>
+      <selection pane="bottomRight" activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2441,7 +2533,7 @@
       <c r="C44" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D44" s="29" t="s">
+      <c r="D44" s="27" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2546,7 +2638,7 @@
       <c r="D56" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I56" s="26"/>
+      <c r="I56" s="25"/>
     </row>
     <row r="57" spans="1:9" ht="15.75" hidden="1">
       <c r="C57" s="2" t="s">
@@ -2557,7 +2649,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" ht="24.95" customHeight="1">
-      <c r="D58" s="25" t="s">
+      <c r="D58" s="31" t="s">
         <v>114</v>
       </c>
       <c r="I58" s="11" t="s">
@@ -2576,7 +2668,7 @@
       <c r="C60" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D60" s="27" t="s">
+      <c r="D60" s="26" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2628,12 +2720,12 @@
       </c>
     </row>
     <row r="68" spans="3:9" ht="24.95" customHeight="1">
-      <c r="D68" s="9" t="s">
+      <c r="D68" s="31" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="69" spans="3:9" ht="63.75" thickBot="1">
-      <c r="D69" s="9" t="s">
+      <c r="D69" s="31" t="s">
         <v>130</v>
       </c>
       <c r="G69" s="19" t="s">
@@ -2656,8 +2748,8 @@
       <c r="C71" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D71" s="30" t="s">
-        <v>147</v>
+      <c r="D71" s="28" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="72" spans="3:9" ht="42" hidden="1" customHeight="1" thickBot="1">
@@ -2670,14 +2762,14 @@
       <c r="G72" s="19"/>
     </row>
     <row r="73" spans="3:9" ht="16.5" thickBot="1">
-      <c r="D73" s="32" t="s">
-        <v>146</v>
+      <c r="D73" s="30" t="s">
+        <v>150</v>
       </c>
       <c r="G73" s="19"/>
     </row>
     <row r="74" spans="3:9" ht="15.75">
       <c r="D74" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G74" s="19"/>
     </row>
@@ -2687,7 +2779,7 @@
       </c>
     </row>
     <row r="77" spans="3:9" ht="34.5" customHeight="1">
-      <c r="D77" s="28" t="s">
+      <c r="D77" s="33" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2698,11 +2790,11 @@
       </c>
     </row>
     <row r="80" spans="3:9" ht="24.95" customHeight="1">
-      <c r="D80" s="27" t="s">
+      <c r="D80" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="I80" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="I80" s="11" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="435" spans="1:1" ht="15.75" hidden="1">
@@ -2732,6 +2824,3548 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8A68F0-A5CC-4F2B-9E7A-D47D3E46C475}">
+  <dimension ref="A1:J435"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="3.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="62.75" style="9" customWidth="1"/>
+    <col min="5" max="5" width="4.5" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.25" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="8.125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="62.625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="32.125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="97.5" customHeight="1">
+      <c r="A1" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" customFormat="1" ht="15.75">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="2:9" ht="15.75">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="2:9" ht="15.75">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="2:9" ht="15.75">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="2:9" ht="15.75">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="2:9" ht="15.75">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="2:9" ht="15.75">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="2:9" ht="15.75">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="2:9" ht="15.75">
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="2:9" ht="15.75">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="2:9" ht="15.75">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="2:9" ht="15.75">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="2:9" ht="15.75">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="2:9" ht="15.75">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="2:9" ht="15.75">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="2:9" ht="15.75">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="2:9" ht="15.75">
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="2:9" ht="15.75">
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="2:9" ht="15.75">
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="2:9" ht="15.75">
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" spans="2:9" ht="15.75">
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" spans="2:9" ht="15.75">
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+    </row>
+    <row r="38" spans="2:9" ht="15.75">
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+    </row>
+    <row r="39" spans="2:9" ht="15.75">
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="2:9" ht="15.75">
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+    </row>
+    <row r="41" spans="2:9" ht="15.75">
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+    </row>
+    <row r="42" spans="2:9" ht="15.75">
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+    </row>
+    <row r="43" spans="2:9" ht="15.75">
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="2:9" ht="39.75" customHeight="1">
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+    </row>
+    <row r="45" spans="2:9" ht="15.75">
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+    </row>
+    <row r="46" spans="2:9" ht="15.75">
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+    </row>
+    <row r="47" spans="2:9" ht="9.75" customHeight="1">
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+    </row>
+    <row r="48" spans="2:9" ht="42" customHeight="1">
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+    </row>
+    <row r="49" spans="2:9" ht="15.75">
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+    </row>
+    <row r="50" spans="2:9" ht="15.75">
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+    </row>
+    <row r="51" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+    </row>
+    <row r="52" spans="2:9" ht="15.75">
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+    </row>
+    <row r="53" spans="2:9" ht="15.75">
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+    </row>
+    <row r="54" spans="2:9" ht="15.75">
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+    </row>
+    <row r="55" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+    </row>
+    <row r="56" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+    </row>
+    <row r="57" spans="2:9" ht="15.75">
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+    </row>
+    <row r="58" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+    </row>
+    <row r="59" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+    </row>
+    <row r="60" spans="2:9" ht="15.75">
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+    </row>
+    <row r="61" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+    </row>
+    <row r="62" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+    </row>
+    <row r="63" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+    </row>
+    <row r="64" spans="2:9" ht="32.25" customHeight="1">
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+    </row>
+    <row r="65" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+    </row>
+    <row r="66" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+    </row>
+    <row r="67" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+    </row>
+    <row r="68" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+    </row>
+    <row r="69" spans="2:9" ht="15.75">
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+    </row>
+    <row r="70" spans="2:9" ht="15.75">
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
+    </row>
+    <row r="71" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+    </row>
+    <row r="72" spans="2:9" ht="42" customHeight="1">
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+    </row>
+    <row r="73" spans="2:9" ht="15.75">
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+    </row>
+    <row r="74" spans="2:9" ht="15.75">
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+    </row>
+    <row r="75" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+    </row>
+    <row r="76" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+    </row>
+    <row r="77" spans="2:9" ht="34.5" customHeight="1">
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+    </row>
+    <row r="78" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+    </row>
+    <row r="79" spans="2:9" ht="15.75">
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+    </row>
+    <row r="80" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+    </row>
+    <row r="81" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+    </row>
+    <row r="82" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+    </row>
+    <row r="83" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+    </row>
+    <row r="84" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+    </row>
+    <row r="85" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+    </row>
+    <row r="86" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+    </row>
+    <row r="87" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+    </row>
+    <row r="88" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+    </row>
+    <row r="89" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
+    </row>
+    <row r="90" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+    </row>
+    <row r="91" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+    </row>
+    <row r="92" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+    </row>
+    <row r="93" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+    </row>
+    <row r="94" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B94" s="6"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+    </row>
+    <row r="95" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+    </row>
+    <row r="96" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+    </row>
+    <row r="97" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B97" s="6"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+    </row>
+    <row r="98" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B98" s="6"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+    </row>
+    <row r="99" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+    </row>
+    <row r="100" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B100" s="6"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="F100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+    </row>
+    <row r="101" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B101" s="6"/>
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="F101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+    </row>
+    <row r="102" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B102" s="6"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+    </row>
+    <row r="103" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+    </row>
+    <row r="104" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B104" s="6"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="6"/>
+    </row>
+    <row r="105" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6"/>
+    </row>
+    <row r="106" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B106" s="6"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="F106" s="6"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6"/>
+    </row>
+    <row r="107" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B107" s="6"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="F107" s="6"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6"/>
+    </row>
+    <row r="108" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B108" s="6"/>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
+    </row>
+    <row r="109" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B109" s="6"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="F109" s="6"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="6"/>
+    </row>
+    <row r="110" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="F110" s="6"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="6"/>
+    </row>
+    <row r="111" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B111" s="6"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="F111" s="6"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="6"/>
+    </row>
+    <row r="112" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B112" s="6"/>
+      <c r="C112" s="6"/>
+      <c r="D112" s="6"/>
+      <c r="F112" s="6"/>
+      <c r="H112" s="6"/>
+      <c r="I112" s="6"/>
+    </row>
+    <row r="113" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B113" s="6"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+    </row>
+    <row r="114" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B114" s="6"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="6"/>
+    </row>
+    <row r="115" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6"/>
+    </row>
+    <row r="116" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B116" s="6"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="H116" s="6"/>
+      <c r="I116" s="6"/>
+    </row>
+    <row r="117" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B117" s="6"/>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="F117" s="6"/>
+      <c r="H117" s="6"/>
+      <c r="I117" s="6"/>
+    </row>
+    <row r="118" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B118" s="6"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="F118" s="6"/>
+      <c r="H118" s="6"/>
+      <c r="I118" s="6"/>
+    </row>
+    <row r="119" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B119" s="6"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+      <c r="F119" s="6"/>
+      <c r="H119" s="6"/>
+      <c r="I119" s="6"/>
+    </row>
+    <row r="120" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B120" s="6"/>
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+      <c r="F120" s="6"/>
+      <c r="H120" s="6"/>
+      <c r="I120" s="6"/>
+    </row>
+    <row r="121" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B121" s="6"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="F121" s="6"/>
+      <c r="H121" s="6"/>
+      <c r="I121" s="6"/>
+    </row>
+    <row r="122" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B122" s="6"/>
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="F122" s="6"/>
+      <c r="H122" s="6"/>
+      <c r="I122" s="6"/>
+    </row>
+    <row r="123" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B123" s="6"/>
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
+      <c r="F123" s="6"/>
+      <c r="H123" s="6"/>
+      <c r="I123" s="6"/>
+    </row>
+    <row r="124" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B124" s="6"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="6"/>
+      <c r="F124" s="6"/>
+      <c r="H124" s="6"/>
+      <c r="I124" s="6"/>
+    </row>
+    <row r="125" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B125" s="6"/>
+      <c r="C125" s="6"/>
+      <c r="D125" s="6"/>
+      <c r="F125" s="6"/>
+      <c r="H125" s="6"/>
+      <c r="I125" s="6"/>
+    </row>
+    <row r="126" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B126" s="6"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
+      <c r="F126" s="6"/>
+      <c r="H126" s="6"/>
+      <c r="I126" s="6"/>
+    </row>
+    <row r="127" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B127" s="6"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="6"/>
+      <c r="F127" s="6"/>
+      <c r="H127" s="6"/>
+      <c r="I127" s="6"/>
+    </row>
+    <row r="128" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B128" s="6"/>
+      <c r="C128" s="6"/>
+      <c r="D128" s="6"/>
+      <c r="F128" s="6"/>
+      <c r="H128" s="6"/>
+      <c r="I128" s="6"/>
+    </row>
+    <row r="129" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B129" s="6"/>
+      <c r="C129" s="6"/>
+      <c r="D129" s="6"/>
+      <c r="F129" s="6"/>
+      <c r="H129" s="6"/>
+      <c r="I129" s="6"/>
+    </row>
+    <row r="130" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B130" s="6"/>
+      <c r="C130" s="6"/>
+      <c r="D130" s="6"/>
+      <c r="F130" s="6"/>
+      <c r="H130" s="6"/>
+      <c r="I130" s="6"/>
+    </row>
+    <row r="131" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B131" s="6"/>
+      <c r="C131" s="6"/>
+      <c r="D131" s="6"/>
+      <c r="F131" s="6"/>
+      <c r="H131" s="6"/>
+      <c r="I131" s="6"/>
+    </row>
+    <row r="132" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B132" s="6"/>
+      <c r="C132" s="6"/>
+      <c r="D132" s="6"/>
+      <c r="F132" s="6"/>
+      <c r="H132" s="6"/>
+      <c r="I132" s="6"/>
+    </row>
+    <row r="133" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B133" s="6"/>
+      <c r="C133" s="6"/>
+      <c r="D133" s="6"/>
+      <c r="F133" s="6"/>
+      <c r="H133" s="6"/>
+      <c r="I133" s="6"/>
+    </row>
+    <row r="134" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B134" s="6"/>
+      <c r="C134" s="6"/>
+      <c r="D134" s="6"/>
+      <c r="F134" s="6"/>
+      <c r="H134" s="6"/>
+      <c r="I134" s="6"/>
+    </row>
+    <row r="135" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B135" s="6"/>
+      <c r="C135" s="6"/>
+      <c r="D135" s="6"/>
+      <c r="F135" s="6"/>
+      <c r="H135" s="6"/>
+      <c r="I135" s="6"/>
+    </row>
+    <row r="136" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B136" s="6"/>
+      <c r="C136" s="6"/>
+      <c r="D136" s="6"/>
+      <c r="F136" s="6"/>
+      <c r="H136" s="6"/>
+      <c r="I136" s="6"/>
+    </row>
+    <row r="137" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B137" s="6"/>
+      <c r="C137" s="6"/>
+      <c r="D137" s="6"/>
+      <c r="F137" s="6"/>
+      <c r="H137" s="6"/>
+      <c r="I137" s="6"/>
+    </row>
+    <row r="138" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B138" s="6"/>
+      <c r="C138" s="6"/>
+      <c r="D138" s="6"/>
+      <c r="F138" s="6"/>
+      <c r="H138" s="6"/>
+      <c r="I138" s="6"/>
+    </row>
+    <row r="139" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B139" s="6"/>
+      <c r="C139" s="6"/>
+      <c r="D139" s="6"/>
+      <c r="F139" s="6"/>
+      <c r="H139" s="6"/>
+      <c r="I139" s="6"/>
+    </row>
+    <row r="140" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B140" s="6"/>
+      <c r="C140" s="6"/>
+      <c r="D140" s="6"/>
+      <c r="F140" s="6"/>
+      <c r="H140" s="6"/>
+      <c r="I140" s="6"/>
+    </row>
+    <row r="141" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B141" s="6"/>
+      <c r="C141" s="6"/>
+      <c r="D141" s="6"/>
+      <c r="F141" s="6"/>
+      <c r="H141" s="6"/>
+      <c r="I141" s="6"/>
+    </row>
+    <row r="142" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B142" s="6"/>
+      <c r="C142" s="6"/>
+      <c r="D142" s="6"/>
+      <c r="F142" s="6"/>
+      <c r="H142" s="6"/>
+      <c r="I142" s="6"/>
+    </row>
+    <row r="143" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B143" s="6"/>
+      <c r="C143" s="6"/>
+      <c r="D143" s="6"/>
+      <c r="F143" s="6"/>
+      <c r="H143" s="6"/>
+      <c r="I143" s="6"/>
+    </row>
+    <row r="144" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B144" s="6"/>
+      <c r="C144" s="6"/>
+      <c r="D144" s="6"/>
+      <c r="F144" s="6"/>
+      <c r="H144" s="6"/>
+      <c r="I144" s="6"/>
+    </row>
+    <row r="145" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B145" s="6"/>
+      <c r="C145" s="6"/>
+      <c r="D145" s="6"/>
+      <c r="F145" s="6"/>
+      <c r="H145" s="6"/>
+      <c r="I145" s="6"/>
+    </row>
+    <row r="146" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B146" s="6"/>
+      <c r="C146" s="6"/>
+      <c r="D146" s="6"/>
+      <c r="F146" s="6"/>
+      <c r="H146" s="6"/>
+      <c r="I146" s="6"/>
+    </row>
+    <row r="147" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B147" s="6"/>
+      <c r="C147" s="6"/>
+      <c r="D147" s="6"/>
+      <c r="F147" s="6"/>
+      <c r="H147" s="6"/>
+      <c r="I147" s="6"/>
+    </row>
+    <row r="148" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B148" s="6"/>
+      <c r="C148" s="6"/>
+      <c r="D148" s="6"/>
+      <c r="F148" s="6"/>
+      <c r="H148" s="6"/>
+      <c r="I148" s="6"/>
+    </row>
+    <row r="149" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B149" s="6"/>
+      <c r="C149" s="6"/>
+      <c r="D149" s="6"/>
+      <c r="F149" s="6"/>
+      <c r="H149" s="6"/>
+      <c r="I149" s="6"/>
+    </row>
+    <row r="150" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B150" s="6"/>
+      <c r="C150" s="6"/>
+      <c r="D150" s="6"/>
+      <c r="F150" s="6"/>
+      <c r="H150" s="6"/>
+      <c r="I150" s="6"/>
+    </row>
+    <row r="151" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B151" s="6"/>
+      <c r="C151" s="6"/>
+      <c r="D151" s="6"/>
+      <c r="F151" s="6"/>
+      <c r="H151" s="6"/>
+      <c r="I151" s="6"/>
+    </row>
+    <row r="152" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B152" s="6"/>
+      <c r="C152" s="6"/>
+      <c r="D152" s="6"/>
+      <c r="F152" s="6"/>
+      <c r="H152" s="6"/>
+      <c r="I152" s="6"/>
+    </row>
+    <row r="153" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B153" s="6"/>
+      <c r="C153" s="6"/>
+      <c r="D153" s="6"/>
+      <c r="F153" s="6"/>
+      <c r="H153" s="6"/>
+      <c r="I153" s="6"/>
+    </row>
+    <row r="154" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B154" s="6"/>
+      <c r="C154" s="6"/>
+      <c r="D154" s="6"/>
+      <c r="F154" s="6"/>
+      <c r="H154" s="6"/>
+      <c r="I154" s="6"/>
+    </row>
+    <row r="155" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B155" s="6"/>
+      <c r="C155" s="6"/>
+      <c r="D155" s="6"/>
+      <c r="F155" s="6"/>
+      <c r="H155" s="6"/>
+      <c r="I155" s="6"/>
+    </row>
+    <row r="156" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B156" s="6"/>
+      <c r="C156" s="6"/>
+      <c r="D156" s="6"/>
+      <c r="F156" s="6"/>
+      <c r="H156" s="6"/>
+      <c r="I156" s="6"/>
+    </row>
+    <row r="157" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B157" s="6"/>
+      <c r="C157" s="6"/>
+      <c r="D157" s="6"/>
+      <c r="F157" s="6"/>
+      <c r="H157" s="6"/>
+      <c r="I157" s="6"/>
+    </row>
+    <row r="158" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B158" s="6"/>
+      <c r="C158" s="6"/>
+      <c r="D158" s="6"/>
+      <c r="F158" s="6"/>
+      <c r="H158" s="6"/>
+      <c r="I158" s="6"/>
+    </row>
+    <row r="159" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B159" s="6"/>
+      <c r="C159" s="6"/>
+      <c r="D159" s="6"/>
+      <c r="F159" s="6"/>
+      <c r="H159" s="6"/>
+      <c r="I159" s="6"/>
+    </row>
+    <row r="160" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B160" s="6"/>
+      <c r="C160" s="6"/>
+      <c r="D160" s="6"/>
+      <c r="F160" s="6"/>
+      <c r="H160" s="6"/>
+      <c r="I160" s="6"/>
+    </row>
+    <row r="161" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B161" s="6"/>
+      <c r="C161" s="6"/>
+      <c r="D161" s="6"/>
+      <c r="F161" s="6"/>
+      <c r="H161" s="6"/>
+      <c r="I161" s="6"/>
+    </row>
+    <row r="162" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B162" s="6"/>
+      <c r="C162" s="6"/>
+      <c r="D162" s="6"/>
+      <c r="F162" s="6"/>
+      <c r="H162" s="6"/>
+      <c r="I162" s="6"/>
+    </row>
+    <row r="163" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B163" s="6"/>
+      <c r="C163" s="6"/>
+      <c r="D163" s="6"/>
+      <c r="F163" s="6"/>
+      <c r="H163" s="6"/>
+      <c r="I163" s="6"/>
+    </row>
+    <row r="164" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B164" s="6"/>
+      <c r="C164" s="6"/>
+      <c r="D164" s="6"/>
+      <c r="F164" s="6"/>
+      <c r="H164" s="6"/>
+      <c r="I164" s="6"/>
+    </row>
+    <row r="165" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B165" s="6"/>
+      <c r="C165" s="6"/>
+      <c r="D165" s="6"/>
+      <c r="F165" s="6"/>
+      <c r="H165" s="6"/>
+      <c r="I165" s="6"/>
+    </row>
+    <row r="166" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B166" s="6"/>
+      <c r="C166" s="6"/>
+      <c r="D166" s="6"/>
+      <c r="F166" s="6"/>
+      <c r="H166" s="6"/>
+      <c r="I166" s="6"/>
+    </row>
+    <row r="167" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B167" s="6"/>
+      <c r="C167" s="6"/>
+      <c r="D167" s="6"/>
+      <c r="F167" s="6"/>
+      <c r="H167" s="6"/>
+      <c r="I167" s="6"/>
+    </row>
+    <row r="168" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B168" s="6"/>
+      <c r="C168" s="6"/>
+      <c r="D168" s="6"/>
+      <c r="F168" s="6"/>
+      <c r="H168" s="6"/>
+      <c r="I168" s="6"/>
+    </row>
+    <row r="169" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B169" s="6"/>
+      <c r="C169" s="6"/>
+      <c r="D169" s="6"/>
+      <c r="F169" s="6"/>
+      <c r="H169" s="6"/>
+      <c r="I169" s="6"/>
+    </row>
+    <row r="170" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B170" s="6"/>
+      <c r="C170" s="6"/>
+      <c r="D170" s="6"/>
+      <c r="F170" s="6"/>
+      <c r="H170" s="6"/>
+      <c r="I170" s="6"/>
+    </row>
+    <row r="171" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B171" s="6"/>
+      <c r="C171" s="6"/>
+      <c r="D171" s="6"/>
+      <c r="F171" s="6"/>
+      <c r="H171" s="6"/>
+      <c r="I171" s="6"/>
+    </row>
+    <row r="172" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B172" s="6"/>
+      <c r="C172" s="6"/>
+      <c r="D172" s="6"/>
+      <c r="F172" s="6"/>
+      <c r="H172" s="6"/>
+      <c r="I172" s="6"/>
+    </row>
+    <row r="173" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B173" s="6"/>
+      <c r="C173" s="6"/>
+      <c r="D173" s="6"/>
+      <c r="F173" s="6"/>
+      <c r="H173" s="6"/>
+      <c r="I173" s="6"/>
+    </row>
+    <row r="174" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B174" s="6"/>
+      <c r="C174" s="6"/>
+      <c r="D174" s="6"/>
+      <c r="F174" s="6"/>
+      <c r="H174" s="6"/>
+      <c r="I174" s="6"/>
+    </row>
+    <row r="175" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B175" s="6"/>
+      <c r="C175" s="6"/>
+      <c r="D175" s="6"/>
+      <c r="F175" s="6"/>
+      <c r="H175" s="6"/>
+      <c r="I175" s="6"/>
+    </row>
+    <row r="176" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B176" s="6"/>
+      <c r="C176" s="6"/>
+      <c r="D176" s="6"/>
+      <c r="F176" s="6"/>
+      <c r="H176" s="6"/>
+      <c r="I176" s="6"/>
+    </row>
+    <row r="177" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B177" s="6"/>
+      <c r="C177" s="6"/>
+      <c r="D177" s="6"/>
+      <c r="F177" s="6"/>
+      <c r="H177" s="6"/>
+      <c r="I177" s="6"/>
+    </row>
+    <row r="178" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B178" s="6"/>
+      <c r="C178" s="6"/>
+      <c r="D178" s="6"/>
+      <c r="F178" s="6"/>
+      <c r="H178" s="6"/>
+      <c r="I178" s="6"/>
+    </row>
+    <row r="179" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B179" s="6"/>
+      <c r="C179" s="6"/>
+      <c r="D179" s="6"/>
+      <c r="F179" s="6"/>
+      <c r="H179" s="6"/>
+      <c r="I179" s="6"/>
+    </row>
+    <row r="180" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B180" s="6"/>
+      <c r="C180" s="6"/>
+      <c r="D180" s="6"/>
+      <c r="F180" s="6"/>
+      <c r="H180" s="6"/>
+      <c r="I180" s="6"/>
+    </row>
+    <row r="181" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B181" s="6"/>
+      <c r="C181" s="6"/>
+      <c r="D181" s="6"/>
+      <c r="F181" s="6"/>
+      <c r="H181" s="6"/>
+      <c r="I181" s="6"/>
+    </row>
+    <row r="182" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B182" s="6"/>
+      <c r="C182" s="6"/>
+      <c r="D182" s="6"/>
+      <c r="F182" s="6"/>
+      <c r="H182" s="6"/>
+      <c r="I182" s="6"/>
+    </row>
+    <row r="183" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B183" s="6"/>
+      <c r="C183" s="6"/>
+      <c r="D183" s="6"/>
+      <c r="F183" s="6"/>
+      <c r="H183" s="6"/>
+      <c r="I183" s="6"/>
+    </row>
+    <row r="184" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B184" s="6"/>
+      <c r="C184" s="6"/>
+      <c r="D184" s="6"/>
+      <c r="F184" s="6"/>
+      <c r="H184" s="6"/>
+      <c r="I184" s="6"/>
+    </row>
+    <row r="185" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B185" s="6"/>
+      <c r="C185" s="6"/>
+      <c r="D185" s="6"/>
+      <c r="F185" s="6"/>
+      <c r="H185" s="6"/>
+      <c r="I185" s="6"/>
+    </row>
+    <row r="186" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B186" s="6"/>
+      <c r="C186" s="6"/>
+      <c r="D186" s="6"/>
+      <c r="F186" s="6"/>
+      <c r="H186" s="6"/>
+      <c r="I186" s="6"/>
+    </row>
+    <row r="187" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B187" s="6"/>
+      <c r="C187" s="6"/>
+      <c r="D187" s="6"/>
+      <c r="F187" s="6"/>
+      <c r="H187" s="6"/>
+      <c r="I187" s="6"/>
+    </row>
+    <row r="188" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B188" s="6"/>
+      <c r="C188" s="6"/>
+      <c r="D188" s="6"/>
+      <c r="F188" s="6"/>
+      <c r="H188" s="6"/>
+      <c r="I188" s="6"/>
+    </row>
+    <row r="189" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B189" s="6"/>
+      <c r="C189" s="6"/>
+      <c r="D189" s="6"/>
+      <c r="F189" s="6"/>
+      <c r="H189" s="6"/>
+      <c r="I189" s="6"/>
+    </row>
+    <row r="190" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B190" s="6"/>
+      <c r="C190" s="6"/>
+      <c r="D190" s="6"/>
+      <c r="F190" s="6"/>
+      <c r="H190" s="6"/>
+      <c r="I190" s="6"/>
+    </row>
+    <row r="191" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B191" s="6"/>
+      <c r="C191" s="6"/>
+      <c r="D191" s="6"/>
+      <c r="F191" s="6"/>
+      <c r="H191" s="6"/>
+      <c r="I191" s="6"/>
+    </row>
+    <row r="192" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B192" s="6"/>
+      <c r="C192" s="6"/>
+      <c r="D192" s="6"/>
+      <c r="F192" s="6"/>
+      <c r="H192" s="6"/>
+      <c r="I192" s="6"/>
+    </row>
+    <row r="193" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B193" s="6"/>
+      <c r="C193" s="6"/>
+      <c r="D193" s="6"/>
+      <c r="F193" s="6"/>
+      <c r="H193" s="6"/>
+      <c r="I193" s="6"/>
+    </row>
+    <row r="194" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B194" s="6"/>
+      <c r="C194" s="6"/>
+      <c r="D194" s="6"/>
+      <c r="F194" s="6"/>
+      <c r="H194" s="6"/>
+      <c r="I194" s="6"/>
+    </row>
+    <row r="195" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B195" s="6"/>
+      <c r="C195" s="6"/>
+      <c r="D195" s="6"/>
+      <c r="F195" s="6"/>
+      <c r="H195" s="6"/>
+      <c r="I195" s="6"/>
+    </row>
+    <row r="196" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B196" s="6"/>
+      <c r="C196" s="6"/>
+      <c r="D196" s="6"/>
+      <c r="F196" s="6"/>
+      <c r="H196" s="6"/>
+      <c r="I196" s="6"/>
+    </row>
+    <row r="197" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B197" s="6"/>
+      <c r="C197" s="6"/>
+      <c r="D197" s="6"/>
+      <c r="F197" s="6"/>
+      <c r="H197" s="6"/>
+      <c r="I197" s="6"/>
+    </row>
+    <row r="198" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B198" s="6"/>
+      <c r="C198" s="6"/>
+      <c r="D198" s="6"/>
+      <c r="F198" s="6"/>
+      <c r="H198" s="6"/>
+      <c r="I198" s="6"/>
+    </row>
+    <row r="199" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B199" s="6"/>
+      <c r="C199" s="6"/>
+      <c r="D199" s="6"/>
+      <c r="F199" s="6"/>
+      <c r="H199" s="6"/>
+      <c r="I199" s="6"/>
+    </row>
+    <row r="200" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B200" s="6"/>
+      <c r="C200" s="6"/>
+      <c r="D200" s="6"/>
+      <c r="F200" s="6"/>
+      <c r="H200" s="6"/>
+      <c r="I200" s="6"/>
+    </row>
+    <row r="201" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B201" s="6"/>
+      <c r="C201" s="6"/>
+      <c r="D201" s="6"/>
+      <c r="F201" s="6"/>
+      <c r="H201" s="6"/>
+      <c r="I201" s="6"/>
+    </row>
+    <row r="202" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B202" s="6"/>
+      <c r="C202" s="6"/>
+      <c r="D202" s="6"/>
+      <c r="F202" s="6"/>
+      <c r="H202" s="6"/>
+      <c r="I202" s="6"/>
+    </row>
+    <row r="203" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B203" s="6"/>
+      <c r="C203" s="6"/>
+      <c r="D203" s="6"/>
+      <c r="F203" s="6"/>
+      <c r="H203" s="6"/>
+      <c r="I203" s="6"/>
+    </row>
+    <row r="204" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B204" s="6"/>
+      <c r="C204" s="6"/>
+      <c r="D204" s="6"/>
+      <c r="F204" s="6"/>
+      <c r="H204" s="6"/>
+      <c r="I204" s="6"/>
+    </row>
+    <row r="205" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B205" s="6"/>
+      <c r="C205" s="6"/>
+      <c r="D205" s="6"/>
+      <c r="F205" s="6"/>
+      <c r="H205" s="6"/>
+      <c r="I205" s="6"/>
+    </row>
+    <row r="206" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B206" s="6"/>
+      <c r="C206" s="6"/>
+      <c r="D206" s="6"/>
+      <c r="F206" s="6"/>
+      <c r="H206" s="6"/>
+      <c r="I206" s="6"/>
+    </row>
+    <row r="207" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B207" s="6"/>
+      <c r="C207" s="6"/>
+      <c r="D207" s="6"/>
+      <c r="F207" s="6"/>
+      <c r="H207" s="6"/>
+      <c r="I207" s="6"/>
+    </row>
+    <row r="208" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B208" s="6"/>
+      <c r="C208" s="6"/>
+      <c r="D208" s="6"/>
+      <c r="F208" s="6"/>
+      <c r="H208" s="6"/>
+      <c r="I208" s="6"/>
+    </row>
+    <row r="209" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B209" s="6"/>
+      <c r="C209" s="6"/>
+      <c r="D209" s="6"/>
+      <c r="F209" s="6"/>
+      <c r="H209" s="6"/>
+      <c r="I209" s="6"/>
+    </row>
+    <row r="210" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B210" s="6"/>
+      <c r="C210" s="6"/>
+      <c r="D210" s="6"/>
+      <c r="F210" s="6"/>
+      <c r="H210" s="6"/>
+      <c r="I210" s="6"/>
+    </row>
+    <row r="211" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B211" s="6"/>
+      <c r="C211" s="6"/>
+      <c r="D211" s="6"/>
+      <c r="F211" s="6"/>
+      <c r="H211" s="6"/>
+      <c r="I211" s="6"/>
+    </row>
+    <row r="212" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B212" s="6"/>
+      <c r="C212" s="6"/>
+      <c r="D212" s="6"/>
+      <c r="F212" s="6"/>
+      <c r="H212" s="6"/>
+      <c r="I212" s="6"/>
+    </row>
+    <row r="213" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B213" s="6"/>
+      <c r="C213" s="6"/>
+      <c r="D213" s="6"/>
+      <c r="F213" s="6"/>
+      <c r="H213" s="6"/>
+      <c r="I213" s="6"/>
+    </row>
+    <row r="214" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B214" s="6"/>
+      <c r="C214" s="6"/>
+      <c r="D214" s="6"/>
+      <c r="F214" s="6"/>
+      <c r="H214" s="6"/>
+      <c r="I214" s="6"/>
+    </row>
+    <row r="215" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B215" s="6"/>
+      <c r="C215" s="6"/>
+      <c r="D215" s="6"/>
+      <c r="F215" s="6"/>
+      <c r="H215" s="6"/>
+      <c r="I215" s="6"/>
+    </row>
+    <row r="216" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B216" s="6"/>
+      <c r="C216" s="6"/>
+      <c r="D216" s="6"/>
+      <c r="F216" s="6"/>
+      <c r="H216" s="6"/>
+      <c r="I216" s="6"/>
+    </row>
+    <row r="217" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B217" s="6"/>
+      <c r="C217" s="6"/>
+      <c r="D217" s="6"/>
+      <c r="F217" s="6"/>
+      <c r="H217" s="6"/>
+      <c r="I217" s="6"/>
+    </row>
+    <row r="218" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B218" s="6"/>
+      <c r="C218" s="6"/>
+      <c r="D218" s="6"/>
+      <c r="F218" s="6"/>
+      <c r="H218" s="6"/>
+      <c r="I218" s="6"/>
+    </row>
+    <row r="219" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B219" s="6"/>
+      <c r="C219" s="6"/>
+      <c r="D219" s="6"/>
+      <c r="F219" s="6"/>
+      <c r="H219" s="6"/>
+      <c r="I219" s="6"/>
+    </row>
+    <row r="220" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B220" s="6"/>
+      <c r="C220" s="6"/>
+      <c r="D220" s="6"/>
+      <c r="F220" s="6"/>
+      <c r="H220" s="6"/>
+      <c r="I220" s="6"/>
+    </row>
+    <row r="221" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B221" s="6"/>
+      <c r="C221" s="6"/>
+      <c r="D221" s="6"/>
+      <c r="F221" s="6"/>
+      <c r="H221" s="6"/>
+      <c r="I221" s="6"/>
+    </row>
+    <row r="222" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B222" s="6"/>
+      <c r="C222" s="6"/>
+      <c r="D222" s="6"/>
+      <c r="F222" s="6"/>
+      <c r="H222" s="6"/>
+      <c r="I222" s="6"/>
+    </row>
+    <row r="223" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B223" s="6"/>
+      <c r="C223" s="6"/>
+      <c r="D223" s="6"/>
+      <c r="F223" s="6"/>
+      <c r="H223" s="6"/>
+      <c r="I223" s="6"/>
+    </row>
+    <row r="224" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B224" s="6"/>
+      <c r="C224" s="6"/>
+      <c r="D224" s="6"/>
+      <c r="F224" s="6"/>
+      <c r="H224" s="6"/>
+      <c r="I224" s="6"/>
+    </row>
+    <row r="225" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B225" s="6"/>
+      <c r="C225" s="6"/>
+      <c r="D225" s="6"/>
+      <c r="F225" s="6"/>
+      <c r="H225" s="6"/>
+      <c r="I225" s="6"/>
+    </row>
+    <row r="226" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B226" s="6"/>
+      <c r="C226" s="6"/>
+      <c r="D226" s="6"/>
+      <c r="F226" s="6"/>
+      <c r="H226" s="6"/>
+      <c r="I226" s="6"/>
+    </row>
+    <row r="227" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B227" s="6"/>
+      <c r="C227" s="6"/>
+      <c r="D227" s="6"/>
+      <c r="F227" s="6"/>
+      <c r="H227" s="6"/>
+      <c r="I227" s="6"/>
+    </row>
+    <row r="228" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B228" s="6"/>
+      <c r="C228" s="6"/>
+      <c r="D228" s="6"/>
+      <c r="F228" s="6"/>
+      <c r="H228" s="6"/>
+      <c r="I228" s="6"/>
+    </row>
+    <row r="229" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B229" s="6"/>
+      <c r="C229" s="6"/>
+      <c r="D229" s="6"/>
+      <c r="F229" s="6"/>
+      <c r="H229" s="6"/>
+      <c r="I229" s="6"/>
+    </row>
+    <row r="230" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B230" s="6"/>
+      <c r="C230" s="6"/>
+      <c r="D230" s="6"/>
+      <c r="F230" s="6"/>
+      <c r="H230" s="6"/>
+      <c r="I230" s="6"/>
+    </row>
+    <row r="231" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B231" s="6"/>
+      <c r="C231" s="6"/>
+      <c r="D231" s="6"/>
+      <c r="F231" s="6"/>
+      <c r="H231" s="6"/>
+      <c r="I231" s="6"/>
+    </row>
+    <row r="232" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B232" s="6"/>
+      <c r="C232" s="6"/>
+      <c r="D232" s="6"/>
+      <c r="F232" s="6"/>
+      <c r="H232" s="6"/>
+      <c r="I232" s="6"/>
+    </row>
+    <row r="233" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B233" s="6"/>
+      <c r="C233" s="6"/>
+      <c r="D233" s="6"/>
+      <c r="F233" s="6"/>
+      <c r="H233" s="6"/>
+      <c r="I233" s="6"/>
+    </row>
+    <row r="234" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B234" s="6"/>
+      <c r="C234" s="6"/>
+      <c r="D234" s="6"/>
+      <c r="F234" s="6"/>
+      <c r="H234" s="6"/>
+      <c r="I234" s="6"/>
+    </row>
+    <row r="235" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B235" s="6"/>
+      <c r="C235" s="6"/>
+      <c r="D235" s="6"/>
+      <c r="F235" s="6"/>
+      <c r="H235" s="6"/>
+      <c r="I235" s="6"/>
+    </row>
+    <row r="236" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B236" s="6"/>
+      <c r="C236" s="6"/>
+      <c r="D236" s="6"/>
+      <c r="F236" s="6"/>
+      <c r="H236" s="6"/>
+      <c r="I236" s="6"/>
+    </row>
+    <row r="237" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B237" s="6"/>
+      <c r="C237" s="6"/>
+      <c r="D237" s="6"/>
+      <c r="F237" s="6"/>
+      <c r="H237" s="6"/>
+      <c r="I237" s="6"/>
+    </row>
+    <row r="238" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B238" s="6"/>
+      <c r="C238" s="6"/>
+      <c r="D238" s="6"/>
+      <c r="F238" s="6"/>
+      <c r="H238" s="6"/>
+      <c r="I238" s="6"/>
+    </row>
+    <row r="239" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B239" s="6"/>
+      <c r="C239" s="6"/>
+      <c r="D239" s="6"/>
+      <c r="F239" s="6"/>
+      <c r="H239" s="6"/>
+      <c r="I239" s="6"/>
+    </row>
+    <row r="240" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B240" s="6"/>
+      <c r="C240" s="6"/>
+      <c r="D240" s="6"/>
+      <c r="F240" s="6"/>
+      <c r="H240" s="6"/>
+      <c r="I240" s="6"/>
+    </row>
+    <row r="241" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B241" s="6"/>
+      <c r="C241" s="6"/>
+      <c r="D241" s="6"/>
+      <c r="F241" s="6"/>
+      <c r="H241" s="6"/>
+      <c r="I241" s="6"/>
+    </row>
+    <row r="242" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B242" s="6"/>
+      <c r="C242" s="6"/>
+      <c r="D242" s="6"/>
+      <c r="F242" s="6"/>
+      <c r="H242" s="6"/>
+      <c r="I242" s="6"/>
+    </row>
+    <row r="243" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B243" s="6"/>
+      <c r="C243" s="6"/>
+      <c r="D243" s="6"/>
+      <c r="F243" s="6"/>
+      <c r="H243" s="6"/>
+      <c r="I243" s="6"/>
+    </row>
+    <row r="244" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B244" s="6"/>
+      <c r="C244" s="6"/>
+      <c r="D244" s="6"/>
+      <c r="F244" s="6"/>
+      <c r="H244" s="6"/>
+      <c r="I244" s="6"/>
+    </row>
+    <row r="245" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B245" s="6"/>
+      <c r="C245" s="6"/>
+      <c r="D245" s="6"/>
+      <c r="F245" s="6"/>
+      <c r="H245" s="6"/>
+      <c r="I245" s="6"/>
+    </row>
+    <row r="246" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B246" s="6"/>
+      <c r="C246" s="6"/>
+      <c r="D246" s="6"/>
+      <c r="F246" s="6"/>
+      <c r="H246" s="6"/>
+      <c r="I246" s="6"/>
+    </row>
+    <row r="247" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B247" s="6"/>
+      <c r="C247" s="6"/>
+      <c r="D247" s="6"/>
+      <c r="F247" s="6"/>
+      <c r="H247" s="6"/>
+      <c r="I247" s="6"/>
+    </row>
+    <row r="248" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B248" s="6"/>
+      <c r="C248" s="6"/>
+      <c r="D248" s="6"/>
+      <c r="F248" s="6"/>
+      <c r="H248" s="6"/>
+      <c r="I248" s="6"/>
+    </row>
+    <row r="249" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B249" s="6"/>
+      <c r="C249" s="6"/>
+      <c r="D249" s="6"/>
+      <c r="F249" s="6"/>
+      <c r="H249" s="6"/>
+      <c r="I249" s="6"/>
+    </row>
+    <row r="250" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B250" s="6"/>
+      <c r="C250" s="6"/>
+      <c r="D250" s="6"/>
+      <c r="F250" s="6"/>
+      <c r="H250" s="6"/>
+      <c r="I250" s="6"/>
+    </row>
+    <row r="251" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B251" s="6"/>
+      <c r="C251" s="6"/>
+      <c r="D251" s="6"/>
+      <c r="F251" s="6"/>
+      <c r="H251" s="6"/>
+      <c r="I251" s="6"/>
+    </row>
+    <row r="252" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B252" s="6"/>
+      <c r="C252" s="6"/>
+      <c r="D252" s="6"/>
+      <c r="F252" s="6"/>
+      <c r="H252" s="6"/>
+      <c r="I252" s="6"/>
+    </row>
+    <row r="253" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B253" s="6"/>
+      <c r="C253" s="6"/>
+      <c r="D253" s="6"/>
+      <c r="F253" s="6"/>
+      <c r="H253" s="6"/>
+      <c r="I253" s="6"/>
+    </row>
+    <row r="254" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B254" s="6"/>
+      <c r="C254" s="6"/>
+      <c r="D254" s="6"/>
+      <c r="F254" s="6"/>
+      <c r="H254" s="6"/>
+      <c r="I254" s="6"/>
+    </row>
+    <row r="255" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B255" s="6"/>
+      <c r="C255" s="6"/>
+      <c r="D255" s="6"/>
+      <c r="F255" s="6"/>
+      <c r="H255" s="6"/>
+      <c r="I255" s="6"/>
+    </row>
+    <row r="256" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B256" s="6"/>
+      <c r="C256" s="6"/>
+      <c r="D256" s="6"/>
+      <c r="F256" s="6"/>
+      <c r="H256" s="6"/>
+      <c r="I256" s="6"/>
+    </row>
+    <row r="257" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B257" s="6"/>
+      <c r="C257" s="6"/>
+      <c r="D257" s="6"/>
+      <c r="F257" s="6"/>
+      <c r="H257" s="6"/>
+      <c r="I257" s="6"/>
+    </row>
+    <row r="258" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B258" s="6"/>
+      <c r="C258" s="6"/>
+      <c r="D258" s="6"/>
+      <c r="F258" s="6"/>
+      <c r="H258" s="6"/>
+      <c r="I258" s="6"/>
+    </row>
+    <row r="259" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B259" s="6"/>
+      <c r="C259" s="6"/>
+      <c r="D259" s="6"/>
+      <c r="F259" s="6"/>
+      <c r="H259" s="6"/>
+      <c r="I259" s="6"/>
+    </row>
+    <row r="260" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B260" s="6"/>
+      <c r="C260" s="6"/>
+      <c r="D260" s="6"/>
+      <c r="F260" s="6"/>
+      <c r="H260" s="6"/>
+      <c r="I260" s="6"/>
+    </row>
+    <row r="261" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B261" s="6"/>
+      <c r="C261" s="6"/>
+      <c r="D261" s="6"/>
+      <c r="F261" s="6"/>
+      <c r="H261" s="6"/>
+      <c r="I261" s="6"/>
+    </row>
+    <row r="262" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B262" s="6"/>
+      <c r="C262" s="6"/>
+      <c r="D262" s="6"/>
+      <c r="F262" s="6"/>
+      <c r="H262" s="6"/>
+      <c r="I262" s="6"/>
+    </row>
+    <row r="263" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B263" s="6"/>
+      <c r="C263" s="6"/>
+      <c r="D263" s="6"/>
+      <c r="F263" s="6"/>
+      <c r="H263" s="6"/>
+      <c r="I263" s="6"/>
+    </row>
+    <row r="264" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B264" s="6"/>
+      <c r="C264" s="6"/>
+      <c r="D264" s="6"/>
+      <c r="F264" s="6"/>
+      <c r="H264" s="6"/>
+      <c r="I264" s="6"/>
+    </row>
+    <row r="265" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B265" s="6"/>
+      <c r="C265" s="6"/>
+      <c r="D265" s="6"/>
+      <c r="F265" s="6"/>
+      <c r="H265" s="6"/>
+      <c r="I265" s="6"/>
+    </row>
+    <row r="266" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B266" s="6"/>
+      <c r="C266" s="6"/>
+      <c r="D266" s="6"/>
+      <c r="F266" s="6"/>
+      <c r="H266" s="6"/>
+      <c r="I266" s="6"/>
+    </row>
+    <row r="267" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B267" s="6"/>
+      <c r="C267" s="6"/>
+      <c r="D267" s="6"/>
+      <c r="F267" s="6"/>
+      <c r="H267" s="6"/>
+      <c r="I267" s="6"/>
+    </row>
+    <row r="268" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B268" s="6"/>
+      <c r="C268" s="6"/>
+      <c r="D268" s="6"/>
+      <c r="F268" s="6"/>
+      <c r="H268" s="6"/>
+      <c r="I268" s="6"/>
+    </row>
+    <row r="269" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B269" s="6"/>
+      <c r="C269" s="6"/>
+      <c r="D269" s="6"/>
+      <c r="F269" s="6"/>
+      <c r="H269" s="6"/>
+      <c r="I269" s="6"/>
+    </row>
+    <row r="270" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B270" s="6"/>
+      <c r="C270" s="6"/>
+      <c r="D270" s="6"/>
+      <c r="F270" s="6"/>
+      <c r="H270" s="6"/>
+      <c r="I270" s="6"/>
+    </row>
+    <row r="271" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B271" s="6"/>
+      <c r="C271" s="6"/>
+      <c r="D271" s="6"/>
+      <c r="F271" s="6"/>
+      <c r="H271" s="6"/>
+      <c r="I271" s="6"/>
+    </row>
+    <row r="272" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B272" s="6"/>
+      <c r="C272" s="6"/>
+      <c r="D272" s="6"/>
+      <c r="F272" s="6"/>
+      <c r="H272" s="6"/>
+      <c r="I272" s="6"/>
+    </row>
+    <row r="273" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B273" s="6"/>
+      <c r="C273" s="6"/>
+      <c r="D273" s="6"/>
+      <c r="F273" s="6"/>
+      <c r="H273" s="6"/>
+      <c r="I273" s="6"/>
+    </row>
+    <row r="274" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B274" s="6"/>
+      <c r="C274" s="6"/>
+      <c r="D274" s="6"/>
+      <c r="F274" s="6"/>
+      <c r="H274" s="6"/>
+      <c r="I274" s="6"/>
+    </row>
+    <row r="275" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B275" s="6"/>
+      <c r="C275" s="6"/>
+      <c r="D275" s="6"/>
+      <c r="F275" s="6"/>
+      <c r="H275" s="6"/>
+      <c r="I275" s="6"/>
+    </row>
+    <row r="276" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B276" s="6"/>
+      <c r="C276" s="6"/>
+      <c r="D276" s="6"/>
+      <c r="F276" s="6"/>
+      <c r="H276" s="6"/>
+      <c r="I276" s="6"/>
+    </row>
+    <row r="277" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B277" s="6"/>
+      <c r="C277" s="6"/>
+      <c r="D277" s="6"/>
+      <c r="F277" s="6"/>
+      <c r="H277" s="6"/>
+      <c r="I277" s="6"/>
+    </row>
+    <row r="278" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B278" s="6"/>
+      <c r="C278" s="6"/>
+      <c r="D278" s="6"/>
+      <c r="F278" s="6"/>
+      <c r="H278" s="6"/>
+      <c r="I278" s="6"/>
+    </row>
+    <row r="279" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B279" s="6"/>
+      <c r="C279" s="6"/>
+      <c r="D279" s="6"/>
+      <c r="F279" s="6"/>
+      <c r="H279" s="6"/>
+      <c r="I279" s="6"/>
+    </row>
+    <row r="280" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B280" s="6"/>
+      <c r="C280" s="6"/>
+      <c r="D280" s="6"/>
+      <c r="F280" s="6"/>
+      <c r="H280" s="6"/>
+      <c r="I280" s="6"/>
+    </row>
+    <row r="281" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B281" s="6"/>
+      <c r="C281" s="6"/>
+      <c r="D281" s="6"/>
+      <c r="F281" s="6"/>
+      <c r="H281" s="6"/>
+      <c r="I281" s="6"/>
+    </row>
+    <row r="282" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B282" s="6"/>
+      <c r="C282" s="6"/>
+      <c r="D282" s="6"/>
+      <c r="F282" s="6"/>
+      <c r="H282" s="6"/>
+      <c r="I282" s="6"/>
+    </row>
+    <row r="283" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B283" s="6"/>
+      <c r="C283" s="6"/>
+      <c r="D283" s="6"/>
+      <c r="F283" s="6"/>
+      <c r="H283" s="6"/>
+      <c r="I283" s="6"/>
+    </row>
+    <row r="284" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B284" s="6"/>
+      <c r="C284" s="6"/>
+      <c r="D284" s="6"/>
+      <c r="F284" s="6"/>
+      <c r="H284" s="6"/>
+      <c r="I284" s="6"/>
+    </row>
+    <row r="285" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B285" s="6"/>
+      <c r="C285" s="6"/>
+      <c r="D285" s="6"/>
+      <c r="F285" s="6"/>
+      <c r="H285" s="6"/>
+      <c r="I285" s="6"/>
+    </row>
+    <row r="286" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B286" s="6"/>
+      <c r="C286" s="6"/>
+      <c r="D286" s="6"/>
+      <c r="F286" s="6"/>
+      <c r="H286" s="6"/>
+      <c r="I286" s="6"/>
+    </row>
+    <row r="287" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B287" s="6"/>
+      <c r="C287" s="6"/>
+      <c r="D287" s="6"/>
+      <c r="F287" s="6"/>
+      <c r="H287" s="6"/>
+      <c r="I287" s="6"/>
+    </row>
+    <row r="288" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B288" s="6"/>
+      <c r="C288" s="6"/>
+      <c r="D288" s="6"/>
+      <c r="F288" s="6"/>
+      <c r="H288" s="6"/>
+      <c r="I288" s="6"/>
+    </row>
+    <row r="289" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B289" s="6"/>
+      <c r="C289" s="6"/>
+      <c r="D289" s="6"/>
+      <c r="F289" s="6"/>
+      <c r="H289" s="6"/>
+      <c r="I289" s="6"/>
+    </row>
+    <row r="290" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B290" s="6"/>
+      <c r="C290" s="6"/>
+      <c r="D290" s="6"/>
+      <c r="F290" s="6"/>
+      <c r="H290" s="6"/>
+      <c r="I290" s="6"/>
+    </row>
+    <row r="291" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B291" s="6"/>
+      <c r="C291" s="6"/>
+      <c r="D291" s="6"/>
+      <c r="F291" s="6"/>
+      <c r="H291" s="6"/>
+      <c r="I291" s="6"/>
+    </row>
+    <row r="292" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B292" s="6"/>
+      <c r="C292" s="6"/>
+      <c r="D292" s="6"/>
+      <c r="F292" s="6"/>
+      <c r="H292" s="6"/>
+      <c r="I292" s="6"/>
+    </row>
+    <row r="293" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B293" s="6"/>
+      <c r="C293" s="6"/>
+      <c r="D293" s="6"/>
+      <c r="F293" s="6"/>
+      <c r="H293" s="6"/>
+      <c r="I293" s="6"/>
+    </row>
+    <row r="294" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B294" s="6"/>
+      <c r="C294" s="6"/>
+      <c r="D294" s="6"/>
+      <c r="F294" s="6"/>
+      <c r="H294" s="6"/>
+      <c r="I294" s="6"/>
+    </row>
+    <row r="295" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B295" s="6"/>
+      <c r="C295" s="6"/>
+      <c r="D295" s="6"/>
+      <c r="F295" s="6"/>
+      <c r="H295" s="6"/>
+      <c r="I295" s="6"/>
+    </row>
+    <row r="296" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B296" s="6"/>
+      <c r="C296" s="6"/>
+      <c r="D296" s="6"/>
+      <c r="F296" s="6"/>
+      <c r="H296" s="6"/>
+      <c r="I296" s="6"/>
+    </row>
+    <row r="297" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B297" s="6"/>
+      <c r="C297" s="6"/>
+      <c r="D297" s="6"/>
+      <c r="F297" s="6"/>
+      <c r="H297" s="6"/>
+      <c r="I297" s="6"/>
+    </row>
+    <row r="298" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B298" s="6"/>
+      <c r="C298" s="6"/>
+      <c r="D298" s="6"/>
+      <c r="F298" s="6"/>
+      <c r="H298" s="6"/>
+      <c r="I298" s="6"/>
+    </row>
+    <row r="299" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B299" s="6"/>
+      <c r="C299" s="6"/>
+      <c r="D299" s="6"/>
+      <c r="F299" s="6"/>
+      <c r="H299" s="6"/>
+      <c r="I299" s="6"/>
+    </row>
+    <row r="300" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B300" s="6"/>
+      <c r="C300" s="6"/>
+      <c r="D300" s="6"/>
+      <c r="F300" s="6"/>
+      <c r="H300" s="6"/>
+      <c r="I300" s="6"/>
+    </row>
+    <row r="301" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B301" s="6"/>
+      <c r="C301" s="6"/>
+      <c r="D301" s="6"/>
+      <c r="F301" s="6"/>
+      <c r="H301" s="6"/>
+      <c r="I301" s="6"/>
+    </row>
+    <row r="302" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B302" s="6"/>
+      <c r="C302" s="6"/>
+      <c r="D302" s="6"/>
+      <c r="F302" s="6"/>
+      <c r="H302" s="6"/>
+      <c r="I302" s="6"/>
+    </row>
+    <row r="303" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B303" s="6"/>
+      <c r="C303" s="6"/>
+      <c r="D303" s="6"/>
+      <c r="F303" s="6"/>
+      <c r="H303" s="6"/>
+      <c r="I303" s="6"/>
+    </row>
+    <row r="304" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B304" s="6"/>
+      <c r="C304" s="6"/>
+      <c r="D304" s="6"/>
+      <c r="F304" s="6"/>
+      <c r="H304" s="6"/>
+      <c r="I304" s="6"/>
+    </row>
+    <row r="305" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B305" s="6"/>
+      <c r="C305" s="6"/>
+      <c r="D305" s="6"/>
+      <c r="F305" s="6"/>
+      <c r="H305" s="6"/>
+      <c r="I305" s="6"/>
+    </row>
+    <row r="306" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B306" s="6"/>
+      <c r="C306" s="6"/>
+      <c r="D306" s="6"/>
+      <c r="F306" s="6"/>
+      <c r="H306" s="6"/>
+      <c r="I306" s="6"/>
+    </row>
+    <row r="307" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B307" s="6"/>
+      <c r="C307" s="6"/>
+      <c r="D307" s="6"/>
+      <c r="F307" s="6"/>
+      <c r="H307" s="6"/>
+      <c r="I307" s="6"/>
+    </row>
+    <row r="308" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B308" s="6"/>
+      <c r="C308" s="6"/>
+      <c r="D308" s="6"/>
+      <c r="F308" s="6"/>
+      <c r="H308" s="6"/>
+      <c r="I308" s="6"/>
+    </row>
+    <row r="309" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B309" s="6"/>
+      <c r="C309" s="6"/>
+      <c r="D309" s="6"/>
+      <c r="F309" s="6"/>
+      <c r="H309" s="6"/>
+      <c r="I309" s="6"/>
+    </row>
+    <row r="310" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B310" s="6"/>
+      <c r="C310" s="6"/>
+      <c r="D310" s="6"/>
+      <c r="F310" s="6"/>
+      <c r="H310" s="6"/>
+      <c r="I310" s="6"/>
+    </row>
+    <row r="311" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B311" s="6"/>
+      <c r="C311" s="6"/>
+      <c r="D311" s="6"/>
+      <c r="F311" s="6"/>
+      <c r="H311" s="6"/>
+      <c r="I311" s="6"/>
+    </row>
+    <row r="312" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B312" s="6"/>
+      <c r="C312" s="6"/>
+      <c r="D312" s="6"/>
+      <c r="F312" s="6"/>
+      <c r="H312" s="6"/>
+      <c r="I312" s="6"/>
+    </row>
+    <row r="313" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B313" s="6"/>
+      <c r="C313" s="6"/>
+      <c r="D313" s="6"/>
+      <c r="F313" s="6"/>
+      <c r="H313" s="6"/>
+      <c r="I313" s="6"/>
+    </row>
+    <row r="314" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B314" s="6"/>
+      <c r="C314" s="6"/>
+      <c r="D314" s="6"/>
+      <c r="F314" s="6"/>
+      <c r="H314" s="6"/>
+      <c r="I314" s="6"/>
+    </row>
+    <row r="315" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B315" s="6"/>
+      <c r="C315" s="6"/>
+      <c r="D315" s="6"/>
+      <c r="F315" s="6"/>
+      <c r="H315" s="6"/>
+      <c r="I315" s="6"/>
+    </row>
+    <row r="316" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B316" s="6"/>
+      <c r="C316" s="6"/>
+      <c r="D316" s="6"/>
+      <c r="F316" s="6"/>
+      <c r="H316" s="6"/>
+      <c r="I316" s="6"/>
+    </row>
+    <row r="317" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B317" s="6"/>
+      <c r="C317" s="6"/>
+      <c r="D317" s="6"/>
+      <c r="F317" s="6"/>
+      <c r="H317" s="6"/>
+      <c r="I317" s="6"/>
+    </row>
+    <row r="318" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B318" s="6"/>
+      <c r="C318" s="6"/>
+      <c r="D318" s="6"/>
+      <c r="F318" s="6"/>
+      <c r="H318" s="6"/>
+      <c r="I318" s="6"/>
+    </row>
+    <row r="319" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B319" s="6"/>
+      <c r="C319" s="6"/>
+      <c r="D319" s="6"/>
+      <c r="F319" s="6"/>
+      <c r="H319" s="6"/>
+      <c r="I319" s="6"/>
+    </row>
+    <row r="320" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B320" s="6"/>
+      <c r="C320" s="6"/>
+      <c r="D320" s="6"/>
+      <c r="F320" s="6"/>
+      <c r="H320" s="6"/>
+      <c r="I320" s="6"/>
+    </row>
+    <row r="321" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B321" s="6"/>
+      <c r="C321" s="6"/>
+      <c r="D321" s="6"/>
+      <c r="F321" s="6"/>
+      <c r="H321" s="6"/>
+      <c r="I321" s="6"/>
+    </row>
+    <row r="322" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B322" s="6"/>
+      <c r="C322" s="6"/>
+      <c r="D322" s="6"/>
+      <c r="F322" s="6"/>
+      <c r="H322" s="6"/>
+      <c r="I322" s="6"/>
+    </row>
+    <row r="323" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B323" s="6"/>
+      <c r="C323" s="6"/>
+      <c r="D323" s="6"/>
+      <c r="F323" s="6"/>
+      <c r="H323" s="6"/>
+      <c r="I323" s="6"/>
+    </row>
+    <row r="324" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B324" s="6"/>
+      <c r="C324" s="6"/>
+      <c r="D324" s="6"/>
+      <c r="F324" s="6"/>
+      <c r="H324" s="6"/>
+      <c r="I324" s="6"/>
+    </row>
+    <row r="325" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B325" s="6"/>
+      <c r="C325" s="6"/>
+      <c r="D325" s="6"/>
+      <c r="F325" s="6"/>
+      <c r="H325" s="6"/>
+      <c r="I325" s="6"/>
+    </row>
+    <row r="326" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B326" s="6"/>
+      <c r="C326" s="6"/>
+      <c r="D326" s="6"/>
+      <c r="F326" s="6"/>
+      <c r="H326" s="6"/>
+      <c r="I326" s="6"/>
+    </row>
+    <row r="327" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B327" s="6"/>
+      <c r="C327" s="6"/>
+      <c r="D327" s="6"/>
+      <c r="F327" s="6"/>
+      <c r="H327" s="6"/>
+      <c r="I327" s="6"/>
+    </row>
+    <row r="328" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B328" s="6"/>
+      <c r="C328" s="6"/>
+      <c r="D328" s="6"/>
+      <c r="F328" s="6"/>
+      <c r="H328" s="6"/>
+      <c r="I328" s="6"/>
+    </row>
+    <row r="329" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B329" s="6"/>
+      <c r="C329" s="6"/>
+      <c r="D329" s="6"/>
+      <c r="F329" s="6"/>
+      <c r="H329" s="6"/>
+      <c r="I329" s="6"/>
+    </row>
+    <row r="330" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B330" s="6"/>
+      <c r="C330" s="6"/>
+      <c r="D330" s="6"/>
+      <c r="F330" s="6"/>
+      <c r="H330" s="6"/>
+      <c r="I330" s="6"/>
+    </row>
+    <row r="331" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B331" s="6"/>
+      <c r="C331" s="6"/>
+      <c r="D331" s="6"/>
+      <c r="F331" s="6"/>
+      <c r="H331" s="6"/>
+      <c r="I331" s="6"/>
+    </row>
+    <row r="332" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B332" s="6"/>
+      <c r="C332" s="6"/>
+      <c r="D332" s="6"/>
+      <c r="F332" s="6"/>
+      <c r="H332" s="6"/>
+      <c r="I332" s="6"/>
+    </row>
+    <row r="333" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B333" s="6"/>
+      <c r="C333" s="6"/>
+      <c r="D333" s="6"/>
+      <c r="F333" s="6"/>
+      <c r="H333" s="6"/>
+      <c r="I333" s="6"/>
+    </row>
+    <row r="334" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B334" s="6"/>
+      <c r="C334" s="6"/>
+      <c r="D334" s="6"/>
+      <c r="F334" s="6"/>
+      <c r="H334" s="6"/>
+      <c r="I334" s="6"/>
+    </row>
+    <row r="335" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B335" s="6"/>
+      <c r="C335" s="6"/>
+      <c r="D335" s="6"/>
+      <c r="F335" s="6"/>
+      <c r="H335" s="6"/>
+      <c r="I335" s="6"/>
+    </row>
+    <row r="336" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B336" s="6"/>
+      <c r="C336" s="6"/>
+      <c r="D336" s="6"/>
+      <c r="F336" s="6"/>
+      <c r="H336" s="6"/>
+      <c r="I336" s="6"/>
+    </row>
+    <row r="337" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B337" s="6"/>
+      <c r="C337" s="6"/>
+      <c r="D337" s="6"/>
+      <c r="F337" s="6"/>
+      <c r="H337" s="6"/>
+      <c r="I337" s="6"/>
+    </row>
+    <row r="338" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B338" s="6"/>
+      <c r="C338" s="6"/>
+      <c r="D338" s="6"/>
+      <c r="F338" s="6"/>
+      <c r="H338" s="6"/>
+      <c r="I338" s="6"/>
+    </row>
+    <row r="339" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B339" s="6"/>
+      <c r="C339" s="6"/>
+      <c r="D339" s="6"/>
+      <c r="F339" s="6"/>
+      <c r="H339" s="6"/>
+      <c r="I339" s="6"/>
+    </row>
+    <row r="340" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B340" s="6"/>
+      <c r="C340" s="6"/>
+      <c r="D340" s="6"/>
+      <c r="F340" s="6"/>
+      <c r="H340" s="6"/>
+      <c r="I340" s="6"/>
+    </row>
+    <row r="341" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B341" s="6"/>
+      <c r="C341" s="6"/>
+      <c r="D341" s="6"/>
+      <c r="F341" s="6"/>
+      <c r="H341" s="6"/>
+      <c r="I341" s="6"/>
+    </row>
+    <row r="342" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B342" s="6"/>
+      <c r="C342" s="6"/>
+      <c r="D342" s="6"/>
+      <c r="F342" s="6"/>
+      <c r="H342" s="6"/>
+      <c r="I342" s="6"/>
+    </row>
+    <row r="343" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B343" s="6"/>
+      <c r="C343" s="6"/>
+      <c r="D343" s="6"/>
+      <c r="F343" s="6"/>
+      <c r="H343" s="6"/>
+      <c r="I343" s="6"/>
+    </row>
+    <row r="344" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B344" s="6"/>
+      <c r="C344" s="6"/>
+      <c r="D344" s="6"/>
+      <c r="F344" s="6"/>
+      <c r="H344" s="6"/>
+      <c r="I344" s="6"/>
+    </row>
+    <row r="345" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B345" s="6"/>
+      <c r="C345" s="6"/>
+      <c r="D345" s="6"/>
+      <c r="F345" s="6"/>
+      <c r="H345" s="6"/>
+      <c r="I345" s="6"/>
+    </row>
+    <row r="346" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B346" s="6"/>
+      <c r="C346" s="6"/>
+      <c r="D346" s="6"/>
+      <c r="F346" s="6"/>
+      <c r="H346" s="6"/>
+      <c r="I346" s="6"/>
+    </row>
+    <row r="347" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B347" s="6"/>
+      <c r="C347" s="6"/>
+      <c r="D347" s="6"/>
+      <c r="F347" s="6"/>
+      <c r="H347" s="6"/>
+      <c r="I347" s="6"/>
+    </row>
+    <row r="348" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B348" s="6"/>
+      <c r="C348" s="6"/>
+      <c r="D348" s="6"/>
+      <c r="F348" s="6"/>
+      <c r="H348" s="6"/>
+      <c r="I348" s="6"/>
+    </row>
+    <row r="349" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B349" s="6"/>
+      <c r="C349" s="6"/>
+      <c r="D349" s="6"/>
+      <c r="F349" s="6"/>
+      <c r="H349" s="6"/>
+      <c r="I349" s="6"/>
+    </row>
+    <row r="350" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B350" s="6"/>
+      <c r="C350" s="6"/>
+      <c r="D350" s="6"/>
+      <c r="F350" s="6"/>
+      <c r="H350" s="6"/>
+      <c r="I350" s="6"/>
+    </row>
+    <row r="351" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B351" s="6"/>
+      <c r="C351" s="6"/>
+      <c r="D351" s="6"/>
+      <c r="F351" s="6"/>
+      <c r="H351" s="6"/>
+      <c r="I351" s="6"/>
+    </row>
+    <row r="352" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B352" s="6"/>
+      <c r="C352" s="6"/>
+      <c r="D352" s="6"/>
+      <c r="F352" s="6"/>
+      <c r="H352" s="6"/>
+      <c r="I352" s="6"/>
+    </row>
+    <row r="353" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B353" s="6"/>
+      <c r="C353" s="6"/>
+      <c r="D353" s="6"/>
+      <c r="F353" s="6"/>
+      <c r="H353" s="6"/>
+      <c r="I353" s="6"/>
+    </row>
+    <row r="354" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B354" s="6"/>
+      <c r="C354" s="6"/>
+      <c r="D354" s="6"/>
+      <c r="F354" s="6"/>
+      <c r="H354" s="6"/>
+      <c r="I354" s="6"/>
+    </row>
+    <row r="355" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B355" s="6"/>
+      <c r="C355" s="6"/>
+      <c r="D355" s="6"/>
+      <c r="F355" s="6"/>
+      <c r="H355" s="6"/>
+      <c r="I355" s="6"/>
+    </row>
+    <row r="356" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B356" s="6"/>
+      <c r="C356" s="6"/>
+      <c r="D356" s="6"/>
+      <c r="F356" s="6"/>
+      <c r="H356" s="6"/>
+      <c r="I356" s="6"/>
+    </row>
+    <row r="357" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B357" s="6"/>
+      <c r="C357" s="6"/>
+      <c r="D357" s="6"/>
+      <c r="F357" s="6"/>
+      <c r="H357" s="6"/>
+      <c r="I357" s="6"/>
+    </row>
+    <row r="358" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B358" s="6"/>
+      <c r="C358" s="6"/>
+      <c r="D358" s="6"/>
+      <c r="F358" s="6"/>
+      <c r="H358" s="6"/>
+      <c r="I358" s="6"/>
+    </row>
+    <row r="359" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B359" s="6"/>
+      <c r="C359" s="6"/>
+      <c r="D359" s="6"/>
+      <c r="F359" s="6"/>
+      <c r="H359" s="6"/>
+      <c r="I359" s="6"/>
+    </row>
+    <row r="360" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B360" s="6"/>
+      <c r="C360" s="6"/>
+      <c r="D360" s="6"/>
+      <c r="F360" s="6"/>
+      <c r="H360" s="6"/>
+      <c r="I360" s="6"/>
+    </row>
+    <row r="361" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B361" s="6"/>
+      <c r="C361" s="6"/>
+      <c r="D361" s="6"/>
+      <c r="F361" s="6"/>
+      <c r="H361" s="6"/>
+      <c r="I361" s="6"/>
+    </row>
+    <row r="362" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B362" s="6"/>
+      <c r="C362" s="6"/>
+      <c r="D362" s="6"/>
+      <c r="F362" s="6"/>
+      <c r="H362" s="6"/>
+      <c r="I362" s="6"/>
+    </row>
+    <row r="363" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B363" s="6"/>
+      <c r="C363" s="6"/>
+      <c r="D363" s="6"/>
+      <c r="F363" s="6"/>
+      <c r="H363" s="6"/>
+      <c r="I363" s="6"/>
+    </row>
+    <row r="364" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B364" s="6"/>
+      <c r="C364" s="6"/>
+      <c r="D364" s="6"/>
+      <c r="F364" s="6"/>
+      <c r="H364" s="6"/>
+      <c r="I364" s="6"/>
+    </row>
+    <row r="365" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B365" s="6"/>
+      <c r="C365" s="6"/>
+      <c r="D365" s="6"/>
+      <c r="F365" s="6"/>
+      <c r="H365" s="6"/>
+      <c r="I365" s="6"/>
+    </row>
+    <row r="366" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B366" s="6"/>
+      <c r="C366" s="6"/>
+      <c r="D366" s="6"/>
+      <c r="F366" s="6"/>
+      <c r="H366" s="6"/>
+      <c r="I366" s="6"/>
+    </row>
+    <row r="367" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B367" s="6"/>
+      <c r="C367" s="6"/>
+      <c r="D367" s="6"/>
+      <c r="F367" s="6"/>
+      <c r="H367" s="6"/>
+      <c r="I367" s="6"/>
+    </row>
+    <row r="368" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B368" s="6"/>
+      <c r="C368" s="6"/>
+      <c r="D368" s="6"/>
+      <c r="F368" s="6"/>
+      <c r="H368" s="6"/>
+      <c r="I368" s="6"/>
+    </row>
+    <row r="369" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B369" s="6"/>
+      <c r="C369" s="6"/>
+      <c r="D369" s="6"/>
+      <c r="F369" s="6"/>
+      <c r="H369" s="6"/>
+      <c r="I369" s="6"/>
+    </row>
+    <row r="370" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B370" s="6"/>
+      <c r="C370" s="6"/>
+      <c r="D370" s="6"/>
+      <c r="F370" s="6"/>
+      <c r="H370" s="6"/>
+      <c r="I370" s="6"/>
+    </row>
+    <row r="371" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B371" s="6"/>
+      <c r="C371" s="6"/>
+      <c r="D371" s="6"/>
+      <c r="F371" s="6"/>
+      <c r="H371" s="6"/>
+      <c r="I371" s="6"/>
+    </row>
+    <row r="372" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B372" s="6"/>
+      <c r="C372" s="6"/>
+      <c r="D372" s="6"/>
+      <c r="F372" s="6"/>
+      <c r="H372" s="6"/>
+      <c r="I372" s="6"/>
+    </row>
+    <row r="373" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B373" s="6"/>
+      <c r="C373" s="6"/>
+      <c r="D373" s="6"/>
+      <c r="F373" s="6"/>
+      <c r="H373" s="6"/>
+      <c r="I373" s="6"/>
+    </row>
+    <row r="374" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B374" s="6"/>
+      <c r="C374" s="6"/>
+      <c r="D374" s="6"/>
+      <c r="F374" s="6"/>
+      <c r="H374" s="6"/>
+      <c r="I374" s="6"/>
+    </row>
+    <row r="375" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B375" s="6"/>
+      <c r="C375" s="6"/>
+      <c r="D375" s="6"/>
+      <c r="F375" s="6"/>
+      <c r="H375" s="6"/>
+      <c r="I375" s="6"/>
+    </row>
+    <row r="376" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B376" s="6"/>
+      <c r="C376" s="6"/>
+      <c r="D376" s="6"/>
+      <c r="F376" s="6"/>
+      <c r="H376" s="6"/>
+      <c r="I376" s="6"/>
+    </row>
+    <row r="377" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B377" s="6"/>
+      <c r="C377" s="6"/>
+      <c r="D377" s="6"/>
+      <c r="F377" s="6"/>
+      <c r="H377" s="6"/>
+      <c r="I377" s="6"/>
+    </row>
+    <row r="378" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B378" s="6"/>
+      <c r="C378" s="6"/>
+      <c r="D378" s="6"/>
+      <c r="F378" s="6"/>
+      <c r="H378" s="6"/>
+      <c r="I378" s="6"/>
+    </row>
+    <row r="379" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B379" s="6"/>
+      <c r="C379" s="6"/>
+      <c r="D379" s="6"/>
+      <c r="F379" s="6"/>
+      <c r="H379" s="6"/>
+      <c r="I379" s="6"/>
+    </row>
+    <row r="380" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B380" s="6"/>
+      <c r="C380" s="6"/>
+      <c r="D380" s="6"/>
+      <c r="F380" s="6"/>
+      <c r="H380" s="6"/>
+      <c r="I380" s="6"/>
+    </row>
+    <row r="381" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B381" s="6"/>
+      <c r="C381" s="6"/>
+      <c r="D381" s="6"/>
+      <c r="F381" s="6"/>
+      <c r="H381" s="6"/>
+      <c r="I381" s="6"/>
+    </row>
+    <row r="382" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B382" s="6"/>
+      <c r="C382" s="6"/>
+      <c r="D382" s="6"/>
+      <c r="F382" s="6"/>
+      <c r="H382" s="6"/>
+      <c r="I382" s="6"/>
+    </row>
+    <row r="383" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B383" s="6"/>
+      <c r="C383" s="6"/>
+      <c r="D383" s="6"/>
+      <c r="F383" s="6"/>
+      <c r="H383" s="6"/>
+      <c r="I383" s="6"/>
+    </row>
+    <row r="384" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B384" s="6"/>
+      <c r="C384" s="6"/>
+      <c r="D384" s="6"/>
+      <c r="F384" s="6"/>
+      <c r="H384" s="6"/>
+      <c r="I384" s="6"/>
+    </row>
+    <row r="385" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B385" s="6"/>
+      <c r="C385" s="6"/>
+      <c r="D385" s="6"/>
+      <c r="F385" s="6"/>
+      <c r="H385" s="6"/>
+      <c r="I385" s="6"/>
+    </row>
+    <row r="386" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B386" s="6"/>
+      <c r="C386" s="6"/>
+      <c r="D386" s="6"/>
+      <c r="F386" s="6"/>
+      <c r="H386" s="6"/>
+      <c r="I386" s="6"/>
+    </row>
+    <row r="387" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B387" s="6"/>
+      <c r="C387" s="6"/>
+      <c r="D387" s="6"/>
+      <c r="F387" s="6"/>
+      <c r="H387" s="6"/>
+      <c r="I387" s="6"/>
+    </row>
+    <row r="388" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B388" s="6"/>
+      <c r="C388" s="6"/>
+      <c r="D388" s="6"/>
+      <c r="F388" s="6"/>
+      <c r="H388" s="6"/>
+      <c r="I388" s="6"/>
+    </row>
+    <row r="389" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B389" s="6"/>
+      <c r="C389" s="6"/>
+      <c r="D389" s="6"/>
+      <c r="F389" s="6"/>
+      <c r="H389" s="6"/>
+      <c r="I389" s="6"/>
+    </row>
+    <row r="390" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B390" s="6"/>
+      <c r="C390" s="6"/>
+      <c r="D390" s="6"/>
+      <c r="F390" s="6"/>
+      <c r="H390" s="6"/>
+      <c r="I390" s="6"/>
+    </row>
+    <row r="391" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B391" s="6"/>
+      <c r="C391" s="6"/>
+      <c r="D391" s="6"/>
+      <c r="F391" s="6"/>
+      <c r="H391" s="6"/>
+      <c r="I391" s="6"/>
+    </row>
+    <row r="392" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B392" s="6"/>
+      <c r="C392" s="6"/>
+      <c r="D392" s="6"/>
+      <c r="F392" s="6"/>
+      <c r="H392" s="6"/>
+      <c r="I392" s="6"/>
+    </row>
+    <row r="393" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B393" s="6"/>
+      <c r="C393" s="6"/>
+      <c r="D393" s="6"/>
+      <c r="F393" s="6"/>
+      <c r="H393" s="6"/>
+      <c r="I393" s="6"/>
+    </row>
+    <row r="394" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B394" s="6"/>
+      <c r="C394" s="6"/>
+      <c r="D394" s="6"/>
+      <c r="F394" s="6"/>
+      <c r="H394" s="6"/>
+      <c r="I394" s="6"/>
+    </row>
+    <row r="395" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B395" s="6"/>
+      <c r="C395" s="6"/>
+      <c r="D395" s="6"/>
+      <c r="F395" s="6"/>
+      <c r="H395" s="6"/>
+      <c r="I395" s="6"/>
+    </row>
+    <row r="396" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B396" s="6"/>
+      <c r="C396" s="6"/>
+      <c r="D396" s="6"/>
+      <c r="F396" s="6"/>
+      <c r="H396" s="6"/>
+      <c r="I396" s="6"/>
+    </row>
+    <row r="397" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B397" s="6"/>
+      <c r="C397" s="6"/>
+      <c r="D397" s="6"/>
+      <c r="F397" s="6"/>
+      <c r="H397" s="6"/>
+      <c r="I397" s="6"/>
+    </row>
+    <row r="398" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B398" s="6"/>
+      <c r="C398" s="6"/>
+      <c r="D398" s="6"/>
+      <c r="F398" s="6"/>
+      <c r="H398" s="6"/>
+      <c r="I398" s="6"/>
+    </row>
+    <row r="399" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B399" s="6"/>
+      <c r="C399" s="6"/>
+      <c r="D399" s="6"/>
+      <c r="F399" s="6"/>
+      <c r="H399" s="6"/>
+      <c r="I399" s="6"/>
+    </row>
+    <row r="400" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B400" s="6"/>
+      <c r="C400" s="6"/>
+      <c r="D400" s="6"/>
+      <c r="F400" s="6"/>
+      <c r="H400" s="6"/>
+      <c r="I400" s="6"/>
+    </row>
+    <row r="401" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B401" s="6"/>
+      <c r="C401" s="6"/>
+      <c r="D401" s="6"/>
+      <c r="F401" s="6"/>
+      <c r="H401" s="6"/>
+      <c r="I401" s="6"/>
+    </row>
+    <row r="402" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B402" s="6"/>
+      <c r="C402" s="6"/>
+      <c r="D402" s="6"/>
+      <c r="F402" s="6"/>
+      <c r="H402" s="6"/>
+      <c r="I402" s="6"/>
+    </row>
+    <row r="403" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B403" s="6"/>
+      <c r="C403" s="6"/>
+      <c r="D403" s="6"/>
+      <c r="F403" s="6"/>
+      <c r="H403" s="6"/>
+      <c r="I403" s="6"/>
+    </row>
+    <row r="404" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B404" s="6"/>
+      <c r="C404" s="6"/>
+      <c r="D404" s="6"/>
+      <c r="F404" s="6"/>
+      <c r="H404" s="6"/>
+      <c r="I404" s="6"/>
+    </row>
+    <row r="405" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B405" s="6"/>
+      <c r="C405" s="6"/>
+      <c r="D405" s="6"/>
+      <c r="F405" s="6"/>
+      <c r="H405" s="6"/>
+      <c r="I405" s="6"/>
+    </row>
+    <row r="406" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B406" s="6"/>
+      <c r="C406" s="6"/>
+      <c r="D406" s="6"/>
+      <c r="F406" s="6"/>
+      <c r="H406" s="6"/>
+      <c r="I406" s="6"/>
+    </row>
+    <row r="407" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B407" s="6"/>
+      <c r="C407" s="6"/>
+      <c r="D407" s="6"/>
+      <c r="F407" s="6"/>
+      <c r="H407" s="6"/>
+      <c r="I407" s="6"/>
+    </row>
+    <row r="408" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B408" s="6"/>
+      <c r="C408" s="6"/>
+      <c r="D408" s="6"/>
+      <c r="F408" s="6"/>
+      <c r="H408" s="6"/>
+      <c r="I408" s="6"/>
+    </row>
+    <row r="409" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B409" s="6"/>
+      <c r="C409" s="6"/>
+      <c r="D409" s="6"/>
+      <c r="F409" s="6"/>
+      <c r="H409" s="6"/>
+      <c r="I409" s="6"/>
+    </row>
+    <row r="410" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B410" s="6"/>
+      <c r="C410" s="6"/>
+      <c r="D410" s="6"/>
+      <c r="F410" s="6"/>
+      <c r="H410" s="6"/>
+      <c r="I410" s="6"/>
+    </row>
+    <row r="411" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B411" s="6"/>
+      <c r="C411" s="6"/>
+      <c r="D411" s="6"/>
+      <c r="F411" s="6"/>
+      <c r="H411" s="6"/>
+      <c r="I411" s="6"/>
+    </row>
+    <row r="412" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B412" s="6"/>
+      <c r="C412" s="6"/>
+      <c r="D412" s="6"/>
+      <c r="F412" s="6"/>
+      <c r="H412" s="6"/>
+      <c r="I412" s="6"/>
+    </row>
+    <row r="413" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B413" s="6"/>
+      <c r="C413" s="6"/>
+      <c r="D413" s="6"/>
+      <c r="F413" s="6"/>
+      <c r="H413" s="6"/>
+      <c r="I413" s="6"/>
+    </row>
+    <row r="414" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B414" s="6"/>
+      <c r="C414" s="6"/>
+      <c r="D414" s="6"/>
+      <c r="F414" s="6"/>
+      <c r="H414" s="6"/>
+      <c r="I414" s="6"/>
+    </row>
+    <row r="415" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B415" s="6"/>
+      <c r="C415" s="6"/>
+      <c r="D415" s="6"/>
+      <c r="F415" s="6"/>
+      <c r="H415" s="6"/>
+      <c r="I415" s="6"/>
+    </row>
+    <row r="416" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B416" s="6"/>
+      <c r="C416" s="6"/>
+      <c r="D416" s="6"/>
+      <c r="F416" s="6"/>
+      <c r="H416" s="6"/>
+      <c r="I416" s="6"/>
+    </row>
+    <row r="417" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B417" s="6"/>
+      <c r="C417" s="6"/>
+      <c r="D417" s="6"/>
+      <c r="F417" s="6"/>
+      <c r="H417" s="6"/>
+      <c r="I417" s="6"/>
+    </row>
+    <row r="418" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B418" s="6"/>
+      <c r="C418" s="6"/>
+      <c r="D418" s="6"/>
+      <c r="F418" s="6"/>
+      <c r="H418" s="6"/>
+      <c r="I418" s="6"/>
+    </row>
+    <row r="419" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B419" s="6"/>
+      <c r="C419" s="6"/>
+      <c r="D419" s="6"/>
+      <c r="F419" s="6"/>
+      <c r="H419" s="6"/>
+      <c r="I419" s="6"/>
+    </row>
+    <row r="420" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B420" s="6"/>
+      <c r="C420" s="6"/>
+      <c r="D420" s="6"/>
+      <c r="F420" s="6"/>
+      <c r="H420" s="6"/>
+      <c r="I420" s="6"/>
+    </row>
+    <row r="421" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B421" s="6"/>
+      <c r="C421" s="6"/>
+      <c r="D421" s="6"/>
+      <c r="F421" s="6"/>
+      <c r="H421" s="6"/>
+      <c r="I421" s="6"/>
+    </row>
+    <row r="422" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B422" s="6"/>
+      <c r="C422" s="6"/>
+      <c r="D422" s="6"/>
+      <c r="F422" s="6"/>
+      <c r="H422" s="6"/>
+      <c r="I422" s="6"/>
+    </row>
+    <row r="423" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B423" s="6"/>
+      <c r="C423" s="6"/>
+      <c r="D423" s="6"/>
+      <c r="F423" s="6"/>
+      <c r="H423" s="6"/>
+      <c r="I423" s="6"/>
+    </row>
+    <row r="424" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B424" s="6"/>
+      <c r="C424" s="6"/>
+      <c r="D424" s="6"/>
+      <c r="F424" s="6"/>
+      <c r="H424" s="6"/>
+      <c r="I424" s="6"/>
+    </row>
+    <row r="425" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B425" s="6"/>
+      <c r="C425" s="6"/>
+      <c r="D425" s="6"/>
+      <c r="F425" s="6"/>
+      <c r="H425" s="6"/>
+      <c r="I425" s="6"/>
+    </row>
+    <row r="426" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B426" s="6"/>
+      <c r="C426" s="6"/>
+      <c r="D426" s="6"/>
+      <c r="F426" s="6"/>
+      <c r="H426" s="6"/>
+      <c r="I426" s="6"/>
+    </row>
+    <row r="427" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B427" s="6"/>
+      <c r="C427" s="6"/>
+      <c r="D427" s="6"/>
+      <c r="F427" s="6"/>
+      <c r="H427" s="6"/>
+      <c r="I427" s="6"/>
+    </row>
+    <row r="428" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B428" s="6"/>
+      <c r="C428" s="6"/>
+      <c r="D428" s="6"/>
+      <c r="F428" s="6"/>
+      <c r="H428" s="6"/>
+      <c r="I428" s="6"/>
+    </row>
+    <row r="429" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B429" s="6"/>
+      <c r="C429" s="6"/>
+      <c r="D429" s="6"/>
+      <c r="F429" s="6"/>
+      <c r="H429" s="6"/>
+      <c r="I429" s="6"/>
+    </row>
+    <row r="430" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B430" s="6"/>
+      <c r="C430" s="6"/>
+      <c r="D430" s="6"/>
+      <c r="F430" s="6"/>
+      <c r="H430" s="6"/>
+      <c r="I430" s="6"/>
+    </row>
+    <row r="431" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B431" s="6"/>
+      <c r="C431" s="6"/>
+      <c r="D431" s="6"/>
+      <c r="F431" s="6"/>
+      <c r="H431" s="6"/>
+      <c r="I431" s="6"/>
+    </row>
+    <row r="432" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B432" s="6"/>
+      <c r="C432" s="6"/>
+      <c r="D432" s="6"/>
+      <c r="F432" s="6"/>
+      <c r="H432" s="6"/>
+      <c r="I432" s="6"/>
+    </row>
+    <row r="433" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B433" s="6"/>
+      <c r="C433" s="6"/>
+      <c r="D433" s="6"/>
+      <c r="F433" s="6"/>
+      <c r="H433" s="6"/>
+      <c r="I433" s="6"/>
+    </row>
+    <row r="434" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B434" s="6"/>
+      <c r="C434" s="6"/>
+      <c r="D434" s="6"/>
+      <c r="F434" s="6"/>
+      <c r="H434" s="6"/>
+      <c r="I434" s="6"/>
+    </row>
+    <row r="435" spans="2:9" ht="15.75">
+      <c r="B435" s="6"/>
+      <c r="C435" s="6"/>
+      <c r="D435" s="6"/>
+      <c r="F435" s="6"/>
+      <c r="H435" s="6"/>
+      <c r="I435" s="6"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:I435" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3521A2-0E46-4626-A556-F81B8258D1DB}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2746,7 +6380,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D90DEFD-D6A8-4BFB-97A2-600F5E7E4446}">
   <dimension ref="B2:C12"/>
   <sheetViews>
@@ -2761,7 +6395,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="18" thickBot="1">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="29" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Error handling for data extract 2
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870278A3-04B6-4822-A0E9-95D40F95C4AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F585618E-2021-4632-8BE1-9C77B5AC6D8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="45" windowWidth="27030" windowHeight="15555" activeTab="2" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="915" yWindow="45" windowWidth="27030" windowHeight="15555" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$435</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$438</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'to do - SS'!$A$1:$I$435</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D69" authorId="0" shapeId="0" xr:uid="{E4E7D546-5501-4B22-B4CB-2D44BAC24129}">
+    <comment ref="D70" authorId="0" shapeId="0" xr:uid="{E4E7D546-5501-4B22-B4CB-2D44BAC24129}">
       <text>
         <r>
           <rPr>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="158">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -687,35 +687,6 @@
     <t>set some kind of flag to let app know it's not a real map panel resize?</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">SZ:  Make manual point regeneration the default, and add map tool for setting this.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">old task:  </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>If (Chrome) downloads panel appears and changes map panel size, don't requery points</t>
-    </r>
-  </si>
-  <si>
     <t>add link to download FA (and SS?) GDB</t>
   </si>
   <si>
@@ -829,6 +800,56 @@
       </rPr>
       <t xml:space="preserve"> option</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>old task</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:  If (Chrome) downloads panel appears and changes map panel size, don't requery points</t>
+    </r>
+  </si>
+  <si>
+    <t>SZ:  Make manual point regeneration the default, and add map tool for setting this.</t>
+  </si>
+  <si>
+    <t>On data extract, get video clip URLs to open in new tab.  Also, handle GP errors.</t>
+  </si>
+  <si>
+    <r>
+      <t>something wrong with</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Limit suggestions to current extent</t>
+    </r>
+  </si>
+  <si>
+    <t>increase height of "offlineAppPanel"</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1118,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1185,6 +1206,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1498,7 +1528,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1723224</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>75975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1955,30 +1985,30 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J435"/>
+  <dimension ref="A1:J438"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G76" sqref="G76"/>
+      <selection pane="bottomRight" activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="62.75" style="9" customWidth="1"/>
+    <col min="4" max="4" width="66.125" style="9" customWidth="1"/>
     <col min="5" max="5" width="4.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="11.25" style="7" customWidth="1"/>
+    <col min="6" max="6" width="6.875" style="7" customWidth="1"/>
     <col min="7" max="7" width="13.875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="8.125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="6.125" style="9" customWidth="1"/>
     <col min="9" max="9" width="62.625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="32.125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="41.125" style="7" customWidth="1"/>
     <col min="11" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="97.5" customHeight="1">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="97.5" customHeight="1">
       <c r="A1" s="17" t="s">
         <v>12</v>
       </c>
@@ -2004,8 +2034,9 @@
       <c r="I1" s="12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" hidden="1">
+      <c r="J1" s="35"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" hidden="1">
       <c r="C2" s="2" t="s">
         <v>72</v>
       </c>
@@ -2014,8 +2045,9 @@
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="9"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" hidden="1">
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" hidden="1">
       <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
@@ -2032,8 +2064,9 @@
         <v>41</v>
       </c>
       <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" hidden="1">
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" hidden="1">
       <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
@@ -2045,8 +2078,9 @@
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" customFormat="1" ht="15.75" hidden="1">
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" customFormat="1" ht="15.75" hidden="1">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2059,7 +2093,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="31.5" hidden="1">
+    <row r="6" spans="1:10" ht="31.5" hidden="1">
       <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
@@ -2079,8 +2113,9 @@
       <c r="I6" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="47.25" hidden="1">
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="47.25" hidden="1">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
@@ -2092,8 +2127,9 @@
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" hidden="1">
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" hidden="1">
       <c r="C8" s="2" t="s">
         <v>72</v>
       </c>
@@ -2102,8 +2138,9 @@
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" hidden="1">
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" hidden="1">
       <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
@@ -2115,8 +2152,9 @@
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" hidden="1">
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" hidden="1">
       <c r="C10" s="2" t="s">
         <v>72</v>
       </c>
@@ -2125,8 +2163,9 @@
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:9" ht="31.5" hidden="1">
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" ht="31.5" hidden="1">
       <c r="C11" s="2" t="s">
         <v>71</v>
       </c>
@@ -2137,8 +2176,9 @@
       <c r="I11" s="11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" hidden="1">
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" hidden="1">
       <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2148,8 +2188,9 @@
       <c r="D12" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="31.5" hidden="1">
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" ht="31.5" hidden="1">
       <c r="C13" s="2" t="s">
         <v>71</v>
       </c>
@@ -2160,8 +2201,9 @@
       <c r="I13" s="11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="31.5" hidden="1">
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" ht="31.5" hidden="1">
       <c r="C14" s="2" t="s">
         <v>72</v>
       </c>
@@ -2172,8 +2214,9 @@
       <c r="I14" s="11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" hidden="1">
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" hidden="1">
       <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
@@ -2186,8 +2229,9 @@
       <c r="I15" s="11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" hidden="1">
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" hidden="1">
       <c r="A16" s="6" t="s">
         <v>11</v>
       </c>
@@ -2201,6 +2245,7 @@
       <c r="I16" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="J16" s="6"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" hidden="1">
       <c r="C17" s="2" t="s">
@@ -2211,6 +2256,7 @@
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="9"/>
+      <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" ht="31.5" hidden="1">
       <c r="B18" s="2" t="s">
@@ -2225,6 +2271,7 @@
       <c r="I18" s="11" t="s">
         <v>111</v>
       </c>
+      <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" hidden="1">
       <c r="B19" s="2" t="s">
@@ -2236,6 +2283,7 @@
       <c r="D19" s="6" t="s">
         <v>68</v>
       </c>
+      <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" hidden="1">
       <c r="A20" s="6" t="s">
@@ -2247,6 +2295,7 @@
       <c r="D20" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" hidden="1">
       <c r="B21" s="2" t="s">
@@ -2258,6 +2307,7 @@
       <c r="D21" s="9" t="s">
         <v>27</v>
       </c>
+      <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" hidden="1">
       <c r="C22" s="2" t="s">
@@ -2267,6 +2317,7 @@
         <v>29</v>
       </c>
       <c r="H22" s="6"/>
+      <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" hidden="1">
       <c r="B23" s="2" t="s">
@@ -2278,6 +2329,7 @@
       <c r="D23" s="9" t="s">
         <v>36</v>
       </c>
+      <c r="J23" s="6"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" hidden="1">
       <c r="B24" s="2" t="s">
@@ -2292,6 +2344,7 @@
       <c r="I24" s="11" t="s">
         <v>66</v>
       </c>
+      <c r="J24" s="6"/>
     </row>
     <row r="25" spans="1:10" ht="126" hidden="1">
       <c r="B25" s="2" t="s">
@@ -2312,8 +2365,9 @@
       <c r="I25" s="11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="94.5" hidden="1">
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:10" ht="110.25" hidden="1">
       <c r="C26" s="2" t="s">
         <v>71</v>
       </c>
@@ -2332,6 +2386,7 @@
       <c r="I26" s="11" t="s">
         <v>49</v>
       </c>
+      <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5" hidden="1">
       <c r="B27" s="2" t="s">
@@ -2366,6 +2421,7 @@
       <c r="D28" s="9" t="s">
         <v>53</v>
       </c>
+      <c r="J28" s="6"/>
     </row>
     <row r="29" spans="1:10" ht="31.5" hidden="1">
       <c r="B29" s="2" t="s">
@@ -2377,6 +2433,7 @@
       <c r="D29" s="9" t="s">
         <v>74</v>
       </c>
+      <c r="J29" s="6"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" hidden="1">
       <c r="A30" s="6" t="s">
@@ -2388,6 +2445,7 @@
       <c r="I30" s="20" t="s">
         <v>75</v>
       </c>
+      <c r="J30" s="6"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" hidden="1">
       <c r="C31" s="2" t="s">
@@ -2396,6 +2454,7 @@
       <c r="D31" s="6" t="s">
         <v>54</v>
       </c>
+      <c r="J31" s="6"/>
     </row>
     <row r="32" spans="1:10" ht="31.5" hidden="1">
       <c r="B32" s="2" t="s">
@@ -2416,8 +2475,9 @@
       <c r="I32" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="31.5" hidden="1">
+      <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="1:10" ht="31.5" hidden="1">
       <c r="B33" s="2" t="s">
         <v>21</v>
       </c>
@@ -2433,8 +2493,9 @@
       <c r="I33" s="19" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="31.5" hidden="1">
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="1:10" ht="31.5" hidden="1">
       <c r="C34" s="2" t="s">
         <v>71</v>
       </c>
@@ -2444,16 +2505,18 @@
       <c r="I34" s="19" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="63" hidden="1">
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="1:10" ht="63" hidden="1">
       <c r="A35" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" hidden="1">
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" hidden="1">
       <c r="B36" s="2" t="s">
         <v>24</v>
       </c>
@@ -2466,8 +2529,9 @@
       <c r="I36" s="11" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="15.75" hidden="1">
+      <c r="J36" s="6"/>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" hidden="1">
       <c r="C37" s="2" t="s">
         <v>71</v>
       </c>
@@ -2477,32 +2541,36 @@
       <c r="I37" s="11" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" hidden="1">
+      <c r="J37" s="6"/>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" hidden="1">
       <c r="C38" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="31.5" hidden="1">
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" hidden="1">
       <c r="C39" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="15.75" hidden="1">
+      <c r="J39" s="6"/>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" hidden="1">
       <c r="A40" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" hidden="1">
+      <c r="J40" s="6"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" hidden="1">
       <c r="C41" s="2" t="s">
         <v>71</v>
       </c>
@@ -2512,69 +2580,77 @@
       <c r="I41" s="11" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" hidden="1">
+      <c r="J41" s="6"/>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" hidden="1">
       <c r="C42" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D42" s="9" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="15.75" hidden="1">
+      <c r="J42" s="6"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" hidden="1">
       <c r="C43" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="39.75" hidden="1" customHeight="1">
+      <c r="J43" s="6"/>
+    </row>
+    <row r="44" spans="1:10" ht="39.75" hidden="1" customHeight="1">
       <c r="C44" s="2" t="s">
         <v>101</v>
       </c>
       <c r="D44" s="27" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" hidden="1">
+      <c r="J44" s="6"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" hidden="1">
       <c r="C45" s="2" t="s">
         <v>101</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="15.75" hidden="1">
+      <c r="J45" s="6"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" hidden="1">
       <c r="C46" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="9.75" hidden="1" customHeight="1">
+      <c r="J46" s="6"/>
+    </row>
+    <row r="47" spans="1:10" ht="9.75" hidden="1" customHeight="1">
       <c r="A47" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="42" customHeight="1">
+      <c r="J47" s="6"/>
+    </row>
+    <row r="48" spans="1:10" ht="42" customHeight="1">
       <c r="D48" s="9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15.75" hidden="1">
+    <row r="49" spans="1:10" ht="15.75" hidden="1">
       <c r="C49" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="31.5" hidden="1">
+      <c r="J49" s="6"/>
+    </row>
+    <row r="50" spans="1:10" ht="31.5" hidden="1">
       <c r="C50" s="2" t="s">
         <v>71</v>
       </c>
@@ -2584,16 +2660,18 @@
       <c r="I50" s="11" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+      <c r="J50" s="6"/>
+    </row>
+    <row r="51" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C51" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" hidden="1">
+      <c r="J51" s="6"/>
+    </row>
+    <row r="52" spans="1:10" ht="15.75" hidden="1">
       <c r="C52" s="2" t="s">
         <v>21</v>
       </c>
@@ -2603,8 +2681,9 @@
       <c r="I52" s="11" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" hidden="1">
+      <c r="J52" s="6"/>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" hidden="1">
       <c r="C53" s="2" t="s">
         <v>71</v>
       </c>
@@ -2614,24 +2693,27 @@
       <c r="I53" s="11" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="15.75" hidden="1">
+      <c r="J53" s="6"/>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" hidden="1">
       <c r="C54" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+      <c r="J54" s="6"/>
+    </row>
+    <row r="55" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="A55" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D55" s="24" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+      <c r="J55" s="6"/>
+    </row>
+    <row r="56" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C56" s="2" t="s">
         <v>21</v>
       </c>
@@ -2639,16 +2721,18 @@
         <v>113</v>
       </c>
       <c r="I56" s="25"/>
-    </row>
-    <row r="57" spans="1:9" ht="15.75" hidden="1">
+      <c r="J56" s="6"/>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" hidden="1">
       <c r="C57" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" ht="24.95" customHeight="1">
+      <c r="J57" s="6"/>
+    </row>
+    <row r="58" spans="1:10" ht="24.95" customHeight="1">
       <c r="D58" s="31" t="s">
         <v>114</v>
       </c>
@@ -2656,154 +2740,188 @@
         <v>115</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+    <row r="59" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="A59" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="31.5" hidden="1">
+      <c r="J59" s="6"/>
+    </row>
+    <row r="60" spans="1:10" ht="15.75" hidden="1">
       <c r="C60" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D60" s="26" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="24.95" customHeight="1">
+      <c r="J60" s="6"/>
+    </row>
+    <row r="61" spans="1:10" ht="24.95" customHeight="1">
       <c r="D61" s="9" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+    <row r="62" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C62" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+      <c r="J62" s="6"/>
+    </row>
+    <row r="63" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C63" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="32.25" hidden="1" customHeight="1">
+      <c r="J63" s="6"/>
+    </row>
+    <row r="64" spans="1:10" ht="32.25" hidden="1" customHeight="1">
       <c r="C64" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D64" s="9" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="65" spans="3:9" ht="24.95" customHeight="1">
+      <c r="J64" s="6"/>
+    </row>
+    <row r="65" spans="3:10" ht="24.95" customHeight="1">
       <c r="D65" s="9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="66" spans="3:9" ht="24.95" hidden="1" customHeight="1">
+    <row r="66" spans="3:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C66" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D66" s="9" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="67" spans="3:9" ht="24.95" customHeight="1">
-      <c r="D67" s="9" t="s">
+      <c r="J66" s="6"/>
+    </row>
+    <row r="67" spans="3:10" ht="24.95" customHeight="1">
+      <c r="D67" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="J67" s="6"/>
+    </row>
+    <row r="68" spans="3:10" ht="24.95" customHeight="1">
+      <c r="D68" s="9" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="68" spans="3:9" ht="24.95" customHeight="1">
-      <c r="D68" s="31" t="s">
+    <row r="69" spans="3:10" ht="24.95" customHeight="1">
+      <c r="D69" s="31" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="3:9" ht="63.75" thickBot="1">
-      <c r="D69" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="G69" s="19" t="s">
+    <row r="70" spans="3:10" ht="48" thickBot="1">
+      <c r="D70" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="G70" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="I69" s="11" t="s">
+      <c r="I70" s="11" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="70" spans="3:9" ht="16.5" hidden="1" thickBot="1">
-      <c r="C70" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="G70" s="19"/>
-    </row>
-    <row r="71" spans="3:9" ht="24.95" hidden="1" customHeight="1" thickBot="1">
+      <c r="J70" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="71" spans="3:10" ht="16.5" hidden="1" thickBot="1">
       <c r="C71" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D71" s="28" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="72" spans="3:9" ht="42" hidden="1" customHeight="1" thickBot="1">
+      <c r="D71" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G71" s="19"/>
+      <c r="J71" s="6"/>
+    </row>
+    <row r="72" spans="3:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C72" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D72" s="9" t="s">
+      <c r="D72" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="J72" s="6"/>
+    </row>
+    <row r="73" spans="3:10" ht="42" hidden="1" customHeight="1" thickBot="1">
+      <c r="C73" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="G73" s="19"/>
+      <c r="J73" s="6"/>
+    </row>
+    <row r="74" spans="3:10" ht="16.5" thickBot="1">
+      <c r="D74" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="G74" s="19"/>
+    </row>
+    <row r="75" spans="3:10" ht="15.75">
+      <c r="D75" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G75" s="19"/>
+    </row>
+    <row r="76" spans="3:10" ht="15.75">
+      <c r="D76" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="G76" s="19"/>
+    </row>
+    <row r="77" spans="3:10" ht="15.75" hidden="1">
+      <c r="C77" s="36">
+        <v>44011</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G77" s="19"/>
+    </row>
+    <row r="79" spans="3:10" ht="24.95" customHeight="1">
+      <c r="D79" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="80" spans="3:10" ht="34.5" customHeight="1">
+      <c r="D80" s="33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="81" spans="4:9" ht="24.95" customHeight="1" thickBot="1"/>
+    <row r="82" spans="4:9" ht="32.25" thickBot="1">
+      <c r="D82" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="G72" s="19"/>
-    </row>
-    <row r="73" spans="3:9" ht="16.5" thickBot="1">
-      <c r="D73" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="G73" s="19"/>
-    </row>
-    <row r="74" spans="3:9" ht="15.75">
-      <c r="D74" s="9" t="s">
+    </row>
+    <row r="83" spans="4:9" ht="24.95" customHeight="1">
+      <c r="D83" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="G74" s="19"/>
-    </row>
-    <row r="76" spans="3:9" ht="24.95" customHeight="1">
-      <c r="D76" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="77" spans="3:9" ht="34.5" customHeight="1">
-      <c r="D77" s="33" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="78" spans="3:9" ht="24.95" customHeight="1" thickBot="1"/>
-    <row r="79" spans="3:9" ht="32.25" thickBot="1">
-      <c r="D79" s="32" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="80" spans="3:9" ht="24.95" customHeight="1">
-      <c r="D80" s="26" t="s">
+      <c r="I83" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="I80" s="11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="435" spans="1:1" ht="15.75" hidden="1">
-      <c r="A435" s="2" t="s">
+    </row>
+    <row r="438" spans="1:10" ht="15.75" hidden="1">
+      <c r="A438" s="2" t="s">
         <v>109</v>
       </c>
+      <c r="J438" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I435" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
+  <autoFilter ref="A1:I438" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
@@ -2815,7 +2933,7 @@
     <hyperlink ref="J27" r:id="rId1" display="https://github.com/SitePen/dgrid/blob/master/doc/components/mixins/Selection.md" xr:uid="{B02003EC-0D72-4D32-86B5-BCB2E4740BDA}"/>
     <hyperlink ref="I33" r:id="rId2" xr:uid="{D7280C89-055C-482B-859C-78DDF371D8BE}"/>
     <hyperlink ref="I34" r:id="rId3" location="release_notes_08_23_2018" display="Can no longer disable showing of &quot;more videos&quot; when video is paused" xr:uid="{75869B48-9B1F-4352-8C34-D2F55186219A}"/>
-    <hyperlink ref="G69" r:id="rId4" display="https://www.google.com/search?sxsrf=ALeKk03fRI45rxW7duPejqDWYRNo315xnA%3A1589067316875Google search" xr:uid="{B59445F6-07F3-4CDD-950F-C113A43BEE63}"/>
+    <hyperlink ref="G70" r:id="rId4" display="https://www.google.com/search?sxsrf=ALeKk03fRI45rxW7duPejqDWYRNo315xnA%3A1589067316875Google search" xr:uid="{B59445F6-07F3-4CDD-950F-C113A43BEE63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId5"/>
@@ -2825,13 +2943,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8A68F0-A5CC-4F2B-9E7A-D47D3E46C475}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J435"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2883,11 +3002,13 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75">
+    <row r="3" spans="1:10" ht="15.75" hidden="1">
       <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="C3" s="34">
+        <v>44006</v>
+      </c>
       <c r="D3" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F3" s="6"/>
       <c r="H3" s="6"/>
@@ -2906,7 +3027,7 @@
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -2919,7 +3040,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F6" s="6"/>
       <c r="H6" s="6"/>
@@ -6358,7 +6479,11 @@
       <c r="I435" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I435" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}"/>
+  <autoFilter ref="A1:I435" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
+    <filterColumn colId="2">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -6396,56 +6521,56 @@
   <sheetData>
     <row r="2" spans="2:3" ht="18" thickBot="1">
       <c r="B2" s="29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="16.5" thickTop="1"/>
     <row r="4" spans="2:3">
       <c r="B4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" t="s">
         <v>136</v>
-      </c>
-      <c r="C7" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" t="s">
         <v>138</v>
-      </c>
-      <c r="C8" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" t="s">
         <v>140</v>
-      </c>
-      <c r="C10" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Algae/Invert filter for SS Species table
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F585618E-2021-4632-8BE1-9C77B5AC6D8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58FD921-3A5F-436A-9349-BE6C88C136E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="45" windowWidth="27030" windowHeight="15555" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="615" yWindow="180" windowWidth="27030" windowHeight="15555" activeTab="2" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$438</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$439</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'to do - SS'!$A$1:$I$435</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="160">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -830,9 +830,6 @@
     <t>SZ:  Make manual point regeneration the default, and add map tool for setting this.</t>
   </si>
   <si>
-    <t>On data extract, get video clip URLs to open in new tab.  Also, handle GP errors.</t>
-  </si>
-  <si>
     <r>
       <t>something wrong with</t>
     </r>
@@ -850,6 +847,15 @@
   </si>
   <si>
     <t>increase height of "offlineAppPanel"</t>
+  </si>
+  <si>
+    <t>changes table header height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On data extract, get video clip URLs to open in new tab.  </t>
+  </si>
+  <si>
+    <t>add algae/invert filters and  "show biobands" option to the species table</t>
   </si>
 </sst>
 </file>
@@ -1985,20 +1991,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J438"/>
+  <dimension ref="A1:J439"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C78" sqref="C78"/>
+      <selection pane="bottomRight" activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="66.125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="70.75" style="9" customWidth="1"/>
     <col min="5" max="5" width="4.5" style="6" customWidth="1"/>
     <col min="6" max="6" width="6.875" style="7" customWidth="1"/>
     <col min="7" max="7" width="13.875" style="6" customWidth="1"/>
@@ -2806,11 +2812,11 @@
     </row>
     <row r="67" spans="3:10" ht="24.95" customHeight="1">
       <c r="D67" s="33" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="J67" s="6"/>
     </row>
-    <row r="68" spans="3:10" ht="24.95" customHeight="1">
+    <row r="68" spans="3:10" ht="20.100000000000001" customHeight="1">
       <c r="D68" s="9" t="s">
         <v>126</v>
       </c>
@@ -2820,7 +2826,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="3:10" ht="48" thickBot="1">
+    <row r="70" spans="3:10" ht="34.5" customHeight="1" thickBot="1">
       <c r="D70" s="31" t="s">
         <v>154</v>
       </c>
@@ -2869,15 +2875,21 @@
       </c>
       <c r="G74" s="19"/>
     </row>
-    <row r="75" spans="3:10" ht="15.75">
+    <row r="75" spans="3:10" ht="20.100000000000001" customHeight="1">
       <c r="D75" s="9" t="s">
         <v>146</v>
       </c>
       <c r="G75" s="19"/>
-    </row>
-    <row r="76" spans="3:10" ht="15.75">
+      <c r="I75" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="76" spans="3:10" ht="15.75" hidden="1">
+      <c r="C76" s="36">
+        <v>44011</v>
+      </c>
       <c r="D76" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G76" s="19"/>
     </row>
@@ -2886,42 +2898,49 @@
         <v>44011</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G77" s="19"/>
     </row>
-    <row r="79" spans="3:10" ht="24.95" customHeight="1">
-      <c r="D79" s="9" t="s">
+    <row r="78" spans="3:10" ht="20.100000000000001" customHeight="1">
+      <c r="C78" s="36"/>
+      <c r="D78" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G78" s="19"/>
+    </row>
+    <row r="80" spans="3:10" ht="24.95" customHeight="1">
+      <c r="D80" s="9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="80" spans="3:10" ht="34.5" customHeight="1">
-      <c r="D80" s="33" t="s">
+    <row r="81" spans="4:9" ht="34.5" customHeight="1">
+      <c r="D81" s="33" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="81" spans="4:9" ht="24.95" customHeight="1" thickBot="1"/>
-    <row r="82" spans="4:9" ht="32.25" thickBot="1">
-      <c r="D82" s="32" t="s">
+    <row r="82" spans="4:9" ht="24.95" customHeight="1" thickBot="1"/>
+    <row r="83" spans="4:9" ht="32.25" thickBot="1">
+      <c r="D83" s="32" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="83" spans="4:9" ht="24.95" customHeight="1">
-      <c r="D83" s="26" t="s">
+    <row r="84" spans="4:9" ht="24.95" customHeight="1">
+      <c r="D84" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="I83" s="11" t="s">
+      <c r="I84" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="438" spans="1:10" ht="15.75" hidden="1">
-      <c r="A438" s="2" t="s">
+    <row r="439" spans="1:10" ht="15.75" hidden="1">
+      <c r="A439" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="J438" s="6"/>
+      <c r="J439" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I438" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
+  <autoFilter ref="A1:I439" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
@@ -2946,7 +2965,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J435"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
last version using old FA with Locales
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58FD921-3A5F-436A-9349-BE6C88C136E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEA9169-A6CB-453B-A5D9-1B1400CCDE19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="180" windowWidth="27030" windowHeight="15555" activeTab="2" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="405" yWindow="45" windowWidth="26265" windowHeight="15555" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -855,7 +855,7 @@
     <t xml:space="preserve">On data extract, get video clip URLs to open in new tab.  </t>
   </si>
   <si>
-    <t>add algae/invert filters and  "show biobands" option to the species table</t>
+    <t>add  "show biobands" option to the species table</t>
   </si>
 </sst>
 </file>
@@ -1993,11 +1993,11 @@
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:J439"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D78" sqref="D78"/>
+      <selection pane="bottomRight" activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2264,7 +2264,7 @@
       <c r="I17" s="9"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10" ht="31.5" hidden="1">
+    <row r="18" spans="1:10" ht="15.75" hidden="1">
       <c r="B18" s="2" t="s">
         <v>24</v>
       </c>
@@ -2429,7 +2429,7 @@
       </c>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:10" ht="31.5" hidden="1">
+    <row r="29" spans="1:10" ht="15.75" hidden="1">
       <c r="B29" s="2" t="s">
         <v>21</v>
       </c>
@@ -2965,11 +2965,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J435"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -3044,7 +3044,9 @@
     <row r="5" spans="1:10" customFormat="1" ht="15.75">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="C5" s="34">
+        <v>44014</v>
+      </c>
       <c r="D5" s="6" t="s">
         <v>151</v>
       </c>

</xml_diff>

<commit_message>
Fix totals query and alignment
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEA9169-A6CB-453B-A5D9-1B1400CCDE19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA25BA27-5E33-407D-A97A-673E9EFF814E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="45" windowWidth="26265" windowHeight="15555" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="7980" yWindow="45" windowWidth="18690" windowHeight="15555" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$439</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$440</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'to do - SS'!$A$1:$I$435</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="161">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -856,6 +856,9 @@
   </si>
   <si>
     <t>add  "show biobands" option to the species table</t>
+  </si>
+  <si>
+    <t>FA:  Change "Species" to "SpCount" in SQL Server views and associated JS code</t>
   </si>
 </sst>
 </file>
@@ -1991,13 +1994,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J439"/>
+  <dimension ref="A1:J440"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D79" sqref="D79"/>
+      <selection pane="bottomRight" activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2909,38 +2912,45 @@
       </c>
       <c r="G78" s="19"/>
     </row>
-    <row r="80" spans="3:10" ht="24.95" customHeight="1">
-      <c r="D80" s="9" t="s">
+    <row r="79" spans="3:10" ht="20.100000000000001" customHeight="1">
+      <c r="C79" s="36"/>
+      <c r="D79" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G79" s="19"/>
+    </row>
+    <row r="81" spans="4:9" ht="24.95" customHeight="1">
+      <c r="D81" s="9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="81" spans="4:9" ht="34.5" customHeight="1">
-      <c r="D81" s="33" t="s">
+    <row r="82" spans="4:9" ht="34.5" customHeight="1">
+      <c r="D82" s="33" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="82" spans="4:9" ht="24.95" customHeight="1" thickBot="1"/>
-    <row r="83" spans="4:9" ht="32.25" thickBot="1">
-      <c r="D83" s="32" t="s">
+    <row r="83" spans="4:9" ht="24.95" customHeight="1" thickBot="1"/>
+    <row r="84" spans="4:9" ht="32.25" thickBot="1">
+      <c r="D84" s="32" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="84" spans="4:9" ht="24.95" customHeight="1">
-      <c r="D84" s="26" t="s">
+    <row r="85" spans="4:9" ht="24.95" customHeight="1">
+      <c r="D85" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="I84" s="11" t="s">
+      <c r="I85" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="439" spans="1:10" ht="15.75" hidden="1">
-      <c r="A439" s="2" t="s">
+    <row r="440" spans="1:10" ht="15.75" hidden="1">
+      <c r="A440" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="J439" s="6"/>
+      <c r="J440" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I439" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
+  <autoFilter ref="A1:I440" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Fixed statewide species query after regional query bug
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA25BA27-5E33-407D-A97A-673E9EFF814E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF1C659-1523-4109-A1AE-EC3C767CF657}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="45" windowWidth="18690" windowHeight="15555" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="390" yWindow="45" windowWidth="25425" windowHeight="15555" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="162">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -859,6 +859,9 @@
   </si>
   <si>
     <t>FA:  Change "Species" to "SpCount" in SQL Server views and associated JS code</t>
+  </si>
+  <si>
+    <t>SS species table:  Statewide table after showing regional table: regional WHERE clause still there</t>
   </si>
 </sst>
 </file>
@@ -2000,7 +2003,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D80" sqref="D80"/>
+      <selection pane="bottomRight" activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2799,12 +2802,12 @@
       </c>
       <c r="J64" s="6"/>
     </row>
-    <row r="65" spans="3:10" ht="24.95" customHeight="1">
+    <row r="65" spans="1:10" ht="24.95" customHeight="1">
       <c r="D65" s="9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="66" spans="3:10" ht="24.95" hidden="1" customHeight="1">
+    <row r="66" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C66" s="2" t="s">
         <v>21</v>
       </c>
@@ -2813,23 +2816,23 @@
       </c>
       <c r="J66" s="6"/>
     </row>
-    <row r="67" spans="3:10" ht="24.95" customHeight="1">
+    <row r="67" spans="1:10" ht="24.95" customHeight="1">
       <c r="D67" s="33" t="s">
         <v>158</v>
       </c>
       <c r="J67" s="6"/>
     </row>
-    <row r="68" spans="3:10" ht="20.100000000000001" customHeight="1">
+    <row r="68" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="D68" s="9" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="69" spans="3:10" ht="24.95" customHeight="1">
+    <row r="69" spans="1:10" ht="24.95" customHeight="1">
       <c r="D69" s="31" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="3:10" ht="34.5" customHeight="1" thickBot="1">
+    <row r="70" spans="1:10" ht="34.5" customHeight="1" thickBot="1">
       <c r="D70" s="31" t="s">
         <v>154</v>
       </c>
@@ -2843,7 +2846,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="71" spans="3:10" ht="16.5" hidden="1" thickBot="1">
+    <row r="71" spans="1:10" ht="16.5" hidden="1" thickBot="1">
       <c r="C71" s="2" t="s">
         <v>21</v>
       </c>
@@ -2853,7 +2856,7 @@
       <c r="G71" s="19"/>
       <c r="J71" s="6"/>
     </row>
-    <row r="72" spans="3:10" ht="24.95" hidden="1" customHeight="1">
+    <row r="72" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C72" s="2" t="s">
         <v>21</v>
       </c>
@@ -2862,7 +2865,7 @@
       </c>
       <c r="J72" s="6"/>
     </row>
-    <row r="73" spans="3:10" ht="42" hidden="1" customHeight="1" thickBot="1">
+    <row r="73" spans="1:10" ht="42" hidden="1" customHeight="1" thickBot="1">
       <c r="C73" s="2" t="s">
         <v>21</v>
       </c>
@@ -2872,13 +2875,13 @@
       <c r="G73" s="19"/>
       <c r="J73" s="6"/>
     </row>
-    <row r="74" spans="3:10" ht="16.5" thickBot="1">
+    <row r="74" spans="1:10" ht="16.5" thickBot="1">
       <c r="D74" s="30" t="s">
         <v>149</v>
       </c>
       <c r="G74" s="19"/>
     </row>
-    <row r="75" spans="3:10" ht="20.100000000000001" customHeight="1">
+    <row r="75" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="D75" s="9" t="s">
         <v>146</v>
       </c>
@@ -2887,7 +2890,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="76" spans="3:10" ht="15.75" hidden="1">
+    <row r="76" spans="1:10" ht="15.75" hidden="1">
       <c r="C76" s="36">
         <v>44011</v>
       </c>
@@ -2896,7 +2899,7 @@
       </c>
       <c r="G76" s="19"/>
     </row>
-    <row r="77" spans="3:10" ht="15.75" hidden="1">
+    <row r="77" spans="1:10" ht="15.75" hidden="1">
       <c r="C77" s="36">
         <v>44011</v>
       </c>
@@ -2905,37 +2908,53 @@
       </c>
       <c r="G77" s="19"/>
     </row>
-    <row r="78" spans="3:10" ht="20.100000000000001" customHeight="1">
+    <row r="78" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="C78" s="36"/>
       <c r="D78" s="9" t="s">
         <v>159</v>
       </c>
       <c r="G78" s="19"/>
     </row>
-    <row r="79" spans="3:10" ht="20.100000000000001" customHeight="1">
+    <row r="79" spans="1:10" ht="20.100000000000001" hidden="1" customHeight="1">
+      <c r="A79" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="C79" s="36"/>
       <c r="D79" s="9" t="s">
         <v>160</v>
       </c>
       <c r="G79" s="19"/>
     </row>
-    <row r="81" spans="4:9" ht="24.95" customHeight="1">
-      <c r="D81" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="82" spans="4:9" ht="34.5" customHeight="1">
+    <row r="80" spans="1:10" ht="39" hidden="1" customHeight="1">
+      <c r="C80" s="36">
+        <v>44029</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="34.5" hidden="1" customHeight="1">
+      <c r="A82" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="D82" s="33" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="83" spans="4:9" ht="24.95" customHeight="1" thickBot="1"/>
-    <row r="84" spans="4:9" ht="32.25" thickBot="1">
+    <row r="83" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D83" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="32.25" hidden="1" thickBot="1">
+      <c r="C84" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="D84" s="32" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="4:9" ht="24.95" customHeight="1">
+    <row r="85" spans="1:9" ht="24.95" customHeight="1">
       <c r="D85" s="26" t="s">
         <v>147</v>
       </c>

</xml_diff>

<commit_message>
Extra fields for SP tables, long display values (e.g. for Abundance)
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF1C659-1523-4109-A1AE-EC3C767CF657}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9E75B0-D393-473B-8677-BECC5349143E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="45" windowWidth="25425" windowHeight="15555" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="390" yWindow="45" windowWidth="25425" windowHeight="15555" activeTab="5" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -18,9 +18,11 @@
     <sheet name="to do - SS" sheetId="16" r:id="rId3"/>
     <sheet name="SZ point regeneration rethink" sheetId="14" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="15" r:id="rId5"/>
+    <sheet name="MPK download" sheetId="17" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'MPK download'!$A$3:$C$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$440</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'to do - SS'!$A$1:$I$435</definedName>
   </definedNames>
@@ -32,7 +34,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -133,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="172">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -863,12 +867,42 @@
   <si>
     <t>SS species table:  Statewide table after showing regional table: regional WHERE clause still there</t>
   </si>
+  <si>
+    <t>https://alaskafisheries.noaa.gov/mapping/shorezonedata/carrymap/</t>
+  </si>
+  <si>
+    <t>FishAtlas_v2020.mpk</t>
+  </si>
+  <si>
+    <t>FishAtlas_wViews_2020_0708.mpk</t>
+  </si>
+  <si>
+    <t>Ports_SSL.mpk</t>
+  </si>
+  <si>
+    <t>ShoreStation2019_2020_0723.mpk</t>
+  </si>
+  <si>
+    <t>ShoreZone.mpk</t>
+  </si>
+  <si>
+    <t>ShoreZoneFlexMapService_2019_0331.mpk</t>
+  </si>
+  <si>
+    <t>MPK</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1036,6 +1070,12 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1130,7 +1170,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1227,6 +1267,20 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1999,7 +2053,7 @@
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:J440"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -6627,4 +6681,118 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392EF631-8DBE-4581-9410-4CF72B20CF9A}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="44.25" customWidth="1"/>
+    <col min="2" max="2" width="16.875" style="40" customWidth="1"/>
+    <col min="3" max="3" width="94" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="37" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="41" customFormat="1">
+      <c r="A3" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="39">
+        <v>44035</v>
+      </c>
+      <c r="C4" s="38" t="str">
+        <f>HYPERLINK($A$1&amp;A4)</f>
+        <v>https://alaskafisheries.noaa.gov/mapping/shorezonedata/carrymap/FishAtlas_v2020.mpk</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="39">
+        <v>44035</v>
+      </c>
+      <c r="C5" s="38" t="str">
+        <f>HYPERLINK($A$1&amp;A5)</f>
+        <v>https://alaskafisheries.noaa.gov/mapping/shorezonedata/carrymap/ShoreStation2019_2020_0723.mpk</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" s="39">
+        <v>44020</v>
+      </c>
+      <c r="C6" s="38" t="str">
+        <f>HYPERLINK($A$1&amp;A6)</f>
+        <v>https://alaskafisheries.noaa.gov/mapping/shorezonedata/carrymap/FishAtlas_wViews_2020_0708.mpk</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="39">
+        <v>43864</v>
+      </c>
+      <c r="C7" s="38" t="str">
+        <f>HYPERLINK($A$1&amp;A7)</f>
+        <v>https://alaskafisheries.noaa.gov/mapping/shorezonedata/carrymap/Ports_SSL.mpk</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="39">
+        <v>43838</v>
+      </c>
+      <c r="C8" s="38" t="str">
+        <f>HYPERLINK($A$1&amp;A8)</f>
+        <v>https://alaskafisheries.noaa.gov/mapping/shorezonedata/carrymap/ShoreZone.mpk</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" s="39">
+        <v>43555</v>
+      </c>
+      <c r="C9" s="38" t="str">
+        <f>HYPERLINK($A$1&amp;A9)</f>
+        <v>https://alaskafisheries.noaa.gov/mapping/shorezonedata/carrymap/ShoreZoneFlexMapService_2019_0331.mpk</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A3:C9" xr:uid="{EF34674F-F350-41F4-8F0D-F23E66B41960}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:C9">
+      <sortCondition descending="1" ref="B3:B9"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add BioBands option to Species table
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,30 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9E75B0-D393-473B-8677-BECC5349143E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D257B1BA-7BF8-46CA-8494-84C1E9B88756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="45" windowWidth="25425" windowHeight="15555" activeTab="5" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="5205" yWindow="45" windowWidth="23430" windowHeight="15555" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
     <sheet name="to do" sheetId="1" r:id="rId2"/>
-    <sheet name="to do - SS" sheetId="16" r:id="rId3"/>
-    <sheet name="SZ point regeneration rethink" sheetId="14" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="15" r:id="rId5"/>
-    <sheet name="MPK download" sheetId="17" r:id="rId6"/>
+    <sheet name="Statistical queries" sheetId="18" r:id="rId3"/>
+    <sheet name="to do - SS" sheetId="16" r:id="rId4"/>
+    <sheet name="SZ point regeneration rethink" sheetId="14" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId6"/>
+    <sheet name="MPK download" sheetId="17" r:id="rId7"/>
+    <sheet name="Sp_BB tables" sheetId="19" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'MPK download'!$A$3:$C$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$440</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'to do - SS'!$A$1:$I$435</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'MPK download'!$A$3:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$441</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'to do - SS'!$A$1:$I$435</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +58,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>4.14 feature</t>
         </r>
@@ -69,7 +71,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Make clickable features invisible, hovering over MapService features?
 (Use views to limit features.)</t>
@@ -126,7 +128,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>not there yet</t>
         </r>
@@ -137,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="278">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -897,14 +899,448 @@
   <si>
     <t>Link</t>
   </si>
+  <si>
+    <t>Statistical queries</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>groupByFieldsForStatistics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> instead of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>outFields</t>
+    </r>
+  </si>
+  <si>
+    <t>outStatistics</t>
+  </si>
+  <si>
+    <t>Values: An array of statistic definitions. A statistic definition specifies the type of statistic, the field on which it is to be calculated, and the resulting output field name.</t>
+  </si>
+  <si>
+    <t>Syntax:</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "statisticType": "&lt;count | sum | min | max | avg | stddev | var&gt;",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "onStatisticField": "Field1", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "outStatisticFieldName": "Out_Field_Name1"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "onStatisticField": "Field2",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "outStatisticFieldName": "Out_Field_Name2"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  }  </t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>Example:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "statisticType": "sum",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "onStatisticField": "GENDER",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "outStatisticFieldName": "PopulationByGender"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "statisticType": "avg",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "onStatisticField": "INCOME",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "outStatisticFieldName": "AverageIncome"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  }</t>
+  </si>
+  <si>
+    <t>https://alaskafisheries.noaa.gov/arcgis/sdk/rest/index.html#//02ss0000000r000000</t>
+  </si>
+  <si>
+    <t>uniqueValues</t>
+  </si>
+  <si>
+    <t>https://developers.arcgis.com/javascript/latest/api-reference/esri-smartMapping-statistics-uniqueValues.html</t>
+  </si>
+  <si>
+    <t>has to be on a FeatureLayer?</t>
+  </si>
+  <si>
+    <t>https://www.google.com/search?q=sql+server+rest+service&amp;oq=sq&amp;aqs=chrome.1.69i57j35i39l2j0l5.4119j0j8&amp;sourceid=chrome&amp;ie=UTF-8</t>
+  </si>
+  <si>
+    <t>https://www.red-gate.com/simple-talk/blogs/setting-up-a-simple-rest-interface-with-sql-server/</t>
+  </si>
+  <si>
+    <t>Rest interface with SQL Server</t>
+  </si>
+  <si>
+    <t>Looks like I will need to use MVCServices to get Hauls and Species count</t>
+  </si>
+  <si>
+    <t>I might look into  whether I can make a GP service that will give counts of unique values, and whether this can be done using a file GDB.  (Might need to be in an ArcGIS Pro file.)</t>
+  </si>
+  <si>
+    <t>https://community.esri.com/community/open-platform-standards-and-interoperability/blog/2020/04/22/etl-file-geodatabase-views</t>
+  </si>
+  <si>
+    <t>SubgroupID</t>
+  </si>
+  <si>
+    <t>esriFieldTypeInteger</t>
+  </si>
+  <si>
+    <t>SubgroupID </t>
+  </si>
+  <si>
+    <t>Subgroup</t>
+  </si>
+  <si>
+    <t>esriFieldTypeString</t>
+  </si>
+  <si>
+    <t>Subgroup </t>
+  </si>
+  <si>
+    <t>station_ID</t>
+  </si>
+  <si>
+    <t>station_ID </t>
+  </si>
+  <si>
+    <t>station</t>
+  </si>
+  <si>
+    <t>station </t>
+  </si>
+  <si>
+    <t>SppTxtCode</t>
+  </si>
+  <si>
+    <t>SppTxtCode </t>
+  </si>
+  <si>
+    <t>SppNameHtml</t>
+  </si>
+  <si>
+    <t>SppNameHtml </t>
+  </si>
+  <si>
+    <t>SppName</t>
+  </si>
+  <si>
+    <t>SppName </t>
+  </si>
+  <si>
+    <t>SpeciesNo</t>
+  </si>
+  <si>
+    <t>esriFieldTypeDouble</t>
+  </si>
+  <si>
+    <t>SpeciesNo </t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>esriFieldTypeGeometry</t>
+  </si>
+  <si>
+    <t>Shape </t>
+  </si>
+  <si>
+    <t>RegionalID</t>
+  </si>
+  <si>
+    <t>RegionalID </t>
+  </si>
+  <si>
+    <t>OBJECTID</t>
+  </si>
+  <si>
+    <t>esriFieldTypeOID</t>
+  </si>
+  <si>
+    <t>OBJECTID </t>
+  </si>
+  <si>
+    <t>LocaleConcat</t>
+  </si>
+  <si>
+    <t>LocaleConcat </t>
+  </si>
+  <si>
+    <t>hasSpecies</t>
+  </si>
+  <si>
+    <t>hasSpecies </t>
+  </si>
+  <si>
+    <t>hasProfile</t>
+  </si>
+  <si>
+    <t>hasProfile </t>
+  </si>
+  <si>
+    <t>hasPhotos</t>
+  </si>
+  <si>
+    <t>hasPhotos </t>
+  </si>
+  <si>
+    <t>GroupID</t>
+  </si>
+  <si>
+    <t>GroupID </t>
+  </si>
+  <si>
+    <t>Group_</t>
+  </si>
+  <si>
+    <t>Group_ </t>
+  </si>
+  <si>
+    <t>ExpBio</t>
+  </si>
+  <si>
+    <t>ExpBio </t>
+  </si>
+  <si>
+    <t>date_</t>
+  </si>
+  <si>
+    <t>esriFieldTypeDate</t>
+  </si>
+  <si>
+    <t>date_ </t>
+  </si>
+  <si>
+    <t>Common_name</t>
+  </si>
+  <si>
+    <t>Common_name </t>
+  </si>
+  <si>
+    <t>CoastalClass</t>
+  </si>
+  <si>
+    <t>esriFieldTypeSmallInteger</t>
+  </si>
+  <si>
+    <t>CoastalClass </t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Fields:</t>
+  </si>
+  <si>
+    <t>records</t>
+  </si>
+  <si>
+    <t>vw_StationPoints_Species </t>
+  </si>
+  <si>
+    <t>vw_StationSpecies </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PSMFC tables:  NOAA tables also have </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>abun</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>abundance </t>
+  </si>
+  <si>
+    <t>abundance</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[ no </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>abundance</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field ]</t>
+    </r>
+  </si>
+  <si>
+    <t>BiobandCode </t>
+  </si>
+  <si>
+    <t>BiobandCode</t>
+  </si>
+  <si>
+    <t>BiobandName </t>
+  </si>
+  <si>
+    <t>BiobandName</t>
+  </si>
+  <si>
+    <t>BiobandDescription </t>
+  </si>
+  <si>
+    <t>BiobandDescription</t>
+  </si>
+  <si>
+    <t>ESRI_OID </t>
+  </si>
+  <si>
+    <t>ESRI_OID</t>
+  </si>
+  <si>
+    <t>BandOrder </t>
+  </si>
+  <si>
+    <t>BandOrder</t>
+  </si>
+  <si>
+    <t>vw_StationPoints_BiobandsSpecies </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">fix </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>vw_StationPoints_BiobandsSpecies</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> table</t>
+    </r>
+  </si>
+  <si>
+    <t>species split out to all biobands</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="34">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1033,7 +1469,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1041,12 +1477,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1064,17 +1494,93 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="9.8000000000000007"/>
       <color rgb="FF067D17"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1160,81 +1666,82 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1246,7 +1753,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="7"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="7"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1262,7 +1769,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1271,19 +1778,40 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="8" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Heading 2" xfId="7" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1292,6 +1820,7 @@
     <cellStyle name="Normal 3" xfId="3" xr:uid="{33E71147-3CE4-45CE-8876-5FF661A1EB4E}"/>
     <cellStyle name="Normal 4" xfId="5" xr:uid="{F641EBF2-1CDA-425E-B5C3-517AF90F4C7A}"/>
     <cellStyle name="Normal 5" xfId="6" xr:uid="{9FC96886-235B-415D-910B-05AF22994145}"/>
+    <cellStyle name="Normal 6" xfId="8" xr:uid="{781E0154-589F-43E9-8A42-FC321BEEB6B8}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1586,6 +2115,55 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6142788</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>104594</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE3345D0-75ED-4F04-9097-BD98E65A35D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="6667500"/>
+          <a:ext cx="6695238" cy="1447619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -1594,7 +2172,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1723224</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>75975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1631,7 +2209,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1683,6 +2261,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5161905" cy="723810"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BE7AA84-411E-41A8-9AF9-D359244A1A12}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5161905" cy="723810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2051,13 +2673,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J440"/>
+  <dimension ref="A1:J441"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C81" sqref="C81"/>
+      <selection pane="bottomRight" activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2987,43 +3609,52 @@
         <v>161</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="34.5" hidden="1" customHeight="1">
-      <c r="A82" s="6" t="s">
+    <row r="81" spans="1:9" ht="15.75">
+      <c r="C81" s="36"/>
+      <c r="D81" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="I81" s="11" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="34.5" hidden="1" customHeight="1">
+      <c r="A83" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D82" s="33" t="s">
+      <c r="D83" s="33" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="24.95" customHeight="1">
-      <c r="D83" s="9" t="s">
+    <row r="84" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D84" s="9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="32.25" hidden="1" thickBot="1">
-      <c r="C84" s="2" t="s">
+    <row r="85" spans="1:9" ht="32.25" hidden="1" thickBot="1">
+      <c r="C85" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D84" s="32" t="s">
+      <c r="D85" s="32" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="24.95" customHeight="1">
-      <c r="D85" s="26" t="s">
+    <row r="86" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D86" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="I85" s="11" t="s">
+      <c r="I86" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="440" spans="1:10" ht="15.75" hidden="1">
-      <c r="A440" s="2" t="s">
+    <row r="441" spans="1:10" ht="15.75" hidden="1">
+      <c r="A441" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="J440" s="6"/>
+      <c r="J441" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I440" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
+  <autoFilter ref="A1:I441" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
@@ -3044,6 +3675,230 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFDF36D1-DE2E-478E-8F20-00E572A1B869}">
+  <dimension ref="B1:E44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="83.875" customWidth="1"/>
+    <col min="3" max="3" width="4.375" customWidth="1"/>
+    <col min="5" max="5" width="30.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5">
+      <c r="B1" s="57" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" ht="31.5">
+      <c r="B2" s="49" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="18.75">
+      <c r="B7" s="43" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="26.25">
+      <c r="B15" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="12" customHeight="1">
+      <c r="B16" s="46" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="12" customHeight="1">
+      <c r="B17" s="45"/>
+    </row>
+    <row r="18" spans="2:5" ht="12" customHeight="1">
+      <c r="B18" s="45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="12" customHeight="1">
+      <c r="B19" s="45" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="12" customHeight="1">
+      <c r="B20" s="45" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="12" customHeight="1">
+      <c r="B21" s="45" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="12" customHeight="1">
+      <c r="B22" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="E22" s="44" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="12" customHeight="1">
+      <c r="B23" s="45" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="12" customHeight="1">
+      <c r="B24" s="45" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="12" customHeight="1">
+      <c r="B25" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="E25" s="38" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="12" customHeight="1">
+      <c r="B26" s="45" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="12" customHeight="1">
+      <c r="B27" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="E27" s="38" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="12" customHeight="1">
+      <c r="B28" s="45" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="12" customHeight="1">
+      <c r="B29" s="45" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="12" customHeight="1">
+      <c r="B30" s="45"/>
+    </row>
+    <row r="31" spans="2:5" ht="12" customHeight="1">
+      <c r="B31" s="46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="12" customHeight="1">
+      <c r="B32" s="45"/>
+    </row>
+    <row r="33" spans="2:2" ht="12" customHeight="1">
+      <c r="B33" s="45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" ht="12" customHeight="1">
+      <c r="B34" s="45" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" ht="12" customHeight="1">
+      <c r="B35" s="45" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" ht="12" customHeight="1">
+      <c r="B36" s="45" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" ht="12" customHeight="1">
+      <c r="B37" s="45" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" ht="12" customHeight="1">
+      <c r="B38" s="45" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" ht="12" customHeight="1">
+      <c r="B39" s="45" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" ht="12" customHeight="1">
+      <c r="B40" s="45" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" ht="12" customHeight="1">
+      <c r="B41" s="45" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" ht="12" customHeight="1">
+      <c r="B42" s="45" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" ht="12" customHeight="1">
+      <c r="B43" s="45" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" ht="12" customHeight="1">
+      <c r="B44" s="45" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" location="//02ss0000000r000000" xr:uid="{FE3FE263-21A4-4264-8B41-7F0895BE4A6F}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{CABDCE2D-23BE-454B-A9E0-2326878E3F45}"/>
+    <hyperlink ref="E25" r:id="rId3" xr:uid="{9B7A1DB2-D1ED-46DC-817E-A567BE3AC29B}"/>
+    <hyperlink ref="E27" r:id="rId4" xr:uid="{F3619D6A-BCA7-44B6-8614-FAD60D558E0E}"/>
+    <hyperlink ref="E2" r:id="rId5" xr:uid="{72EC7B0B-3160-43E4-8583-453DC2293ED5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+  <drawing r:id="rId7"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8A68F0-A5CC-4F2B-9E7A-D47D3E46C475}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J435"/>
@@ -3124,7 +3979,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:10" customFormat="1" ht="15.75">
+    <row r="5" spans="1:10" customFormat="1" ht="15.75" hidden="1">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="34">
@@ -6594,7 +7449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3521A2-0E46-4626-A556-F81B8258D1DB}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6609,7 +7464,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D90DEFD-D6A8-4BFB-97A2-600F5E7E4446}">
   <dimension ref="B2:C12"/>
   <sheetViews>
@@ -6683,12 +7538,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392EF631-8DBE-4581-9410-4CF72B20CF9A}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -6722,7 +7577,7 @@
         <v>44035</v>
       </c>
       <c r="C4" s="38" t="str">
-        <f>HYPERLINK($A$1&amp;A4)</f>
+        <f t="shared" ref="C4:C9" si="0">HYPERLINK($A$1&amp;A4)</f>
         <v>https://alaskafisheries.noaa.gov/mapping/shorezonedata/carrymap/FishAtlas_v2020.mpk</v>
       </c>
     </row>
@@ -6734,7 +7589,7 @@
         <v>44035</v>
       </c>
       <c r="C5" s="38" t="str">
-        <f>HYPERLINK($A$1&amp;A5)</f>
+        <f t="shared" si="0"/>
         <v>https://alaskafisheries.noaa.gov/mapping/shorezonedata/carrymap/ShoreStation2019_2020_0723.mpk</v>
       </c>
     </row>
@@ -6746,7 +7601,7 @@
         <v>44020</v>
       </c>
       <c r="C6" s="38" t="str">
-        <f>HYPERLINK($A$1&amp;A6)</f>
+        <f t="shared" si="0"/>
         <v>https://alaskafisheries.noaa.gov/mapping/shorezonedata/carrymap/FishAtlas_wViews_2020_0708.mpk</v>
       </c>
     </row>
@@ -6758,7 +7613,7 @@
         <v>43864</v>
       </c>
       <c r="C7" s="38" t="str">
-        <f>HYPERLINK($A$1&amp;A7)</f>
+        <f t="shared" si="0"/>
         <v>https://alaskafisheries.noaa.gov/mapping/shorezonedata/carrymap/Ports_SSL.mpk</v>
       </c>
     </row>
@@ -6770,7 +7625,7 @@
         <v>43838</v>
       </c>
       <c r="C8" s="38" t="str">
-        <f>HYPERLINK($A$1&amp;A8)</f>
+        <f t="shared" si="0"/>
         <v>https://alaskafisheries.noaa.gov/mapping/shorezonedata/carrymap/ShoreZone.mpk</v>
       </c>
     </row>
@@ -6782,7 +7637,7 @@
         <v>43555</v>
       </c>
       <c r="C9" s="38" t="str">
-        <f>HYPERLINK($A$1&amp;A9)</f>
+        <f t="shared" si="0"/>
         <v>https://alaskafisheries.noaa.gov/mapping/shorezonedata/carrymap/ShoreZoneFlexMapService_2019_0331.mpk</v>
       </c>
     </row>
@@ -6795,4 +7650,828 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073BA0C8-793A-470F-9811-FE4A219663BF}">
+  <dimension ref="A1:N36"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.625" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.625" style="50" customWidth="1"/>
+    <col min="3" max="3" width="14.875" style="50" customWidth="1"/>
+    <col min="4" max="5" width="9" style="50"/>
+    <col min="6" max="6" width="28.25" style="50" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.625" style="50" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.25" style="50" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9" style="50"/>
+    <col min="11" max="11" width="16.625" style="50" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.625" style="50" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.25" style="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="50"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75">
+      <c r="F1" s="56" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="55" customFormat="1" ht="18.75">
+      <c r="A7" s="55" t="s">
+        <v>260</v>
+      </c>
+      <c r="F7" s="55" t="s">
+        <v>259</v>
+      </c>
+      <c r="K7" s="55" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="54">
+        <v>16099</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>258</v>
+      </c>
+      <c r="F8" s="54">
+        <v>16099</v>
+      </c>
+      <c r="G8" s="53" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="52"/>
+    </row>
+    <row r="10" spans="1:14" s="51" customFormat="1">
+      <c r="A10" s="51" t="s">
+        <v>257</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" s="51" t="s">
+        <v>255</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>254</v>
+      </c>
+      <c r="F10" s="51" t="s">
+        <v>257</v>
+      </c>
+      <c r="G10" s="51" t="s">
+        <v>256</v>
+      </c>
+      <c r="H10" s="51" t="s">
+        <v>255</v>
+      </c>
+      <c r="I10" s="51" t="s">
+        <v>254</v>
+      </c>
+      <c r="K10" s="51" t="s">
+        <v>257</v>
+      </c>
+      <c r="L10" s="51" t="s">
+        <v>256</v>
+      </c>
+      <c r="M10" s="51" t="s">
+        <v>255</v>
+      </c>
+      <c r="N10" s="51" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="51"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="F11" s="50" t="s">
+        <v>253</v>
+      </c>
+      <c r="G11" s="50" t="s">
+        <v>252</v>
+      </c>
+      <c r="H11" s="50" t="s">
+        <v>251</v>
+      </c>
+      <c r="K11" s="50" t="s">
+        <v>253</v>
+      </c>
+      <c r="L11" s="50" t="s">
+        <v>252</v>
+      </c>
+      <c r="M11" s="50" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="50" t="s">
+        <v>250</v>
+      </c>
+      <c r="B12" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>249</v>
+      </c>
+      <c r="D12" s="50">
+        <v>255</v>
+      </c>
+      <c r="F12" s="50" t="s">
+        <v>250</v>
+      </c>
+      <c r="G12" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="H12" s="50" t="s">
+        <v>249</v>
+      </c>
+      <c r="I12" s="50">
+        <v>255</v>
+      </c>
+      <c r="K12" s="50" t="s">
+        <v>250</v>
+      </c>
+      <c r="L12" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M12" s="50" t="s">
+        <v>249</v>
+      </c>
+      <c r="N12" s="50">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="F13" s="50" t="s">
+        <v>248</v>
+      </c>
+      <c r="G13" s="50" t="s">
+        <v>247</v>
+      </c>
+      <c r="H13" s="50" t="s">
+        <v>246</v>
+      </c>
+      <c r="I13" s="50">
+        <v>8</v>
+      </c>
+      <c r="K13" s="50" t="s">
+        <v>248</v>
+      </c>
+      <c r="L13" s="50" t="s">
+        <v>247</v>
+      </c>
+      <c r="M13" s="50" t="s">
+        <v>246</v>
+      </c>
+      <c r="N13" s="50">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="F14" s="50" t="s">
+        <v>245</v>
+      </c>
+      <c r="G14" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="H14" s="50" t="s">
+        <v>244</v>
+      </c>
+      <c r="I14" s="50">
+        <v>2</v>
+      </c>
+      <c r="K14" s="50" t="s">
+        <v>245</v>
+      </c>
+      <c r="L14" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M14" s="50" t="s">
+        <v>244</v>
+      </c>
+      <c r="N14" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="B15" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>242</v>
+      </c>
+      <c r="D15" s="50">
+        <v>255</v>
+      </c>
+      <c r="F15" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="G15" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="H15" s="50" t="s">
+        <v>242</v>
+      </c>
+      <c r="I15" s="50">
+        <v>255</v>
+      </c>
+      <c r="K15" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="L15" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M15" s="50" t="s">
+        <v>242</v>
+      </c>
+      <c r="N15" s="50">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="50" t="s">
+        <v>241</v>
+      </c>
+      <c r="B16" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>240</v>
+      </c>
+      <c r="F16" s="50" t="s">
+        <v>241</v>
+      </c>
+      <c r="G16" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="H16" s="50" t="s">
+        <v>240</v>
+      </c>
+      <c r="K16" s="50" t="s">
+        <v>241</v>
+      </c>
+      <c r="L16" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="M16" s="50" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="F17" s="50" t="s">
+        <v>239</v>
+      </c>
+      <c r="G17" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="H17" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="I17" s="50">
+        <v>5</v>
+      </c>
+      <c r="K17" s="50" t="s">
+        <v>239</v>
+      </c>
+      <c r="L17" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M17" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="N17" s="50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="F18" s="50" t="s">
+        <v>237</v>
+      </c>
+      <c r="G18" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="H18" s="50" t="s">
+        <v>236</v>
+      </c>
+      <c r="I18" s="50">
+        <v>5</v>
+      </c>
+      <c r="K18" s="50" t="s">
+        <v>237</v>
+      </c>
+      <c r="L18" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M18" s="50" t="s">
+        <v>236</v>
+      </c>
+      <c r="N18" s="50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="F19" s="50" t="s">
+        <v>235</v>
+      </c>
+      <c r="G19" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="H19" s="50" t="s">
+        <v>234</v>
+      </c>
+      <c r="I19" s="50">
+        <v>5</v>
+      </c>
+      <c r="K19" s="50" t="s">
+        <v>235</v>
+      </c>
+      <c r="L19" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M19" s="50" t="s">
+        <v>234</v>
+      </c>
+      <c r="N19" s="50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="F20" s="50" t="s">
+        <v>233</v>
+      </c>
+      <c r="G20" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="H20" s="50" t="s">
+        <v>232</v>
+      </c>
+      <c r="I20" s="50">
+        <v>150</v>
+      </c>
+      <c r="K20" s="50" t="s">
+        <v>233</v>
+      </c>
+      <c r="L20" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M20" s="50" t="s">
+        <v>232</v>
+      </c>
+      <c r="N20" s="50">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="50" t="s">
+        <v>231</v>
+      </c>
+      <c r="B21" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>229</v>
+      </c>
+      <c r="F21" s="50" t="s">
+        <v>231</v>
+      </c>
+      <c r="G21" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="H21" s="50" t="s">
+        <v>229</v>
+      </c>
+      <c r="K21" s="50" t="s">
+        <v>271</v>
+      </c>
+      <c r="L21" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="M21" s="50" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="F22" s="50" t="s">
+        <v>228</v>
+      </c>
+      <c r="G22" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="H22" s="50" t="s">
+        <v>227</v>
+      </c>
+      <c r="I22" s="50">
+        <v>25</v>
+      </c>
+      <c r="K22" s="50" t="s">
+        <v>228</v>
+      </c>
+      <c r="L22" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M22" s="50" t="s">
+        <v>227</v>
+      </c>
+      <c r="N22" s="50">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="F23" s="50" t="s">
+        <v>226</v>
+      </c>
+      <c r="G23" s="50" t="s">
+        <v>225</v>
+      </c>
+      <c r="H23" s="50" t="s">
+        <v>224</v>
+      </c>
+      <c r="K23" s="50" t="s">
+        <v>226</v>
+      </c>
+      <c r="L23" s="50" t="s">
+        <v>225</v>
+      </c>
+      <c r="M23" s="50" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="50" t="s">
+        <v>223</v>
+      </c>
+      <c r="B24" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>221</v>
+      </c>
+      <c r="F24" s="50" t="s">
+        <v>223</v>
+      </c>
+      <c r="G24" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="H24" s="50" t="s">
+        <v>221</v>
+      </c>
+      <c r="K24" s="50" t="s">
+        <v>223</v>
+      </c>
+      <c r="L24" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="M24" s="50" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="B25" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="C25" s="50" t="s">
+        <v>219</v>
+      </c>
+      <c r="D25" s="50">
+        <v>255</v>
+      </c>
+      <c r="F25" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="G25" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="H25" s="50" t="s">
+        <v>219</v>
+      </c>
+      <c r="I25" s="50">
+        <v>255</v>
+      </c>
+      <c r="K25" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="L25" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M25" s="50" t="s">
+        <v>219</v>
+      </c>
+      <c r="N25" s="50">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="B26" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="C26" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="D26" s="50">
+        <v>801</v>
+      </c>
+      <c r="F26" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="G26" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="H26" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="I26" s="50">
+        <v>801</v>
+      </c>
+      <c r="K26" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="L26" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M26" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="N26" s="50">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="B27" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="C27" s="50" t="s">
+        <v>215</v>
+      </c>
+      <c r="D27" s="50">
+        <v>255</v>
+      </c>
+      <c r="F27" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="G27" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="H27" s="50" t="s">
+        <v>215</v>
+      </c>
+      <c r="I27" s="50">
+        <v>255</v>
+      </c>
+      <c r="K27" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="L27" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M27" s="50" t="s">
+        <v>215</v>
+      </c>
+      <c r="N27" s="50">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="B28" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="C28" s="50" t="s">
+        <v>213</v>
+      </c>
+      <c r="D28" s="50">
+        <v>12</v>
+      </c>
+      <c r="F28" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="G28" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="H28" s="50" t="s">
+        <v>213</v>
+      </c>
+      <c r="I28" s="50">
+        <v>12</v>
+      </c>
+      <c r="K28" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="L28" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M28" s="50" t="s">
+        <v>213</v>
+      </c>
+      <c r="N28" s="50">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="50" t="s">
+        <v>212</v>
+      </c>
+      <c r="B29" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="C29" s="50" t="s">
+        <v>211</v>
+      </c>
+      <c r="F29" s="50" t="s">
+        <v>212</v>
+      </c>
+      <c r="G29" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="H29" s="50" t="s">
+        <v>211</v>
+      </c>
+      <c r="K29" s="50" t="s">
+        <v>212</v>
+      </c>
+      <c r="L29" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="M29" s="50" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="50" t="s">
+        <v>210</v>
+      </c>
+      <c r="B30" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="C30" s="50" t="s">
+        <v>208</v>
+      </c>
+      <c r="D30" s="50">
+        <v>255</v>
+      </c>
+      <c r="F30" s="50" t="s">
+        <v>210</v>
+      </c>
+      <c r="G30" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="H30" s="50" t="s">
+        <v>208</v>
+      </c>
+      <c r="I30" s="50">
+        <v>255</v>
+      </c>
+      <c r="K30" s="50" t="s">
+        <v>210</v>
+      </c>
+      <c r="L30" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M30" s="50" t="s">
+        <v>208</v>
+      </c>
+      <c r="N30" s="50">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="B31" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="C31" s="50" t="s">
+        <v>205</v>
+      </c>
+      <c r="F31" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="G31" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="H31" s="50" t="s">
+        <v>205</v>
+      </c>
+      <c r="K31" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="L31" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="M31" s="50" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="58" t="s">
+        <v>262</v>
+      </c>
+      <c r="B32" s="58" t="s">
+        <v>209</v>
+      </c>
+      <c r="C32" s="58" t="s">
+        <v>263</v>
+      </c>
+      <c r="D32" s="50">
+        <v>1</v>
+      </c>
+      <c r="F32" s="59" t="s">
+        <v>264</v>
+      </c>
+      <c r="K32" s="50" t="s">
+        <v>262</v>
+      </c>
+      <c r="L32" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M32" s="50" t="s">
+        <v>263</v>
+      </c>
+      <c r="N32" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="11:14">
+      <c r="K33" s="50" t="s">
+        <v>273</v>
+      </c>
+      <c r="L33" s="50" t="s">
+        <v>252</v>
+      </c>
+      <c r="M33" s="50" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="34" spans="11:14">
+      <c r="K34" s="50" t="s">
+        <v>265</v>
+      </c>
+      <c r="L34" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M34" s="50" t="s">
+        <v>266</v>
+      </c>
+      <c r="N34" s="50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="11:14">
+      <c r="K35" s="50" t="s">
+        <v>269</v>
+      </c>
+      <c r="L35" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M35" s="50" t="s">
+        <v>270</v>
+      </c>
+      <c r="N35" s="50">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="36" spans="11:14">
+      <c r="K36" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="L36" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="M36" s="50" t="s">
+        <v>268</v>
+      </c>
+      <c r="N36" s="50">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K11:N31">
+    <sortCondition ref="K11:K31"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix ShoreStations Species query panel issue, start on data download issue.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D257B1BA-7BF8-46CA-8494-84C1E9B88756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA72A75-5B9E-430C-94EB-ED742C3D8E29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5205" yWindow="45" windowWidth="23430" windowHeight="15555" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="5205" yWindow="45" windowWidth="23430" windowHeight="15555" tabRatio="736" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -23,9 +23,9 @@
     <sheet name="Sp_BB tables" sheetId="19" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'MPK download'!$A$3:$C$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$441</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$442</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'to do - SS'!$A$1:$I$435</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -139,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="280">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -1319,12 +1319,18 @@
   <si>
     <t>species split out to all biobands</t>
   </si>
+  <si>
+    <t>fix GP</t>
+  </si>
+  <si>
+    <t>July 2020?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="34">
+  <fonts count="35">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1582,6 +1588,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1677,7 +1691,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1810,6 +1824,9 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Heading 2" xfId="7" builtinId="17"/>
@@ -1848,13 +1865,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>203201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>4791076</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1892,13 +1909,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>538480</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>695326</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1936,13 +1953,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>215901</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>1694816</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1980,13 +1997,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>863600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2024,13 +2041,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>424180</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>1899286</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2068,13 +2085,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>101601</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>308610</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>2012316</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2605,10 +2622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2BFB56-BD70-FD45-AC33-49638CF763A3}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="21"/>
@@ -2624,62 +2641,72 @@
     </row>
     <row r="3" spans="1:2" ht="23.25">
       <c r="A3" s="22">
+        <v>4.16</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="23.25">
+      <c r="A7" s="22">
         <v>4.13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="408.95" customHeight="1">
-      <c r="B4" s="23" t="s">
+    <row r="8" spans="1:2" ht="408.95" customHeight="1">
+      <c r="B8" s="23" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="72" customHeight="1"/>
-    <row r="6" spans="1:2" ht="144" customHeight="1">
-      <c r="B6" s="23" t="s">
+    <row r="9" spans="1:2" ht="72" customHeight="1"/>
+    <row r="10" spans="1:2" ht="144" customHeight="1">
+      <c r="B10" s="23" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="398.1" customHeight="1">
-      <c r="B7" s="23" t="s">
+    <row r="11" spans="1:2" ht="398.1" customHeight="1">
+      <c r="B11" s="23" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.25">
-      <c r="A8" s="22">
+    <row r="12" spans="1:2" ht="23.25">
+      <c r="A12" s="22">
         <v>4.12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="75.95" customHeight="1">
-      <c r="B9" s="23" t="s">
+    <row r="13" spans="1:2" ht="75.95" customHeight="1">
+      <c r="B13" s="23" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="408.95" customHeight="1">
-      <c r="B10" s="23" t="s">
+    <row r="14" spans="1:2" ht="408.95" customHeight="1">
+      <c r="B14" s="23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="177" customHeight="1"/>
-    <row r="12" spans="1:2" ht="185.1" customHeight="1"/>
+    <row r="15" spans="1:2" ht="177" customHeight="1"/>
+    <row r="16" spans="1:2" ht="185.1" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://developers.arcgis.com/javascript/latest/guide/release-notes/" xr:uid="{9B90A93B-81C7-0348-B902-045AB450F6B0}"/>
-    <hyperlink ref="A8" r:id="rId2" display="https://developers.arcgis.com/javascript/latest/guide/4.12/index.html" xr:uid="{61356492-1618-A948-A250-8B62E3FA344C}"/>
+    <hyperlink ref="A7" r:id="rId1" display="https://developers.arcgis.com/javascript/latest/guide/4.13/index.html" xr:uid="{9B90A93B-81C7-0348-B902-045AB450F6B0}"/>
+    <hyperlink ref="A12" r:id="rId2" display="https://developers.arcgis.com/javascript/latest/guide/4.12/index.html" xr:uid="{61356492-1618-A948-A250-8B62E3FA344C}"/>
+    <hyperlink ref="A3" r:id="rId3" display="https://developers.arcgis.com/javascript/latest/guide/release-notes/" xr:uid="{74479A76-EC03-4AE1-AD61-B66E1A0897BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J441"/>
+  <dimension ref="A1:J442"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D81" sqref="D81"/>
+      <selection pane="bottomRight" activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -3584,8 +3611,10 @@
       </c>
       <c r="G77" s="19"/>
     </row>
-    <row r="78" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="C78" s="36"/>
+    <row r="78" spans="1:10" ht="20.100000000000001" hidden="1" customHeight="1">
+      <c r="C78" s="36">
+        <v>44064</v>
+      </c>
       <c r="D78" s="9" t="s">
         <v>159</v>
       </c>
@@ -3618,43 +3647,49 @@
         <v>277</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="34.5" hidden="1" customHeight="1">
-      <c r="A83" s="6" t="s">
+    <row r="82" spans="1:9" ht="18.75">
+      <c r="C82" s="36"/>
+      <c r="D82" s="60" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="34.5" hidden="1" customHeight="1">
+      <c r="A84" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D83" s="33" t="s">
+      <c r="D84" s="33" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="24.95" customHeight="1">
-      <c r="D84" s="9" t="s">
+    <row r="85" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D85" s="9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="32.25" hidden="1" thickBot="1">
-      <c r="C85" s="2" t="s">
+    <row r="86" spans="1:9" ht="32.25" hidden="1" thickBot="1">
+      <c r="C86" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D85" s="32" t="s">
+      <c r="D86" s="32" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="24.95" customHeight="1">
-      <c r="D86" s="26" t="s">
+    <row r="87" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D87" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="I86" s="11" t="s">
+      <c r="I87" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="441" spans="1:10" ht="15.75" hidden="1">
-      <c r="A441" s="2" t="s">
+    <row r="442" spans="1:10" ht="15.75" hidden="1">
+      <c r="A442" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="J441" s="6"/>
+      <c r="J442" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I441" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
+  <autoFilter ref="A1:I442" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Skip refresh on minor extent change or when file downloads bar appears/disappears. Clean up data download code.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA72A75-5B9E-430C-94EB-ED742C3D8E29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14E391C-887D-44A0-8E0B-1C54BF4B1BF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5205" yWindow="45" windowWidth="23430" windowHeight="15555" tabRatio="736" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="2805" yWindow="135" windowWidth="11790" windowHeight="15555" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
-    <sheet name="to do" sheetId="1" r:id="rId2"/>
-    <sheet name="Statistical queries" sheetId="18" r:id="rId3"/>
-    <sheet name="to do - SS" sheetId="16" r:id="rId4"/>
-    <sheet name="SZ point regeneration rethink" sheetId="14" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="15" r:id="rId6"/>
-    <sheet name="MPK download" sheetId="17" r:id="rId7"/>
-    <sheet name="Sp_BB tables" sheetId="19" r:id="rId8"/>
+    <sheet name="browser heights" sheetId="20" r:id="rId2"/>
+    <sheet name="to do" sheetId="1" r:id="rId3"/>
+    <sheet name="Statistical queries" sheetId="18" r:id="rId4"/>
+    <sheet name="to do - SS" sheetId="16" r:id="rId5"/>
+    <sheet name="SZ point regeneration rethink" sheetId="14" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId7"/>
+    <sheet name="MPK download" sheetId="17" r:id="rId8"/>
+    <sheet name="Sp_BB tables" sheetId="19" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'MPK download'!$A$3:$C$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$442</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'to do - SS'!$A$1:$I$435</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'MPK download'!$A$3:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'to do'!$A$1:$I$442</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'to do - SS'!$A$1:$I$435</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -139,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="284">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -1325,14 +1326,33 @@
   <si>
     <t>July 2020?</t>
   </si>
+  <si>
+    <t>download bar closed, window maximized</t>
+  </si>
+  <si>
+    <t>download bar closed</t>
+  </si>
+  <si>
+    <t>JetBrains debugging bar closed</t>
+  </si>
+  <si>
+    <t>window maximized</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="35">
+  <fonts count="36">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1680,82 +1700,83 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1767,7 +1788,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="7"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="7"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1783,52 +1804,56 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="8"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="8" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="8" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="8" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="Heading 2" xfId="7" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1838,6 +1863,7 @@
     <cellStyle name="Normal 4" xfId="5" xr:uid="{F641EBF2-1CDA-425E-B5C3-517AF90F4C7A}"/>
     <cellStyle name="Normal 5" xfId="6" xr:uid="{9FC96886-235B-415D-910B-05AF22994145}"/>
     <cellStyle name="Normal 6" xfId="8" xr:uid="{781E0154-589F-43E9-8A42-FC321BEEB6B8}"/>
+    <cellStyle name="Normal 7" xfId="9" xr:uid="{FFCA2E3A-85FA-46D9-AFDD-5663A69045BD}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2624,7 +2650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2BFB56-BD70-FD45-AC33-49638CF763A3}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -2698,6 +2724,134 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD2386D-2AF1-4B5F-9842-EBCA886CA8B5}">
+  <dimension ref="B3:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="5" width="9" style="61"/>
+    <col min="6" max="6" width="25.125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="61"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7">
+      <c r="B3" s="61">
+        <v>994</v>
+      </c>
+      <c r="C3" s="61">
+        <v>776</v>
+      </c>
+      <c r="D3" s="61">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="61">
+        <v>1040</v>
+      </c>
+      <c r="C4" s="61">
+        <v>839</v>
+      </c>
+      <c r="D4" s="61">
+        <v>201</v>
+      </c>
+      <c r="F4" s="61" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="61">
+        <v>849</v>
+      </c>
+      <c r="C5" s="61">
+        <v>631</v>
+      </c>
+      <c r="D5" s="61">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="61">
+        <v>480</v>
+      </c>
+      <c r="C6" s="61">
+        <v>262</v>
+      </c>
+      <c r="D6" s="61">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="61">
+        <v>480</v>
+      </c>
+      <c r="C8" s="61">
+        <v>311</v>
+      </c>
+      <c r="D8" s="61">
+        <v>169</v>
+      </c>
+      <c r="F8" s="61" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="61">
+        <v>480</v>
+      </c>
+      <c r="C9" s="61">
+        <v>311</v>
+      </c>
+      <c r="D9" s="61">
+        <v>169</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>281</v>
+      </c>
+      <c r="G9" s="61">
+        <f>D6-D9</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="30">
+      <c r="B10" s="61">
+        <v>1040</v>
+      </c>
+      <c r="C10" s="61">
+        <v>888</v>
+      </c>
+      <c r="D10" s="61">
+        <v>152</v>
+      </c>
+      <c r="F10" s="62" t="s">
+        <v>280</v>
+      </c>
+      <c r="G10" s="61">
+        <f>D4-D10</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="61">
+        <v>774</v>
+      </c>
+      <c r="C13" s="61">
+        <v>605</v>
+      </c>
+      <c r="D13" s="61">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:J442"/>
@@ -3709,7 +3863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFDF36D1-DE2E-478E-8F20-00E572A1B869}">
   <dimension ref="B1:E44"/>
   <sheetViews>
@@ -3933,7 +4087,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8A68F0-A5CC-4F2B-9E7A-D47D3E46C475}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J435"/>
@@ -7484,7 +7638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3521A2-0E46-4626-A556-F81B8258D1DB}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -7499,7 +7653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D90DEFD-D6A8-4BFB-97A2-600F5E7E4446}">
   <dimension ref="B2:C12"/>
   <sheetViews>
@@ -7573,7 +7727,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392EF631-8DBE-4581-9410-4CF72B20CF9A}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -7687,7 +7841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073BA0C8-793A-470F-9811-FE4A219663BF}">
   <dimension ref="A1:N36"/>
   <sheetViews>

</xml_diff>

<commit_message>
Show CoastalClass description in Shore Stations tables.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,26 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14E391C-887D-44A0-8E0B-1C54BF4B1BF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13A37FB-B6A5-420D-9CD5-FB25FA64E347}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2805" yWindow="135" windowWidth="11790" windowHeight="15555" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="3510" yWindow="750" windowWidth="24750" windowHeight="14145" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
-    <sheet name="browser heights" sheetId="20" r:id="rId2"/>
-    <sheet name="to do" sheetId="1" r:id="rId3"/>
-    <sheet name="Statistical queries" sheetId="18" r:id="rId4"/>
-    <sheet name="to do - SS" sheetId="16" r:id="rId5"/>
-    <sheet name="SZ point regeneration rethink" sheetId="14" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="15" r:id="rId7"/>
-    <sheet name="MPK download" sheetId="17" r:id="rId8"/>
-    <sheet name="Sp_BB tables" sheetId="19" r:id="rId9"/>
+    <sheet name="to do" sheetId="1" r:id="rId2"/>
+    <sheet name="Statistical queries" sheetId="18" r:id="rId3"/>
+    <sheet name="to do - SS" sheetId="16" r:id="rId4"/>
+    <sheet name="SZ point regeneration rethink" sheetId="14" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId6"/>
+    <sheet name="MPK download" sheetId="17" r:id="rId7"/>
+    <sheet name="Sp_BB tables" sheetId="19" r:id="rId8"/>
+    <sheet name="browser heights" sheetId="20" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'MPK download'!$A$3:$C$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'to do'!$A$1:$I$442</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'to do - SS'!$A$1:$I$435</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'MPK download'!$A$3:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$443</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'to do - SS'!$A$1:$I$435</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="287">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -742,9 +742,6 @@
     <t>get table back after previous query returns no rows</t>
   </si>
   <si>
-    <t>Update to 4.15 API</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Use </t>
     </r>
@@ -1337,6 +1334,18 @@
   </si>
   <si>
     <t>window maximized</t>
+  </si>
+  <si>
+    <t>fix 1-day date discerpancies in Station tables</t>
+  </si>
+  <si>
+    <t>JS Date() issue with SQL Server date values</t>
+  </si>
+  <si>
+    <t>Update to 4.16 API</t>
+  </si>
+  <si>
+    <t>long values for SS Coastal Class values</t>
   </si>
 </sst>
 </file>
@@ -2670,7 +2679,7 @@
         <v>4.16</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="23.25">
@@ -2724,143 +2733,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD2386D-2AF1-4B5F-9842-EBCA886CA8B5}">
-  <dimension ref="B3:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
+  <sheetPr codeName="Sheet1" filterMode="1"/>
+  <dimension ref="A1:J443"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="5" width="9" style="61"/>
-    <col min="6" max="6" width="25.125" style="61" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="61"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:7">
-      <c r="B3" s="61">
-        <v>994</v>
-      </c>
-      <c r="C3" s="61">
-        <v>776</v>
-      </c>
-      <c r="D3" s="61">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7">
-      <c r="B4" s="61">
-        <v>1040</v>
-      </c>
-      <c r="C4" s="61">
-        <v>839</v>
-      </c>
-      <c r="D4" s="61">
-        <v>201</v>
-      </c>
-      <c r="F4" s="61" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="61">
-        <v>849</v>
-      </c>
-      <c r="C5" s="61">
-        <v>631</v>
-      </c>
-      <c r="D5" s="61">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7">
-      <c r="B6" s="61">
-        <v>480</v>
-      </c>
-      <c r="C6" s="61">
-        <v>262</v>
-      </c>
-      <c r="D6" s="61">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="61">
-        <v>480</v>
-      </c>
-      <c r="C8" s="61">
-        <v>311</v>
-      </c>
-      <c r="D8" s="61">
-        <v>169</v>
-      </c>
-      <c r="F8" s="61" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="61">
-        <v>480</v>
-      </c>
-      <c r="C9" s="61">
-        <v>311</v>
-      </c>
-      <c r="D9" s="61">
-        <v>169</v>
-      </c>
-      <c r="F9" s="61" t="s">
-        <v>281</v>
-      </c>
-      <c r="G9" s="61">
-        <f>D6-D9</f>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="30">
-      <c r="B10" s="61">
-        <v>1040</v>
-      </c>
-      <c r="C10" s="61">
-        <v>888</v>
-      </c>
-      <c r="D10" s="61">
-        <v>152</v>
-      </c>
-      <c r="F10" s="62" t="s">
-        <v>280</v>
-      </c>
-      <c r="G10" s="61">
-        <f>D4-D10</f>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="61">
-        <v>774</v>
-      </c>
-      <c r="C13" s="61">
-        <v>605</v>
-      </c>
-      <c r="D13" s="61">
-        <v>169</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
-  <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J442"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D82" sqref="D82"/>
+      <selection pane="bottomRight" activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -3675,7 +3556,7 @@
     </row>
     <row r="67" spans="1:10" ht="24.95" customHeight="1">
       <c r="D67" s="33" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J67" s="6"/>
     </row>
@@ -3691,7 +3572,7 @@
     </row>
     <row r="70" spans="1:10" ht="34.5" customHeight="1" thickBot="1">
       <c r="D70" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G70" s="19" t="s">
         <v>128</v>
@@ -3700,7 +3581,7 @@
         <v>129</v>
       </c>
       <c r="J70" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="16.5" hidden="1" thickBot="1">
@@ -3734,17 +3615,17 @@
     </row>
     <row r="74" spans="1:10" ht="16.5" thickBot="1">
       <c r="D74" s="30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G74" s="19"/>
     </row>
     <row r="75" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="D75" s="9" t="s">
-        <v>146</v>
+        <v>285</v>
       </c>
       <c r="G75" s="19"/>
       <c r="I75" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="15.75" hidden="1">
@@ -3752,7 +3633,7 @@
         <v>44011</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G76" s="19"/>
     </row>
@@ -3761,7 +3642,7 @@
         <v>44011</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G77" s="19"/>
     </row>
@@ -3770,7 +3651,7 @@
         <v>44064</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G78" s="19"/>
     </row>
@@ -3780,7 +3661,7 @@
       </c>
       <c r="C79" s="36"/>
       <c r="D79" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G79" s="19"/>
     </row>
@@ -3789,61 +3670,82 @@
         <v>44029</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="15.75">
-      <c r="C81" s="36"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="15.75" hidden="1">
+      <c r="C81" s="36">
+        <v>44075</v>
+      </c>
       <c r="D81" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="I81" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="I81" s="11" t="s">
+    </row>
+    <row r="82" spans="1:9" ht="18.75" hidden="1">
+      <c r="C82" s="36">
+        <v>44075</v>
+      </c>
+      <c r="D82" s="60" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="18.75">
-      <c r="C82" s="36"/>
-      <c r="D82" s="60" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" ht="34.5" hidden="1" customHeight="1">
+    <row r="83" spans="1:9" ht="15.75">
+      <c r="C83" s="36"/>
+      <c r="D83" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="24.95" hidden="1" customHeight="1">
       <c r="A84" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D84" s="33" t="s">
+      <c r="D84" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="I84" s="11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="34.5" hidden="1" customHeight="1">
+      <c r="A85" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85" s="33" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="24.95" customHeight="1">
-      <c r="D85" s="9" t="s">
+    <row r="86" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D86" s="9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="32.25" hidden="1" thickBot="1">
-      <c r="C86" s="2" t="s">
+    <row r="87" spans="1:9" ht="32.25" hidden="1" thickBot="1">
+      <c r="C87" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D86" s="32" t="s">
+      <c r="D87" s="32" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="24.95" customHeight="1">
-      <c r="D87" s="26" t="s">
+    <row r="88" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D88" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="I88" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="I87" s="11" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="442" spans="1:10" ht="15.75" hidden="1">
-      <c r="A442" s="2" t="s">
+    </row>
+    <row r="443" spans="1:10" ht="15.75" hidden="1">
+      <c r="A443" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="J442" s="6"/>
+      <c r="J443" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I442" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
+  <autoFilter ref="A1:I443" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
@@ -3863,7 +3765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFDF36D1-DE2E-478E-8F20-00E572A1B869}">
   <dimension ref="B1:E44"/>
   <sheetViews>
@@ -3880,54 +3782,54 @@
   <sheetData>
     <row r="1" spans="2:5">
       <c r="B1" s="57" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="31.5">
       <c r="B2" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>203</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75">
       <c r="B7" s="43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="44" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="26.25">
       <c r="B15" s="47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E15" s="48" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="12" customHeight="1">
       <c r="B16" s="46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="12" customHeight="1">
@@ -3935,71 +3837,71 @@
     </row>
     <row r="18" spans="2:5" ht="12" customHeight="1">
       <c r="B18" s="45" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="12" customHeight="1">
       <c r="B19" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="12" customHeight="1">
       <c r="B20" s="45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="12" customHeight="1">
       <c r="B21" s="45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="12" customHeight="1">
       <c r="B22" s="45" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E22" s="44" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="12" customHeight="1">
       <c r="B23" s="45" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="12" customHeight="1">
       <c r="B24" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="12" customHeight="1">
       <c r="B25" s="45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="12" customHeight="1">
       <c r="B26" s="45" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="12" customHeight="1">
       <c r="B27" s="45" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E27" s="38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="12" customHeight="1">
       <c r="B28" s="45" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="12" customHeight="1">
       <c r="B29" s="45" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="12" customHeight="1">
@@ -4007,7 +3909,7 @@
     </row>
     <row r="31" spans="2:5" ht="12" customHeight="1">
       <c r="B31" s="46" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="12" customHeight="1">
@@ -4015,62 +3917,62 @@
     </row>
     <row r="33" spans="2:2" ht="12" customHeight="1">
       <c r="B33" s="45" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="12" customHeight="1">
       <c r="B34" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="12" customHeight="1">
       <c r="B35" s="45" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="12" customHeight="1">
       <c r="B36" s="45" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="12" customHeight="1">
       <c r="B37" s="45" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="12" customHeight="1">
       <c r="B38" s="45" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="12" customHeight="1">
       <c r="B39" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="12" customHeight="1">
       <c r="B40" s="45" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="12" customHeight="1">
       <c r="B41" s="45" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="12" customHeight="1">
       <c r="B42" s="45" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="2:2" ht="12" customHeight="1">
       <c r="B43" s="45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="12" customHeight="1">
       <c r="B44" s="45" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -4087,7 +3989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8A68F0-A5CC-4F2B-9E7A-D47D3E46C475}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J435"/>
@@ -4154,7 +4056,7 @@
         <v>44006</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F3" s="6"/>
       <c r="H3" s="6"/>
@@ -4175,7 +4077,7 @@
         <v>44014</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -4188,7 +4090,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F6" s="6"/>
       <c r="H6" s="6"/>
@@ -7638,7 +7540,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3521A2-0E46-4626-A556-F81B8258D1DB}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -7653,7 +7555,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D90DEFD-D6A8-4BFB-97A2-600F5E7E4446}">
   <dimension ref="B2:C12"/>
   <sheetViews>
@@ -7727,7 +7629,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392EF631-8DBE-4581-9410-4CF72B20CF9A}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -7744,23 +7646,23 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="37" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="41" customFormat="1">
       <c r="A3" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="C3" s="41" t="s">
         <v>170</v>
-      </c>
-      <c r="C3" s="41" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B4" s="39">
         <v>44035</v>
@@ -7772,7 +7674,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B5" s="39">
         <v>44035</v>
@@ -7784,7 +7686,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="39">
         <v>44020</v>
@@ -7796,7 +7698,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B7" s="39">
         <v>43864</v>
@@ -7808,7 +7710,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B8" s="39">
         <v>43838</v>
@@ -7820,7 +7722,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9" s="39">
         <v>43555</v>
@@ -7841,7 +7743,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073BA0C8-793A-470F-9811-FE4A219663BF}">
   <dimension ref="A1:N36"/>
   <sheetViews>
@@ -7867,18 +7769,18 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75">
       <c r="F1" s="56" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="55" customFormat="1" ht="18.75">
       <c r="A7" s="55" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F7" s="55" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K7" s="55" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -7886,13 +7788,13 @@
         <v>16099</v>
       </c>
       <c r="B8" s="53" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F8" s="54">
         <v>16099</v>
       </c>
       <c r="G8" s="53" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -7900,40 +7802,40 @@
     </row>
     <row r="10" spans="1:14" s="51" customFormat="1">
       <c r="A10" s="51" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B10" s="51" t="s">
+        <v>255</v>
+      </c>
+      <c r="C10" s="51" t="s">
+        <v>254</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>253</v>
+      </c>
+      <c r="F10" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="G10" s="51" t="s">
         <v>255</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="H10" s="51" t="s">
         <v>254</v>
       </c>
-      <c r="F10" s="51" t="s">
-        <v>257</v>
-      </c>
-      <c r="G10" s="51" t="s">
+      <c r="I10" s="51" t="s">
+        <v>253</v>
+      </c>
+      <c r="K10" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="H10" s="51" t="s">
+      <c r="L10" s="51" t="s">
         <v>255</v>
       </c>
-      <c r="I10" s="51" t="s">
+      <c r="M10" s="51" t="s">
         <v>254</v>
       </c>
-      <c r="K10" s="51" t="s">
-        <v>257</v>
-      </c>
-      <c r="L10" s="51" t="s">
-        <v>256</v>
-      </c>
-      <c r="M10" s="51" t="s">
-        <v>255</v>
-      </c>
       <c r="N10" s="51" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -7942,57 +7844,57 @@
       <c r="C11" s="51"/>
       <c r="D11" s="51"/>
       <c r="F11" s="50" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G11" s="50" t="s">
+        <v>251</v>
+      </c>
+      <c r="H11" s="50" t="s">
+        <v>250</v>
+      </c>
+      <c r="K11" s="50" t="s">
         <v>252</v>
       </c>
-      <c r="H11" s="50" t="s">
+      <c r="L11" s="50" t="s">
         <v>251</v>
       </c>
-      <c r="K11" s="50" t="s">
-        <v>253</v>
-      </c>
-      <c r="L11" s="50" t="s">
-        <v>252</v>
-      </c>
       <c r="M11" s="50" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="50" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D12" s="50">
         <v>255</v>
       </c>
       <c r="F12" s="50" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G12" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H12" s="50" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I12" s="50">
         <v>255</v>
       </c>
       <c r="K12" s="50" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L12" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M12" s="50" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N12" s="50">
         <v>255</v>
@@ -8000,25 +7902,25 @@
     </row>
     <row r="13" spans="1:14">
       <c r="F13" s="50" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G13" s="50" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H13" s="50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I13" s="50">
         <v>8</v>
       </c>
       <c r="K13" s="50" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L13" s="50" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M13" s="50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N13" s="50">
         <v>8</v>
@@ -8026,25 +7928,25 @@
     </row>
     <row r="14" spans="1:14">
       <c r="F14" s="50" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G14" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H14" s="50" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I14" s="50">
         <v>2</v>
       </c>
       <c r="K14" s="50" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L14" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M14" s="50" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N14" s="50">
         <v>2</v>
@@ -8052,37 +7954,37 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="50" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D15" s="50">
         <v>255</v>
       </c>
       <c r="F15" s="50" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G15" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H15" s="50" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I15" s="50">
         <v>255</v>
       </c>
       <c r="K15" s="50" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L15" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M15" s="50" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N15" s="50">
         <v>255</v>
@@ -8090,54 +7992,54 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="50" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C16" s="50" t="s">
+        <v>239</v>
+      </c>
+      <c r="F16" s="50" t="s">
         <v>240</v>
       </c>
-      <c r="F16" s="50" t="s">
-        <v>241</v>
-      </c>
       <c r="G16" s="50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H16" s="50" t="s">
+        <v>239</v>
+      </c>
+      <c r="K16" s="50" t="s">
         <v>240</v>
       </c>
-      <c r="K16" s="50" t="s">
-        <v>241</v>
-      </c>
       <c r="L16" s="50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M16" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="F17" s="50" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G17" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H17" s="50" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I17" s="50">
         <v>5</v>
       </c>
       <c r="K17" s="50" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L17" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M17" s="50" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N17" s="50">
         <v>5</v>
@@ -8145,25 +8047,25 @@
     </row>
     <row r="18" spans="1:14">
       <c r="F18" s="50" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G18" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H18" s="50" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I18" s="50">
         <v>5</v>
       </c>
       <c r="K18" s="50" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L18" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M18" s="50" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N18" s="50">
         <v>5</v>
@@ -8171,25 +8073,25 @@
     </row>
     <row r="19" spans="1:14">
       <c r="F19" s="50" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G19" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H19" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I19" s="50">
         <v>5</v>
       </c>
       <c r="K19" s="50" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L19" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M19" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N19" s="50">
         <v>5</v>
@@ -8197,25 +8099,25 @@
     </row>
     <row r="20" spans="1:14">
       <c r="F20" s="50" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G20" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H20" s="50" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I20" s="50">
         <v>150</v>
       </c>
       <c r="K20" s="50" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L20" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M20" s="50" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N20" s="50">
         <v>150</v>
@@ -8223,54 +8125,54 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="50" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B21" s="50" t="s">
+        <v>229</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>228</v>
+      </c>
+      <c r="F21" s="50" t="s">
         <v>230</v>
       </c>
-      <c r="C21" s="50" t="s">
+      <c r="G21" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="F21" s="50" t="s">
-        <v>231</v>
-      </c>
-      <c r="G21" s="50" t="s">
-        <v>230</v>
-      </c>
       <c r="H21" s="50" t="s">
+        <v>228</v>
+      </c>
+      <c r="K21" s="50" t="s">
+        <v>270</v>
+      </c>
+      <c r="L21" s="50" t="s">
         <v>229</v>
       </c>
-      <c r="K21" s="50" t="s">
+      <c r="M21" s="50" t="s">
         <v>271</v>
-      </c>
-      <c r="L21" s="50" t="s">
-        <v>230</v>
-      </c>
-      <c r="M21" s="50" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:14">
       <c r="F22" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G22" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H22" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I22" s="50">
         <v>25</v>
       </c>
       <c r="K22" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L22" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M22" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N22" s="50">
         <v>25</v>
@@ -8278,86 +8180,86 @@
     </row>
     <row r="23" spans="1:14">
       <c r="F23" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G23" s="50" t="s">
+        <v>224</v>
+      </c>
+      <c r="H23" s="50" t="s">
+        <v>223</v>
+      </c>
+      <c r="K23" s="50" t="s">
         <v>225</v>
       </c>
-      <c r="H23" s="50" t="s">
+      <c r="L23" s="50" t="s">
         <v>224</v>
       </c>
-      <c r="K23" s="50" t="s">
-        <v>226</v>
-      </c>
-      <c r="L23" s="50" t="s">
-        <v>225</v>
-      </c>
       <c r="M23" s="50" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="50" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B24" s="50" t="s">
+        <v>221</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="F24" s="50" t="s">
         <v>222</v>
       </c>
-      <c r="C24" s="50" t="s">
+      <c r="G24" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="F24" s="50" t="s">
-        <v>223</v>
-      </c>
-      <c r="G24" s="50" t="s">
+      <c r="H24" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="K24" s="50" t="s">
         <v>222</v>
       </c>
-      <c r="H24" s="50" t="s">
+      <c r="L24" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="K24" s="50" t="s">
-        <v>223</v>
-      </c>
-      <c r="L24" s="50" t="s">
-        <v>222</v>
-      </c>
       <c r="M24" s="50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="50" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C25" s="50" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D25" s="50">
         <v>255</v>
       </c>
       <c r="F25" s="50" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G25" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H25" s="50" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I25" s="50">
         <v>255</v>
       </c>
       <c r="K25" s="50" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L25" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M25" s="50" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N25" s="50">
         <v>255</v>
@@ -8365,37 +8267,37 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C26" s="50" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D26" s="50">
         <v>801</v>
       </c>
       <c r="F26" s="50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G26" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H26" s="50" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I26" s="50">
         <v>801</v>
       </c>
       <c r="K26" s="50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L26" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M26" s="50" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N26" s="50">
         <v>801</v>
@@ -8403,37 +8305,37 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D27" s="50">
         <v>255</v>
       </c>
       <c r="F27" s="50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G27" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H27" s="50" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I27" s="50">
         <v>255</v>
       </c>
       <c r="K27" s="50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L27" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M27" s="50" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N27" s="50">
         <v>255</v>
@@ -8441,37 +8343,37 @@
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="50" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C28" s="50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D28" s="50">
         <v>12</v>
       </c>
       <c r="F28" s="50" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G28" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H28" s="50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I28" s="50">
         <v>12</v>
       </c>
       <c r="K28" s="50" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L28" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M28" s="50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N28" s="50">
         <v>12</v>
@@ -8479,66 +8381,66 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="50" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C29" s="50" t="s">
+        <v>210</v>
+      </c>
+      <c r="F29" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="F29" s="50" t="s">
-        <v>212</v>
-      </c>
       <c r="G29" s="50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H29" s="50" t="s">
+        <v>210</v>
+      </c>
+      <c r="K29" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="K29" s="50" t="s">
-        <v>212</v>
-      </c>
       <c r="L29" s="50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M29" s="50" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B30" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D30" s="50">
         <v>255</v>
       </c>
       <c r="F30" s="50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G30" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H30" s="50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I30" s="50">
         <v>255</v>
       </c>
       <c r="K30" s="50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L30" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M30" s="50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="N30" s="50">
         <v>255</v>
@@ -8546,57 +8448,57 @@
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="50" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B31" s="50" t="s">
+        <v>205</v>
+      </c>
+      <c r="C31" s="50" t="s">
+        <v>204</v>
+      </c>
+      <c r="F31" s="50" t="s">
         <v>206</v>
       </c>
-      <c r="C31" s="50" t="s">
+      <c r="G31" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="F31" s="50" t="s">
-        <v>207</v>
-      </c>
-      <c r="G31" s="50" t="s">
+      <c r="H31" s="50" t="s">
+        <v>204</v>
+      </c>
+      <c r="K31" s="50" t="s">
         <v>206</v>
       </c>
-      <c r="H31" s="50" t="s">
+      <c r="L31" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="K31" s="50" t="s">
-        <v>207</v>
-      </c>
-      <c r="L31" s="50" t="s">
-        <v>206</v>
-      </c>
       <c r="M31" s="50" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="58" t="s">
+        <v>261</v>
+      </c>
+      <c r="B32" s="58" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" s="58" t="s">
         <v>262</v>
-      </c>
-      <c r="B32" s="58" t="s">
-        <v>209</v>
-      </c>
-      <c r="C32" s="58" t="s">
-        <v>263</v>
       </c>
       <c r="D32" s="50">
         <v>1</v>
       </c>
       <c r="F32" s="59" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K32" s="50" t="s">
+        <v>261</v>
+      </c>
+      <c r="L32" s="50" t="s">
+        <v>208</v>
+      </c>
+      <c r="M32" s="50" t="s">
         <v>262</v>
-      </c>
-      <c r="L32" s="50" t="s">
-        <v>209</v>
-      </c>
-      <c r="M32" s="50" t="s">
-        <v>263</v>
       </c>
       <c r="N32" s="50">
         <v>1</v>
@@ -8604,24 +8506,24 @@
     </row>
     <row r="33" spans="11:14">
       <c r="K33" s="50" t="s">
+        <v>272</v>
+      </c>
+      <c r="L33" s="50" t="s">
+        <v>251</v>
+      </c>
+      <c r="M33" s="50" t="s">
         <v>273</v>
-      </c>
-      <c r="L33" s="50" t="s">
-        <v>252</v>
-      </c>
-      <c r="M33" s="50" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="34" spans="11:14">
       <c r="K34" s="50" t="s">
+        <v>264</v>
+      </c>
+      <c r="L34" s="50" t="s">
+        <v>208</v>
+      </c>
+      <c r="M34" s="50" t="s">
         <v>265</v>
-      </c>
-      <c r="L34" s="50" t="s">
-        <v>209</v>
-      </c>
-      <c r="M34" s="50" t="s">
-        <v>266</v>
       </c>
       <c r="N34" s="50">
         <v>6</v>
@@ -8629,13 +8531,13 @@
     </row>
     <row r="35" spans="11:14">
       <c r="K35" s="50" t="s">
+        <v>268</v>
+      </c>
+      <c r="L35" s="50" t="s">
+        <v>208</v>
+      </c>
+      <c r="M35" s="50" t="s">
         <v>269</v>
-      </c>
-      <c r="L35" s="50" t="s">
-        <v>209</v>
-      </c>
-      <c r="M35" s="50" t="s">
-        <v>270</v>
       </c>
       <c r="N35" s="50">
         <v>255</v>
@@ -8643,13 +8545,13 @@
     </row>
     <row r="36" spans="11:14">
       <c r="K36" s="50" t="s">
+        <v>266</v>
+      </c>
+      <c r="L36" s="50" t="s">
+        <v>208</v>
+      </c>
+      <c r="M36" s="50" t="s">
         <v>267</v>
-      </c>
-      <c r="L36" s="50" t="s">
-        <v>209</v>
-      </c>
-      <c r="M36" s="50" t="s">
-        <v>268</v>
       </c>
       <c r="N36" s="50">
         <v>255</v>
@@ -8663,4 +8565,132 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD2386D-2AF1-4B5F-9842-EBCA886CA8B5}">
+  <dimension ref="B3:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="5" width="9" style="61"/>
+    <col min="6" max="6" width="25.125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="61"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7">
+      <c r="B3" s="61">
+        <v>994</v>
+      </c>
+      <c r="C3" s="61">
+        <v>776</v>
+      </c>
+      <c r="D3" s="61">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="61">
+        <v>1040</v>
+      </c>
+      <c r="C4" s="61">
+        <v>839</v>
+      </c>
+      <c r="D4" s="61">
+        <v>201</v>
+      </c>
+      <c r="F4" s="61" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="61">
+        <v>849</v>
+      </c>
+      <c r="C5" s="61">
+        <v>631</v>
+      </c>
+      <c r="D5" s="61">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="61">
+        <v>480</v>
+      </c>
+      <c r="C6" s="61">
+        <v>262</v>
+      </c>
+      <c r="D6" s="61">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="61">
+        <v>480</v>
+      </c>
+      <c r="C8" s="61">
+        <v>311</v>
+      </c>
+      <c r="D8" s="61">
+        <v>169</v>
+      </c>
+      <c r="F8" s="61" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="61">
+        <v>480</v>
+      </c>
+      <c r="C9" s="61">
+        <v>311</v>
+      </c>
+      <c r="D9" s="61">
+        <v>169</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>280</v>
+      </c>
+      <c r="G9" s="61">
+        <f>D6-D9</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="30">
+      <c r="B10" s="61">
+        <v>1040</v>
+      </c>
+      <c r="C10" s="61">
+        <v>888</v>
+      </c>
+      <c r="D10" s="61">
+        <v>152</v>
+      </c>
+      <c r="F10" s="62" t="s">
+        <v>279</v>
+      </c>
+      <c r="G10" s="61">
+        <f>D4-D10</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="61">
+        <v>774</v>
+      </c>
+      <c r="C13" s="61">
+        <v>605</v>
+      </c>
+      <c r="D13" s="61">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix FishDisplayPage, add columnsHideable option.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13A37FB-B6A5-420D-9CD5-FB25FA64E347}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B32E7E-32BA-4F2B-A4DB-8C2496FF2523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="750" windowWidth="24750" windowHeight="14145" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="287">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -2741,7 +2741,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D86" sqref="D86"/>
+      <selection pane="bottomRight" activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -3692,8 +3692,10 @@
         <v>277</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15.75">
-      <c r="C83" s="36"/>
+    <row r="83" spans="1:9" ht="15.75" hidden="1">
+      <c r="C83" s="36" t="s">
+        <v>21</v>
+      </c>
       <c r="D83" t="s">
         <v>286</v>
       </c>

</xml_diff>

<commit_message>
Restore FA Regions tab
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B32E7E-32BA-4F2B-A4DB-8C2496FF2523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34619630-326B-4AB7-AABD-44BB7A6D5726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="750" windowWidth="24750" windowHeight="14145" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="1005" yWindow="390" windowWidth="20925" windowHeight="14850" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="287">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -2741,7 +2741,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C83" sqref="C83"/>
+      <selection pane="bottomRight" activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -3386,7 +3386,10 @@
       </c>
       <c r="J47" s="6"/>
     </row>
-    <row r="48" spans="1:10" ht="42" customHeight="1">
+    <row r="48" spans="1:10" ht="42" hidden="1" customHeight="1">
+      <c r="A48" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="D48" s="9" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
Update to API 4.17, add copy of DGrid CSS, modify Bookmarks for 4.17
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34619630-326B-4AB7-AABD-44BB7A6D5726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3FE6B7-A4C3-4569-A063-EC5F68DD7E41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="390" windowWidth="20925" windowHeight="14850" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="1605" yWindow="180" windowWidth="25320" windowHeight="14820" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -2747,7 +2747,8 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="5.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="70.75" style="9" customWidth="1"/>
     <col min="5" max="5" width="4.5" style="6" customWidth="1"/>
     <col min="6" max="6" width="6.875" style="7" customWidth="1"/>
@@ -3557,7 +3558,10 @@
       </c>
       <c r="J66" s="6"/>
     </row>
-    <row r="67" spans="1:10" ht="24.95" customHeight="1">
+    <row r="67" spans="1:10" ht="24.95" hidden="1" customHeight="1">
+      <c r="C67" s="36">
+        <v>44129</v>
+      </c>
       <c r="D67" s="33" t="s">
         <v>157</v>
       </c>
@@ -3622,7 +3626,10 @@
       </c>
       <c r="G74" s="19"/>
     </row>
-    <row r="75" spans="1:10" ht="20.100000000000001" customHeight="1">
+    <row r="75" spans="1:10" ht="20.100000000000001" hidden="1" customHeight="1">
+      <c r="C75" s="36">
+        <v>44129</v>
+      </c>
       <c r="D75" s="9" t="s">
         <v>285</v>
       </c>

</xml_diff>

<commit_message>
Species table layerNames & extra fields for statewide/Region/Station
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3FE6B7-A4C3-4569-A063-EC5F68DD7E41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52E70AF-B6A3-4969-BA85-F410E3E925C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1605" yWindow="180" windowWidth="25320" windowHeight="14820" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="288">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -1346,6 +1346,9 @@
   </si>
   <si>
     <t>long values for SS Coastal Class values</t>
+  </si>
+  <si>
+    <t>Shore Stations species table:  Reset to default mode (no GroupID filter) on switch between statewide/Region/Station.  Also, numbers are still not right when switching between.</t>
   </si>
 </sst>
 </file>
@@ -1721,7 +1724,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1861,6 +1864,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Heading 2" xfId="7" builtinId="17"/>
@@ -1878,9 +1884,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFA7A7"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FFFFE5FF"/>
-      <color rgb="FFFFA7A7"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2741,7 +2747,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D91" sqref="D91"/>
+      <selection pane="bottomRight" activeCell="I91" sqref="I91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -3748,6 +3754,11 @@
       </c>
       <c r="I88" s="11" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="47.25">
+      <c r="D89" s="63" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="443" spans="1:10" ht="15.75" hidden="1">

</xml_diff>

<commit_message>
Attempt at handling missing lowres SZ photos folder, make layout preview images smaller.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52E70AF-B6A3-4969-BA85-F410E3E925C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0381D8B-F948-4DF8-A6F4-D89E71EB2B06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="180" windowWidth="25320" windowHeight="14820" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="10980" yWindow="345" windowWidth="17445" windowHeight="14820" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="289">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -1349,6 +1349,9 @@
   </si>
   <si>
     <t>Shore Stations species table:  Reset to default mode (no GroupID filter) on switch between statewide/Region/Station.  Also, numbers are still not right when switching between.</t>
+  </si>
+  <si>
+    <t>Bioband &amp; Substrate chart labels not showing up in Safari</t>
   </si>
 </sst>
 </file>
@@ -2744,10 +2747,10 @@
   <dimension ref="A1:J443"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I91" sqref="I91"/>
+      <selection pane="bottomRight" activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -3756,9 +3759,17 @@
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="47.25">
+    <row r="89" spans="1:9" ht="47.25" hidden="1">
+      <c r="C89" s="36">
+        <v>44140</v>
+      </c>
       <c r="D89" s="63" t="s">
         <v>287</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D90" s="9" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="443" spans="1:10" ht="15.75" hidden="1">

</xml_diff>

<commit_message>
Initial work on changing totals calc
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0381D8B-F948-4DF8-A6F4-D89E71EB2B06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F45DCB-715A-4B7F-BF74-C568640C58DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10980" yWindow="345" windowWidth="17445" windowHeight="14820" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="8070" yWindow="780" windowWidth="19995" windowHeight="14820" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="290">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -1352,6 +1352,9 @@
   </si>
   <si>
     <t>Bioband &amp; Substrate chart labels not showing up in Safari</t>
+  </si>
+  <si>
+    <t>Figure out why photos aren't displaying in WA/OR</t>
   </si>
 </sst>
 </file>
@@ -2750,7 +2753,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D91" sqref="D91"/>
+      <selection pane="bottomRight" activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -3770,6 +3773,11 @@
     <row r="90" spans="1:9" ht="24.95" customHeight="1">
       <c r="D90" s="9" t="s">
         <v>288</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D91" s="9" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="443" spans="1:10" ht="15.75" hidden="1">
@@ -4210,3358 +4218,425 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="2:9" ht="15.75">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="2:9" ht="15.75">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-    </row>
-    <row r="19" spans="2:9" ht="15.75">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-    </row>
-    <row r="20" spans="2:9" ht="15.75">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-    </row>
-    <row r="21" spans="2:9" ht="15.75">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-    </row>
-    <row r="22" spans="2:9" ht="15.75">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-    </row>
-    <row r="23" spans="2:9" ht="15.75">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-    </row>
-    <row r="24" spans="2:9" ht="15.75">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-    </row>
-    <row r="25" spans="2:9" ht="15.75">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-    </row>
-    <row r="26" spans="2:9" ht="15.75">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-    </row>
-    <row r="27" spans="2:9" ht="15.75">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-    </row>
-    <row r="28" spans="2:9" ht="15.75">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-    </row>
-    <row r="29" spans="2:9" ht="15.75">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-    </row>
-    <row r="30" spans="2:9" ht="15.75">
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-    </row>
-    <row r="31" spans="2:9" ht="15.75">
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-    </row>
-    <row r="32" spans="2:9" ht="15.75">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-    </row>
-    <row r="33" spans="2:9" ht="15.75">
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-    </row>
-    <row r="34" spans="2:9" ht="15.75">
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-    </row>
-    <row r="35" spans="2:9" ht="15.75">
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-    </row>
-    <row r="36" spans="2:9" ht="15.75">
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-    </row>
-    <row r="37" spans="2:9" ht="15.75">
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-    </row>
-    <row r="38" spans="2:9" ht="15.75">
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-    </row>
-    <row r="39" spans="2:9" ht="15.75">
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-    </row>
-    <row r="40" spans="2:9" ht="15.75">
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-    </row>
-    <row r="41" spans="2:9" ht="15.75">
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-    </row>
-    <row r="42" spans="2:9" ht="15.75">
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-    </row>
-    <row r="43" spans="2:9" ht="15.75">
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-    </row>
-    <row r="44" spans="2:9" ht="39.75" customHeight="1">
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-    </row>
-    <row r="45" spans="2:9" ht="15.75">
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-    </row>
-    <row r="46" spans="2:9" ht="15.75">
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-    </row>
-    <row r="47" spans="2:9" ht="9.75" customHeight="1">
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-    </row>
-    <row r="48" spans="2:9" ht="42" customHeight="1">
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-    </row>
-    <row r="49" spans="2:9" ht="15.75">
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-    </row>
-    <row r="50" spans="2:9" ht="15.75">
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-    </row>
-    <row r="51" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-    </row>
-    <row r="52" spans="2:9" ht="15.75">
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-    </row>
-    <row r="53" spans="2:9" ht="15.75">
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6"/>
-    </row>
-    <row r="54" spans="2:9" ht="15.75">
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="6"/>
-    </row>
-    <row r="55" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="H55" s="6"/>
-      <c r="I55" s="6"/>
-    </row>
-    <row r="56" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="F56" s="6"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="6"/>
-    </row>
-    <row r="57" spans="2:9" ht="15.75">
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="H57" s="6"/>
-      <c r="I57" s="6"/>
-    </row>
-    <row r="58" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="H58" s="6"/>
-      <c r="I58" s="6"/>
-    </row>
-    <row r="59" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="F59" s="6"/>
-      <c r="H59" s="6"/>
-      <c r="I59" s="6"/>
-    </row>
-    <row r="60" spans="2:9" ht="15.75">
-      <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="F60" s="6"/>
-      <c r="H60" s="6"/>
-      <c r="I60" s="6"/>
-    </row>
-    <row r="61" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
-      <c r="F61" s="6"/>
-      <c r="H61" s="6"/>
-      <c r="I61" s="6"/>
-    </row>
-    <row r="62" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="F62" s="6"/>
-      <c r="H62" s="6"/>
-      <c r="I62" s="6"/>
-    </row>
-    <row r="63" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B63" s="6"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
-      <c r="F63" s="6"/>
-      <c r="H63" s="6"/>
-      <c r="I63" s="6"/>
-    </row>
-    <row r="64" spans="2:9" ht="32.25" customHeight="1">
-      <c r="B64" s="6"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="6"/>
-      <c r="F64" s="6"/>
-      <c r="H64" s="6"/>
-      <c r="I64" s="6"/>
-    </row>
-    <row r="65" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B65" s="6"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="6"/>
-      <c r="F65" s="6"/>
-      <c r="H65" s="6"/>
-      <c r="I65" s="6"/>
-    </row>
-    <row r="66" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B66" s="6"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="6"/>
-      <c r="F66" s="6"/>
-      <c r="H66" s="6"/>
-      <c r="I66" s="6"/>
-    </row>
-    <row r="67" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
-      <c r="F67" s="6"/>
-      <c r="H67" s="6"/>
-      <c r="I67" s="6"/>
-    </row>
-    <row r="68" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B68" s="6"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="F68" s="6"/>
-      <c r="H68" s="6"/>
-      <c r="I68" s="6"/>
-    </row>
-    <row r="69" spans="2:9" ht="15.75">
-      <c r="B69" s="6"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="F69" s="6"/>
-      <c r="H69" s="6"/>
-      <c r="I69" s="6"/>
-    </row>
-    <row r="70" spans="2:9" ht="15.75">
-      <c r="B70" s="6"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-      <c r="F70" s="6"/>
-      <c r="H70" s="6"/>
-      <c r="I70" s="6"/>
-    </row>
-    <row r="71" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B71" s="6"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="F71" s="6"/>
-      <c r="H71" s="6"/>
-      <c r="I71" s="6"/>
-    </row>
-    <row r="72" spans="2:9" ht="42" customHeight="1">
-      <c r="B72" s="6"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6"/>
-      <c r="F72" s="6"/>
-      <c r="H72" s="6"/>
-      <c r="I72" s="6"/>
-    </row>
-    <row r="73" spans="2:9" ht="15.75">
-      <c r="B73" s="6"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="F73" s="6"/>
-      <c r="H73" s="6"/>
-      <c r="I73" s="6"/>
-    </row>
-    <row r="74" spans="2:9" ht="15.75">
-      <c r="B74" s="6"/>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="F74" s="6"/>
-      <c r="H74" s="6"/>
-      <c r="I74" s="6"/>
-    </row>
-    <row r="75" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B75" s="6"/>
-      <c r="C75" s="6"/>
-      <c r="D75" s="6"/>
-      <c r="F75" s="6"/>
-      <c r="H75" s="6"/>
-      <c r="I75" s="6"/>
-    </row>
-    <row r="76" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B76" s="6"/>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="F76" s="6"/>
-      <c r="H76" s="6"/>
-      <c r="I76" s="6"/>
-    </row>
-    <row r="77" spans="2:9" ht="34.5" customHeight="1">
-      <c r="B77" s="6"/>
-      <c r="C77" s="6"/>
-      <c r="D77" s="6"/>
-      <c r="F77" s="6"/>
-      <c r="H77" s="6"/>
-      <c r="I77" s="6"/>
-    </row>
-    <row r="78" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B78" s="6"/>
-      <c r="C78" s="6"/>
-      <c r="D78" s="6"/>
-      <c r="F78" s="6"/>
-      <c r="H78" s="6"/>
-      <c r="I78" s="6"/>
-    </row>
-    <row r="79" spans="2:9" ht="15.75">
-      <c r="B79" s="6"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="F79" s="6"/>
-      <c r="H79" s="6"/>
-      <c r="I79" s="6"/>
-    </row>
-    <row r="80" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B80" s="6"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="F80" s="6"/>
-      <c r="H80" s="6"/>
-      <c r="I80" s="6"/>
-    </row>
-    <row r="81" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B81" s="6"/>
-      <c r="C81" s="6"/>
-      <c r="D81" s="6"/>
-      <c r="F81" s="6"/>
-      <c r="H81" s="6"/>
-      <c r="I81" s="6"/>
-    </row>
-    <row r="82" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B82" s="6"/>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6"/>
-      <c r="F82" s="6"/>
-      <c r="H82" s="6"/>
-      <c r="I82" s="6"/>
-    </row>
-    <row r="83" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B83" s="6"/>
-      <c r="C83" s="6"/>
-      <c r="D83" s="6"/>
-      <c r="F83" s="6"/>
-      <c r="H83" s="6"/>
-      <c r="I83" s="6"/>
-    </row>
-    <row r="84" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
-      <c r="D84" s="6"/>
-      <c r="F84" s="6"/>
-      <c r="H84" s="6"/>
-      <c r="I84" s="6"/>
-    </row>
-    <row r="85" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
-      <c r="D85" s="6"/>
-      <c r="F85" s="6"/>
-      <c r="H85" s="6"/>
-      <c r="I85" s="6"/>
-    </row>
-    <row r="86" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
-      <c r="D86" s="6"/>
-      <c r="F86" s="6"/>
-      <c r="H86" s="6"/>
-      <c r="I86" s="6"/>
-    </row>
-    <row r="87" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B87" s="6"/>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6"/>
-      <c r="F87" s="6"/>
-      <c r="H87" s="6"/>
-      <c r="I87" s="6"/>
-    </row>
-    <row r="88" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B88" s="6"/>
-      <c r="C88" s="6"/>
-      <c r="D88" s="6"/>
-      <c r="F88" s="6"/>
-      <c r="H88" s="6"/>
-      <c r="I88" s="6"/>
-    </row>
-    <row r="89" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B89" s="6"/>
-      <c r="C89" s="6"/>
-      <c r="D89" s="6"/>
-      <c r="F89" s="6"/>
-      <c r="H89" s="6"/>
-      <c r="I89" s="6"/>
-    </row>
-    <row r="90" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B90" s="6"/>
-      <c r="C90" s="6"/>
-      <c r="D90" s="6"/>
-      <c r="F90" s="6"/>
-      <c r="H90" s="6"/>
-      <c r="I90" s="6"/>
-    </row>
-    <row r="91" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B91" s="6"/>
-      <c r="C91" s="6"/>
-      <c r="D91" s="6"/>
-      <c r="F91" s="6"/>
-      <c r="H91" s="6"/>
-      <c r="I91" s="6"/>
-    </row>
-    <row r="92" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B92" s="6"/>
-      <c r="C92" s="6"/>
-      <c r="D92" s="6"/>
-      <c r="F92" s="6"/>
-      <c r="H92" s="6"/>
-      <c r="I92" s="6"/>
-    </row>
-    <row r="93" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B93" s="6"/>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
-      <c r="F93" s="6"/>
-      <c r="H93" s="6"/>
-      <c r="I93" s="6"/>
-    </row>
-    <row r="94" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B94" s="6"/>
-      <c r="C94" s="6"/>
-      <c r="D94" s="6"/>
-      <c r="F94" s="6"/>
-      <c r="H94" s="6"/>
-      <c r="I94" s="6"/>
-    </row>
-    <row r="95" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B95" s="6"/>
-      <c r="C95" s="6"/>
-      <c r="D95" s="6"/>
-      <c r="F95" s="6"/>
-      <c r="H95" s="6"/>
-      <c r="I95" s="6"/>
-    </row>
-    <row r="96" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B96" s="6"/>
-      <c r="C96" s="6"/>
-      <c r="D96" s="6"/>
-      <c r="F96" s="6"/>
-      <c r="H96" s="6"/>
-      <c r="I96" s="6"/>
-    </row>
-    <row r="97" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B97" s="6"/>
-      <c r="C97" s="6"/>
-      <c r="D97" s="6"/>
-      <c r="F97" s="6"/>
-      <c r="H97" s="6"/>
-      <c r="I97" s="6"/>
-    </row>
-    <row r="98" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B98" s="6"/>
-      <c r="C98" s="6"/>
-      <c r="D98" s="6"/>
-      <c r="F98" s="6"/>
-      <c r="H98" s="6"/>
-      <c r="I98" s="6"/>
-    </row>
-    <row r="99" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B99" s="6"/>
-      <c r="C99" s="6"/>
-      <c r="D99" s="6"/>
-      <c r="F99" s="6"/>
-      <c r="H99" s="6"/>
-      <c r="I99" s="6"/>
-    </row>
-    <row r="100" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B100" s="6"/>
-      <c r="C100" s="6"/>
-      <c r="D100" s="6"/>
-      <c r="F100" s="6"/>
-      <c r="H100" s="6"/>
-      <c r="I100" s="6"/>
-    </row>
-    <row r="101" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B101" s="6"/>
-      <c r="C101" s="6"/>
-      <c r="D101" s="6"/>
-      <c r="F101" s="6"/>
-      <c r="H101" s="6"/>
-      <c r="I101" s="6"/>
-    </row>
-    <row r="102" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B102" s="6"/>
-      <c r="C102" s="6"/>
-      <c r="D102" s="6"/>
-      <c r="F102" s="6"/>
-      <c r="H102" s="6"/>
-      <c r="I102" s="6"/>
-    </row>
-    <row r="103" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B103" s="6"/>
-      <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
-      <c r="F103" s="6"/>
-      <c r="H103" s="6"/>
-      <c r="I103" s="6"/>
-    </row>
-    <row r="104" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B104" s="6"/>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
-      <c r="F104" s="6"/>
-      <c r="H104" s="6"/>
-      <c r="I104" s="6"/>
-    </row>
-    <row r="105" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B105" s="6"/>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="F105" s="6"/>
-      <c r="H105" s="6"/>
-      <c r="I105" s="6"/>
-    </row>
-    <row r="106" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B106" s="6"/>
-      <c r="C106" s="6"/>
-      <c r="D106" s="6"/>
-      <c r="F106" s="6"/>
-      <c r="H106" s="6"/>
-      <c r="I106" s="6"/>
-    </row>
-    <row r="107" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B107" s="6"/>
-      <c r="C107" s="6"/>
-      <c r="D107" s="6"/>
-      <c r="F107" s="6"/>
-      <c r="H107" s="6"/>
-      <c r="I107" s="6"/>
-    </row>
-    <row r="108" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B108" s="6"/>
-      <c r="C108" s="6"/>
-      <c r="D108" s="6"/>
-      <c r="F108" s="6"/>
-      <c r="H108" s="6"/>
-      <c r="I108" s="6"/>
-    </row>
-    <row r="109" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B109" s="6"/>
-      <c r="C109" s="6"/>
-      <c r="D109" s="6"/>
-      <c r="F109" s="6"/>
-      <c r="H109" s="6"/>
-      <c r="I109" s="6"/>
-    </row>
-    <row r="110" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B110" s="6"/>
-      <c r="C110" s="6"/>
-      <c r="D110" s="6"/>
-      <c r="F110" s="6"/>
-      <c r="H110" s="6"/>
-      <c r="I110" s="6"/>
-    </row>
-    <row r="111" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B111" s="6"/>
-      <c r="C111" s="6"/>
-      <c r="D111" s="6"/>
-      <c r="F111" s="6"/>
-      <c r="H111" s="6"/>
-      <c r="I111" s="6"/>
-    </row>
-    <row r="112" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B112" s="6"/>
-      <c r="C112" s="6"/>
-      <c r="D112" s="6"/>
-      <c r="F112" s="6"/>
-      <c r="H112" s="6"/>
-      <c r="I112" s="6"/>
-    </row>
-    <row r="113" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B113" s="6"/>
-      <c r="C113" s="6"/>
-      <c r="D113" s="6"/>
-      <c r="F113" s="6"/>
-      <c r="H113" s="6"/>
-      <c r="I113" s="6"/>
-    </row>
-    <row r="114" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B114" s="6"/>
-      <c r="C114" s="6"/>
-      <c r="D114" s="6"/>
-      <c r="F114" s="6"/>
-      <c r="H114" s="6"/>
-      <c r="I114" s="6"/>
-    </row>
-    <row r="115" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B115" s="6"/>
-      <c r="C115" s="6"/>
-      <c r="D115" s="6"/>
-      <c r="F115" s="6"/>
-      <c r="H115" s="6"/>
-      <c r="I115" s="6"/>
-    </row>
-    <row r="116" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B116" s="6"/>
-      <c r="C116" s="6"/>
-      <c r="D116" s="6"/>
-      <c r="F116" s="6"/>
-      <c r="H116" s="6"/>
-      <c r="I116" s="6"/>
-    </row>
-    <row r="117" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B117" s="6"/>
-      <c r="C117" s="6"/>
-      <c r="D117" s="6"/>
-      <c r="F117" s="6"/>
-      <c r="H117" s="6"/>
-      <c r="I117" s="6"/>
-    </row>
-    <row r="118" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B118" s="6"/>
-      <c r="C118" s="6"/>
-      <c r="D118" s="6"/>
-      <c r="F118" s="6"/>
-      <c r="H118" s="6"/>
-      <c r="I118" s="6"/>
-    </row>
-    <row r="119" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B119" s="6"/>
-      <c r="C119" s="6"/>
-      <c r="D119" s="6"/>
-      <c r="F119" s="6"/>
-      <c r="H119" s="6"/>
-      <c r="I119" s="6"/>
-    </row>
-    <row r="120" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B120" s="6"/>
-      <c r="C120" s="6"/>
-      <c r="D120" s="6"/>
-      <c r="F120" s="6"/>
-      <c r="H120" s="6"/>
-      <c r="I120" s="6"/>
-    </row>
-    <row r="121" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B121" s="6"/>
-      <c r="C121" s="6"/>
-      <c r="D121" s="6"/>
-      <c r="F121" s="6"/>
-      <c r="H121" s="6"/>
-      <c r="I121" s="6"/>
-    </row>
-    <row r="122" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B122" s="6"/>
-      <c r="C122" s="6"/>
-      <c r="D122" s="6"/>
-      <c r="F122" s="6"/>
-      <c r="H122" s="6"/>
-      <c r="I122" s="6"/>
-    </row>
-    <row r="123" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B123" s="6"/>
-      <c r="C123" s="6"/>
-      <c r="D123" s="6"/>
-      <c r="F123" s="6"/>
-      <c r="H123" s="6"/>
-      <c r="I123" s="6"/>
-    </row>
-    <row r="124" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B124" s="6"/>
-      <c r="C124" s="6"/>
-      <c r="D124" s="6"/>
-      <c r="F124" s="6"/>
-      <c r="H124" s="6"/>
-      <c r="I124" s="6"/>
-    </row>
-    <row r="125" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B125" s="6"/>
-      <c r="C125" s="6"/>
-      <c r="D125" s="6"/>
-      <c r="F125" s="6"/>
-      <c r="H125" s="6"/>
-      <c r="I125" s="6"/>
-    </row>
-    <row r="126" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B126" s="6"/>
-      <c r="C126" s="6"/>
-      <c r="D126" s="6"/>
-      <c r="F126" s="6"/>
-      <c r="H126" s="6"/>
-      <c r="I126" s="6"/>
-    </row>
-    <row r="127" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B127" s="6"/>
-      <c r="C127" s="6"/>
-      <c r="D127" s="6"/>
-      <c r="F127" s="6"/>
-      <c r="H127" s="6"/>
-      <c r="I127" s="6"/>
-    </row>
-    <row r="128" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B128" s="6"/>
-      <c r="C128" s="6"/>
-      <c r="D128" s="6"/>
-      <c r="F128" s="6"/>
-      <c r="H128" s="6"/>
-      <c r="I128" s="6"/>
-    </row>
-    <row r="129" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B129" s="6"/>
-      <c r="C129" s="6"/>
-      <c r="D129" s="6"/>
-      <c r="F129" s="6"/>
-      <c r="H129" s="6"/>
-      <c r="I129" s="6"/>
-    </row>
-    <row r="130" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B130" s="6"/>
-      <c r="C130" s="6"/>
-      <c r="D130" s="6"/>
-      <c r="F130" s="6"/>
-      <c r="H130" s="6"/>
-      <c r="I130" s="6"/>
-    </row>
-    <row r="131" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B131" s="6"/>
-      <c r="C131" s="6"/>
-      <c r="D131" s="6"/>
-      <c r="F131" s="6"/>
-      <c r="H131" s="6"/>
-      <c r="I131" s="6"/>
-    </row>
-    <row r="132" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B132" s="6"/>
-      <c r="C132" s="6"/>
-      <c r="D132" s="6"/>
-      <c r="F132" s="6"/>
-      <c r="H132" s="6"/>
-      <c r="I132" s="6"/>
-    </row>
-    <row r="133" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B133" s="6"/>
-      <c r="C133" s="6"/>
-      <c r="D133" s="6"/>
-      <c r="F133" s="6"/>
-      <c r="H133" s="6"/>
-      <c r="I133" s="6"/>
-    </row>
-    <row r="134" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B134" s="6"/>
-      <c r="C134" s="6"/>
-      <c r="D134" s="6"/>
-      <c r="F134" s="6"/>
-      <c r="H134" s="6"/>
-      <c r="I134" s="6"/>
-    </row>
-    <row r="135" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B135" s="6"/>
-      <c r="C135" s="6"/>
-      <c r="D135" s="6"/>
-      <c r="F135" s="6"/>
-      <c r="H135" s="6"/>
-      <c r="I135" s="6"/>
-    </row>
-    <row r="136" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B136" s="6"/>
-      <c r="C136" s="6"/>
-      <c r="D136" s="6"/>
-      <c r="F136" s="6"/>
-      <c r="H136" s="6"/>
-      <c r="I136" s="6"/>
-    </row>
-    <row r="137" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B137" s="6"/>
-      <c r="C137" s="6"/>
-      <c r="D137" s="6"/>
-      <c r="F137" s="6"/>
-      <c r="H137" s="6"/>
-      <c r="I137" s="6"/>
-    </row>
-    <row r="138" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B138" s="6"/>
-      <c r="C138" s="6"/>
-      <c r="D138" s="6"/>
-      <c r="F138" s="6"/>
-      <c r="H138" s="6"/>
-      <c r="I138" s="6"/>
-    </row>
-    <row r="139" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B139" s="6"/>
-      <c r="C139" s="6"/>
-      <c r="D139" s="6"/>
-      <c r="F139" s="6"/>
-      <c r="H139" s="6"/>
-      <c r="I139" s="6"/>
-    </row>
-    <row r="140" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B140" s="6"/>
-      <c r="C140" s="6"/>
-      <c r="D140" s="6"/>
-      <c r="F140" s="6"/>
-      <c r="H140" s="6"/>
-      <c r="I140" s="6"/>
-    </row>
-    <row r="141" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B141" s="6"/>
-      <c r="C141" s="6"/>
-      <c r="D141" s="6"/>
-      <c r="F141" s="6"/>
-      <c r="H141" s="6"/>
-      <c r="I141" s="6"/>
-    </row>
-    <row r="142" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B142" s="6"/>
-      <c r="C142" s="6"/>
-      <c r="D142" s="6"/>
-      <c r="F142" s="6"/>
-      <c r="H142" s="6"/>
-      <c r="I142" s="6"/>
-    </row>
-    <row r="143" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B143" s="6"/>
-      <c r="C143" s="6"/>
-      <c r="D143" s="6"/>
-      <c r="F143" s="6"/>
-      <c r="H143" s="6"/>
-      <c r="I143" s="6"/>
-    </row>
-    <row r="144" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B144" s="6"/>
-      <c r="C144" s="6"/>
-      <c r="D144" s="6"/>
-      <c r="F144" s="6"/>
-      <c r="H144" s="6"/>
-      <c r="I144" s="6"/>
-    </row>
-    <row r="145" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B145" s="6"/>
-      <c r="C145" s="6"/>
-      <c r="D145" s="6"/>
-      <c r="F145" s="6"/>
-      <c r="H145" s="6"/>
-      <c r="I145" s="6"/>
-    </row>
-    <row r="146" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B146" s="6"/>
-      <c r="C146" s="6"/>
-      <c r="D146" s="6"/>
-      <c r="F146" s="6"/>
-      <c r="H146" s="6"/>
-      <c r="I146" s="6"/>
-    </row>
-    <row r="147" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B147" s="6"/>
-      <c r="C147" s="6"/>
-      <c r="D147" s="6"/>
-      <c r="F147" s="6"/>
-      <c r="H147" s="6"/>
-      <c r="I147" s="6"/>
-    </row>
-    <row r="148" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B148" s="6"/>
-      <c r="C148" s="6"/>
-      <c r="D148" s="6"/>
-      <c r="F148" s="6"/>
-      <c r="H148" s="6"/>
-      <c r="I148" s="6"/>
-    </row>
-    <row r="149" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B149" s="6"/>
-      <c r="C149" s="6"/>
-      <c r="D149" s="6"/>
-      <c r="F149" s="6"/>
-      <c r="H149" s="6"/>
-      <c r="I149" s="6"/>
-    </row>
-    <row r="150" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B150" s="6"/>
-      <c r="C150" s="6"/>
-      <c r="D150" s="6"/>
-      <c r="F150" s="6"/>
-      <c r="H150" s="6"/>
-      <c r="I150" s="6"/>
-    </row>
-    <row r="151" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B151" s="6"/>
-      <c r="C151" s="6"/>
-      <c r="D151" s="6"/>
-      <c r="F151" s="6"/>
-      <c r="H151" s="6"/>
-      <c r="I151" s="6"/>
-    </row>
-    <row r="152" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B152" s="6"/>
-      <c r="C152" s="6"/>
-      <c r="D152" s="6"/>
-      <c r="F152" s="6"/>
-      <c r="H152" s="6"/>
-      <c r="I152" s="6"/>
-    </row>
-    <row r="153" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B153" s="6"/>
-      <c r="C153" s="6"/>
-      <c r="D153" s="6"/>
-      <c r="F153" s="6"/>
-      <c r="H153" s="6"/>
-      <c r="I153" s="6"/>
-    </row>
-    <row r="154" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B154" s="6"/>
-      <c r="C154" s="6"/>
-      <c r="D154" s="6"/>
-      <c r="F154" s="6"/>
-      <c r="H154" s="6"/>
-      <c r="I154" s="6"/>
-    </row>
-    <row r="155" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B155" s="6"/>
-      <c r="C155" s="6"/>
-      <c r="D155" s="6"/>
-      <c r="F155" s="6"/>
-      <c r="H155" s="6"/>
-      <c r="I155" s="6"/>
-    </row>
-    <row r="156" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B156" s="6"/>
-      <c r="C156" s="6"/>
-      <c r="D156" s="6"/>
-      <c r="F156" s="6"/>
-      <c r="H156" s="6"/>
-      <c r="I156" s="6"/>
-    </row>
-    <row r="157" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B157" s="6"/>
-      <c r="C157" s="6"/>
-      <c r="D157" s="6"/>
-      <c r="F157" s="6"/>
-      <c r="H157" s="6"/>
-      <c r="I157" s="6"/>
-    </row>
-    <row r="158" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B158" s="6"/>
-      <c r="C158" s="6"/>
-      <c r="D158" s="6"/>
-      <c r="F158" s="6"/>
-      <c r="H158" s="6"/>
-      <c r="I158" s="6"/>
-    </row>
-    <row r="159" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B159" s="6"/>
-      <c r="C159" s="6"/>
-      <c r="D159" s="6"/>
-      <c r="F159" s="6"/>
-      <c r="H159" s="6"/>
-      <c r="I159" s="6"/>
-    </row>
-    <row r="160" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B160" s="6"/>
-      <c r="C160" s="6"/>
-      <c r="D160" s="6"/>
-      <c r="F160" s="6"/>
-      <c r="H160" s="6"/>
-      <c r="I160" s="6"/>
-    </row>
-    <row r="161" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B161" s="6"/>
-      <c r="C161" s="6"/>
-      <c r="D161" s="6"/>
-      <c r="F161" s="6"/>
-      <c r="H161" s="6"/>
-      <c r="I161" s="6"/>
-    </row>
-    <row r="162" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B162" s="6"/>
-      <c r="C162" s="6"/>
-      <c r="D162" s="6"/>
-      <c r="F162" s="6"/>
-      <c r="H162" s="6"/>
-      <c r="I162" s="6"/>
-    </row>
-    <row r="163" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B163" s="6"/>
-      <c r="C163" s="6"/>
-      <c r="D163" s="6"/>
-      <c r="F163" s="6"/>
-      <c r="H163" s="6"/>
-      <c r="I163" s="6"/>
-    </row>
-    <row r="164" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B164" s="6"/>
-      <c r="C164" s="6"/>
-      <c r="D164" s="6"/>
-      <c r="F164" s="6"/>
-      <c r="H164" s="6"/>
-      <c r="I164" s="6"/>
-    </row>
-    <row r="165" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B165" s="6"/>
-      <c r="C165" s="6"/>
-      <c r="D165" s="6"/>
-      <c r="F165" s="6"/>
-      <c r="H165" s="6"/>
-      <c r="I165" s="6"/>
-    </row>
-    <row r="166" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B166" s="6"/>
-      <c r="C166" s="6"/>
-      <c r="D166" s="6"/>
-      <c r="F166" s="6"/>
-      <c r="H166" s="6"/>
-      <c r="I166" s="6"/>
-    </row>
-    <row r="167" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B167" s="6"/>
-      <c r="C167" s="6"/>
-      <c r="D167" s="6"/>
-      <c r="F167" s="6"/>
-      <c r="H167" s="6"/>
-      <c r="I167" s="6"/>
-    </row>
-    <row r="168" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B168" s="6"/>
-      <c r="C168" s="6"/>
-      <c r="D168" s="6"/>
-      <c r="F168" s="6"/>
-      <c r="H168" s="6"/>
-      <c r="I168" s="6"/>
-    </row>
-    <row r="169" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B169" s="6"/>
-      <c r="C169" s="6"/>
-      <c r="D169" s="6"/>
-      <c r="F169" s="6"/>
-      <c r="H169" s="6"/>
-      <c r="I169" s="6"/>
-    </row>
-    <row r="170" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B170" s="6"/>
-      <c r="C170" s="6"/>
-      <c r="D170" s="6"/>
-      <c r="F170" s="6"/>
-      <c r="H170" s="6"/>
-      <c r="I170" s="6"/>
-    </row>
-    <row r="171" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B171" s="6"/>
-      <c r="C171" s="6"/>
-      <c r="D171" s="6"/>
-      <c r="F171" s="6"/>
-      <c r="H171" s="6"/>
-      <c r="I171" s="6"/>
-    </row>
-    <row r="172" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B172" s="6"/>
-      <c r="C172" s="6"/>
-      <c r="D172" s="6"/>
-      <c r="F172" s="6"/>
-      <c r="H172" s="6"/>
-      <c r="I172" s="6"/>
-    </row>
-    <row r="173" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B173" s="6"/>
-      <c r="C173" s="6"/>
-      <c r="D173" s="6"/>
-      <c r="F173" s="6"/>
-      <c r="H173" s="6"/>
-      <c r="I173" s="6"/>
-    </row>
-    <row r="174" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B174" s="6"/>
-      <c r="C174" s="6"/>
-      <c r="D174" s="6"/>
-      <c r="F174" s="6"/>
-      <c r="H174" s="6"/>
-      <c r="I174" s="6"/>
-    </row>
-    <row r="175" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B175" s="6"/>
-      <c r="C175" s="6"/>
-      <c r="D175" s="6"/>
-      <c r="F175" s="6"/>
-      <c r="H175" s="6"/>
-      <c r="I175" s="6"/>
-    </row>
-    <row r="176" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B176" s="6"/>
-      <c r="C176" s="6"/>
-      <c r="D176" s="6"/>
-      <c r="F176" s="6"/>
-      <c r="H176" s="6"/>
-      <c r="I176" s="6"/>
-    </row>
-    <row r="177" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B177" s="6"/>
-      <c r="C177" s="6"/>
-      <c r="D177" s="6"/>
-      <c r="F177" s="6"/>
-      <c r="H177" s="6"/>
-      <c r="I177" s="6"/>
-    </row>
-    <row r="178" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B178" s="6"/>
-      <c r="C178" s="6"/>
-      <c r="D178" s="6"/>
-      <c r="F178" s="6"/>
-      <c r="H178" s="6"/>
-      <c r="I178" s="6"/>
-    </row>
-    <row r="179" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B179" s="6"/>
-      <c r="C179" s="6"/>
-      <c r="D179" s="6"/>
-      <c r="F179" s="6"/>
-      <c r="H179" s="6"/>
-      <c r="I179" s="6"/>
-    </row>
-    <row r="180" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B180" s="6"/>
-      <c r="C180" s="6"/>
-      <c r="D180" s="6"/>
-      <c r="F180" s="6"/>
-      <c r="H180" s="6"/>
-      <c r="I180" s="6"/>
-    </row>
-    <row r="181" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B181" s="6"/>
-      <c r="C181" s="6"/>
-      <c r="D181" s="6"/>
-      <c r="F181" s="6"/>
-      <c r="H181" s="6"/>
-      <c r="I181" s="6"/>
-    </row>
-    <row r="182" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B182" s="6"/>
-      <c r="C182" s="6"/>
-      <c r="D182" s="6"/>
-      <c r="F182" s="6"/>
-      <c r="H182" s="6"/>
-      <c r="I182" s="6"/>
-    </row>
-    <row r="183" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B183" s="6"/>
-      <c r="C183" s="6"/>
-      <c r="D183" s="6"/>
-      <c r="F183" s="6"/>
-      <c r="H183" s="6"/>
-      <c r="I183" s="6"/>
-    </row>
-    <row r="184" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B184" s="6"/>
-      <c r="C184" s="6"/>
-      <c r="D184" s="6"/>
-      <c r="F184" s="6"/>
-      <c r="H184" s="6"/>
-      <c r="I184" s="6"/>
-    </row>
-    <row r="185" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B185" s="6"/>
-      <c r="C185" s="6"/>
-      <c r="D185" s="6"/>
-      <c r="F185" s="6"/>
-      <c r="H185" s="6"/>
-      <c r="I185" s="6"/>
-    </row>
-    <row r="186" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B186" s="6"/>
-      <c r="C186" s="6"/>
-      <c r="D186" s="6"/>
-      <c r="F186" s="6"/>
-      <c r="H186" s="6"/>
-      <c r="I186" s="6"/>
-    </row>
-    <row r="187" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B187" s="6"/>
-      <c r="C187" s="6"/>
-      <c r="D187" s="6"/>
-      <c r="F187" s="6"/>
-      <c r="H187" s="6"/>
-      <c r="I187" s="6"/>
-    </row>
-    <row r="188" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B188" s="6"/>
-      <c r="C188" s="6"/>
-      <c r="D188" s="6"/>
-      <c r="F188" s="6"/>
-      <c r="H188" s="6"/>
-      <c r="I188" s="6"/>
-    </row>
-    <row r="189" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B189" s="6"/>
-      <c r="C189" s="6"/>
-      <c r="D189" s="6"/>
-      <c r="F189" s="6"/>
-      <c r="H189" s="6"/>
-      <c r="I189" s="6"/>
-    </row>
-    <row r="190" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B190" s="6"/>
-      <c r="C190" s="6"/>
-      <c r="D190" s="6"/>
-      <c r="F190" s="6"/>
-      <c r="H190" s="6"/>
-      <c r="I190" s="6"/>
-    </row>
-    <row r="191" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B191" s="6"/>
-      <c r="C191" s="6"/>
-      <c r="D191" s="6"/>
-      <c r="F191" s="6"/>
-      <c r="H191" s="6"/>
-      <c r="I191" s="6"/>
-    </row>
-    <row r="192" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B192" s="6"/>
-      <c r="C192" s="6"/>
-      <c r="D192" s="6"/>
-      <c r="F192" s="6"/>
-      <c r="H192" s="6"/>
-      <c r="I192" s="6"/>
-    </row>
-    <row r="193" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B193" s="6"/>
-      <c r="C193" s="6"/>
-      <c r="D193" s="6"/>
-      <c r="F193" s="6"/>
-      <c r="H193" s="6"/>
-      <c r="I193" s="6"/>
-    </row>
-    <row r="194" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B194" s="6"/>
-      <c r="C194" s="6"/>
-      <c r="D194" s="6"/>
-      <c r="F194" s="6"/>
-      <c r="H194" s="6"/>
-      <c r="I194" s="6"/>
-    </row>
-    <row r="195" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B195" s="6"/>
-      <c r="C195" s="6"/>
-      <c r="D195" s="6"/>
-      <c r="F195" s="6"/>
-      <c r="H195" s="6"/>
-      <c r="I195" s="6"/>
-    </row>
-    <row r="196" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B196" s="6"/>
-      <c r="C196" s="6"/>
-      <c r="D196" s="6"/>
-      <c r="F196" s="6"/>
-      <c r="H196" s="6"/>
-      <c r="I196" s="6"/>
-    </row>
-    <row r="197" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B197" s="6"/>
-      <c r="C197" s="6"/>
-      <c r="D197" s="6"/>
-      <c r="F197" s="6"/>
-      <c r="H197" s="6"/>
-      <c r="I197" s="6"/>
-    </row>
-    <row r="198" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B198" s="6"/>
-      <c r="C198" s="6"/>
-      <c r="D198" s="6"/>
-      <c r="F198" s="6"/>
-      <c r="H198" s="6"/>
-      <c r="I198" s="6"/>
-    </row>
-    <row r="199" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B199" s="6"/>
-      <c r="C199" s="6"/>
-      <c r="D199" s="6"/>
-      <c r="F199" s="6"/>
-      <c r="H199" s="6"/>
-      <c r="I199" s="6"/>
-    </row>
-    <row r="200" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B200" s="6"/>
-      <c r="C200" s="6"/>
-      <c r="D200" s="6"/>
-      <c r="F200" s="6"/>
-      <c r="H200" s="6"/>
-      <c r="I200" s="6"/>
-    </row>
-    <row r="201" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B201" s="6"/>
-      <c r="C201" s="6"/>
-      <c r="D201" s="6"/>
-      <c r="F201" s="6"/>
-      <c r="H201" s="6"/>
-      <c r="I201" s="6"/>
-    </row>
-    <row r="202" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B202" s="6"/>
-      <c r="C202" s="6"/>
-      <c r="D202" s="6"/>
-      <c r="F202" s="6"/>
-      <c r="H202" s="6"/>
-      <c r="I202" s="6"/>
-    </row>
-    <row r="203" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B203" s="6"/>
-      <c r="C203" s="6"/>
-      <c r="D203" s="6"/>
-      <c r="F203" s="6"/>
-      <c r="H203" s="6"/>
-      <c r="I203" s="6"/>
-    </row>
-    <row r="204" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B204" s="6"/>
-      <c r="C204" s="6"/>
-      <c r="D204" s="6"/>
-      <c r="F204" s="6"/>
-      <c r="H204" s="6"/>
-      <c r="I204" s="6"/>
-    </row>
-    <row r="205" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B205" s="6"/>
-      <c r="C205" s="6"/>
-      <c r="D205" s="6"/>
-      <c r="F205" s="6"/>
-      <c r="H205" s="6"/>
-      <c r="I205" s="6"/>
-    </row>
-    <row r="206" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B206" s="6"/>
-      <c r="C206" s="6"/>
-      <c r="D206" s="6"/>
-      <c r="F206" s="6"/>
-      <c r="H206" s="6"/>
-      <c r="I206" s="6"/>
-    </row>
-    <row r="207" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B207" s="6"/>
-      <c r="C207" s="6"/>
-      <c r="D207" s="6"/>
-      <c r="F207" s="6"/>
-      <c r="H207" s="6"/>
-      <c r="I207" s="6"/>
-    </row>
-    <row r="208" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B208" s="6"/>
-      <c r="C208" s="6"/>
-      <c r="D208" s="6"/>
-      <c r="F208" s="6"/>
-      <c r="H208" s="6"/>
-      <c r="I208" s="6"/>
-    </row>
-    <row r="209" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B209" s="6"/>
-      <c r="C209" s="6"/>
-      <c r="D209" s="6"/>
-      <c r="F209" s="6"/>
-      <c r="H209" s="6"/>
-      <c r="I209" s="6"/>
-    </row>
-    <row r="210" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B210" s="6"/>
-      <c r="C210" s="6"/>
-      <c r="D210" s="6"/>
-      <c r="F210" s="6"/>
-      <c r="H210" s="6"/>
-      <c r="I210" s="6"/>
-    </row>
-    <row r="211" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B211" s="6"/>
-      <c r="C211" s="6"/>
-      <c r="D211" s="6"/>
-      <c r="F211" s="6"/>
-      <c r="H211" s="6"/>
-      <c r="I211" s="6"/>
-    </row>
-    <row r="212" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B212" s="6"/>
-      <c r="C212" s="6"/>
-      <c r="D212" s="6"/>
-      <c r="F212" s="6"/>
-      <c r="H212" s="6"/>
-      <c r="I212" s="6"/>
-    </row>
-    <row r="213" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B213" s="6"/>
-      <c r="C213" s="6"/>
-      <c r="D213" s="6"/>
-      <c r="F213" s="6"/>
-      <c r="H213" s="6"/>
-      <c r="I213" s="6"/>
-    </row>
-    <row r="214" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B214" s="6"/>
-      <c r="C214" s="6"/>
-      <c r="D214" s="6"/>
-      <c r="F214" s="6"/>
-      <c r="H214" s="6"/>
-      <c r="I214" s="6"/>
-    </row>
-    <row r="215" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B215" s="6"/>
-      <c r="C215" s="6"/>
-      <c r="D215" s="6"/>
-      <c r="F215" s="6"/>
-      <c r="H215" s="6"/>
-      <c r="I215" s="6"/>
-    </row>
-    <row r="216" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B216" s="6"/>
-      <c r="C216" s="6"/>
-      <c r="D216" s="6"/>
-      <c r="F216" s="6"/>
-      <c r="H216" s="6"/>
-      <c r="I216" s="6"/>
-    </row>
-    <row r="217" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B217" s="6"/>
-      <c r="C217" s="6"/>
-      <c r="D217" s="6"/>
-      <c r="F217" s="6"/>
-      <c r="H217" s="6"/>
-      <c r="I217" s="6"/>
-    </row>
-    <row r="218" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B218" s="6"/>
-      <c r="C218" s="6"/>
-      <c r="D218" s="6"/>
-      <c r="F218" s="6"/>
-      <c r="H218" s="6"/>
-      <c r="I218" s="6"/>
-    </row>
-    <row r="219" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B219" s="6"/>
-      <c r="C219" s="6"/>
-      <c r="D219" s="6"/>
-      <c r="F219" s="6"/>
-      <c r="H219" s="6"/>
-      <c r="I219" s="6"/>
-    </row>
-    <row r="220" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B220" s="6"/>
-      <c r="C220" s="6"/>
-      <c r="D220" s="6"/>
-      <c r="F220" s="6"/>
-      <c r="H220" s="6"/>
-      <c r="I220" s="6"/>
-    </row>
-    <row r="221" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B221" s="6"/>
-      <c r="C221" s="6"/>
-      <c r="D221" s="6"/>
-      <c r="F221" s="6"/>
-      <c r="H221" s="6"/>
-      <c r="I221" s="6"/>
-    </row>
-    <row r="222" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B222" s="6"/>
-      <c r="C222" s="6"/>
-      <c r="D222" s="6"/>
-      <c r="F222" s="6"/>
-      <c r="H222" s="6"/>
-      <c r="I222" s="6"/>
-    </row>
-    <row r="223" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B223" s="6"/>
-      <c r="C223" s="6"/>
-      <c r="D223" s="6"/>
-      <c r="F223" s="6"/>
-      <c r="H223" s="6"/>
-      <c r="I223" s="6"/>
-    </row>
-    <row r="224" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B224" s="6"/>
-      <c r="C224" s="6"/>
-      <c r="D224" s="6"/>
-      <c r="F224" s="6"/>
-      <c r="H224" s="6"/>
-      <c r="I224" s="6"/>
-    </row>
-    <row r="225" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B225" s="6"/>
-      <c r="C225" s="6"/>
-      <c r="D225" s="6"/>
-      <c r="F225" s="6"/>
-      <c r="H225" s="6"/>
-      <c r="I225" s="6"/>
-    </row>
-    <row r="226" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B226" s="6"/>
-      <c r="C226" s="6"/>
-      <c r="D226" s="6"/>
-      <c r="F226" s="6"/>
-      <c r="H226" s="6"/>
-      <c r="I226" s="6"/>
-    </row>
-    <row r="227" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B227" s="6"/>
-      <c r="C227" s="6"/>
-      <c r="D227" s="6"/>
-      <c r="F227" s="6"/>
-      <c r="H227" s="6"/>
-      <c r="I227" s="6"/>
-    </row>
-    <row r="228" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B228" s="6"/>
-      <c r="C228" s="6"/>
-      <c r="D228" s="6"/>
-      <c r="F228" s="6"/>
-      <c r="H228" s="6"/>
-      <c r="I228" s="6"/>
-    </row>
-    <row r="229" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B229" s="6"/>
-      <c r="C229" s="6"/>
-      <c r="D229" s="6"/>
-      <c r="F229" s="6"/>
-      <c r="H229" s="6"/>
-      <c r="I229" s="6"/>
-    </row>
-    <row r="230" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B230" s="6"/>
-      <c r="C230" s="6"/>
-      <c r="D230" s="6"/>
-      <c r="F230" s="6"/>
-      <c r="H230" s="6"/>
-      <c r="I230" s="6"/>
-    </row>
-    <row r="231" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B231" s="6"/>
-      <c r="C231" s="6"/>
-      <c r="D231" s="6"/>
-      <c r="F231" s="6"/>
-      <c r="H231" s="6"/>
-      <c r="I231" s="6"/>
-    </row>
-    <row r="232" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B232" s="6"/>
-      <c r="C232" s="6"/>
-      <c r="D232" s="6"/>
-      <c r="F232" s="6"/>
-      <c r="H232" s="6"/>
-      <c r="I232" s="6"/>
-    </row>
-    <row r="233" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B233" s="6"/>
-      <c r="C233" s="6"/>
-      <c r="D233" s="6"/>
-      <c r="F233" s="6"/>
-      <c r="H233" s="6"/>
-      <c r="I233" s="6"/>
-    </row>
-    <row r="234" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B234" s="6"/>
-      <c r="C234" s="6"/>
-      <c r="D234" s="6"/>
-      <c r="F234" s="6"/>
-      <c r="H234" s="6"/>
-      <c r="I234" s="6"/>
-    </row>
-    <row r="235" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B235" s="6"/>
-      <c r="C235" s="6"/>
-      <c r="D235" s="6"/>
-      <c r="F235" s="6"/>
-      <c r="H235" s="6"/>
-      <c r="I235" s="6"/>
-    </row>
-    <row r="236" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B236" s="6"/>
-      <c r="C236" s="6"/>
-      <c r="D236" s="6"/>
-      <c r="F236" s="6"/>
-      <c r="H236" s="6"/>
-      <c r="I236" s="6"/>
-    </row>
-    <row r="237" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B237" s="6"/>
-      <c r="C237" s="6"/>
-      <c r="D237" s="6"/>
-      <c r="F237" s="6"/>
-      <c r="H237" s="6"/>
-      <c r="I237" s="6"/>
-    </row>
-    <row r="238" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B238" s="6"/>
-      <c r="C238" s="6"/>
-      <c r="D238" s="6"/>
-      <c r="F238" s="6"/>
-      <c r="H238" s="6"/>
-      <c r="I238" s="6"/>
-    </row>
-    <row r="239" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B239" s="6"/>
-      <c r="C239" s="6"/>
-      <c r="D239" s="6"/>
-      <c r="F239" s="6"/>
-      <c r="H239" s="6"/>
-      <c r="I239" s="6"/>
-    </row>
-    <row r="240" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B240" s="6"/>
-      <c r="C240" s="6"/>
-      <c r="D240" s="6"/>
-      <c r="F240" s="6"/>
-      <c r="H240" s="6"/>
-      <c r="I240" s="6"/>
-    </row>
-    <row r="241" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B241" s="6"/>
-      <c r="C241" s="6"/>
-      <c r="D241" s="6"/>
-      <c r="F241" s="6"/>
-      <c r="H241" s="6"/>
-      <c r="I241" s="6"/>
-    </row>
-    <row r="242" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B242" s="6"/>
-      <c r="C242" s="6"/>
-      <c r="D242" s="6"/>
-      <c r="F242" s="6"/>
-      <c r="H242" s="6"/>
-      <c r="I242" s="6"/>
-    </row>
-    <row r="243" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B243" s="6"/>
-      <c r="C243" s="6"/>
-      <c r="D243" s="6"/>
-      <c r="F243" s="6"/>
-      <c r="H243" s="6"/>
-      <c r="I243" s="6"/>
-    </row>
-    <row r="244" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B244" s="6"/>
-      <c r="C244" s="6"/>
-      <c r="D244" s="6"/>
-      <c r="F244" s="6"/>
-      <c r="H244" s="6"/>
-      <c r="I244" s="6"/>
-    </row>
-    <row r="245" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B245" s="6"/>
-      <c r="C245" s="6"/>
-      <c r="D245" s="6"/>
-      <c r="F245" s="6"/>
-      <c r="H245" s="6"/>
-      <c r="I245" s="6"/>
-    </row>
-    <row r="246" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B246" s="6"/>
-      <c r="C246" s="6"/>
-      <c r="D246" s="6"/>
-      <c r="F246" s="6"/>
-      <c r="H246" s="6"/>
-      <c r="I246" s="6"/>
-    </row>
-    <row r="247" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B247" s="6"/>
-      <c r="C247" s="6"/>
-      <c r="D247" s="6"/>
-      <c r="F247" s="6"/>
-      <c r="H247" s="6"/>
-      <c r="I247" s="6"/>
-    </row>
-    <row r="248" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B248" s="6"/>
-      <c r="C248" s="6"/>
-      <c r="D248" s="6"/>
-      <c r="F248" s="6"/>
-      <c r="H248" s="6"/>
-      <c r="I248" s="6"/>
-    </row>
-    <row r="249" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B249" s="6"/>
-      <c r="C249" s="6"/>
-      <c r="D249" s="6"/>
-      <c r="F249" s="6"/>
-      <c r="H249" s="6"/>
-      <c r="I249" s="6"/>
-    </row>
-    <row r="250" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B250" s="6"/>
-      <c r="C250" s="6"/>
-      <c r="D250" s="6"/>
-      <c r="F250" s="6"/>
-      <c r="H250" s="6"/>
-      <c r="I250" s="6"/>
-    </row>
-    <row r="251" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B251" s="6"/>
-      <c r="C251" s="6"/>
-      <c r="D251" s="6"/>
-      <c r="F251" s="6"/>
-      <c r="H251" s="6"/>
-      <c r="I251" s="6"/>
-    </row>
-    <row r="252" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B252" s="6"/>
-      <c r="C252" s="6"/>
-      <c r="D252" s="6"/>
-      <c r="F252" s="6"/>
-      <c r="H252" s="6"/>
-      <c r="I252" s="6"/>
-    </row>
-    <row r="253" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B253" s="6"/>
-      <c r="C253" s="6"/>
-      <c r="D253" s="6"/>
-      <c r="F253" s="6"/>
-      <c r="H253" s="6"/>
-      <c r="I253" s="6"/>
-    </row>
-    <row r="254" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B254" s="6"/>
-      <c r="C254" s="6"/>
-      <c r="D254" s="6"/>
-      <c r="F254" s="6"/>
-      <c r="H254" s="6"/>
-      <c r="I254" s="6"/>
-    </row>
-    <row r="255" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B255" s="6"/>
-      <c r="C255" s="6"/>
-      <c r="D255" s="6"/>
-      <c r="F255" s="6"/>
-      <c r="H255" s="6"/>
-      <c r="I255" s="6"/>
-    </row>
-    <row r="256" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B256" s="6"/>
-      <c r="C256" s="6"/>
-      <c r="D256" s="6"/>
-      <c r="F256" s="6"/>
-      <c r="H256" s="6"/>
-      <c r="I256" s="6"/>
-    </row>
-    <row r="257" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B257" s="6"/>
-      <c r="C257" s="6"/>
-      <c r="D257" s="6"/>
-      <c r="F257" s="6"/>
-      <c r="H257" s="6"/>
-      <c r="I257" s="6"/>
-    </row>
-    <row r="258" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B258" s="6"/>
-      <c r="C258" s="6"/>
-      <c r="D258" s="6"/>
-      <c r="F258" s="6"/>
-      <c r="H258" s="6"/>
-      <c r="I258" s="6"/>
-    </row>
-    <row r="259" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B259" s="6"/>
-      <c r="C259" s="6"/>
-      <c r="D259" s="6"/>
-      <c r="F259" s="6"/>
-      <c r="H259" s="6"/>
-      <c r="I259" s="6"/>
-    </row>
-    <row r="260" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B260" s="6"/>
-      <c r="C260" s="6"/>
-      <c r="D260" s="6"/>
-      <c r="F260" s="6"/>
-      <c r="H260" s="6"/>
-      <c r="I260" s="6"/>
-    </row>
-    <row r="261" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B261" s="6"/>
-      <c r="C261" s="6"/>
-      <c r="D261" s="6"/>
-      <c r="F261" s="6"/>
-      <c r="H261" s="6"/>
-      <c r="I261" s="6"/>
-    </row>
-    <row r="262" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B262" s="6"/>
-      <c r="C262" s="6"/>
-      <c r="D262" s="6"/>
-      <c r="F262" s="6"/>
-      <c r="H262" s="6"/>
-      <c r="I262" s="6"/>
-    </row>
-    <row r="263" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B263" s="6"/>
-      <c r="C263" s="6"/>
-      <c r="D263" s="6"/>
-      <c r="F263" s="6"/>
-      <c r="H263" s="6"/>
-      <c r="I263" s="6"/>
-    </row>
-    <row r="264" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B264" s="6"/>
-      <c r="C264" s="6"/>
-      <c r="D264" s="6"/>
-      <c r="F264" s="6"/>
-      <c r="H264" s="6"/>
-      <c r="I264" s="6"/>
-    </row>
-    <row r="265" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B265" s="6"/>
-      <c r="C265" s="6"/>
-      <c r="D265" s="6"/>
-      <c r="F265" s="6"/>
-      <c r="H265" s="6"/>
-      <c r="I265" s="6"/>
-    </row>
-    <row r="266" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B266" s="6"/>
-      <c r="C266" s="6"/>
-      <c r="D266" s="6"/>
-      <c r="F266" s="6"/>
-      <c r="H266" s="6"/>
-      <c r="I266" s="6"/>
-    </row>
-    <row r="267" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B267" s="6"/>
-      <c r="C267" s="6"/>
-      <c r="D267" s="6"/>
-      <c r="F267" s="6"/>
-      <c r="H267" s="6"/>
-      <c r="I267" s="6"/>
-    </row>
-    <row r="268" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B268" s="6"/>
-      <c r="C268" s="6"/>
-      <c r="D268" s="6"/>
-      <c r="F268" s="6"/>
-      <c r="H268" s="6"/>
-      <c r="I268" s="6"/>
-    </row>
-    <row r="269" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B269" s="6"/>
-      <c r="C269" s="6"/>
-      <c r="D269" s="6"/>
-      <c r="F269" s="6"/>
-      <c r="H269" s="6"/>
-      <c r="I269" s="6"/>
-    </row>
-    <row r="270" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B270" s="6"/>
-      <c r="C270" s="6"/>
-      <c r="D270" s="6"/>
-      <c r="F270" s="6"/>
-      <c r="H270" s="6"/>
-      <c r="I270" s="6"/>
-    </row>
-    <row r="271" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B271" s="6"/>
-      <c r="C271" s="6"/>
-      <c r="D271" s="6"/>
-      <c r="F271" s="6"/>
-      <c r="H271" s="6"/>
-      <c r="I271" s="6"/>
-    </row>
-    <row r="272" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B272" s="6"/>
-      <c r="C272" s="6"/>
-      <c r="D272" s="6"/>
-      <c r="F272" s="6"/>
-      <c r="H272" s="6"/>
-      <c r="I272" s="6"/>
-    </row>
-    <row r="273" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B273" s="6"/>
-      <c r="C273" s="6"/>
-      <c r="D273" s="6"/>
-      <c r="F273" s="6"/>
-      <c r="H273" s="6"/>
-      <c r="I273" s="6"/>
-    </row>
-    <row r="274" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B274" s="6"/>
-      <c r="C274" s="6"/>
-      <c r="D274" s="6"/>
-      <c r="F274" s="6"/>
-      <c r="H274" s="6"/>
-      <c r="I274" s="6"/>
-    </row>
-    <row r="275" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B275" s="6"/>
-      <c r="C275" s="6"/>
-      <c r="D275" s="6"/>
-      <c r="F275" s="6"/>
-      <c r="H275" s="6"/>
-      <c r="I275" s="6"/>
-    </row>
-    <row r="276" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B276" s="6"/>
-      <c r="C276" s="6"/>
-      <c r="D276" s="6"/>
-      <c r="F276" s="6"/>
-      <c r="H276" s="6"/>
-      <c r="I276" s="6"/>
-    </row>
-    <row r="277" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B277" s="6"/>
-      <c r="C277" s="6"/>
-      <c r="D277" s="6"/>
-      <c r="F277" s="6"/>
-      <c r="H277" s="6"/>
-      <c r="I277" s="6"/>
-    </row>
-    <row r="278" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B278" s="6"/>
-      <c r="C278" s="6"/>
-      <c r="D278" s="6"/>
-      <c r="F278" s="6"/>
-      <c r="H278" s="6"/>
-      <c r="I278" s="6"/>
-    </row>
-    <row r="279" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B279" s="6"/>
-      <c r="C279" s="6"/>
-      <c r="D279" s="6"/>
-      <c r="F279" s="6"/>
-      <c r="H279" s="6"/>
-      <c r="I279" s="6"/>
-    </row>
-    <row r="280" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B280" s="6"/>
-      <c r="C280" s="6"/>
-      <c r="D280" s="6"/>
-      <c r="F280" s="6"/>
-      <c r="H280" s="6"/>
-      <c r="I280" s="6"/>
-    </row>
-    <row r="281" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B281" s="6"/>
-      <c r="C281" s="6"/>
-      <c r="D281" s="6"/>
-      <c r="F281" s="6"/>
-      <c r="H281" s="6"/>
-      <c r="I281" s="6"/>
-    </row>
-    <row r="282" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B282" s="6"/>
-      <c r="C282" s="6"/>
-      <c r="D282" s="6"/>
-      <c r="F282" s="6"/>
-      <c r="H282" s="6"/>
-      <c r="I282" s="6"/>
-    </row>
-    <row r="283" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B283" s="6"/>
-      <c r="C283" s="6"/>
-      <c r="D283" s="6"/>
-      <c r="F283" s="6"/>
-      <c r="H283" s="6"/>
-      <c r="I283" s="6"/>
-    </row>
-    <row r="284" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B284" s="6"/>
-      <c r="C284" s="6"/>
-      <c r="D284" s="6"/>
-      <c r="F284" s="6"/>
-      <c r="H284" s="6"/>
-      <c r="I284" s="6"/>
-    </row>
-    <row r="285" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B285" s="6"/>
-      <c r="C285" s="6"/>
-      <c r="D285" s="6"/>
-      <c r="F285" s="6"/>
-      <c r="H285" s="6"/>
-      <c r="I285" s="6"/>
-    </row>
-    <row r="286" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B286" s="6"/>
-      <c r="C286" s="6"/>
-      <c r="D286" s="6"/>
-      <c r="F286" s="6"/>
-      <c r="H286" s="6"/>
-      <c r="I286" s="6"/>
-    </row>
-    <row r="287" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B287" s="6"/>
-      <c r="C287" s="6"/>
-      <c r="D287" s="6"/>
-      <c r="F287" s="6"/>
-      <c r="H287" s="6"/>
-      <c r="I287" s="6"/>
-    </row>
-    <row r="288" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B288" s="6"/>
-      <c r="C288" s="6"/>
-      <c r="D288" s="6"/>
-      <c r="F288" s="6"/>
-      <c r="H288" s="6"/>
-      <c r="I288" s="6"/>
-    </row>
-    <row r="289" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B289" s="6"/>
-      <c r="C289" s="6"/>
-      <c r="D289" s="6"/>
-      <c r="F289" s="6"/>
-      <c r="H289" s="6"/>
-      <c r="I289" s="6"/>
-    </row>
-    <row r="290" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B290" s="6"/>
-      <c r="C290" s="6"/>
-      <c r="D290" s="6"/>
-      <c r="F290" s="6"/>
-      <c r="H290" s="6"/>
-      <c r="I290" s="6"/>
-    </row>
-    <row r="291" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B291" s="6"/>
-      <c r="C291" s="6"/>
-      <c r="D291" s="6"/>
-      <c r="F291" s="6"/>
-      <c r="H291" s="6"/>
-      <c r="I291" s="6"/>
-    </row>
-    <row r="292" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B292" s="6"/>
-      <c r="C292" s="6"/>
-      <c r="D292" s="6"/>
-      <c r="F292" s="6"/>
-      <c r="H292" s="6"/>
-      <c r="I292" s="6"/>
-    </row>
-    <row r="293" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B293" s="6"/>
-      <c r="C293" s="6"/>
-      <c r="D293" s="6"/>
-      <c r="F293" s="6"/>
-      <c r="H293" s="6"/>
-      <c r="I293" s="6"/>
-    </row>
-    <row r="294" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B294" s="6"/>
-      <c r="C294" s="6"/>
-      <c r="D294" s="6"/>
-      <c r="F294" s="6"/>
-      <c r="H294" s="6"/>
-      <c r="I294" s="6"/>
-    </row>
-    <row r="295" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B295" s="6"/>
-      <c r="C295" s="6"/>
-      <c r="D295" s="6"/>
-      <c r="F295" s="6"/>
-      <c r="H295" s="6"/>
-      <c r="I295" s="6"/>
-    </row>
-    <row r="296" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B296" s="6"/>
-      <c r="C296" s="6"/>
-      <c r="D296" s="6"/>
-      <c r="F296" s="6"/>
-      <c r="H296" s="6"/>
-      <c r="I296" s="6"/>
-    </row>
-    <row r="297" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B297" s="6"/>
-      <c r="C297" s="6"/>
-      <c r="D297" s="6"/>
-      <c r="F297" s="6"/>
-      <c r="H297" s="6"/>
-      <c r="I297" s="6"/>
-    </row>
-    <row r="298" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B298" s="6"/>
-      <c r="C298" s="6"/>
-      <c r="D298" s="6"/>
-      <c r="F298" s="6"/>
-      <c r="H298" s="6"/>
-      <c r="I298" s="6"/>
-    </row>
-    <row r="299" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B299" s="6"/>
-      <c r="C299" s="6"/>
-      <c r="D299" s="6"/>
-      <c r="F299" s="6"/>
-      <c r="H299" s="6"/>
-      <c r="I299" s="6"/>
-    </row>
-    <row r="300" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B300" s="6"/>
-      <c r="C300" s="6"/>
-      <c r="D300" s="6"/>
-      <c r="F300" s="6"/>
-      <c r="H300" s="6"/>
-      <c r="I300" s="6"/>
-    </row>
-    <row r="301" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B301" s="6"/>
-      <c r="C301" s="6"/>
-      <c r="D301" s="6"/>
-      <c r="F301" s="6"/>
-      <c r="H301" s="6"/>
-      <c r="I301" s="6"/>
-    </row>
-    <row r="302" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B302" s="6"/>
-      <c r="C302" s="6"/>
-      <c r="D302" s="6"/>
-      <c r="F302" s="6"/>
-      <c r="H302" s="6"/>
-      <c r="I302" s="6"/>
-    </row>
-    <row r="303" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B303" s="6"/>
-      <c r="C303" s="6"/>
-      <c r="D303" s="6"/>
-      <c r="F303" s="6"/>
-      <c r="H303" s="6"/>
-      <c r="I303" s="6"/>
-    </row>
-    <row r="304" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B304" s="6"/>
-      <c r="C304" s="6"/>
-      <c r="D304" s="6"/>
-      <c r="F304" s="6"/>
-      <c r="H304" s="6"/>
-      <c r="I304" s="6"/>
-    </row>
-    <row r="305" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B305" s="6"/>
-      <c r="C305" s="6"/>
-      <c r="D305" s="6"/>
-      <c r="F305" s="6"/>
-      <c r="H305" s="6"/>
-      <c r="I305" s="6"/>
-    </row>
-    <row r="306" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B306" s="6"/>
-      <c r="C306" s="6"/>
-      <c r="D306" s="6"/>
-      <c r="F306" s="6"/>
-      <c r="H306" s="6"/>
-      <c r="I306" s="6"/>
-    </row>
-    <row r="307" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B307" s="6"/>
-      <c r="C307" s="6"/>
-      <c r="D307" s="6"/>
-      <c r="F307" s="6"/>
-      <c r="H307" s="6"/>
-      <c r="I307" s="6"/>
-    </row>
-    <row r="308" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B308" s="6"/>
-      <c r="C308" s="6"/>
-      <c r="D308" s="6"/>
-      <c r="F308" s="6"/>
-      <c r="H308" s="6"/>
-      <c r="I308" s="6"/>
-    </row>
-    <row r="309" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B309" s="6"/>
-      <c r="C309" s="6"/>
-      <c r="D309" s="6"/>
-      <c r="F309" s="6"/>
-      <c r="H309" s="6"/>
-      <c r="I309" s="6"/>
-    </row>
-    <row r="310" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B310" s="6"/>
-      <c r="C310" s="6"/>
-      <c r="D310" s="6"/>
-      <c r="F310" s="6"/>
-      <c r="H310" s="6"/>
-      <c r="I310" s="6"/>
-    </row>
-    <row r="311" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B311" s="6"/>
-      <c r="C311" s="6"/>
-      <c r="D311" s="6"/>
-      <c r="F311" s="6"/>
-      <c r="H311" s="6"/>
-      <c r="I311" s="6"/>
-    </row>
-    <row r="312" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B312" s="6"/>
-      <c r="C312" s="6"/>
-      <c r="D312" s="6"/>
-      <c r="F312" s="6"/>
-      <c r="H312" s="6"/>
-      <c r="I312" s="6"/>
-    </row>
-    <row r="313" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B313" s="6"/>
-      <c r="C313" s="6"/>
-      <c r="D313" s="6"/>
-      <c r="F313" s="6"/>
-      <c r="H313" s="6"/>
-      <c r="I313" s="6"/>
-    </row>
-    <row r="314" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B314" s="6"/>
-      <c r="C314" s="6"/>
-      <c r="D314" s="6"/>
-      <c r="F314" s="6"/>
-      <c r="H314" s="6"/>
-      <c r="I314" s="6"/>
-    </row>
-    <row r="315" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B315" s="6"/>
-      <c r="C315" s="6"/>
-      <c r="D315" s="6"/>
-      <c r="F315" s="6"/>
-      <c r="H315" s="6"/>
-      <c r="I315" s="6"/>
-    </row>
-    <row r="316" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B316" s="6"/>
-      <c r="C316" s="6"/>
-      <c r="D316" s="6"/>
-      <c r="F316" s="6"/>
-      <c r="H316" s="6"/>
-      <c r="I316" s="6"/>
-    </row>
-    <row r="317" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B317" s="6"/>
-      <c r="C317" s="6"/>
-      <c r="D317" s="6"/>
-      <c r="F317" s="6"/>
-      <c r="H317" s="6"/>
-      <c r="I317" s="6"/>
-    </row>
-    <row r="318" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B318" s="6"/>
-      <c r="C318" s="6"/>
-      <c r="D318" s="6"/>
-      <c r="F318" s="6"/>
-      <c r="H318" s="6"/>
-      <c r="I318" s="6"/>
-    </row>
-    <row r="319" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B319" s="6"/>
-      <c r="C319" s="6"/>
-      <c r="D319" s="6"/>
-      <c r="F319" s="6"/>
-      <c r="H319" s="6"/>
-      <c r="I319" s="6"/>
-    </row>
-    <row r="320" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B320" s="6"/>
-      <c r="C320" s="6"/>
-      <c r="D320" s="6"/>
-      <c r="F320" s="6"/>
-      <c r="H320" s="6"/>
-      <c r="I320" s="6"/>
-    </row>
-    <row r="321" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B321" s="6"/>
-      <c r="C321" s="6"/>
-      <c r="D321" s="6"/>
-      <c r="F321" s="6"/>
-      <c r="H321" s="6"/>
-      <c r="I321" s="6"/>
-    </row>
-    <row r="322" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B322" s="6"/>
-      <c r="C322" s="6"/>
-      <c r="D322" s="6"/>
-      <c r="F322" s="6"/>
-      <c r="H322" s="6"/>
-      <c r="I322" s="6"/>
-    </row>
-    <row r="323" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B323" s="6"/>
-      <c r="C323" s="6"/>
-      <c r="D323" s="6"/>
-      <c r="F323" s="6"/>
-      <c r="H323" s="6"/>
-      <c r="I323" s="6"/>
-    </row>
-    <row r="324" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B324" s="6"/>
-      <c r="C324" s="6"/>
-      <c r="D324" s="6"/>
-      <c r="F324" s="6"/>
-      <c r="H324" s="6"/>
-      <c r="I324" s="6"/>
-    </row>
-    <row r="325" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B325" s="6"/>
-      <c r="C325" s="6"/>
-      <c r="D325" s="6"/>
-      <c r="F325" s="6"/>
-      <c r="H325" s="6"/>
-      <c r="I325" s="6"/>
-    </row>
-    <row r="326" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B326" s="6"/>
-      <c r="C326" s="6"/>
-      <c r="D326" s="6"/>
-      <c r="F326" s="6"/>
-      <c r="H326" s="6"/>
-      <c r="I326" s="6"/>
-    </row>
-    <row r="327" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B327" s="6"/>
-      <c r="C327" s="6"/>
-      <c r="D327" s="6"/>
-      <c r="F327" s="6"/>
-      <c r="H327" s="6"/>
-      <c r="I327" s="6"/>
-    </row>
-    <row r="328" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B328" s="6"/>
-      <c r="C328" s="6"/>
-      <c r="D328" s="6"/>
-      <c r="F328" s="6"/>
-      <c r="H328" s="6"/>
-      <c r="I328" s="6"/>
-    </row>
-    <row r="329" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B329" s="6"/>
-      <c r="C329" s="6"/>
-      <c r="D329" s="6"/>
-      <c r="F329" s="6"/>
-      <c r="H329" s="6"/>
-      <c r="I329" s="6"/>
-    </row>
-    <row r="330" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B330" s="6"/>
-      <c r="C330" s="6"/>
-      <c r="D330" s="6"/>
-      <c r="F330" s="6"/>
-      <c r="H330" s="6"/>
-      <c r="I330" s="6"/>
-    </row>
-    <row r="331" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B331" s="6"/>
-      <c r="C331" s="6"/>
-      <c r="D331" s="6"/>
-      <c r="F331" s="6"/>
-      <c r="H331" s="6"/>
-      <c r="I331" s="6"/>
-    </row>
-    <row r="332" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B332" s="6"/>
-      <c r="C332" s="6"/>
-      <c r="D332" s="6"/>
-      <c r="F332" s="6"/>
-      <c r="H332" s="6"/>
-      <c r="I332" s="6"/>
-    </row>
-    <row r="333" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B333" s="6"/>
-      <c r="C333" s="6"/>
-      <c r="D333" s="6"/>
-      <c r="F333" s="6"/>
-      <c r="H333" s="6"/>
-      <c r="I333" s="6"/>
-    </row>
-    <row r="334" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B334" s="6"/>
-      <c r="C334" s="6"/>
-      <c r="D334" s="6"/>
-      <c r="F334" s="6"/>
-      <c r="H334" s="6"/>
-      <c r="I334" s="6"/>
-    </row>
-    <row r="335" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B335" s="6"/>
-      <c r="C335" s="6"/>
-      <c r="D335" s="6"/>
-      <c r="F335" s="6"/>
-      <c r="H335" s="6"/>
-      <c r="I335" s="6"/>
-    </row>
-    <row r="336" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B336" s="6"/>
-      <c r="C336" s="6"/>
-      <c r="D336" s="6"/>
-      <c r="F336" s="6"/>
-      <c r="H336" s="6"/>
-      <c r="I336" s="6"/>
-    </row>
-    <row r="337" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B337" s="6"/>
-      <c r="C337" s="6"/>
-      <c r="D337" s="6"/>
-      <c r="F337" s="6"/>
-      <c r="H337" s="6"/>
-      <c r="I337" s="6"/>
-    </row>
-    <row r="338" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B338" s="6"/>
-      <c r="C338" s="6"/>
-      <c r="D338" s="6"/>
-      <c r="F338" s="6"/>
-      <c r="H338" s="6"/>
-      <c r="I338" s="6"/>
-    </row>
-    <row r="339" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B339" s="6"/>
-      <c r="C339" s="6"/>
-      <c r="D339" s="6"/>
-      <c r="F339" s="6"/>
-      <c r="H339" s="6"/>
-      <c r="I339" s="6"/>
-    </row>
-    <row r="340" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B340" s="6"/>
-      <c r="C340" s="6"/>
-      <c r="D340" s="6"/>
-      <c r="F340" s="6"/>
-      <c r="H340" s="6"/>
-      <c r="I340" s="6"/>
-    </row>
-    <row r="341" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B341" s="6"/>
-      <c r="C341" s="6"/>
-      <c r="D341" s="6"/>
-      <c r="F341" s="6"/>
-      <c r="H341" s="6"/>
-      <c r="I341" s="6"/>
-    </row>
-    <row r="342" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B342" s="6"/>
-      <c r="C342" s="6"/>
-      <c r="D342" s="6"/>
-      <c r="F342" s="6"/>
-      <c r="H342" s="6"/>
-      <c r="I342" s="6"/>
-    </row>
-    <row r="343" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B343" s="6"/>
-      <c r="C343" s="6"/>
-      <c r="D343" s="6"/>
-      <c r="F343" s="6"/>
-      <c r="H343" s="6"/>
-      <c r="I343" s="6"/>
-    </row>
-    <row r="344" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B344" s="6"/>
-      <c r="C344" s="6"/>
-      <c r="D344" s="6"/>
-      <c r="F344" s="6"/>
-      <c r="H344" s="6"/>
-      <c r="I344" s="6"/>
-    </row>
-    <row r="345" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B345" s="6"/>
-      <c r="C345" s="6"/>
-      <c r="D345" s="6"/>
-      <c r="F345" s="6"/>
-      <c r="H345" s="6"/>
-      <c r="I345" s="6"/>
-    </row>
-    <row r="346" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B346" s="6"/>
-      <c r="C346" s="6"/>
-      <c r="D346" s="6"/>
-      <c r="F346" s="6"/>
-      <c r="H346" s="6"/>
-      <c r="I346" s="6"/>
-    </row>
-    <row r="347" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B347" s="6"/>
-      <c r="C347" s="6"/>
-      <c r="D347" s="6"/>
-      <c r="F347" s="6"/>
-      <c r="H347" s="6"/>
-      <c r="I347" s="6"/>
-    </row>
-    <row r="348" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B348" s="6"/>
-      <c r="C348" s="6"/>
-      <c r="D348" s="6"/>
-      <c r="F348" s="6"/>
-      <c r="H348" s="6"/>
-      <c r="I348" s="6"/>
-    </row>
-    <row r="349" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B349" s="6"/>
-      <c r="C349" s="6"/>
-      <c r="D349" s="6"/>
-      <c r="F349" s="6"/>
-      <c r="H349" s="6"/>
-      <c r="I349" s="6"/>
-    </row>
-    <row r="350" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B350" s="6"/>
-      <c r="C350" s="6"/>
-      <c r="D350" s="6"/>
-      <c r="F350" s="6"/>
-      <c r="H350" s="6"/>
-      <c r="I350" s="6"/>
-    </row>
-    <row r="351" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B351" s="6"/>
-      <c r="C351" s="6"/>
-      <c r="D351" s="6"/>
-      <c r="F351" s="6"/>
-      <c r="H351" s="6"/>
-      <c r="I351" s="6"/>
-    </row>
-    <row r="352" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B352" s="6"/>
-      <c r="C352" s="6"/>
-      <c r="D352" s="6"/>
-      <c r="F352" s="6"/>
-      <c r="H352" s="6"/>
-      <c r="I352" s="6"/>
-    </row>
-    <row r="353" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B353" s="6"/>
-      <c r="C353" s="6"/>
-      <c r="D353" s="6"/>
-      <c r="F353" s="6"/>
-      <c r="H353" s="6"/>
-      <c r="I353" s="6"/>
-    </row>
-    <row r="354" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B354" s="6"/>
-      <c r="C354" s="6"/>
-      <c r="D354" s="6"/>
-      <c r="F354" s="6"/>
-      <c r="H354" s="6"/>
-      <c r="I354" s="6"/>
-    </row>
-    <row r="355" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B355" s="6"/>
-      <c r="C355" s="6"/>
-      <c r="D355" s="6"/>
-      <c r="F355" s="6"/>
-      <c r="H355" s="6"/>
-      <c r="I355" s="6"/>
-    </row>
-    <row r="356" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B356" s="6"/>
-      <c r="C356" s="6"/>
-      <c r="D356" s="6"/>
-      <c r="F356" s="6"/>
-      <c r="H356" s="6"/>
-      <c r="I356" s="6"/>
-    </row>
-    <row r="357" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B357" s="6"/>
-      <c r="C357" s="6"/>
-      <c r="D357" s="6"/>
-      <c r="F357" s="6"/>
-      <c r="H357" s="6"/>
-      <c r="I357" s="6"/>
-    </row>
-    <row r="358" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B358" s="6"/>
-      <c r="C358" s="6"/>
-      <c r="D358" s="6"/>
-      <c r="F358" s="6"/>
-      <c r="H358" s="6"/>
-      <c r="I358" s="6"/>
-    </row>
-    <row r="359" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B359" s="6"/>
-      <c r="C359" s="6"/>
-      <c r="D359" s="6"/>
-      <c r="F359" s="6"/>
-      <c r="H359" s="6"/>
-      <c r="I359" s="6"/>
-    </row>
-    <row r="360" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B360" s="6"/>
-      <c r="C360" s="6"/>
-      <c r="D360" s="6"/>
-      <c r="F360" s="6"/>
-      <c r="H360" s="6"/>
-      <c r="I360" s="6"/>
-    </row>
-    <row r="361" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B361" s="6"/>
-      <c r="C361" s="6"/>
-      <c r="D361" s="6"/>
-      <c r="F361" s="6"/>
-      <c r="H361" s="6"/>
-      <c r="I361" s="6"/>
-    </row>
-    <row r="362" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B362" s="6"/>
-      <c r="C362" s="6"/>
-      <c r="D362" s="6"/>
-      <c r="F362" s="6"/>
-      <c r="H362" s="6"/>
-      <c r="I362" s="6"/>
-    </row>
-    <row r="363" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B363" s="6"/>
-      <c r="C363" s="6"/>
-      <c r="D363" s="6"/>
-      <c r="F363" s="6"/>
-      <c r="H363" s="6"/>
-      <c r="I363" s="6"/>
-    </row>
-    <row r="364" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B364" s="6"/>
-      <c r="C364" s="6"/>
-      <c r="D364" s="6"/>
-      <c r="F364" s="6"/>
-      <c r="H364" s="6"/>
-      <c r="I364" s="6"/>
-    </row>
-    <row r="365" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B365" s="6"/>
-      <c r="C365" s="6"/>
-      <c r="D365" s="6"/>
-      <c r="F365" s="6"/>
-      <c r="H365" s="6"/>
-      <c r="I365" s="6"/>
-    </row>
-    <row r="366" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B366" s="6"/>
-      <c r="C366" s="6"/>
-      <c r="D366" s="6"/>
-      <c r="F366" s="6"/>
-      <c r="H366" s="6"/>
-      <c r="I366" s="6"/>
-    </row>
-    <row r="367" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B367" s="6"/>
-      <c r="C367" s="6"/>
-      <c r="D367" s="6"/>
-      <c r="F367" s="6"/>
-      <c r="H367" s="6"/>
-      <c r="I367" s="6"/>
-    </row>
-    <row r="368" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B368" s="6"/>
-      <c r="C368" s="6"/>
-      <c r="D368" s="6"/>
-      <c r="F368" s="6"/>
-      <c r="H368" s="6"/>
-      <c r="I368" s="6"/>
-    </row>
-    <row r="369" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B369" s="6"/>
-      <c r="C369" s="6"/>
-      <c r="D369" s="6"/>
-      <c r="F369" s="6"/>
-      <c r="H369" s="6"/>
-      <c r="I369" s="6"/>
-    </row>
-    <row r="370" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B370" s="6"/>
-      <c r="C370" s="6"/>
-      <c r="D370" s="6"/>
-      <c r="F370" s="6"/>
-      <c r="H370" s="6"/>
-      <c r="I370" s="6"/>
-    </row>
-    <row r="371" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B371" s="6"/>
-      <c r="C371" s="6"/>
-      <c r="D371" s="6"/>
-      <c r="F371" s="6"/>
-      <c r="H371" s="6"/>
-      <c r="I371" s="6"/>
-    </row>
-    <row r="372" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B372" s="6"/>
-      <c r="C372" s="6"/>
-      <c r="D372" s="6"/>
-      <c r="F372" s="6"/>
-      <c r="H372" s="6"/>
-      <c r="I372" s="6"/>
-    </row>
-    <row r="373" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B373" s="6"/>
-      <c r="C373" s="6"/>
-      <c r="D373" s="6"/>
-      <c r="F373" s="6"/>
-      <c r="H373" s="6"/>
-      <c r="I373" s="6"/>
-    </row>
-    <row r="374" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B374" s="6"/>
-      <c r="C374" s="6"/>
-      <c r="D374" s="6"/>
-      <c r="F374" s="6"/>
-      <c r="H374" s="6"/>
-      <c r="I374" s="6"/>
-    </row>
-    <row r="375" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B375" s="6"/>
-      <c r="C375" s="6"/>
-      <c r="D375" s="6"/>
-      <c r="F375" s="6"/>
-      <c r="H375" s="6"/>
-      <c r="I375" s="6"/>
-    </row>
-    <row r="376" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B376" s="6"/>
-      <c r="C376" s="6"/>
-      <c r="D376" s="6"/>
-      <c r="F376" s="6"/>
-      <c r="H376" s="6"/>
-      <c r="I376" s="6"/>
-    </row>
-    <row r="377" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B377" s="6"/>
-      <c r="C377" s="6"/>
-      <c r="D377" s="6"/>
-      <c r="F377" s="6"/>
-      <c r="H377" s="6"/>
-      <c r="I377" s="6"/>
-    </row>
-    <row r="378" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B378" s="6"/>
-      <c r="C378" s="6"/>
-      <c r="D378" s="6"/>
-      <c r="F378" s="6"/>
-      <c r="H378" s="6"/>
-      <c r="I378" s="6"/>
-    </row>
-    <row r="379" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B379" s="6"/>
-      <c r="C379" s="6"/>
-      <c r="D379" s="6"/>
-      <c r="F379" s="6"/>
-      <c r="H379" s="6"/>
-      <c r="I379" s="6"/>
-    </row>
-    <row r="380" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B380" s="6"/>
-      <c r="C380" s="6"/>
-      <c r="D380" s="6"/>
-      <c r="F380" s="6"/>
-      <c r="H380" s="6"/>
-      <c r="I380" s="6"/>
-    </row>
-    <row r="381" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B381" s="6"/>
-      <c r="C381" s="6"/>
-      <c r="D381" s="6"/>
-      <c r="F381" s="6"/>
-      <c r="H381" s="6"/>
-      <c r="I381" s="6"/>
-    </row>
-    <row r="382" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B382" s="6"/>
-      <c r="C382" s="6"/>
-      <c r="D382" s="6"/>
-      <c r="F382" s="6"/>
-      <c r="H382" s="6"/>
-      <c r="I382" s="6"/>
-    </row>
-    <row r="383" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B383" s="6"/>
-      <c r="C383" s="6"/>
-      <c r="D383" s="6"/>
-      <c r="F383" s="6"/>
-      <c r="H383" s="6"/>
-      <c r="I383" s="6"/>
-    </row>
-    <row r="384" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B384" s="6"/>
-      <c r="C384" s="6"/>
-      <c r="D384" s="6"/>
-      <c r="F384" s="6"/>
-      <c r="H384" s="6"/>
-      <c r="I384" s="6"/>
-    </row>
-    <row r="385" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B385" s="6"/>
-      <c r="C385" s="6"/>
-      <c r="D385" s="6"/>
-      <c r="F385" s="6"/>
-      <c r="H385" s="6"/>
-      <c r="I385" s="6"/>
-    </row>
-    <row r="386" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B386" s="6"/>
-      <c r="C386" s="6"/>
-      <c r="D386" s="6"/>
-      <c r="F386" s="6"/>
-      <c r="H386" s="6"/>
-      <c r="I386" s="6"/>
-    </row>
-    <row r="387" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B387" s="6"/>
-      <c r="C387" s="6"/>
-      <c r="D387" s="6"/>
-      <c r="F387" s="6"/>
-      <c r="H387" s="6"/>
-      <c r="I387" s="6"/>
-    </row>
-    <row r="388" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B388" s="6"/>
-      <c r="C388" s="6"/>
-      <c r="D388" s="6"/>
-      <c r="F388" s="6"/>
-      <c r="H388" s="6"/>
-      <c r="I388" s="6"/>
-    </row>
-    <row r="389" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B389" s="6"/>
-      <c r="C389" s="6"/>
-      <c r="D389" s="6"/>
-      <c r="F389" s="6"/>
-      <c r="H389" s="6"/>
-      <c r="I389" s="6"/>
-    </row>
-    <row r="390" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B390" s="6"/>
-      <c r="C390" s="6"/>
-      <c r="D390" s="6"/>
-      <c r="F390" s="6"/>
-      <c r="H390" s="6"/>
-      <c r="I390" s="6"/>
-    </row>
-    <row r="391" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B391" s="6"/>
-      <c r="C391" s="6"/>
-      <c r="D391" s="6"/>
-      <c r="F391" s="6"/>
-      <c r="H391" s="6"/>
-      <c r="I391" s="6"/>
-    </row>
-    <row r="392" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B392" s="6"/>
-      <c r="C392" s="6"/>
-      <c r="D392" s="6"/>
-      <c r="F392" s="6"/>
-      <c r="H392" s="6"/>
-      <c r="I392" s="6"/>
-    </row>
-    <row r="393" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B393" s="6"/>
-      <c r="C393" s="6"/>
-      <c r="D393" s="6"/>
-      <c r="F393" s="6"/>
-      <c r="H393" s="6"/>
-      <c r="I393" s="6"/>
-    </row>
-    <row r="394" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B394" s="6"/>
-      <c r="C394" s="6"/>
-      <c r="D394" s="6"/>
-      <c r="F394" s="6"/>
-      <c r="H394" s="6"/>
-      <c r="I394" s="6"/>
-    </row>
-    <row r="395" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B395" s="6"/>
-      <c r="C395" s="6"/>
-      <c r="D395" s="6"/>
-      <c r="F395" s="6"/>
-      <c r="H395" s="6"/>
-      <c r="I395" s="6"/>
-    </row>
-    <row r="396" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B396" s="6"/>
-      <c r="C396" s="6"/>
-      <c r="D396" s="6"/>
-      <c r="F396" s="6"/>
-      <c r="H396" s="6"/>
-      <c r="I396" s="6"/>
-    </row>
-    <row r="397" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B397" s="6"/>
-      <c r="C397" s="6"/>
-      <c r="D397" s="6"/>
-      <c r="F397" s="6"/>
-      <c r="H397" s="6"/>
-      <c r="I397" s="6"/>
-    </row>
-    <row r="398" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B398" s="6"/>
-      <c r="C398" s="6"/>
-      <c r="D398" s="6"/>
-      <c r="F398" s="6"/>
-      <c r="H398" s="6"/>
-      <c r="I398" s="6"/>
-    </row>
-    <row r="399" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B399" s="6"/>
-      <c r="C399" s="6"/>
-      <c r="D399" s="6"/>
-      <c r="F399" s="6"/>
-      <c r="H399" s="6"/>
-      <c r="I399" s="6"/>
-    </row>
-    <row r="400" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B400" s="6"/>
-      <c r="C400" s="6"/>
-      <c r="D400" s="6"/>
-      <c r="F400" s="6"/>
-      <c r="H400" s="6"/>
-      <c r="I400" s="6"/>
-    </row>
-    <row r="401" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B401" s="6"/>
-      <c r="C401" s="6"/>
-      <c r="D401" s="6"/>
-      <c r="F401" s="6"/>
-      <c r="H401" s="6"/>
-      <c r="I401" s="6"/>
-    </row>
-    <row r="402" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B402" s="6"/>
-      <c r="C402" s="6"/>
-      <c r="D402" s="6"/>
-      <c r="F402" s="6"/>
-      <c r="H402" s="6"/>
-      <c r="I402" s="6"/>
-    </row>
-    <row r="403" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B403" s="6"/>
-      <c r="C403" s="6"/>
-      <c r="D403" s="6"/>
-      <c r="F403" s="6"/>
-      <c r="H403" s="6"/>
-      <c r="I403" s="6"/>
-    </row>
-    <row r="404" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B404" s="6"/>
-      <c r="C404" s="6"/>
-      <c r="D404" s="6"/>
-      <c r="F404" s="6"/>
-      <c r="H404" s="6"/>
-      <c r="I404" s="6"/>
-    </row>
-    <row r="405" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B405" s="6"/>
-      <c r="C405" s="6"/>
-      <c r="D405" s="6"/>
-      <c r="F405" s="6"/>
-      <c r="H405" s="6"/>
-      <c r="I405" s="6"/>
-    </row>
-    <row r="406" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B406" s="6"/>
-      <c r="C406" s="6"/>
-      <c r="D406" s="6"/>
-      <c r="F406" s="6"/>
-      <c r="H406" s="6"/>
-      <c r="I406" s="6"/>
-    </row>
-    <row r="407" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B407" s="6"/>
-      <c r="C407" s="6"/>
-      <c r="D407" s="6"/>
-      <c r="F407" s="6"/>
-      <c r="H407" s="6"/>
-      <c r="I407" s="6"/>
-    </row>
-    <row r="408" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B408" s="6"/>
-      <c r="C408" s="6"/>
-      <c r="D408" s="6"/>
-      <c r="F408" s="6"/>
-      <c r="H408" s="6"/>
-      <c r="I408" s="6"/>
-    </row>
-    <row r="409" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B409" s="6"/>
-      <c r="C409" s="6"/>
-      <c r="D409" s="6"/>
-      <c r="F409" s="6"/>
-      <c r="H409" s="6"/>
-      <c r="I409" s="6"/>
-    </row>
-    <row r="410" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B410" s="6"/>
-      <c r="C410" s="6"/>
-      <c r="D410" s="6"/>
-      <c r="F410" s="6"/>
-      <c r="H410" s="6"/>
-      <c r="I410" s="6"/>
-    </row>
-    <row r="411" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B411" s="6"/>
-      <c r="C411" s="6"/>
-      <c r="D411" s="6"/>
-      <c r="F411" s="6"/>
-      <c r="H411" s="6"/>
-      <c r="I411" s="6"/>
-    </row>
-    <row r="412" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B412" s="6"/>
-      <c r="C412" s="6"/>
-      <c r="D412" s="6"/>
-      <c r="F412" s="6"/>
-      <c r="H412" s="6"/>
-      <c r="I412" s="6"/>
-    </row>
-    <row r="413" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B413" s="6"/>
-      <c r="C413" s="6"/>
-      <c r="D413" s="6"/>
-      <c r="F413" s="6"/>
-      <c r="H413" s="6"/>
-      <c r="I413" s="6"/>
-    </row>
-    <row r="414" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B414" s="6"/>
-      <c r="C414" s="6"/>
-      <c r="D414" s="6"/>
-      <c r="F414" s="6"/>
-      <c r="H414" s="6"/>
-      <c r="I414" s="6"/>
-    </row>
-    <row r="415" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B415" s="6"/>
-      <c r="C415" s="6"/>
-      <c r="D415" s="6"/>
-      <c r="F415" s="6"/>
-      <c r="H415" s="6"/>
-      <c r="I415" s="6"/>
-    </row>
-    <row r="416" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B416" s="6"/>
-      <c r="C416" s="6"/>
-      <c r="D416" s="6"/>
-      <c r="F416" s="6"/>
-      <c r="H416" s="6"/>
-      <c r="I416" s="6"/>
-    </row>
-    <row r="417" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B417" s="6"/>
-      <c r="C417" s="6"/>
-      <c r="D417" s="6"/>
-      <c r="F417" s="6"/>
-      <c r="H417" s="6"/>
-      <c r="I417" s="6"/>
-    </row>
-    <row r="418" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B418" s="6"/>
-      <c r="C418" s="6"/>
-      <c r="D418" s="6"/>
-      <c r="F418" s="6"/>
-      <c r="H418" s="6"/>
-      <c r="I418" s="6"/>
-    </row>
-    <row r="419" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B419" s="6"/>
-      <c r="C419" s="6"/>
-      <c r="D419" s="6"/>
-      <c r="F419" s="6"/>
-      <c r="H419" s="6"/>
-      <c r="I419" s="6"/>
-    </row>
-    <row r="420" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B420" s="6"/>
-      <c r="C420" s="6"/>
-      <c r="D420" s="6"/>
-      <c r="F420" s="6"/>
-      <c r="H420" s="6"/>
-      <c r="I420" s="6"/>
-    </row>
-    <row r="421" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B421" s="6"/>
-      <c r="C421" s="6"/>
-      <c r="D421" s="6"/>
-      <c r="F421" s="6"/>
-      <c r="H421" s="6"/>
-      <c r="I421" s="6"/>
-    </row>
-    <row r="422" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B422" s="6"/>
-      <c r="C422" s="6"/>
-      <c r="D422" s="6"/>
-      <c r="F422" s="6"/>
-      <c r="H422" s="6"/>
-      <c r="I422" s="6"/>
-    </row>
-    <row r="423" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B423" s="6"/>
-      <c r="C423" s="6"/>
-      <c r="D423" s="6"/>
-      <c r="F423" s="6"/>
-      <c r="H423" s="6"/>
-      <c r="I423" s="6"/>
-    </row>
-    <row r="424" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B424" s="6"/>
-      <c r="C424" s="6"/>
-      <c r="D424" s="6"/>
-      <c r="F424" s="6"/>
-      <c r="H424" s="6"/>
-      <c r="I424" s="6"/>
-    </row>
-    <row r="425" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B425" s="6"/>
-      <c r="C425" s="6"/>
-      <c r="D425" s="6"/>
-      <c r="F425" s="6"/>
-      <c r="H425" s="6"/>
-      <c r="I425" s="6"/>
-    </row>
-    <row r="426" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B426" s="6"/>
-      <c r="C426" s="6"/>
-      <c r="D426" s="6"/>
-      <c r="F426" s="6"/>
-      <c r="H426" s="6"/>
-      <c r="I426" s="6"/>
-    </row>
-    <row r="427" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B427" s="6"/>
-      <c r="C427" s="6"/>
-      <c r="D427" s="6"/>
-      <c r="F427" s="6"/>
-      <c r="H427" s="6"/>
-      <c r="I427" s="6"/>
-    </row>
-    <row r="428" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B428" s="6"/>
-      <c r="C428" s="6"/>
-      <c r="D428" s="6"/>
-      <c r="F428" s="6"/>
-      <c r="H428" s="6"/>
-      <c r="I428" s="6"/>
-    </row>
-    <row r="429" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B429" s="6"/>
-      <c r="C429" s="6"/>
-      <c r="D429" s="6"/>
-      <c r="F429" s="6"/>
-      <c r="H429" s="6"/>
-      <c r="I429" s="6"/>
-    </row>
-    <row r="430" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B430" s="6"/>
-      <c r="C430" s="6"/>
-      <c r="D430" s="6"/>
-      <c r="F430" s="6"/>
-      <c r="H430" s="6"/>
-      <c r="I430" s="6"/>
-    </row>
-    <row r="431" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B431" s="6"/>
-      <c r="C431" s="6"/>
-      <c r="D431" s="6"/>
-      <c r="F431" s="6"/>
-      <c r="H431" s="6"/>
-      <c r="I431" s="6"/>
-    </row>
-    <row r="432" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B432" s="6"/>
-      <c r="C432" s="6"/>
-      <c r="D432" s="6"/>
-      <c r="F432" s="6"/>
-      <c r="H432" s="6"/>
-      <c r="I432" s="6"/>
-    </row>
-    <row r="433" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B433" s="6"/>
-      <c r="C433" s="6"/>
-      <c r="D433" s="6"/>
-      <c r="F433" s="6"/>
-      <c r="H433" s="6"/>
-      <c r="I433" s="6"/>
-    </row>
-    <row r="434" spans="2:9" ht="24.95" customHeight="1">
-      <c r="B434" s="6"/>
-      <c r="C434" s="6"/>
-      <c r="D434" s="6"/>
-      <c r="F434" s="6"/>
-      <c r="H434" s="6"/>
-      <c r="I434" s="6"/>
-    </row>
-    <row r="435" spans="2:9" ht="15.75">
-      <c r="B435" s="6"/>
-      <c r="C435" s="6"/>
-      <c r="D435" s="6"/>
-      <c r="F435" s="6"/>
-      <c r="H435" s="6"/>
-      <c r="I435" s="6"/>
-    </row>
+    <row r="17" s="6" customFormat="1" ht="15.75"/>
+    <row r="18" s="6" customFormat="1" ht="15.75"/>
+    <row r="19" s="6" customFormat="1" ht="15.75"/>
+    <row r="20" s="6" customFormat="1" ht="15.75"/>
+    <row r="21" s="6" customFormat="1" ht="15.75"/>
+    <row r="22" s="6" customFormat="1" ht="15.75"/>
+    <row r="23" s="6" customFormat="1" ht="15.75"/>
+    <row r="24" s="6" customFormat="1" ht="15.75"/>
+    <row r="25" s="6" customFormat="1" ht="15.75"/>
+    <row r="26" s="6" customFormat="1" ht="15.75"/>
+    <row r="27" s="6" customFormat="1" ht="15.75"/>
+    <row r="28" s="6" customFormat="1" ht="15.75"/>
+    <row r="29" s="6" customFormat="1" ht="15.75"/>
+    <row r="30" s="6" customFormat="1" ht="15.75"/>
+    <row r="31" s="6" customFormat="1" ht="15.75"/>
+    <row r="32" s="6" customFormat="1" ht="15.75"/>
+    <row r="33" s="6" customFormat="1" ht="15.75"/>
+    <row r="34" s="6" customFormat="1" ht="15.75"/>
+    <row r="35" s="6" customFormat="1" ht="15.75"/>
+    <row r="36" s="6" customFormat="1" ht="15.75"/>
+    <row r="37" s="6" customFormat="1" ht="15.75"/>
+    <row r="38" s="6" customFormat="1" ht="15.75"/>
+    <row r="39" s="6" customFormat="1" ht="15.75"/>
+    <row r="40" s="6" customFormat="1" ht="15.75"/>
+    <row r="41" s="6" customFormat="1" ht="15.75"/>
+    <row r="42" s="6" customFormat="1" ht="15.75"/>
+    <row r="43" s="6" customFormat="1" ht="15.75"/>
+    <row r="44" s="6" customFormat="1" ht="39.75" customHeight="1"/>
+    <row r="45" s="6" customFormat="1" ht="15.75"/>
+    <row r="46" s="6" customFormat="1" ht="15.75"/>
+    <row r="47" s="6" customFormat="1" ht="9.75" customHeight="1"/>
+    <row r="48" s="6" customFormat="1" ht="42" customHeight="1"/>
+    <row r="49" s="6" customFormat="1" ht="15.75"/>
+    <row r="50" s="6" customFormat="1" ht="15.75"/>
+    <row r="51" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="52" s="6" customFormat="1" ht="15.75"/>
+    <row r="53" s="6" customFormat="1" ht="15.75"/>
+    <row r="54" s="6" customFormat="1" ht="15.75"/>
+    <row r="55" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="56" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="57" s="6" customFormat="1" ht="15.75"/>
+    <row r="58" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="59" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="60" s="6" customFormat="1" ht="15.75"/>
+    <row r="61" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="62" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="63" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="64" s="6" customFormat="1" ht="32.25" customHeight="1"/>
+    <row r="65" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="66" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="67" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="68" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="69" s="6" customFormat="1" ht="15.75"/>
+    <row r="70" s="6" customFormat="1" ht="15.75"/>
+    <row r="71" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="72" s="6" customFormat="1" ht="42" customHeight="1"/>
+    <row r="73" s="6" customFormat="1" ht="15.75"/>
+    <row r="74" s="6" customFormat="1" ht="15.75"/>
+    <row r="75" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="76" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="77" s="6" customFormat="1" ht="34.5" customHeight="1"/>
+    <row r="78" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="79" s="6" customFormat="1" ht="15.75"/>
+    <row r="80" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="81" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="82" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="83" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="84" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="85" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="86" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="87" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="88" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="89" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="90" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="91" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="92" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="93" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="94" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="95" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="96" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="97" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="98" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="99" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="100" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="101" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="102" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="103" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="104" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="105" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="106" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="107" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="108" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="109" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="110" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="111" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="112" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="113" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="114" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="115" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="116" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="117" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="118" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="119" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="120" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="121" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="122" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="123" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="124" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="125" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="126" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="127" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="128" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="129" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="130" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="131" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="132" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="133" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="134" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="135" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="136" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="137" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="138" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="139" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="140" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="141" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="142" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="143" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="144" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="145" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="146" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="147" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="148" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="149" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="150" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="151" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="152" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="153" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="154" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="155" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="156" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="157" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="158" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="159" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="160" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="161" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="162" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="163" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="164" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="165" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="166" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="167" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="168" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="169" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="170" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="171" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="172" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="173" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="174" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="175" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="176" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="177" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="178" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="179" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="180" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="181" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="182" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="183" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="184" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="185" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="186" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="187" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="188" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="189" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="190" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="191" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="192" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="193" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="194" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="195" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="196" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="197" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="198" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="199" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="200" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="201" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="202" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="203" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="204" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="205" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="206" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="207" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="208" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="209" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="210" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="211" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="212" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="213" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="214" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="215" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="216" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="217" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="218" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="219" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="220" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="221" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="222" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="223" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="224" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="225" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="226" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="227" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="228" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="229" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="230" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="231" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="232" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="233" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="234" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="235" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="236" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="237" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="238" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="239" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="240" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="241" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="242" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="243" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="244" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="245" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="246" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="247" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="248" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="249" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="250" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="251" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="252" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="253" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="254" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="255" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="256" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="257" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="258" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="259" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="260" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="261" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="262" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="263" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="264" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="265" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="266" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="267" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="268" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="269" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="270" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="271" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="272" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="273" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="274" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="275" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="276" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="277" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="278" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="279" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="280" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="281" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="282" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="283" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="284" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="285" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="286" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="287" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="288" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="289" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="290" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="291" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="292" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="293" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="294" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="295" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="296" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="297" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="298" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="299" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="300" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="301" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="302" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="303" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="304" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="305" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="306" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="307" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="308" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="309" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="310" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="311" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="312" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="313" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="314" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="315" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="316" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="317" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="318" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="319" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="320" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="321" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="322" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="323" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="324" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="325" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="326" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="327" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="328" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="329" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="330" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="331" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="332" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="333" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="334" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="335" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="336" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="337" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="338" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="339" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="340" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="341" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="342" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="343" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="344" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="345" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="346" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="347" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="348" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="349" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="350" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="351" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="352" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="353" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="354" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="355" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="356" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="357" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="358" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="359" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="360" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="361" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="362" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="363" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="364" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="365" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="366" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="367" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="368" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="369" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="370" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="371" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="372" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="373" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="374" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="375" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="376" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="377" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="378" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="379" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="380" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="381" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="382" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="383" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="384" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="385" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="386" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="387" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="388" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="389" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="390" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="391" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="392" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="393" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="394" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="395" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="396" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="397" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="398" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="399" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="400" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="401" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="402" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="403" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="404" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="405" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="406" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="407" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="408" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="409" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="410" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="411" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="412" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="413" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="414" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="415" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="416" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="417" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="418" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="419" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="420" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="421" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="422" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="423" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="424" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="425" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="426" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="427" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="428" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="429" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="430" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="431" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="432" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="433" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="434" s="6" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="435" s="6" customFormat="1" ht="15.75"/>
   </sheetData>
   <autoFilter ref="A1:I435" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
     <filterColumn colId="2">

</xml_diff>

<commit_message>
Fish Atlas with Gear types
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F45DCB-715A-4B7F-BF74-C568640C58DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0688F06D-E47B-48A6-9298-7D71E7629F63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8070" yWindow="780" windowWidth="19995" windowHeight="14820" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="3705" yWindow="735" windowWidth="21600" windowHeight="12735" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="291">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -1355,6 +1355,9 @@
   </si>
   <si>
     <t>Figure out why photos aren't displaying in WA/OR</t>
+  </si>
+  <si>
+    <t>FA:  Update displayed features when filtered</t>
   </si>
 </sst>
 </file>
@@ -2753,7 +2756,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D95" sqref="D95"/>
+      <selection pane="bottomRight" activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -3778,6 +3781,11 @@
     <row r="91" spans="1:9" ht="24.95" customHeight="1">
       <c r="D91" s="9" t="s">
         <v>289</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D92" s="9" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="443" spans="1:10" ht="15.75" hidden="1">

</xml_diff>

<commit_message>
Test filter using MP4_Seconds_binary
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,33 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCD07D1-5D75-4BE2-AFCB-64773F6EF9E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F905A69F-228E-4D2B-A182-3E449348C16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7230" yWindow="345" windowWidth="21570" windowHeight="15255" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="1950" yWindow="435" windowWidth="23865" windowHeight="15045" tabRatio="736" activeTab="2" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
     <sheet name="to do" sheetId="1" r:id="rId2"/>
-    <sheet name="Statistical queries" sheetId="18" r:id="rId3"/>
-    <sheet name="to do - SS" sheetId="16" r:id="rId4"/>
-    <sheet name="SZ point regeneration rethink" sheetId="14" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="15" r:id="rId6"/>
-    <sheet name="MPK download" sheetId="17" r:id="rId7"/>
-    <sheet name="Sp_BB tables" sheetId="19" r:id="rId8"/>
-    <sheet name="browser heights" sheetId="20" r:id="rId9"/>
+    <sheet name="filter on MP4_Seconds_binary" sheetId="21" r:id="rId3"/>
+    <sheet name="Statistical queries" sheetId="18" r:id="rId4"/>
+    <sheet name="to do - SS" sheetId="16" r:id="rId5"/>
+    <sheet name="SZ point regeneration rethink" sheetId="14" r:id="rId6"/>
+    <sheet name="Downloads" sheetId="15" r:id="rId7"/>
+    <sheet name="MPK download" sheetId="17" r:id="rId8"/>
+    <sheet name="Sp_BB tables" sheetId="19" r:id="rId9"/>
+    <sheet name="browser heights" sheetId="20" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'MPK download'!$A$3:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'MPK download'!$A$3:$C$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$443</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'to do - SS'!$A$1:$I$435</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'to do - SS'!$A$1:$I$435</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -140,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="296">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -1478,6 +1479,12 @@
       </rPr>
       <t xml:space="preserve"> method, and make a version for FA.</t>
     </r>
+  </si>
+  <si>
+    <t>nearly full extent</t>
+  </si>
+  <si>
+    <t>Tee Harbor</t>
   </si>
 </sst>
 </file>
@@ -1859,7 +1866,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2004,6 +2011,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2312,6 +2322,55 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>570220</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>199550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61DF525B-1D39-46A6-9C17-2E39E51E57D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="400050"/>
+          <a:ext cx="10238095" cy="3800000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -2356,7 +2415,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2405,7 +2464,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2460,7 +2519,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -2876,12 +2935,140 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD2386D-2AF1-4B5F-9842-EBCA886CA8B5}">
+  <dimension ref="B3:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="5" width="9" style="61"/>
+    <col min="6" max="6" width="25.125" style="61" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="61"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7">
+      <c r="B3" s="61">
+        <v>994</v>
+      </c>
+      <c r="C3" s="61">
+        <v>776</v>
+      </c>
+      <c r="D3" s="61">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="61">
+        <v>1040</v>
+      </c>
+      <c r="C4" s="61">
+        <v>839</v>
+      </c>
+      <c r="D4" s="61">
+        <v>201</v>
+      </c>
+      <c r="F4" s="61" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="61">
+        <v>849</v>
+      </c>
+      <c r="C5" s="61">
+        <v>631</v>
+      </c>
+      <c r="D5" s="61">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="61">
+        <v>480</v>
+      </c>
+      <c r="C6" s="61">
+        <v>262</v>
+      </c>
+      <c r="D6" s="61">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="61">
+        <v>480</v>
+      </c>
+      <c r="C8" s="61">
+        <v>311</v>
+      </c>
+      <c r="D8" s="61">
+        <v>169</v>
+      </c>
+      <c r="F8" s="61" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="61">
+        <v>480</v>
+      </c>
+      <c r="C9" s="61">
+        <v>311</v>
+      </c>
+      <c r="D9" s="61">
+        <v>169</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>280</v>
+      </c>
+      <c r="G9" s="61">
+        <f>D6-D9</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="30">
+      <c r="B10" s="61">
+        <v>1040</v>
+      </c>
+      <c r="C10" s="61">
+        <v>888</v>
+      </c>
+      <c r="D10" s="61">
+        <v>152</v>
+      </c>
+      <c r="F10" s="62" t="s">
+        <v>279</v>
+      </c>
+      <c r="G10" s="61">
+        <f>D4-D10</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="61">
+        <v>774</v>
+      </c>
+      <c r="C13" s="61">
+        <v>605</v>
+      </c>
+      <c r="D13" s="61">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:J443"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3960,6 +4147,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661E4574-B315-4CFC-8EA2-13147AE35708}">
+  <dimension ref="A3:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="117.875" customWidth="1"/>
+    <col min="4" max="4" width="14.75" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4">
+      <c r="A3" s="65"/>
+      <c r="D3" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="D14" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFDF36D1-DE2E-478E-8F20-00E572A1B869}">
   <dimension ref="B1:E44"/>
   <sheetViews>
@@ -4183,7 +4402,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8A68F0-A5CC-4F2B-9E7A-D47D3E46C475}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J435"/>
@@ -4801,7 +5020,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3521A2-0E46-4626-A556-F81B8258D1DB}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4816,7 +5035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D90DEFD-D6A8-4BFB-97A2-600F5E7E4446}">
   <dimension ref="B2:C12"/>
   <sheetViews>
@@ -4890,7 +5109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392EF631-8DBE-4581-9410-4CF72B20CF9A}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -5004,7 +5223,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073BA0C8-793A-470F-9811-FE4A219663BF}">
   <dimension ref="A1:N36"/>
   <sheetViews>
@@ -5826,132 +6045,4 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD2386D-2AF1-4B5F-9842-EBCA886CA8B5}">
-  <dimension ref="B3:G13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="5" width="9" style="61"/>
-    <col min="6" max="6" width="25.125" style="61" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="61"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:7">
-      <c r="B3" s="61">
-        <v>994</v>
-      </c>
-      <c r="C3" s="61">
-        <v>776</v>
-      </c>
-      <c r="D3" s="61">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7">
-      <c r="B4" s="61">
-        <v>1040</v>
-      </c>
-      <c r="C4" s="61">
-        <v>839</v>
-      </c>
-      <c r="D4" s="61">
-        <v>201</v>
-      </c>
-      <c r="F4" s="61" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="61">
-        <v>849</v>
-      </c>
-      <c r="C5" s="61">
-        <v>631</v>
-      </c>
-      <c r="D5" s="61">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7">
-      <c r="B6" s="61">
-        <v>480</v>
-      </c>
-      <c r="C6" s="61">
-        <v>262</v>
-      </c>
-      <c r="D6" s="61">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="61">
-        <v>480</v>
-      </c>
-      <c r="C8" s="61">
-        <v>311</v>
-      </c>
-      <c r="D8" s="61">
-        <v>169</v>
-      </c>
-      <c r="F8" s="61" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="61">
-        <v>480</v>
-      </c>
-      <c r="C9" s="61">
-        <v>311</v>
-      </c>
-      <c r="D9" s="61">
-        <v>169</v>
-      </c>
-      <c r="F9" s="61" t="s">
-        <v>280</v>
-      </c>
-      <c r="G9" s="61">
-        <f>D6-D9</f>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="30">
-      <c r="B10" s="61">
-        <v>1040</v>
-      </c>
-      <c r="C10" s="61">
-        <v>888</v>
-      </c>
-      <c r="D10" s="61">
-        <v>152</v>
-      </c>
-      <c r="F10" s="62" t="s">
-        <v>279</v>
-      </c>
-      <c r="G10" s="61">
-        <f>D4-D10</f>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="61">
-        <v>774</v>
-      </c>
-      <c r="C13" s="61">
-        <v>605</v>
-      </c>
-      <c r="D13" s="61">
-        <v>169</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaned up updateAllDropdowns, upDateDropdown, filterDropdown
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F905A69F-228E-4D2B-A182-3E449348C16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1718CF-FF08-4FBF-B45D-1BB1817A5C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="435" windowWidth="23865" windowHeight="15045" tabRatio="736" activeTab="2" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="2760" yWindow="555" windowWidth="22695" windowHeight="15045" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="297">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -1485,6 +1485,9 @@
   </si>
   <si>
     <t>Tee Harbor</t>
+  </si>
+  <si>
+    <t>Clean up Gear/Date for Site &amp; Species tables</t>
   </si>
 </sst>
 </file>
@@ -3068,11 +3071,11 @@
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:J443"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G94" sqref="G94"/>
+      <selection pane="bottomRight" activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -4117,6 +4120,11 @@
     <row r="95" spans="1:9" ht="39.75" customHeight="1">
       <c r="D95" s="9" t="s">
         <v>293</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D96" s="9" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="443" spans="1:10" ht="15.75" hidden="1">
@@ -4150,7 +4158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661E4574-B315-4CFC-8EA2-13147AE35708}">
   <dimension ref="A3:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Get counts from custom REST service
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1718CF-FF08-4FBF-B45D-1BB1817A5C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F627882C-6E3B-4FAD-93D5-A47BA421C605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="555" windowWidth="22695" windowHeight="15045" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="297">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -3075,7 +3075,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D97" sqref="D97"/>
+      <selection pane="bottomRight" activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -4123,6 +4123,9 @@
       </c>
     </row>
     <row r="96" spans="1:9" ht="24.95" customHeight="1">
+      <c r="C96" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="D96" s="9" t="s">
         <v>296</v>
       </c>

</xml_diff>

<commit_message>
If extent width of search result selection is 4453, then use zoom=9 for goTo
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B657B2E8-9F32-4769-A6FF-C6148C839FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933D1E5C-8A3F-4CBB-A4FB-617F4CC0ED27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="780" windowWidth="28290" windowHeight="13830" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21000" windowHeight="14175" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="297">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -3075,7 +3075,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -4113,7 +4113,10 @@
         <v>290</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="24.95" customHeight="1">
+    <row r="93" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+      <c r="C93" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="D93" s="33" t="s">
         <v>291</v>
       </c>

</xml_diff>

<commit_message>
Added counts to FA dropdowns (subject to approval)
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933D1E5C-8A3F-4CBB-A4FB-617F4CC0ED27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0E5097-20FA-473D-9AA2-7E5148039804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21000" windowHeight="14175" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="1275" yWindow="555" windowWidth="24810" windowHeight="14100" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -22,12 +22,11 @@
     <sheet name="Downloads" sheetId="15" r:id="rId7"/>
     <sheet name="MPK download" sheetId="17" r:id="rId8"/>
     <sheet name="Sp_BB tables" sheetId="19" r:id="rId9"/>
-    <sheet name="browser heights" sheetId="20" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'API updates'!$B$1:$B$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'MPK download'!$A$3:$C$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$443</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'to do'!$A$1:$I$442</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'to do - SS'!$A$1:$I$435</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -141,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="291">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -572,9 +571,6 @@
     <t>keep track of user state, so stays off in SZ mode when user has turned off?</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>go to locale/site from popup</t>
   </si>
   <si>
@@ -622,9 +618,6 @@
   </si>
   <si>
     <t>new icons for map widgets</t>
-  </si>
-  <si>
-    <t>Flex site:  1) restore mapping/DotNet folder?     2)  ArcGis Server queries set to return in AMF format, which is no longer supported.</t>
   </si>
   <si>
     <t>default to independent habitat dropdowns between Region/Locale/Site tabs</t>
@@ -1323,18 +1316,6 @@
   </si>
   <si>
     <t>July 2020?</t>
-  </si>
-  <si>
-    <t>download bar closed, window maximized</t>
-  </si>
-  <si>
-    <t>download bar closed</t>
-  </si>
-  <si>
-    <t>JetBrains debugging bar closed</t>
-  </si>
-  <si>
-    <t>window maximized</t>
   </si>
   <si>
     <t>fix 1-day date discerpancies in Station tables</t>
@@ -1869,7 +1850,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2004,10 +1985,6 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2885,7 +2862,7 @@
         <v>4.16</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="23.25">
@@ -2938,144 +2915,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD2386D-2AF1-4B5F-9842-EBCA886CA8B5}">
-  <dimension ref="B3:G13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="5" width="9" style="61"/>
-    <col min="6" max="6" width="25.125" style="61" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="61"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:7">
-      <c r="B3" s="61">
-        <v>994</v>
-      </c>
-      <c r="C3" s="61">
-        <v>776</v>
-      </c>
-      <c r="D3" s="61">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7">
-      <c r="B4" s="61">
-        <v>1040</v>
-      </c>
-      <c r="C4" s="61">
-        <v>839</v>
-      </c>
-      <c r="D4" s="61">
-        <v>201</v>
-      </c>
-      <c r="F4" s="61" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="61">
-        <v>849</v>
-      </c>
-      <c r="C5" s="61">
-        <v>631</v>
-      </c>
-      <c r="D5" s="61">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7">
-      <c r="B6" s="61">
-        <v>480</v>
-      </c>
-      <c r="C6" s="61">
-        <v>262</v>
-      </c>
-      <c r="D6" s="61">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="61">
-        <v>480</v>
-      </c>
-      <c r="C8" s="61">
-        <v>311</v>
-      </c>
-      <c r="D8" s="61">
-        <v>169</v>
-      </c>
-      <c r="F8" s="61" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="61">
-        <v>480</v>
-      </c>
-      <c r="C9" s="61">
-        <v>311</v>
-      </c>
-      <c r="D9" s="61">
-        <v>169</v>
-      </c>
-      <c r="F9" s="61" t="s">
-        <v>280</v>
-      </c>
-      <c r="G9" s="61">
-        <f>D6-D9</f>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="30">
-      <c r="B10" s="61">
-        <v>1040</v>
-      </c>
-      <c r="C10" s="61">
-        <v>888</v>
-      </c>
-      <c r="D10" s="61">
-        <v>152</v>
-      </c>
-      <c r="F10" s="62" t="s">
-        <v>279</v>
-      </c>
-      <c r="G10" s="61">
-        <f>D4-D10</f>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="61">
-        <v>774</v>
-      </c>
-      <c r="C13" s="61">
-        <v>605</v>
-      </c>
-      <c r="D13" s="61">
-        <v>169</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J443"/>
+  <dimension ref="A1:J442"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D65" sqref="D65"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -3354,7 +3203,7 @@
         <v>22</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J18" s="6"/>
     </row>
@@ -3746,7 +3595,7 @@
         <v>100</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J50" s="6"/>
     </row>
@@ -3806,7 +3655,7 @@
         <v>21</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I56" s="25"/>
       <c r="J56" s="6"/>
@@ -3816,16 +3665,16 @@
         <v>21</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J57" s="6"/>
     </row>
     <row r="58" spans="1:10" ht="24.95" customHeight="1">
       <c r="D58" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="I58" s="11" t="s">
         <v>114</v>
-      </c>
-      <c r="I58" s="11" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="24.95" hidden="1" customHeight="1">
@@ -3833,7 +3682,7 @@
         <v>11</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J59" s="6"/>
     </row>
@@ -3842,13 +3691,13 @@
         <v>72</v>
       </c>
       <c r="D60" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J60" s="6"/>
     </row>
     <row r="61" spans="1:10" ht="24.95" customHeight="1">
       <c r="D61" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="24.95" hidden="1" customHeight="1">
@@ -3856,7 +3705,7 @@
         <v>21</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J62" s="6"/>
     </row>
@@ -3865,7 +3714,7 @@
         <v>21</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J63" s="6"/>
     </row>
@@ -3874,13 +3723,13 @@
         <v>21</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J64" s="6"/>
     </row>
     <row r="65" spans="1:10" ht="24.95" customHeight="1">
       <c r="D65" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="24.95" hidden="1" customHeight="1">
@@ -3888,7 +3737,7 @@
         <v>21</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J66" s="6"/>
     </row>
@@ -3897,13 +3746,13 @@
         <v>44129</v>
       </c>
       <c r="D67" s="33" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J67" s="6"/>
     </row>
     <row r="68" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="D68" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="24.95" hidden="1" customHeight="1">
@@ -3911,21 +3760,21 @@
         <v>72</v>
       </c>
       <c r="D69" s="31" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="34.5" customHeight="1" thickBot="1">
       <c r="D70" s="31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G70" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I70" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J70" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="16.5" hidden="1" thickBot="1">
@@ -3933,7 +3782,7 @@
         <v>21</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G71" s="19"/>
       <c r="J71" s="6"/>
@@ -3943,7 +3792,7 @@
         <v>21</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J72" s="6"/>
     </row>
@@ -3952,14 +3801,14 @@
         <v>21</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G73" s="19"/>
       <c r="J73" s="6"/>
     </row>
     <row r="74" spans="1:10" ht="16.5" thickBot="1">
       <c r="D74" s="30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G74" s="19"/>
     </row>
@@ -3968,11 +3817,11 @@
         <v>44129</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="G75" s="19"/>
       <c r="I75" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="15.75" hidden="1">
@@ -3980,7 +3829,7 @@
         <v>44011</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G76" s="19"/>
     </row>
@@ -3989,7 +3838,7 @@
         <v>44011</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G77" s="19"/>
     </row>
@@ -3998,7 +3847,7 @@
         <v>44064</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G78" s="19"/>
     </row>
@@ -4008,7 +3857,7 @@
       </c>
       <c r="C79" s="36"/>
       <c r="D79" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G79" s="19"/>
     </row>
@@ -4017,7 +3866,7 @@
         <v>44029</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="15.75" hidden="1">
@@ -4025,10 +3874,10 @@
         <v>44075</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I81" s="11" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="18.75" hidden="1">
@@ -4036,7 +3885,7 @@
         <v>44075</v>
       </c>
       <c r="D82" s="60" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="15.75" hidden="1">
@@ -4044,7 +3893,7 @@
         <v>21</v>
       </c>
       <c r="D83" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="24.95" hidden="1" customHeight="1">
@@ -4052,101 +3901,91 @@
         <v>11</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="I84" s="11" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="34.5" hidden="1" customHeight="1">
-      <c r="A85" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D85" s="33" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="24.95" customHeight="1">
-      <c r="D86" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" ht="32.25" hidden="1" thickBot="1">
-      <c r="C87" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D85" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="32.25" hidden="1" thickBot="1">
+      <c r="C86" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D87" s="32" t="s">
+      <c r="D86" s="32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D87" s="26" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" ht="24.95" customHeight="1">
-      <c r="D88" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="I88" s="11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="47.25" hidden="1">
-      <c r="C89" s="36">
+      <c r="I87" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="47.25" hidden="1">
+      <c r="C88" s="36">
         <v>44140</v>
       </c>
-      <c r="D89" s="63" t="s">
-        <v>287</v>
+      <c r="D88" s="61" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D89" s="9" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="24.95" customHeight="1">
       <c r="D90" s="9" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="24.95" customHeight="1">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+      <c r="C91" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="D91" s="9" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="24.95" hidden="1" customHeight="1">
       <c r="C92" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D92" s="9" t="s">
+      <c r="D92" s="33" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="38.25" customHeight="1">
+      <c r="D93" s="62" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="39.75" customHeight="1">
+      <c r="D94" s="9" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+      <c r="C95" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D95" s="9" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="24.95" hidden="1" customHeight="1">
-      <c r="C93" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D93" s="33" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="38.25" customHeight="1">
-      <c r="D94" s="64" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="39.75" customHeight="1">
-      <c r="D95" s="9" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="24.95" hidden="1" customHeight="1">
-      <c r="C96" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D96" s="9" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="443" spans="1:10" ht="15.75" hidden="1">
-      <c r="A443" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="J443" s="6"/>
+    <row r="442" spans="1:10" ht="15.75">
+      <c r="A442" s="2"/>
+      <c r="J442" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I443" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
+  <autoFilter ref="A1:I442" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
@@ -4181,14 +4020,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
-      <c r="A3" s="65"/>
+      <c r="A3" s="63"/>
       <c r="D3" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="D14" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -4215,54 +4054,54 @@
   <sheetData>
     <row r="1" spans="2:5">
       <c r="B1" s="57" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="31.5">
       <c r="B2" s="49" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="E6" s="38" t="s">
         <v>194</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75">
       <c r="B7" s="43" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="44" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="26.25">
       <c r="B15" s="47" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E15" s="48" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="12" customHeight="1">
       <c r="B16" s="46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="12" customHeight="1">
@@ -4270,71 +4109,71 @@
     </row>
     <row r="18" spans="2:5" ht="12" customHeight="1">
       <c r="B18" s="45" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="12" customHeight="1">
       <c r="B19" s="45" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="12" customHeight="1">
       <c r="B20" s="45" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="12" customHeight="1">
       <c r="B21" s="45" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="12" customHeight="1">
       <c r="B22" s="45" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E22" s="44" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="12" customHeight="1">
       <c r="B23" s="45" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="12" customHeight="1">
       <c r="B24" s="45" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="12" customHeight="1">
       <c r="B25" s="45" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="12" customHeight="1">
       <c r="B26" s="45" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="12" customHeight="1">
       <c r="B27" s="45" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E27" s="38" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="12" customHeight="1">
       <c r="B28" s="45" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="12" customHeight="1">
       <c r="B29" s="45" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="12" customHeight="1">
@@ -4342,7 +4181,7 @@
     </row>
     <row r="31" spans="2:5" ht="12" customHeight="1">
       <c r="B31" s="46" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="12" customHeight="1">
@@ -4350,62 +4189,62 @@
     </row>
     <row r="33" spans="2:2" ht="12" customHeight="1">
       <c r="B33" s="45" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="12" customHeight="1">
       <c r="B34" s="45" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="12" customHeight="1">
       <c r="B35" s="45" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="12" customHeight="1">
       <c r="B36" s="45" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="12" customHeight="1">
       <c r="B37" s="45" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="12" customHeight="1">
       <c r="B38" s="45" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="12" customHeight="1">
       <c r="B39" s="45" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="12" customHeight="1">
       <c r="B40" s="45" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="12" customHeight="1">
       <c r="B41" s="45" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="12" customHeight="1">
       <c r="B42" s="45" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="2:2" ht="12" customHeight="1">
       <c r="B43" s="45" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="12" customHeight="1">
       <c r="B44" s="45" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -4489,7 +4328,7 @@
         <v>44006</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F3" s="6"/>
       <c r="H3" s="6"/>
@@ -4510,7 +4349,7 @@
         <v>44014</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -4523,7 +4362,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F6" s="6"/>
       <c r="H6" s="6"/>
@@ -5071,56 +4910,56 @@
   <sheetData>
     <row r="2" spans="2:3" ht="18" thickBot="1">
       <c r="B2" s="29" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="16.5" thickTop="1"/>
     <row r="4" spans="2:3">
       <c r="B4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -5146,23 +4985,23 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="37" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="41" customFormat="1">
       <c r="A3" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>168</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>169</v>
-      </c>
-      <c r="C3" s="41" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B4" s="39">
         <v>44035</v>
@@ -5174,7 +5013,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B5" s="39">
         <v>44035</v>
@@ -5186,7 +5025,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B6" s="39">
         <v>44020</v>
@@ -5198,7 +5037,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B7" s="39">
         <v>43864</v>
@@ -5210,7 +5049,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B8" s="39">
         <v>43838</v>
@@ -5222,7 +5061,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B9" s="39">
         <v>43555</v>
@@ -5269,18 +5108,18 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75">
       <c r="F1" s="56" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="55" customFormat="1" ht="18.75">
       <c r="A7" s="55" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F7" s="55" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="K7" s="55" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -5288,13 +5127,13 @@
         <v>16099</v>
       </c>
       <c r="B8" s="53" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F8" s="54">
         <v>16099</v>
       </c>
       <c r="G8" s="53" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -5302,40 +5141,40 @@
     </row>
     <row r="10" spans="1:14" s="51" customFormat="1">
       <c r="A10" s="51" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C10" s="51" t="s">
+        <v>252</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>251</v>
+      </c>
+      <c r="F10" s="51" t="s">
         <v>254</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="G10" s="51" t="s">
         <v>253</v>
       </c>
-      <c r="F10" s="51" t="s">
-        <v>256</v>
-      </c>
-      <c r="G10" s="51" t="s">
-        <v>255</v>
-      </c>
       <c r="H10" s="51" t="s">
+        <v>252</v>
+      </c>
+      <c r="I10" s="51" t="s">
+        <v>251</v>
+      </c>
+      <c r="K10" s="51" t="s">
         <v>254</v>
       </c>
-      <c r="I10" s="51" t="s">
+      <c r="L10" s="51" t="s">
         <v>253</v>
       </c>
-      <c r="K10" s="51" t="s">
-        <v>256</v>
-      </c>
-      <c r="L10" s="51" t="s">
-        <v>255</v>
-      </c>
       <c r="M10" s="51" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="N10" s="51" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -5344,57 +5183,57 @@
       <c r="C11" s="51"/>
       <c r="D11" s="51"/>
       <c r="F11" s="50" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G11" s="50" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H11" s="50" t="s">
+        <v>248</v>
+      </c>
+      <c r="K11" s="50" t="s">
         <v>250</v>
       </c>
-      <c r="K11" s="50" t="s">
-        <v>252</v>
-      </c>
       <c r="L11" s="50" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="M11" s="50" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="50" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D12" s="50">
         <v>255</v>
       </c>
       <c r="F12" s="50" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G12" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H12" s="50" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I12" s="50">
         <v>255</v>
       </c>
       <c r="K12" s="50" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="L12" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M12" s="50" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="N12" s="50">
         <v>255</v>
@@ -5402,25 +5241,25 @@
     </row>
     <row r="13" spans="1:14">
       <c r="F13" s="50" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G13" s="50" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H13" s="50" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I13" s="50">
         <v>8</v>
       </c>
       <c r="K13" s="50" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="L13" s="50" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="M13" s="50" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="N13" s="50">
         <v>8</v>
@@ -5428,25 +5267,25 @@
     </row>
     <row r="14" spans="1:14">
       <c r="F14" s="50" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G14" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H14" s="50" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I14" s="50">
         <v>2</v>
       </c>
       <c r="K14" s="50" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="L14" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M14" s="50" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="N14" s="50">
         <v>2</v>
@@ -5454,37 +5293,37 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="50" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D15" s="50">
         <v>255</v>
       </c>
       <c r="F15" s="50" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G15" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H15" s="50" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I15" s="50">
         <v>255</v>
       </c>
       <c r="K15" s="50" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="L15" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M15" s="50" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="N15" s="50">
         <v>255</v>
@@ -5492,54 +5331,54 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="50" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F16" s="50" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G16" s="50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H16" s="50" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K16" s="50" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="L16" s="50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M16" s="50" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="F17" s="50" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G17" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H17" s="50" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I17" s="50">
         <v>5</v>
       </c>
       <c r="K17" s="50" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L17" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M17" s="50" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="N17" s="50">
         <v>5</v>
@@ -5547,25 +5386,25 @@
     </row>
     <row r="18" spans="1:14">
       <c r="F18" s="50" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G18" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H18" s="50" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I18" s="50">
         <v>5</v>
       </c>
       <c r="K18" s="50" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L18" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M18" s="50" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="N18" s="50">
         <v>5</v>
@@ -5573,25 +5412,25 @@
     </row>
     <row r="19" spans="1:14">
       <c r="F19" s="50" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G19" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H19" s="50" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I19" s="50">
         <v>5</v>
       </c>
       <c r="K19" s="50" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="L19" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M19" s="50" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="N19" s="50">
         <v>5</v>
@@ -5599,25 +5438,25 @@
     </row>
     <row r="20" spans="1:14">
       <c r="F20" s="50" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G20" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H20" s="50" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I20" s="50">
         <v>150</v>
       </c>
       <c r="K20" s="50" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="L20" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M20" s="50" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="N20" s="50">
         <v>150</v>
@@ -5625,54 +5464,54 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="50" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C21" s="50" t="s">
+        <v>226</v>
+      </c>
+      <c r="F21" s="50" t="s">
         <v>228</v>
       </c>
-      <c r="F21" s="50" t="s">
-        <v>230</v>
-      </c>
       <c r="G21" s="50" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H21" s="50" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K21" s="50" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L21" s="50" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M21" s="50" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:14">
       <c r="F22" s="50" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G22" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H22" s="50" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I22" s="50">
         <v>25</v>
       </c>
       <c r="K22" s="50" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L22" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M22" s="50" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="N22" s="50">
         <v>25</v>
@@ -5680,86 +5519,86 @@
     </row>
     <row r="23" spans="1:14">
       <c r="F23" s="50" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G23" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H23" s="50" t="s">
+        <v>221</v>
+      </c>
+      <c r="K23" s="50" t="s">
         <v>223</v>
       </c>
-      <c r="K23" s="50" t="s">
-        <v>225</v>
-      </c>
       <c r="L23" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="M23" s="50" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C24" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="F24" s="50" t="s">
         <v>220</v>
       </c>
-      <c r="F24" s="50" t="s">
-        <v>222</v>
-      </c>
       <c r="G24" s="50" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H24" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="K24" s="50" t="s">
         <v>220</v>
       </c>
-      <c r="K24" s="50" t="s">
-        <v>222</v>
-      </c>
       <c r="L24" s="50" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M24" s="50" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="50" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C25" s="50" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D25" s="50">
         <v>255</v>
       </c>
       <c r="F25" s="50" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G25" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H25" s="50" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I25" s="50">
         <v>255</v>
       </c>
       <c r="K25" s="50" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="L25" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M25" s="50" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N25" s="50">
         <v>255</v>
@@ -5767,37 +5606,37 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="50" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C26" s="50" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D26" s="50">
         <v>801</v>
       </c>
       <c r="F26" s="50" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G26" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H26" s="50" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I26" s="50">
         <v>801</v>
       </c>
       <c r="K26" s="50" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="L26" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M26" s="50" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="N26" s="50">
         <v>801</v>
@@ -5805,37 +5644,37 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="50" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D27" s="50">
         <v>255</v>
       </c>
       <c r="F27" s="50" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G27" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H27" s="50" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I27" s="50">
         <v>255</v>
       </c>
       <c r="K27" s="50" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="L27" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M27" s="50" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="N27" s="50">
         <v>255</v>
@@ -5843,37 +5682,37 @@
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="50" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C28" s="50" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D28" s="50">
         <v>12</v>
       </c>
       <c r="F28" s="50" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G28" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H28" s="50" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I28" s="50">
         <v>12</v>
       </c>
       <c r="K28" s="50" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L28" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M28" s="50" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="N28" s="50">
         <v>12</v>
@@ -5881,66 +5720,66 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="50" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F29" s="50" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G29" s="50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H29" s="50" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K29" s="50" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L29" s="50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M29" s="50" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="50" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B30" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D30" s="50">
         <v>255</v>
       </c>
       <c r="F30" s="50" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G30" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H30" s="50" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I30" s="50">
         <v>255</v>
       </c>
       <c r="K30" s="50" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="L30" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M30" s="50" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="N30" s="50">
         <v>255</v>
@@ -5948,57 +5787,57 @@
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B31" s="50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C31" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="F31" s="50" t="s">
         <v>204</v>
       </c>
-      <c r="F31" s="50" t="s">
-        <v>206</v>
-      </c>
       <c r="G31" s="50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H31" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="K31" s="50" t="s">
         <v>204</v>
       </c>
-      <c r="K31" s="50" t="s">
-        <v>206</v>
-      </c>
       <c r="L31" s="50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M31" s="50" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="58" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B32" s="58" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C32" s="58" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D32" s="50">
         <v>1</v>
       </c>
       <c r="F32" s="59" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K32" s="50" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="L32" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M32" s="50" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="N32" s="50">
         <v>1</v>
@@ -6006,24 +5845,24 @@
     </row>
     <row r="33" spans="11:14">
       <c r="K33" s="50" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L33" s="50" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="M33" s="50" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="34" spans="11:14">
       <c r="K34" s="50" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L34" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M34" s="50" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="N34" s="50">
         <v>6</v>
@@ -6031,13 +5870,13 @@
     </row>
     <row r="35" spans="11:14">
       <c r="K35" s="50" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="L35" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M35" s="50" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="N35" s="50">
         <v>255</v>
@@ -6045,13 +5884,13 @@
     </row>
     <row r="36" spans="11:14">
       <c r="K36" s="50" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L36" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M36" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="N36" s="50">
         <v>255</v>

</xml_diff>

<commit_message>
FishDisplayPage altered to use vw_HtmlCode_FishPages.  (So domain name changes can be more easily accommodated.)
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0E5097-20FA-473D-9AA2-7E5148039804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5687478-6D9B-4352-8F34-748BFC8F94A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="555" windowWidth="24810" windowHeight="14100" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
+    <workbookView xWindow="0" yWindow="210" windowWidth="28455" windowHeight="15210" tabRatio="736" activeTab="1" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
   <sheets>
     <sheet name="API updates" sheetId="13" r:id="rId1"/>
@@ -111,6 +111,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D98" authorId="0" shapeId="0" xr:uid="{3B37A8B9-B1DA-48B6-B3C3-ED336BFA71E9}">
+      <text>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>I will probably be converting tables to use the new ESRI FeatureTable widget (using SZ money) fairly soon.  This may handle column widths differently, so it makes sense to wait until this conversion is done before addressing the column widths issue.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -140,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="298">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -171,9 +185,6 @@
     </r>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>VideoPanelWidget.js, PhotoPlaybackWidget</t>
   </si>
   <si>
@@ -352,9 +363,6 @@
   </si>
   <si>
     <t>saved extents</t>
-  </si>
-  <si>
-    <t>TS?</t>
   </si>
   <si>
     <t>Because I'm currently using OnDemandGrid, only partial set of rows are present at any on time</t>
@@ -1470,12 +1478,39 @@
   <si>
     <t>Clean up Gear/Date for Site &amp; Species tables</t>
   </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>add item counts to dropdowns</t>
+  </si>
+  <si>
+    <t>Modify "Fish Catch for All Regions" table (button is in the "Fish Atlas Regions" table header), so it agrees with Regions table numbers when filters are applied</t>
+  </si>
+  <si>
+    <t>Add similar button and table for sites table header</t>
+  </si>
+  <si>
+    <t>demo</t>
+  </si>
+  <si>
+    <t>improve column widths for data tables</t>
+  </si>
+  <si>
+    <t>see note</t>
+  </si>
+  <si>
+    <t>Add "clear filters" button?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="36">
+  <fonts count="37">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1748,6 +1783,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -1850,7 +1892,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1993,6 +2035,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2854,7 +2905,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26.25">
       <c r="A1" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="23.25">
@@ -2862,7 +2913,7 @@
         <v>4.16</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="23.25">
@@ -2872,18 +2923,18 @@
     </row>
     <row r="8" spans="1:2" ht="408.95" customHeight="1">
       <c r="B8" s="23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="72" customHeight="1"/>
     <row r="10" spans="1:2" ht="144" customHeight="1">
       <c r="B10" s="23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="398.1" customHeight="1">
       <c r="B11" s="23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="23.25">
@@ -2893,12 +2944,12 @@
     </row>
     <row r="13" spans="1:2" ht="75.95" customHeight="1">
       <c r="B13" s="23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="408.95" customHeight="1">
       <c r="B14" s="23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="177" customHeight="1"/>
@@ -2921,10 +2972,10 @@
   <dimension ref="A1:J442"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2944,71 +2995,65 @@
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="97.5" customHeight="1">
       <c r="A1" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>15</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>40</v>
-      </c>
       <c r="I1" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" s="35"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" hidden="1">
       <c r="C2" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="9"/>
       <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" hidden="1">
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" hidden="1">
-      <c r="B4" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -3016,45 +3061,37 @@
     </row>
     <row r="5" spans="1:10" customFormat="1" ht="15.75" hidden="1">
       <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="31.5" hidden="1">
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="47.25" hidden="1">
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>2</v>
@@ -3065,7 +3102,7 @@
     </row>
     <row r="8" spans="1:10" ht="15.75" hidden="1">
       <c r="C8" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>1</v>
@@ -3075,14 +3112,11 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" hidden="1">
-      <c r="B9" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="9"/>
@@ -3090,10 +3124,10 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" hidden="1">
       <c r="C10" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="9"/>
@@ -3101,643 +3135,598 @@
     </row>
     <row r="11" spans="1:10" ht="31.5" hidden="1">
       <c r="C11" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>0</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" hidden="1">
-      <c r="B12" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="31.5" hidden="1">
       <c r="C13" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" ht="31.5" hidden="1">
       <c r="C14" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" hidden="1">
       <c r="A15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>35</v>
       </c>
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" hidden="1">
       <c r="A16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J16" s="6"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" hidden="1">
       <c r="C17" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="9"/>
       <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" hidden="1">
-      <c r="B18" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="I18" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" hidden="1">
-      <c r="B19" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" hidden="1">
       <c r="A20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" hidden="1">
+      <c r="C21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" hidden="1">
-      <c r="B21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" hidden="1">
       <c r="C22" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H22" s="6"/>
       <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" hidden="1">
-      <c r="B23" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C23" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D23" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" hidden="1">
+      <c r="C24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" hidden="1">
-      <c r="B24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>37</v>
-      </c>
       <c r="I24" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J24" s="6"/>
     </row>
     <row r="25" spans="1:10" ht="126" hidden="1">
-      <c r="B25" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C25" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H25" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>62</v>
       </c>
       <c r="J25" s="6"/>
     </row>
     <row r="26" spans="1:10" ht="110.25" hidden="1">
       <c r="C26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D26" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" ht="31.5" hidden="1">
+      <c r="C27" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I26" s="11" t="s">
+      <c r="F27" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="J26" s="6"/>
-    </row>
-    <row r="27" spans="1:10" ht="31.5" hidden="1">
-      <c r="B27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="2" t="s">
+    </row>
+    <row r="28" spans="1:10" ht="15.75" hidden="1">
+      <c r="C28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="J28" s="6"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" hidden="1">
+      <c r="C29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="J27" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" hidden="1">
-      <c r="B28" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="J28" s="6"/>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" hidden="1">
-      <c r="B29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="J29" s="6"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" hidden="1">
       <c r="A30" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D30" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I30" s="20" t="s">
         <v>73</v>
-      </c>
-      <c r="I30" s="20" t="s">
-        <v>75</v>
       </c>
       <c r="J30" s="6"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" hidden="1">
       <c r="C31" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J31" s="6"/>
     </row>
     <row r="32" spans="1:10" ht="31.5" hidden="1">
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="9" t="s">
+      <c r="F32" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I32" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F32" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I32" s="11" t="s">
-        <v>59</v>
-      </c>
       <c r="J32" s="6"/>
     </row>
     <row r="33" spans="1:10" ht="31.5" hidden="1">
-      <c r="B33" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C33" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D33" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="I33" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J33" s="6"/>
     </row>
     <row r="34" spans="1:10" ht="31.5" hidden="1">
       <c r="C34" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J34" s="6"/>
     </row>
     <row r="35" spans="1:10" ht="63" hidden="1">
       <c r="A35" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D35" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" hidden="1">
+      <c r="C36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I36" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="J35" s="6"/>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" hidden="1">
-      <c r="B36" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="I36" s="11" t="s">
-        <v>78</v>
       </c>
       <c r="J36" s="6"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" hidden="1">
       <c r="C37" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J37" s="6"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" hidden="1">
       <c r="C38" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J38" s="6"/>
     </row>
     <row r="39" spans="1:10" ht="15.75" hidden="1">
       <c r="C39" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J39" s="6"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" hidden="1">
       <c r="A40" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J40" s="6"/>
     </row>
     <row r="41" spans="1:10" ht="15.75" hidden="1">
       <c r="C41" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" hidden="1">
       <c r="C42" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75" hidden="1">
       <c r="C43" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J43" s="6"/>
     </row>
     <row r="44" spans="1:10" ht="39.75" hidden="1" customHeight="1">
       <c r="C44" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J44" s="6"/>
     </row>
     <row r="45" spans="1:10" ht="15.75" hidden="1">
       <c r="C45" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J45" s="6"/>
     </row>
     <row r="46" spans="1:10" ht="15.75" hidden="1">
       <c r="C46" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J46" s="6"/>
     </row>
     <row r="47" spans="1:10" ht="9.75" hidden="1" customHeight="1">
       <c r="A47" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J47" s="6"/>
     </row>
     <row r="48" spans="1:10" ht="42" hidden="1" customHeight="1">
       <c r="A48" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15.75" hidden="1">
       <c r="C49" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J49" s="6"/>
     </row>
     <row r="50" spans="1:10" ht="31.5" hidden="1">
       <c r="C50" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J50" s="6"/>
     </row>
     <row r="51" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C51" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J51" s="6"/>
     </row>
     <row r="52" spans="1:10" ht="15.75" hidden="1">
       <c r="C52" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J52" s="6"/>
     </row>
     <row r="53" spans="1:10" ht="15.75" hidden="1">
       <c r="C53" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I53" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J53" s="6"/>
     </row>
     <row r="54" spans="1:10" ht="15.75" hidden="1">
       <c r="C54" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J54" s="6"/>
     </row>
     <row r="55" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="A55" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D55" s="24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J55" s="6"/>
     </row>
     <row r="56" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C56" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I56" s="25"/>
       <c r="J56" s="6"/>
     </row>
     <row r="57" spans="1:10" ht="15.75" hidden="1">
       <c r="C57" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J57" s="6"/>
     </row>
     <row r="58" spans="1:10" ht="24.95" customHeight="1">
       <c r="D58" s="31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="A59" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J59" s="6"/>
     </row>
     <row r="60" spans="1:10" ht="15.75" hidden="1">
       <c r="C60" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D60" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J60" s="6"/>
     </row>
     <row r="61" spans="1:10" ht="24.95" customHeight="1">
       <c r="D61" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C62" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J62" s="6"/>
     </row>
     <row r="63" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C63" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J63" s="6"/>
     </row>
     <row r="64" spans="1:10" ht="32.25" hidden="1" customHeight="1">
       <c r="C64" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J64" s="6"/>
     </row>
     <row r="65" spans="1:10" ht="24.95" customHeight="1">
+      <c r="B65" s="2" t="s">
+        <v>290</v>
+      </c>
       <c r="D65" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C66" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J66" s="6"/>
     </row>
@@ -3746,69 +3735,69 @@
         <v>44129</v>
       </c>
       <c r="D67" s="33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J67" s="6"/>
     </row>
     <row r="68" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="D68" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C69" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D69" s="31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="34.5" customHeight="1" thickBot="1">
       <c r="D70" s="31" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G70" s="19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I70" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J70" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="16.5" hidden="1" thickBot="1">
       <c r="C71" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G71" s="19"/>
       <c r="J71" s="6"/>
     </row>
     <row r="72" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C72" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J72" s="6"/>
     </row>
     <row r="73" spans="1:10" ht="42" hidden="1" customHeight="1" thickBot="1">
       <c r="C73" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G73" s="19"/>
       <c r="J73" s="6"/>
     </row>
     <row r="74" spans="1:10" ht="16.5" thickBot="1">
       <c r="D74" s="30" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G74" s="19"/>
     </row>
@@ -3817,11 +3806,11 @@
         <v>44129</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G75" s="19"/>
       <c r="I75" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="15.75" hidden="1">
@@ -3829,7 +3818,7 @@
         <v>44011</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G76" s="19"/>
     </row>
@@ -3838,7 +3827,7 @@
         <v>44011</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G77" s="19"/>
     </row>
@@ -3847,17 +3836,17 @@
         <v>44064</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G78" s="19"/>
     </row>
     <row r="79" spans="1:10" ht="20.100000000000001" hidden="1" customHeight="1">
       <c r="A79" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C79" s="36"/>
       <c r="D79" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G79" s="19"/>
     </row>
@@ -3866,7 +3855,7 @@
         <v>44029</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="15.75" hidden="1">
@@ -3874,10 +3863,10 @@
         <v>44075</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I81" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="18.75" hidden="1">
@@ -3885,47 +3874,47 @@
         <v>44075</v>
       </c>
       <c r="D82" s="60" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="15.75" hidden="1">
       <c r="C83" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D83" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="24.95" hidden="1" customHeight="1">
       <c r="A84" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I84" s="11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="24.95" customHeight="1">
       <c r="D85" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="32.25" hidden="1" thickBot="1">
       <c r="C86" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D86" s="32" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="24.95" customHeight="1">
       <c r="D87" s="26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I87" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="47.25" hidden="1">
@@ -3933,51 +3922,92 @@
         <v>44140</v>
       </c>
       <c r="D88" s="61" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="24.95" customHeight="1">
       <c r="D89" s="9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="24.95" customHeight="1">
       <c r="D90" s="9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="24.95" hidden="1" customHeight="1">
       <c r="C91" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="24.95" hidden="1" customHeight="1">
       <c r="C92" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D92" s="33" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="38.25" customHeight="1">
       <c r="D93" s="62" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="39.75" customHeight="1">
       <c r="D94" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="24.95" hidden="1" customHeight="1">
       <c r="C95" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D95" s="9" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="24.95" customHeight="1">
+      <c r="B96" s="2" t="s">
         <v>290</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D96" s="64" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" ht="31.5">
+      <c r="B97" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D97" s="65" t="s">
+        <v>292</v>
+      </c>
+      <c r="I97" s="64" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" ht="15.75">
+      <c r="B98" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D98" t="s">
+        <v>295</v>
+      </c>
+      <c r="I98" s="66" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B99" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="442" spans="1:10" ht="15.75">
@@ -4022,12 +4052,12 @@
     <row r="3" spans="1:4">
       <c r="A3" s="63"/>
       <c r="D3" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="D14" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -4054,54 +4084,54 @@
   <sheetData>
     <row r="1" spans="2:5">
       <c r="B1" s="57" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="31.5">
       <c r="B2" s="49" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="38" t="s">
         <v>192</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75">
       <c r="B7" s="43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="44" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="26.25">
       <c r="B15" s="47" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E15" s="48" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="12" customHeight="1">
       <c r="B16" s="46" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="12" customHeight="1">
@@ -4109,71 +4139,71 @@
     </row>
     <row r="18" spans="2:5" ht="12" customHeight="1">
       <c r="B18" s="45" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="12" customHeight="1">
       <c r="B19" s="45" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="12" customHeight="1">
       <c r="B20" s="45" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="12" customHeight="1">
       <c r="B21" s="45" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="12" customHeight="1">
       <c r="B22" s="45" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E22" s="44" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="12" customHeight="1">
       <c r="B23" s="45" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="12" customHeight="1">
       <c r="B24" s="45" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="12" customHeight="1">
       <c r="B25" s="45" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="12" customHeight="1">
       <c r="B26" s="45" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="12" customHeight="1">
       <c r="B27" s="45" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E27" s="38" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="12" customHeight="1">
       <c r="B28" s="45" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="12" customHeight="1">
       <c r="B29" s="45" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="12" customHeight="1">
@@ -4181,7 +4211,7 @@
     </row>
     <row r="31" spans="2:5" ht="12" customHeight="1">
       <c r="B31" s="46" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="12" customHeight="1">
@@ -4189,62 +4219,62 @@
     </row>
     <row r="33" spans="2:2" ht="12" customHeight="1">
       <c r="B33" s="45" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="12" customHeight="1">
       <c r="B34" s="45" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="12" customHeight="1">
       <c r="B35" s="45" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="12" customHeight="1">
       <c r="B36" s="45" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="12" customHeight="1">
       <c r="B37" s="45" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="12" customHeight="1">
       <c r="B38" s="45" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="12" customHeight="1">
       <c r="B39" s="45" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="12" customHeight="1">
       <c r="B40" s="45" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="12" customHeight="1">
       <c r="B41" s="45" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="12" customHeight="1">
       <c r="B42" s="45" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="2:2" ht="12" customHeight="1">
       <c r="B43" s="45" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="12" customHeight="1">
       <c r="B44" s="45" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -4289,29 +4319,29 @@
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="97.5" customHeight="1">
       <c r="A1" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>15</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>40</v>
-      </c>
       <c r="I1" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75">
@@ -4328,7 +4358,7 @@
         <v>44006</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F3" s="6"/>
       <c r="H3" s="6"/>
@@ -4349,7 +4379,7 @@
         <v>44014</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -4362,7 +4392,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F6" s="6"/>
       <c r="H6" s="6"/>
@@ -4910,56 +4940,56 @@
   <sheetData>
     <row r="2" spans="2:3" ht="18" thickBot="1">
       <c r="B2" s="29" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="16.5" thickTop="1"/>
     <row r="4" spans="2:3">
       <c r="B4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -4985,23 +5015,23 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="37" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="41" customFormat="1">
       <c r="A3" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>166</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>167</v>
-      </c>
-      <c r="C3" s="41" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B4" s="39">
         <v>44035</v>
@@ -5013,7 +5043,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B5" s="39">
         <v>44035</v>
@@ -5025,7 +5055,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B6" s="39">
         <v>44020</v>
@@ -5037,7 +5067,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B7" s="39">
         <v>43864</v>
@@ -5049,7 +5079,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B8" s="39">
         <v>43838</v>
@@ -5061,7 +5091,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B9" s="39">
         <v>43555</v>
@@ -5108,18 +5138,18 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75">
       <c r="F1" s="56" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="55" customFormat="1" ht="18.75">
       <c r="A7" s="55" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F7" s="55" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="K7" s="55" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -5127,13 +5157,13 @@
         <v>16099</v>
       </c>
       <c r="B8" s="53" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F8" s="54">
         <v>16099</v>
       </c>
       <c r="G8" s="53" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -5141,40 +5171,40 @@
     </row>
     <row r="10" spans="1:14" s="51" customFormat="1">
       <c r="A10" s="51" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C10" s="51" t="s">
+        <v>250</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="F10" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="G10" s="51" t="s">
         <v>251</v>
       </c>
-      <c r="F10" s="51" t="s">
-        <v>254</v>
-      </c>
-      <c r="G10" s="51" t="s">
-        <v>253</v>
-      </c>
       <c r="H10" s="51" t="s">
+        <v>250</v>
+      </c>
+      <c r="I10" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="K10" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="I10" s="51" t="s">
+      <c r="L10" s="51" t="s">
         <v>251</v>
       </c>
-      <c r="K10" s="51" t="s">
-        <v>254</v>
-      </c>
-      <c r="L10" s="51" t="s">
-        <v>253</v>
-      </c>
       <c r="M10" s="51" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N10" s="51" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -5183,57 +5213,57 @@
       <c r="C11" s="51"/>
       <c r="D11" s="51"/>
       <c r="F11" s="50" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G11" s="50" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H11" s="50" t="s">
+        <v>246</v>
+      </c>
+      <c r="K11" s="50" t="s">
         <v>248</v>
       </c>
-      <c r="K11" s="50" t="s">
-        <v>250</v>
-      </c>
       <c r="L11" s="50" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="M11" s="50" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="50" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D12" s="50">
         <v>255</v>
       </c>
       <c r="F12" s="50" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G12" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H12" s="50" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I12" s="50">
         <v>255</v>
       </c>
       <c r="K12" s="50" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="L12" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M12" s="50" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="N12" s="50">
         <v>255</v>
@@ -5241,25 +5271,25 @@
     </row>
     <row r="13" spans="1:14">
       <c r="F13" s="50" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G13" s="50" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H13" s="50" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I13" s="50">
         <v>8</v>
       </c>
       <c r="K13" s="50" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="L13" s="50" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="M13" s="50" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="N13" s="50">
         <v>8</v>
@@ -5267,25 +5297,25 @@
     </row>
     <row r="14" spans="1:14">
       <c r="F14" s="50" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G14" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H14" s="50" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I14" s="50">
         <v>2</v>
       </c>
       <c r="K14" s="50" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="L14" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M14" s="50" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="N14" s="50">
         <v>2</v>
@@ -5293,37 +5323,37 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="50" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D15" s="50">
         <v>255</v>
       </c>
       <c r="F15" s="50" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G15" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H15" s="50" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I15" s="50">
         <v>255</v>
       </c>
       <c r="K15" s="50" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="L15" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M15" s="50" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="N15" s="50">
         <v>255</v>
@@ -5331,54 +5361,54 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="50" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F16" s="50" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G16" s="50" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H16" s="50" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K16" s="50" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L16" s="50" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="M16" s="50" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="F17" s="50" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G17" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H17" s="50" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I17" s="50">
         <v>5</v>
       </c>
       <c r="K17" s="50" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L17" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M17" s="50" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="N17" s="50">
         <v>5</v>
@@ -5386,25 +5416,25 @@
     </row>
     <row r="18" spans="1:14">
       <c r="F18" s="50" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G18" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H18" s="50" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I18" s="50">
         <v>5</v>
       </c>
       <c r="K18" s="50" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="L18" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M18" s="50" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="N18" s="50">
         <v>5</v>
@@ -5412,25 +5442,25 @@
     </row>
     <row r="19" spans="1:14">
       <c r="F19" s="50" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G19" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H19" s="50" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I19" s="50">
         <v>5</v>
       </c>
       <c r="K19" s="50" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="L19" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M19" s="50" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="N19" s="50">
         <v>5</v>
@@ -5438,25 +5468,25 @@
     </row>
     <row r="20" spans="1:14">
       <c r="F20" s="50" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G20" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H20" s="50" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I20" s="50">
         <v>150</v>
       </c>
       <c r="K20" s="50" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="L20" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M20" s="50" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="N20" s="50">
         <v>150</v>
@@ -5464,54 +5494,54 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="50" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C21" s="50" t="s">
+        <v>224</v>
+      </c>
+      <c r="F21" s="50" t="s">
         <v>226</v>
       </c>
-      <c r="F21" s="50" t="s">
-        <v>228</v>
-      </c>
       <c r="G21" s="50" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H21" s="50" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K21" s="50" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="L21" s="50" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M21" s="50" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="1:14">
       <c r="F22" s="50" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G22" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H22" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I22" s="50">
         <v>25</v>
       </c>
       <c r="K22" s="50" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="L22" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M22" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="N22" s="50">
         <v>25</v>
@@ -5519,86 +5549,86 @@
     </row>
     <row r="23" spans="1:14">
       <c r="F23" s="50" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G23" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H23" s="50" t="s">
+        <v>219</v>
+      </c>
+      <c r="K23" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="K23" s="50" t="s">
-        <v>223</v>
-      </c>
       <c r="L23" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="M23" s="50" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="50" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C24" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="F24" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="F24" s="50" t="s">
-        <v>220</v>
-      </c>
       <c r="G24" s="50" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H24" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="K24" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="K24" s="50" t="s">
-        <v>220</v>
-      </c>
       <c r="L24" s="50" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="M24" s="50" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="50" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C25" s="50" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D25" s="50">
         <v>255</v>
       </c>
       <c r="F25" s="50" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G25" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H25" s="50" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I25" s="50">
         <v>255</v>
       </c>
       <c r="K25" s="50" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="L25" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M25" s="50" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="N25" s="50">
         <v>255</v>
@@ -5606,37 +5636,37 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="50" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C26" s="50" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D26" s="50">
         <v>801</v>
       </c>
       <c r="F26" s="50" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G26" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H26" s="50" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I26" s="50">
         <v>801</v>
       </c>
       <c r="K26" s="50" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="L26" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M26" s="50" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="N26" s="50">
         <v>801</v>
@@ -5644,37 +5674,37 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="50" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D27" s="50">
         <v>255</v>
       </c>
       <c r="F27" s="50" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G27" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H27" s="50" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I27" s="50">
         <v>255</v>
       </c>
       <c r="K27" s="50" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L27" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M27" s="50" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="N27" s="50">
         <v>255</v>
@@ -5682,37 +5712,37 @@
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="50" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C28" s="50" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D28" s="50">
         <v>12</v>
       </c>
       <c r="F28" s="50" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G28" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H28" s="50" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I28" s="50">
         <v>12</v>
       </c>
       <c r="K28" s="50" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L28" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M28" s="50" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N28" s="50">
         <v>12</v>
@@ -5720,66 +5750,66 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="50" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F29" s="50" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G29" s="50" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H29" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K29" s="50" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="L29" s="50" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="M29" s="50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="50" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B30" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D30" s="50">
         <v>255</v>
       </c>
       <c r="F30" s="50" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G30" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H30" s="50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I30" s="50">
         <v>255</v>
       </c>
       <c r="K30" s="50" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="L30" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M30" s="50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="N30" s="50">
         <v>255</v>
@@ -5787,57 +5817,57 @@
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="50" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B31" s="50" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C31" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="F31" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="F31" s="50" t="s">
-        <v>204</v>
-      </c>
       <c r="G31" s="50" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H31" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="K31" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="K31" s="50" t="s">
-        <v>204</v>
-      </c>
       <c r="L31" s="50" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="M31" s="50" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="58" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B32" s="58" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C32" s="58" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D32" s="50">
         <v>1</v>
       </c>
       <c r="F32" s="59" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="K32" s="50" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="L32" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M32" s="50" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="N32" s="50">
         <v>1</v>
@@ -5845,24 +5875,24 @@
     </row>
     <row r="33" spans="11:14">
       <c r="K33" s="50" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L33" s="50" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="M33" s="50" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="34" spans="11:14">
       <c r="K34" s="50" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="L34" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M34" s="50" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="N34" s="50">
         <v>6</v>
@@ -5870,13 +5900,13 @@
     </row>
     <row r="35" spans="11:14">
       <c r="K35" s="50" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L35" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M35" s="50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="N35" s="50">
         <v>255</v>
@@ -5884,13 +5914,13 @@
     </row>
     <row r="36" spans="11:14">
       <c r="K36" s="50" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L36" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M36" s="50" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="N36" s="50">
         <v>255</v>

</xml_diff>

<commit_message>
Move unused functions to "deprecatedFunctions.js"
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site ToDos.xlsx
+++ b/Docs/SZ JS site ToDos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\ShoreZoneDev_Dec2023\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9ECBB0-5547-4150-8058-3645DC6A7006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C825383-6E53-4A4C-9E65-312DC2118798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="736" xr2:uid="{E79FFD7B-6BA3-4D36-BD34-AA94A5290057}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="to do" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'to do'!$A$1:$I$442</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'to do'!$A$1:$I$443</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
     <author>Jim</author>
   </authors>
   <commentList>
-    <comment ref="D59" authorId="0" shapeId="0" xr:uid="{8BE8D365-4202-41D2-8F8C-D33F0829961C}">
+    <comment ref="D60" authorId="0" shapeId="0" xr:uid="{8BE8D365-4202-41D2-8F8C-D33F0829961C}">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D62" authorId="0" shapeId="0" xr:uid="{F4FBDC21-E4A6-4952-845B-FA2AABFC0B3B}">
+    <comment ref="D63" authorId="0" shapeId="0" xr:uid="{F4FBDC21-E4A6-4952-845B-FA2AABFC0B3B}">
       <text>
         <r>
           <rPr>
@@ -68,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D70" authorId="0" shapeId="0" xr:uid="{E4E7D546-5501-4B22-B4CB-2D44BAC24129}">
+    <comment ref="D71" authorId="0" shapeId="0" xr:uid="{E4E7D546-5501-4B22-B4CB-2D44BAC24129}">
       <text>
         <r>
           <rPr>
@@ -100,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D98" authorId="0" shapeId="0" xr:uid="{3B37A8B9-B1DA-48B6-B3C3-ED336BFA71E9}">
+    <comment ref="D99" authorId="0" shapeId="0" xr:uid="{3B37A8B9-B1DA-48B6-B3C3-ED336BFA71E9}">
       <text>
         <r>
           <rPr>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="160">
   <si>
     <t>and on point/unit popup</t>
   </si>
@@ -950,6 +950,9 @@
   </si>
   <si>
     <t>Add "clear filters" button?</t>
+  </si>
+  <si>
+    <t>IDEA:  Filter for Survey &amp; Survey Year legend display?  (incl. current extent)</t>
   </si>
 </sst>
 </file>
@@ -1340,9 +1343,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1380,7 +1383,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1486,7 +1489,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1628,7 +1631,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1637,13 +1640,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CE3068-557B-489F-8687-397203D47683}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:J442"/>
+  <dimension ref="A1:J443"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B100" sqref="B100"/>
+      <selection pane="bottomRight" activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1"/>
@@ -2323,367 +2326,373 @@
       </c>
       <c r="J57" s="6"/>
     </row>
-    <row r="58" spans="1:10" ht="24.95" customHeight="1">
-      <c r="D58" s="27" t="s">
+    <row r="58" spans="1:10" ht="15.75">
+      <c r="D58" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="J58" s="6"/>
+    </row>
+    <row r="59" spans="1:10" ht="24.95" customHeight="1">
+      <c r="D59" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="I58" s="11" t="s">
+      <c r="I59" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="24.95" hidden="1" customHeight="1">
-      <c r="A59" s="6" t="s">
+    <row r="60" spans="1:10" ht="24.95" hidden="1" customHeight="1">
+      <c r="A60" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D59" s="9" t="s">
+      <c r="D60" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="J59" s="6"/>
-    </row>
-    <row r="60" spans="1:10" ht="15.75" hidden="1">
-      <c r="C60" s="2" t="s">
+      <c r="J60" s="6"/>
+    </row>
+    <row r="61" spans="1:10" ht="15.75" hidden="1">
+      <c r="C61" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D60" s="23" t="s">
+      <c r="D61" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="J60" s="6"/>
-    </row>
-    <row r="61" spans="1:10" ht="24.95" customHeight="1">
-      <c r="D61" s="9" t="s">
+      <c r="J61" s="6"/>
+    </row>
+    <row r="62" spans="1:10" ht="24.95" customHeight="1">
+      <c r="D62" s="9" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" ht="24.95" hidden="1" customHeight="1">
-      <c r="C62" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="J62" s="6"/>
     </row>
     <row r="63" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C63" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J63" s="6"/>
     </row>
-    <row r="64" spans="1:10" ht="32.25" hidden="1" customHeight="1">
+    <row r="64" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C64" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D64" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="J64" s="6"/>
+    </row>
+    <row r="65" spans="1:10" ht="32.25" hidden="1" customHeight="1">
+      <c r="C65" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="J64" s="6"/>
-    </row>
-    <row r="65" spans="1:10" ht="24.95" customHeight="1">
-      <c r="B65" s="2" t="s">
+      <c r="J65" s="6"/>
+    </row>
+    <row r="66" spans="1:10" ht="24.95" customHeight="1">
+      <c r="B66" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D65" s="9" t="s">
+      <c r="D66" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="24.95" hidden="1" customHeight="1">
-      <c r="C66" s="2" t="s">
+    <row r="67" spans="1:10" ht="24.95" hidden="1" customHeight="1">
+      <c r="C67" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D66" s="9" t="s">
+      <c r="D67" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="J66" s="6"/>
-    </row>
-    <row r="67" spans="1:10" ht="24.95" hidden="1" customHeight="1">
-      <c r="C67" s="31">
+      <c r="J67" s="6"/>
+    </row>
+    <row r="68" spans="1:10" ht="24.95" hidden="1" customHeight="1">
+      <c r="C68" s="31">
         <v>44129</v>
       </c>
-      <c r="D67" s="29" t="s">
+      <c r="D68" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="J67" s="6"/>
-    </row>
-    <row r="68" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="D68" s="9" t="s">
+      <c r="J68" s="6"/>
+    </row>
+    <row r="69" spans="1:10" ht="20.100000000000001" customHeight="1">
+      <c r="D69" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="24.95" hidden="1" customHeight="1">
-      <c r="C69" s="2" t="s">
+    <row r="70" spans="1:10" ht="24.95" hidden="1" customHeight="1">
+      <c r="C70" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D69" s="27" t="s">
+      <c r="D70" s="27" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="34.5" customHeight="1" thickBot="1">
-      <c r="D70" s="27" t="s">
+    <row r="71" spans="1:10" ht="34.5" customHeight="1" thickBot="1">
+      <c r="D71" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G70" s="19" t="s">
+      <c r="G71" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="I70" s="11" t="s">
+      <c r="I71" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="J70" s="11" t="s">
+      <c r="J71" s="11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="16.5" hidden="1" thickBot="1">
-      <c r="C71" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="G71" s="19"/>
-      <c r="J71" s="6"/>
-    </row>
-    <row r="72" spans="1:10" ht="24.95" hidden="1" customHeight="1">
+    <row r="72" spans="1:10" ht="16.5" hidden="1" thickBot="1">
       <c r="C72" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D72" s="25" t="s">
-        <v>122</v>
-      </c>
+      <c r="D72" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G72" s="19"/>
       <c r="J72" s="6"/>
     </row>
-    <row r="73" spans="1:10" ht="42" hidden="1" customHeight="1" thickBot="1">
+    <row r="73" spans="1:10" ht="24.95" hidden="1" customHeight="1">
       <c r="C73" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D73" s="9" t="s">
+      <c r="D73" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="J73" s="6"/>
+    </row>
+    <row r="74" spans="1:10" ht="42" hidden="1" customHeight="1" thickBot="1">
+      <c r="C74" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D74" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="G73" s="19"/>
-      <c r="J73" s="6"/>
-    </row>
-    <row r="74" spans="1:10" ht="16.5" thickBot="1">
-      <c r="D74" s="26" t="s">
+      <c r="G74" s="19"/>
+      <c r="J74" s="6"/>
+    </row>
+    <row r="75" spans="1:10" ht="16.5" thickBot="1">
+      <c r="D75" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="G74" s="19"/>
-    </row>
-    <row r="75" spans="1:10" ht="20.100000000000001" hidden="1" customHeight="1">
-      <c r="C75" s="31">
+      <c r="G75" s="19"/>
+    </row>
+    <row r="76" spans="1:10" ht="20.100000000000001" hidden="1" customHeight="1">
+      <c r="C76" s="31">
         <v>44129</v>
       </c>
-      <c r="D75" s="9" t="s">
+      <c r="D76" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G75" s="19"/>
-      <c r="I75" s="11" t="s">
+      <c r="G76" s="19"/>
+      <c r="I76" s="11" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" ht="15.75" hidden="1">
-      <c r="C76" s="31">
-        <v>44011</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="G76" s="19"/>
     </row>
     <row r="77" spans="1:10" ht="15.75" hidden="1">
       <c r="C77" s="31">
         <v>44011</v>
       </c>
       <c r="D77" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G77" s="19"/>
+    </row>
+    <row r="78" spans="1:10" ht="15.75" hidden="1">
+      <c r="C78" s="31">
+        <v>44011</v>
+      </c>
+      <c r="D78" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G77" s="19"/>
-    </row>
-    <row r="78" spans="1:10" ht="20.100000000000001" hidden="1" customHeight="1">
-      <c r="C78" s="31">
+      <c r="G78" s="19"/>
+    </row>
+    <row r="79" spans="1:10" ht="20.100000000000001" hidden="1" customHeight="1">
+      <c r="C79" s="31">
         <v>44064</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="D79" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="G78" s="19"/>
-    </row>
-    <row r="79" spans="1:10" ht="20.100000000000001" hidden="1" customHeight="1">
-      <c r="A79" s="6" t="s">
+      <c r="G79" s="19"/>
+    </row>
+    <row r="80" spans="1:10" ht="20.100000000000001" hidden="1" customHeight="1">
+      <c r="A80" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C79" s="31"/>
-      <c r="D79" s="9" t="s">
+      <c r="C80" s="31"/>
+      <c r="D80" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="G79" s="19"/>
-    </row>
-    <row r="80" spans="1:10" ht="39" hidden="1" customHeight="1">
-      <c r="C80" s="31">
+      <c r="G80" s="19"/>
+    </row>
+    <row r="81" spans="1:9" ht="39" hidden="1" customHeight="1">
+      <c r="C81" s="31">
         <v>44029</v>
       </c>
-      <c r="D80" s="9" t="s">
+      <c r="D81" s="9" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="15.75" hidden="1">
-      <c r="C81" s="31">
-        <v>44075</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="I81" s="11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="18.75" hidden="1">
+    <row r="82" spans="1:9" ht="15.75" hidden="1">
       <c r="C82" s="31">
         <v>44075</v>
       </c>
-      <c r="D82" s="32" t="s">
+      <c r="D82" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="I82" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="18.75" hidden="1">
+      <c r="C83" s="31">
+        <v>44075</v>
+      </c>
+      <c r="D83" s="32" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15.75" hidden="1">
-      <c r="C83" s="31" t="s">
+    <row r="84" spans="1:9" ht="15.75" hidden="1">
+      <c r="C84" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D84" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="24.95" hidden="1" customHeight="1">
-      <c r="A84" s="6" t="s">
+    <row r="85" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+      <c r="A85" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D84" s="9" t="s">
+      <c r="D85" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="I84" s="11" t="s">
+      <c r="I85" s="11" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="24.95" customHeight="1">
-      <c r="D85" s="9" t="s">
+    <row r="86" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D86" s="9" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="32.25" hidden="1" thickBot="1">
-      <c r="C86" s="2" t="s">
+    <row r="87" spans="1:9" ht="32.25" hidden="1" thickBot="1">
+      <c r="C87" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D86" s="28" t="s">
+      <c r="D87" s="28" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="24.95" customHeight="1">
-      <c r="D87" s="23" t="s">
+    <row r="88" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D88" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="I87" s="11" t="s">
+      <c r="I88" s="11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="47.25" hidden="1">
-      <c r="C88" s="31">
+    <row r="89" spans="1:9" ht="47.25" hidden="1">
+      <c r="C89" s="31">
         <v>44140</v>
       </c>
-      <c r="D88" s="33" t="s">
+      <c r="D89" s="33" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="24.95" customHeight="1">
-      <c r="D89" s="9" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="24.95" customHeight="1">
       <c r="D90" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D91" s="9" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="24.95" hidden="1" customHeight="1">
-      <c r="C91" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D91" s="9" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="24.95" hidden="1" customHeight="1">
       <c r="C92" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D92" s="29" t="s">
+      <c r="D92" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+      <c r="C93" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D93" s="29" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="38.25" customHeight="1">
-      <c r="D93" s="34" t="s">
+    <row r="94" spans="1:9" ht="38.25" customHeight="1">
+      <c r="D94" s="34" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="39.75" customHeight="1">
-      <c r="D94" s="9" t="s">
+    <row r="95" spans="1:9" ht="39.75" customHeight="1">
+      <c r="D95" s="9" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="24.95" hidden="1" customHeight="1">
-      <c r="C95" s="2" t="s">
+    <row r="96" spans="1:9" ht="24.95" hidden="1" customHeight="1">
+      <c r="C96" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D95" s="9" t="s">
+      <c r="D96" s="9" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="24.95" customHeight="1">
-      <c r="B96" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D96" s="35" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="97" spans="2:9" ht="31.5">
+    <row r="97" spans="2:9" ht="24.95" customHeight="1">
       <c r="B97" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D97" s="36" t="s">
-        <v>153</v>
-      </c>
-      <c r="I97" s="35" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="98" spans="2:9" ht="15.75">
+      <c r="C97" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D97" s="35" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" ht="31.5">
       <c r="B98" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D98" t="s">
-        <v>156</v>
-      </c>
-      <c r="I98" s="37" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="99" spans="2:9" ht="24.95" customHeight="1">
+      <c r="D98" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="I98" s="35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" ht="15.75">
       <c r="B99" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D99" s="9" t="s">
+      <c r="D99" t="s">
+        <v>156</v>
+      </c>
+      <c r="I99" s="37" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B100" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D100" s="9" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="442" spans="1:10" ht="15.75">
-      <c r="A442" s="2"/>
-      <c r="J442" s="6"/>
+    <row r="443" spans="1:10" ht="15.75">
+      <c r="A443" s="2"/>
+      <c r="J443" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I442" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
+  <autoFilter ref="A1:I443" xr:uid="{5181A141-DBC1-468E-AB21-28EAEB759146}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
@@ -2695,7 +2704,7 @@
     <hyperlink ref="J27" r:id="rId1" display="https://github.com/SitePen/dgrid/blob/master/doc/components/mixins/Selection.md" xr:uid="{B02003EC-0D72-4D32-86B5-BCB2E4740BDA}"/>
     <hyperlink ref="I33" r:id="rId2" xr:uid="{D7280C89-055C-482B-859C-78DDF371D8BE}"/>
     <hyperlink ref="I34" r:id="rId3" location="release_notes_08_23_2018" display="Can no longer disable showing of &quot;more videos&quot; when video is paused" xr:uid="{75869B48-9B1F-4352-8C34-D2F55186219A}"/>
-    <hyperlink ref="G70" r:id="rId4" display="https://www.google.com/search?sxsrf=ALeKk03fRI45rxW7duPejqDWYRNo315xnA%3A1589067316875Google search" xr:uid="{B59445F6-07F3-4CDD-950F-C113A43BEE63}"/>
+    <hyperlink ref="G71" r:id="rId4" display="https://www.google.com/search?sxsrf=ALeKk03fRI45rxW7duPejqDWYRNo315xnA%3A1589067316875Google search" xr:uid="{B59445F6-07F3-4CDD-950F-C113A43BEE63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId5"/>

</xml_diff>